<commit_message>
Auto push 2023-03-23 18:00:22.21
</commit_message>
<xml_diff>
--- a/project/CheeYoonMovie.xlsx
+++ b/project/CheeYoonMovie.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12240" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12240" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="8" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="214">
   <si>
     <t>이용자 권한과 기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -307,13 +307,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MLoginService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>main/main.jsp</t>
-  </si>
-  <si>
     <t>로그아웃</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -322,14 +315,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>logout.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MLogoutService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>정보수정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -338,22 +323,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>modifyView.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>modify.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>main/main.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MModifyService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MAllViewService.java</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -362,9 +331,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>withdrawal.do</t>
-  </si>
-  <si>
     <t>회원탈퇴</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -373,14 +339,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MWithdrawalService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>main/main.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>boardWriteView.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -389,90 +347,70 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>boardModifyView.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardModify.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardDelete.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardReplyView.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardReply.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardWriteService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardModifyService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardDeleteService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardReplyViewService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardReplyService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardDto 속성들</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardDto 속성들</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardDto 속성들</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardModifyViewService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">member/mAllView.jsp </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>boardList.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boardContent.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boardModifyView.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boardModify.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boardDelete.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boardReplyView.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boardReply.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MemberDto속성들</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardWriteService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardListService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardContentService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardModifyService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardDeleteService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardReplyViewService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardReplyService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardDto 속성들</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardDto 속성들</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardDto 속성들</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardModifyViewService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">member/mAllView.jsp </t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>boardList.do</t>
-  </si>
-  <si>
-    <t>boardList.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -501,14 +439,6 @@
   </si>
   <si>
     <t xml:space="preserve">fileBoard/boardWrite.jsp </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">fileBoard/boardList.jsp </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">fileBoard/boardContent.jsp </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -685,18 +615,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>searchMovie.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>movieName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SearchMovie.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>userId, userPw</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -705,10 +623,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>boardId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>영화 등록</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -729,18 +643,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>검색 결과페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>searchResult.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>searchResult.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>loginView.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -761,7 +663,130 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>main/main.jsp</t>
+    <t>RegisterService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>loginView.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserIdConfirmService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userEmail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user/userEmailConfirm.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ppt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMDb 헤더색상 18 18 18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMDb 카드리스트2  44 44 44</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMDb 카드리스트1  26 26 26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리얼블랙 0 0 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100 100 100   64 64 64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 0 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>75 75 75   4b 4b 4b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>44 44 44 2c2c2c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>130 130 130   82 82 82</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20월요일 dao dto 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21화요일 회원가입,로그인페이지생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22수요일 메인페이지css조정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 그라데이션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">bg-dark 활용하자 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>searchName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Search.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main/search.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserLogoutService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserDto속성들</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserLoginService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main.do</t>
+  </si>
+  <si>
+    <t>logout.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>modifyView.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -769,91 +794,79 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RegisterService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>loginView.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UserIdConfirmService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userEmail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user/userEmailConfirm.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ppt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IMDb 헤더색상 18 18 18</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IMDb 카드리스트2  44 44 44</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IMDb 카드리스트1  26 26 26</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>리얼블랙 0 0 0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100 100 100   64 64 64</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 0 0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>75 75 75   4b 4b 4b</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>44 44 44 2c2c2c</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>130 130 130   82 82 82</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>배경</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20월요일 dao dto 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>21화요일 회원가입,로그인페이지생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>22수요일 메인페이지css조정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그인 그라데이션</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">bg-dark 활용하자 </t>
+    <t>modify.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserModifyService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>withdrawal.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserWithdrawalService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardList.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardListService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pageNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardContentService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>board/boardContent.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>board/boardList.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>댓글 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>commentWrite.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>commentDto속성들</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardNo,pageNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CommentWriteService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardContent.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardContent.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1391,7 +1404,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1545,23 +1558,140 @@
     <xf numFmtId="0" fontId="11" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1569,163 +1699,43 @@
     <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2096,41 +2106,41 @@
     <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="88" t="s">
-        <v>128</v>
-      </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
+      <c r="B2" s="79" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="80"/>
+      <c r="O3" s="80"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
@@ -2175,32 +2185,32 @@
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20"/>
-      <c r="C6" s="90" t="s">
+      <c r="C6" s="81" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="39"/>
-      <c r="E6" s="92" t="s">
+      <c r="E6" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="94" t="s">
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="83"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="84"/>
+      <c r="L6" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="M6" s="92"/>
-      <c r="N6" s="92"/>
-      <c r="O6" s="92"/>
+      <c r="M6" s="83"/>
+      <c r="N6" s="83"/>
+      <c r="O6" s="83"/>
       <c r="P6" s="21"/>
       <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="91"/>
+      <c r="C7" s="82"/>
       <c r="D7" s="22"/>
       <c r="E7" s="13">
         <v>20</v>
@@ -2300,7 +2310,7 @@
     <row r="11" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="84" t="s">
+      <c r="C11" s="86" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="10"/>
@@ -2321,7 +2331,7 @@
     <row r="12" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="84"/>
+      <c r="C12" s="86"/>
       <c r="D12" s="10"/>
       <c r="E12" s="8"/>
       <c r="F12" s="6"/>
@@ -2359,7 +2369,7 @@
     <row r="14" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="87" t="s">
+      <c r="C14" s="78" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="10"/>
@@ -2380,7 +2390,7 @@
     <row r="15" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="87"/>
+      <c r="C15" s="78"/>
       <c r="D15" s="10"/>
       <c r="E15" s="8"/>
       <c r="F15" s="6"/>
@@ -2418,7 +2428,7 @@
     <row r="17" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="84" t="s">
+      <c r="C17" s="86" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="10"/>
@@ -2439,7 +2449,7 @@
     <row r="18" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="84"/>
+      <c r="C18" s="86"/>
       <c r="D18" s="10"/>
       <c r="E18" s="6"/>
       <c r="F18" s="8"/>
@@ -2498,7 +2508,7 @@
     <row r="21" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="85" t="s">
+      <c r="C21" s="88" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="10"/>
@@ -2519,7 +2529,7 @@
     <row r="22" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="85"/>
+      <c r="C22" s="88"/>
       <c r="D22" s="10"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -2557,7 +2567,7 @@
     <row r="24" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="85" t="s">
+      <c r="C24" s="88" t="s">
         <v>16</v>
       </c>
       <c r="D24" s="10"/>
@@ -2578,7 +2588,7 @@
     <row r="25" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="85"/>
+      <c r="C25" s="88"/>
       <c r="D25" s="10"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -2616,8 +2626,8 @@
     <row r="27" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="85" t="s">
-        <v>129</v>
+      <c r="C27" s="88" t="s">
+        <v>111</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="6"/>
@@ -2637,7 +2647,7 @@
     <row r="28" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="85"/>
+      <c r="C28" s="88"/>
       <c r="D28" s="10"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -2675,8 +2685,8 @@
     <row r="30" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="85" t="s">
-        <v>130</v>
+      <c r="C30" s="88" t="s">
+        <v>112</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="6"/>
@@ -2696,7 +2706,7 @@
     <row r="31" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="85"/>
+      <c r="C31" s="88"/>
       <c r="D31" s="10"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -2734,8 +2744,8 @@
     <row r="33" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="85" t="s">
-        <v>131</v>
+      <c r="C33" s="88" t="s">
+        <v>113</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="6"/>
@@ -2755,7 +2765,7 @@
     <row r="34" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="6"/>
-      <c r="C34" s="85"/>
+      <c r="C34" s="88"/>
       <c r="D34" s="10"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -2833,7 +2843,7 @@
     <row r="38" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
       <c r="B38" s="6"/>
-      <c r="C38" s="86" t="s">
+      <c r="C38" s="89" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="10"/>
@@ -2854,7 +2864,7 @@
     <row r="39" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
       <c r="B39" s="6"/>
-      <c r="C39" s="86"/>
+      <c r="C39" s="89"/>
       <c r="D39" s="10"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
@@ -2892,7 +2902,7 @@
     <row r="41" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="86" t="s">
+      <c r="C41" s="89" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="10"/>
@@ -2913,7 +2923,7 @@
     <row r="42" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16"/>
       <c r="B42" s="6"/>
-      <c r="C42" s="86"/>
+      <c r="C42" s="89"/>
       <c r="D42" s="10"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
@@ -2951,8 +2961,8 @@
     <row r="44" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="86" t="s">
-        <v>155</v>
+      <c r="C44" s="89" t="s">
+        <v>137</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="6"/>
@@ -2972,7 +2982,7 @@
     <row r="45" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="16"/>
       <c r="B45" s="6"/>
-      <c r="C45" s="86"/>
+      <c r="C45" s="89"/>
       <c r="D45" s="10"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
@@ -3010,8 +3020,8 @@
     <row r="47" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="86" t="s">
-        <v>132</v>
+      <c r="C47" s="89" t="s">
+        <v>114</v>
       </c>
       <c r="D47" s="10"/>
       <c r="E47" s="6"/>
@@ -3031,7 +3041,7 @@
     <row r="48" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="16"/>
       <c r="B48" s="6"/>
-      <c r="C48" s="86"/>
+      <c r="C48" s="89"/>
       <c r="D48" s="10"/>
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
@@ -3069,8 +3079,8 @@
     <row r="50" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="86" t="s">
-        <v>156</v>
+      <c r="C50" s="89" t="s">
+        <v>138</v>
       </c>
       <c r="D50" s="10"/>
       <c r="E50" s="6"/>
@@ -3090,7 +3100,7 @@
     <row r="51" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="16"/>
       <c r="B51" s="6"/>
-      <c r="C51" s="86"/>
+      <c r="C51" s="89"/>
       <c r="D51" s="10"/>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
@@ -3149,8 +3159,8 @@
     <row r="54" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16"/>
       <c r="B54" s="6"/>
-      <c r="C54" s="80" t="s">
-        <v>133</v>
+      <c r="C54" s="87" t="s">
+        <v>115</v>
       </c>
       <c r="D54" s="10"/>
       <c r="E54" s="6"/>
@@ -3170,7 +3180,7 @@
     <row r="55" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="80"/>
+      <c r="C55" s="87"/>
       <c r="D55" s="10"/>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
@@ -3208,8 +3218,8 @@
     <row r="57" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="16"/>
       <c r="B57" s="6"/>
-      <c r="C57" s="80" t="s">
-        <v>134</v>
+      <c r="C57" s="87" t="s">
+        <v>116</v>
       </c>
       <c r="D57" s="10"/>
       <c r="E57" s="6"/>
@@ -3229,7 +3239,7 @@
     <row r="58" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="80"/>
+      <c r="C58" s="87"/>
       <c r="D58" s="10"/>
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
@@ -3267,8 +3277,8 @@
     <row r="60" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="16"/>
       <c r="B60" s="6"/>
-      <c r="C60" s="80" t="s">
-        <v>154</v>
+      <c r="C60" s="87" t="s">
+        <v>136</v>
       </c>
       <c r="D60" s="10"/>
       <c r="E60" s="6"/>
@@ -3288,7 +3298,7 @@
     <row r="61" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="16"/>
       <c r="B61" s="6"/>
-      <c r="C61" s="80"/>
+      <c r="C61" s="87"/>
       <c r="D61" s="10"/>
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
@@ -3326,8 +3336,8 @@
     <row r="63" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="16"/>
       <c r="B63" s="6"/>
-      <c r="C63" s="80" t="s">
-        <v>153</v>
+      <c r="C63" s="87" t="s">
+        <v>135</v>
       </c>
       <c r="D63" s="10"/>
       <c r="E63" s="6"/>
@@ -3347,7 +3357,7 @@
     <row r="64" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="16"/>
       <c r="B64" s="6"/>
-      <c r="C64" s="80"/>
+      <c r="C64" s="87"/>
       <c r="D64" s="10"/>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
@@ -3385,8 +3395,8 @@
     <row r="66" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="16"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="80" t="s">
-        <v>152</v>
+      <c r="C66" s="87" t="s">
+        <v>134</v>
       </c>
       <c r="D66" s="10"/>
       <c r="E66" s="6"/>
@@ -3406,7 +3416,7 @@
     <row r="67" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="16"/>
       <c r="B67" s="6"/>
-      <c r="C67" s="80"/>
+      <c r="C67" s="87"/>
       <c r="D67" s="10"/>
       <c r="E67" s="6"/>
       <c r="F67" s="6"/>
@@ -3444,8 +3454,8 @@
     <row r="69" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="80" t="s">
-        <v>151</v>
+      <c r="C69" s="87" t="s">
+        <v>133</v>
       </c>
       <c r="D69" s="10"/>
       <c r="E69" s="6"/>
@@ -3465,7 +3475,7 @@
     <row r="70" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="16"/>
       <c r="B70" s="6"/>
-      <c r="C70" s="80"/>
+      <c r="C70" s="87"/>
       <c r="D70" s="10"/>
       <c r="E70" s="6"/>
       <c r="F70" s="6"/>
@@ -3503,7 +3513,7 @@
     <row r="72" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16"/>
       <c r="B72" s="6"/>
-      <c r="C72" s="81" t="s">
+      <c r="C72" s="91" t="s">
         <v>56</v>
       </c>
       <c r="D72" s="7"/>
@@ -3524,7 +3534,7 @@
     <row r="73" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="16"/>
       <c r="B73" s="6"/>
-      <c r="C73" s="81"/>
+      <c r="C73" s="91"/>
       <c r="D73" s="7"/>
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
@@ -3543,8 +3553,8 @@
     <row r="74" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16"/>
       <c r="B74" s="6"/>
-      <c r="C74" s="83" t="s">
-        <v>127</v>
+      <c r="C74" s="93" t="s">
+        <v>109</v>
       </c>
       <c r="D74" s="7"/>
       <c r="E74" s="6"/>
@@ -3559,62 +3569,62 @@
       <c r="N74" s="6"/>
       <c r="O74" s="38"/>
       <c r="P74" s="16"/>
-      <c r="R74" s="54"/>
-      <c r="S74" s="54"/>
-      <c r="T74" s="54"/>
-      <c r="U74" s="54"/>
-      <c r="V74" s="54"/>
-      <c r="W74" s="54"/>
-      <c r="X74" s="54"/>
-      <c r="Y74" s="54"/>
-      <c r="Z74" s="54"/>
-      <c r="AA74" s="54"/>
-      <c r="AB74" s="54"/>
-      <c r="AC74" s="54"/>
-      <c r="AD74" s="54"/>
-      <c r="AE74" s="54"/>
-      <c r="AF74" s="54"/>
-      <c r="AG74" s="54"/>
-      <c r="AH74" s="54"/>
-      <c r="AI74" s="54"/>
-      <c r="AJ74" s="54"/>
-      <c r="AK74" s="54"/>
-      <c r="AL74" s="54"/>
-      <c r="AM74" s="54"/>
-      <c r="AN74" s="54"/>
-      <c r="AO74" s="54"/>
-      <c r="AP74" s="54"/>
-      <c r="AQ74" s="54"/>
-      <c r="AR74" s="54"/>
-      <c r="AS74" s="54"/>
-      <c r="AT74" s="54"/>
-      <c r="AU74" s="54"/>
-      <c r="AV74" s="54"/>
-      <c r="AW74" s="54"/>
-      <c r="AX74" s="54"/>
-      <c r="AY74" s="54"/>
-      <c r="AZ74" s="54"/>
-      <c r="BA74" s="54"/>
-      <c r="BB74" s="54"/>
-      <c r="BC74" s="54"/>
-      <c r="BD74" s="54"/>
-      <c r="BE74" s="54"/>
-      <c r="BF74" s="54"/>
-      <c r="BG74" s="54"/>
-      <c r="BH74" s="54"/>
-      <c r="BI74" s="54"/>
-      <c r="BJ74" s="54"/>
-      <c r="BK74" s="54"/>
-      <c r="BL74" s="54"/>
-      <c r="BM74" s="54"/>
-      <c r="BN74" s="54"/>
-      <c r="BO74" s="54"/>
-      <c r="BP74" s="54"/>
+      <c r="R74" s="53"/>
+      <c r="S74" s="53"/>
+      <c r="T74" s="53"/>
+      <c r="U74" s="53"/>
+      <c r="V74" s="53"/>
+      <c r="W74" s="53"/>
+      <c r="X74" s="53"/>
+      <c r="Y74" s="53"/>
+      <c r="Z74" s="53"/>
+      <c r="AA74" s="53"/>
+      <c r="AB74" s="53"/>
+      <c r="AC74" s="53"/>
+      <c r="AD74" s="53"/>
+      <c r="AE74" s="53"/>
+      <c r="AF74" s="53"/>
+      <c r="AG74" s="53"/>
+      <c r="AH74" s="53"/>
+      <c r="AI74" s="53"/>
+      <c r="AJ74" s="53"/>
+      <c r="AK74" s="53"/>
+      <c r="AL74" s="53"/>
+      <c r="AM74" s="53"/>
+      <c r="AN74" s="53"/>
+      <c r="AO74" s="53"/>
+      <c r="AP74" s="53"/>
+      <c r="AQ74" s="53"/>
+      <c r="AR74" s="53"/>
+      <c r="AS74" s="53"/>
+      <c r="AT74" s="53"/>
+      <c r="AU74" s="53"/>
+      <c r="AV74" s="53"/>
+      <c r="AW74" s="53"/>
+      <c r="AX74" s="53"/>
+      <c r="AY74" s="53"/>
+      <c r="AZ74" s="53"/>
+      <c r="BA74" s="53"/>
+      <c r="BB74" s="53"/>
+      <c r="BC74" s="53"/>
+      <c r="BD74" s="53"/>
+      <c r="BE74" s="53"/>
+      <c r="BF74" s="53"/>
+      <c r="BG74" s="53"/>
+      <c r="BH74" s="53"/>
+      <c r="BI74" s="53"/>
+      <c r="BJ74" s="53"/>
+      <c r="BK74" s="53"/>
+      <c r="BL74" s="53"/>
+      <c r="BM74" s="53"/>
+      <c r="BN74" s="53"/>
+      <c r="BO74" s="53"/>
+      <c r="BP74" s="53"/>
     </row>
     <row r="75" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="16"/>
       <c r="B75" s="6"/>
-      <c r="C75" s="83"/>
+      <c r="C75" s="93"/>
       <c r="D75" s="7"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
@@ -3628,62 +3638,62 @@
       <c r="N75" s="6"/>
       <c r="O75" s="8"/>
       <c r="P75" s="16"/>
-      <c r="R75" s="54"/>
-      <c r="S75" s="54"/>
-      <c r="T75" s="54"/>
-      <c r="U75" s="54"/>
-      <c r="V75" s="54"/>
-      <c r="W75" s="54"/>
-      <c r="X75" s="54"/>
-      <c r="Y75" s="54"/>
-      <c r="Z75" s="54"/>
-      <c r="AA75" s="54"/>
-      <c r="AB75" s="54"/>
-      <c r="AC75" s="54"/>
-      <c r="AD75" s="54"/>
-      <c r="AE75" s="54"/>
-      <c r="AF75" s="54"/>
-      <c r="AG75" s="54"/>
-      <c r="AH75" s="54"/>
-      <c r="AI75" s="54"/>
-      <c r="AJ75" s="54"/>
-      <c r="AK75" s="54"/>
-      <c r="AL75" s="54"/>
-      <c r="AM75" s="54"/>
-      <c r="AN75" s="54"/>
-      <c r="AO75" s="54"/>
-      <c r="AP75" s="54"/>
-      <c r="AQ75" s="54"/>
-      <c r="AR75" s="54"/>
-      <c r="AS75" s="54"/>
-      <c r="AT75" s="54"/>
-      <c r="AU75" s="54"/>
-      <c r="AV75" s="54"/>
-      <c r="AW75" s="54"/>
-      <c r="AX75" s="54"/>
-      <c r="AY75" s="54"/>
-      <c r="AZ75" s="54"/>
-      <c r="BA75" s="54"/>
-      <c r="BB75" s="54"/>
-      <c r="BC75" s="54"/>
-      <c r="BD75" s="54"/>
-      <c r="BE75" s="54"/>
-      <c r="BF75" s="54"/>
-      <c r="BG75" s="54"/>
-      <c r="BH75" s="54"/>
-      <c r="BI75" s="54"/>
-      <c r="BJ75" s="54"/>
-      <c r="BK75" s="54"/>
-      <c r="BL75" s="54"/>
-      <c r="BM75" s="54"/>
-      <c r="BN75" s="54"/>
-      <c r="BO75" s="54"/>
-      <c r="BP75" s="54"/>
-    </row>
-    <row r="76" spans="1:68" s="54" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="52"/>
-      <c r="B76" s="53"/>
-      <c r="C76" s="55"/>
+      <c r="R75" s="53"/>
+      <c r="S75" s="53"/>
+      <c r="T75" s="53"/>
+      <c r="U75" s="53"/>
+      <c r="V75" s="53"/>
+      <c r="W75" s="53"/>
+      <c r="X75" s="53"/>
+      <c r="Y75" s="53"/>
+      <c r="Z75" s="53"/>
+      <c r="AA75" s="53"/>
+      <c r="AB75" s="53"/>
+      <c r="AC75" s="53"/>
+      <c r="AD75" s="53"/>
+      <c r="AE75" s="53"/>
+      <c r="AF75" s="53"/>
+      <c r="AG75" s="53"/>
+      <c r="AH75" s="53"/>
+      <c r="AI75" s="53"/>
+      <c r="AJ75" s="53"/>
+      <c r="AK75" s="53"/>
+      <c r="AL75" s="53"/>
+      <c r="AM75" s="53"/>
+      <c r="AN75" s="53"/>
+      <c r="AO75" s="53"/>
+      <c r="AP75" s="53"/>
+      <c r="AQ75" s="53"/>
+      <c r="AR75" s="53"/>
+      <c r="AS75" s="53"/>
+      <c r="AT75" s="53"/>
+      <c r="AU75" s="53"/>
+      <c r="AV75" s="53"/>
+      <c r="AW75" s="53"/>
+      <c r="AX75" s="53"/>
+      <c r="AY75" s="53"/>
+      <c r="AZ75" s="53"/>
+      <c r="BA75" s="53"/>
+      <c r="BB75" s="53"/>
+      <c r="BC75" s="53"/>
+      <c r="BD75" s="53"/>
+      <c r="BE75" s="53"/>
+      <c r="BF75" s="53"/>
+      <c r="BG75" s="53"/>
+      <c r="BH75" s="53"/>
+      <c r="BI75" s="53"/>
+      <c r="BJ75" s="53"/>
+      <c r="BK75" s="53"/>
+      <c r="BL75" s="53"/>
+      <c r="BM75" s="53"/>
+      <c r="BN75" s="53"/>
+      <c r="BO75" s="53"/>
+      <c r="BP75" s="53"/>
+    </row>
+    <row r="76" spans="1:68" s="53" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="51"/>
+      <c r="B76" s="52"/>
+      <c r="C76" s="54"/>
       <c r="D76" s="7"/>
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
@@ -3696,7 +3706,7 @@
       <c r="M76" s="6"/>
       <c r="N76" s="6"/>
       <c r="O76" s="6"/>
-      <c r="P76" s="52"/>
+      <c r="P76" s="51"/>
     </row>
     <row r="77" spans="1:68" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="16"/>
@@ -3742,18 +3752,18 @@
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
-      <c r="F79" s="82"/>
-      <c r="G79" s="82"/>
+      <c r="F79" s="92"/>
+      <c r="G79" s="92"/>
       <c r="H79" s="6"/>
       <c r="I79" s="38" t="s">
         <v>58</v>
       </c>
       <c r="J79" s="38"/>
       <c r="K79" s="6"/>
-      <c r="L79" s="79" t="s">
+      <c r="L79" s="90" t="s">
         <v>57</v>
       </c>
-      <c r="M79" s="79"/>
+      <c r="M79" s="90"/>
       <c r="N79" s="40"/>
       <c r="O79" s="5"/>
       <c r="P79" s="5"/>
@@ -3779,27 +3789,30 @@
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C82" s="4" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C83" s="4" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C84" s="4" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B2:O3"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="E6:K6"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="L79:M79"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C69:C70"/>
     <mergeCell ref="C54:C55"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C21:C22"/>
@@ -3812,15 +3825,12 @@
     <mergeCell ref="C44:C45"/>
     <mergeCell ref="C50:C51"/>
     <mergeCell ref="C47:C48"/>
-    <mergeCell ref="L79:M79"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B2:O3"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="C11:C12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3851,46 +3861,46 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="94" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
+        <v>125</v>
+      </c>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="95"/>
+      <c r="A4" s="94"/>
       <c r="B4" s="1" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="95"/>
+      <c r="A5" s="94"/>
       <c r="B5" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -3904,19 +3914,19 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F6" s="62" t="s">
-        <v>159</v>
+        <v>122</v>
+      </c>
+      <c r="F6" s="61" t="s">
+        <v>141</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -3938,8 +3948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3949,92 +3959,92 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C1" s="75"/>
+        <v>172</v>
+      </c>
+      <c r="C1" s="70"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C2" s="61"/>
+        <v>131</v>
+      </c>
+      <c r="C2" s="60"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C3" s="60"/>
+        <v>130</v>
+      </c>
+      <c r="C3" s="59"/>
       <c r="E3" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C5" s="72"/>
+        <v>169</v>
+      </c>
+      <c r="C5" s="67"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>198</v>
-      </c>
-      <c r="C6" s="73"/>
+        <v>171</v>
+      </c>
+      <c r="C6" s="68"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>197</v>
-      </c>
-      <c r="C7" s="74"/>
+        <v>170</v>
+      </c>
+      <c r="C7" s="69"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>209</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>204</v>
-      </c>
-      <c r="C10" s="76"/>
+        <v>177</v>
+      </c>
+      <c r="C10" s="71"/>
       <c r="D10" t="s">
-        <v>205</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>200</v>
-      </c>
-      <c r="C11" s="77"/>
+        <v>173</v>
+      </c>
+      <c r="C11" s="72"/>
       <c r="D11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>202</v>
-      </c>
-      <c r="C12" s="78"/>
+        <v>175</v>
+      </c>
+      <c r="C12" s="73"/>
       <c r="D12">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>203</v>
-      </c>
-      <c r="C13" s="74"/>
+        <v>176</v>
+      </c>
+      <c r="C13" s="69"/>
       <c r="D13">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>201</v>
+        <v>174</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -4042,14 +4052,14 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>210</v>
+        <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>147</v>
-      </c>
-      <c r="C40" s="56"/>
+        <v>129</v>
+      </c>
+      <c r="C40" s="55"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
@@ -4153,10 +4163,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H48"/>
+  <dimension ref="B2:H54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4175,26 +4185,26 @@
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="41"/>
       <c r="C2" s="42" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D2" s="42" t="s">
         <v>36</v>
       </c>
       <c r="E2" s="42" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="F2" s="42" t="s">
         <v>37</v>
       </c>
       <c r="G2" s="42" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="H2" s="42" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="95" t="s">
         <v>41</v>
       </c>
       <c r="C3" s="44" t="s">
@@ -4213,657 +4223,717 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="109"/>
-      <c r="C4" s="111" t="s">
+      <c r="B4" s="96"/>
+      <c r="C4" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="111" t="s">
+      <c r="D4" s="99" t="s">
         <v>40</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="F4" s="45"/>
       <c r="G4" s="45"/>
       <c r="H4" s="45" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="109"/>
-      <c r="C5" s="109"/>
-      <c r="D5" s="109"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
       <c r="E5" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="F5" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="G5" s="45" t="s">
+        <v>165</v>
+      </c>
+      <c r="H5" s="45" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="F6" s="45" t="s">
+        <v>166</v>
+      </c>
+      <c r="G6" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="H6" s="45" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="97"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="45" t="s">
+        <v>160</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="G7" s="45" t="s">
         <v>162</v>
       </c>
-      <c r="F5" s="45" t="s">
-        <v>191</v>
-      </c>
-      <c r="G5" s="45" t="s">
-        <v>192</v>
-      </c>
-      <c r="H5" s="45" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="109"/>
-      <c r="C6" s="109"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="45" t="s">
+      <c r="H7" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="F6" s="45" t="s">
-        <v>193</v>
-      </c>
-      <c r="G6" s="45" t="s">
-        <v>165</v>
-      </c>
-      <c r="H6" s="45" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="110"/>
-      <c r="C7" s="110"/>
-      <c r="D7" s="110"/>
-      <c r="E7" s="45" t="s">
-        <v>185</v>
-      </c>
-      <c r="F7" s="45" t="s">
-        <v>160</v>
-      </c>
-      <c r="G7" s="45" t="s">
-        <v>189</v>
-      </c>
-      <c r="H7" s="45" t="s">
-        <v>190</v>
-      </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="57"/>
-      <c r="C8" s="58" t="s">
-        <v>166</v>
-      </c>
-      <c r="D8" s="58" t="s">
-        <v>167</v>
-      </c>
-      <c r="E8" s="45" t="s">
-        <v>168</v>
-      </c>
-      <c r="F8" s="45" t="s">
-        <v>169</v>
-      </c>
-      <c r="G8" s="45" t="s">
-        <v>170</v>
-      </c>
-      <c r="H8" s="45" t="s">
-        <v>181</v>
-      </c>
+      <c r="B8" s="56"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="57"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58" t="s">
-        <v>179</v>
-      </c>
-      <c r="E9" s="45" t="s">
-        <v>180</v>
-      </c>
+      <c r="B9" s="56"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="45"/>
       <c r="G9" s="45"/>
       <c r="H9" s="45"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="67"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="57" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" s="57" t="s">
+        <v>149</v>
+      </c>
+      <c r="E10" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="F10" s="45" t="s">
+        <v>185</v>
+      </c>
+      <c r="G10" s="45" t="s">
+        <v>186</v>
+      </c>
+      <c r="H10" s="45" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="11" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="57"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
       <c r="E11" s="45"/>
       <c r="F11" s="45"/>
       <c r="G11" s="45"/>
       <c r="H11" s="45"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="57"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
       <c r="E12" s="45"/>
       <c r="F12" s="45"/>
       <c r="G12" s="45"/>
       <c r="H12" s="45"/>
     </row>
     <row r="13" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="101" t="s">
+      <c r="B13" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="99" t="s">
+      <c r="C13" s="103" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="99" t="s">
+      <c r="D13" s="103" t="s">
         <v>71</v>
       </c>
       <c r="E13" s="47" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="F13" s="47"/>
       <c r="G13" s="47"/>
       <c r="H13" s="47" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="102"/>
-      <c r="C14" s="100"/>
-      <c r="D14" s="100"/>
+      <c r="B14" s="106"/>
+      <c r="C14" s="104"/>
+      <c r="D14" s="104"/>
       <c r="E14" s="47" t="s">
         <v>72</v>
       </c>
       <c r="F14" s="47" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="G14" s="47" t="s">
+        <v>190</v>
+      </c>
+      <c r="H14" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="106"/>
+      <c r="C15" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="H14" s="48" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="102"/>
-      <c r="C15" s="47" t="s">
-        <v>75</v>
-      </c>
       <c r="D15" s="47" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E15" s="47" t="s">
-        <v>77</v>
+        <v>192</v>
       </c>
       <c r="F15" s="47"/>
       <c r="G15" s="47" t="s">
-        <v>78</v>
+        <v>188</v>
       </c>
       <c r="H15" s="48" t="s">
-        <v>74</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="102"/>
-      <c r="C16" s="99" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="99" t="s">
-        <v>80</v>
+      <c r="B16" s="106"/>
+      <c r="C16" s="103" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="103" t="s">
+        <v>76</v>
       </c>
       <c r="E16" s="47" t="s">
-        <v>81</v>
+        <v>193</v>
       </c>
       <c r="F16" s="47"/>
       <c r="G16" s="47"/>
       <c r="H16" s="47" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="102"/>
-      <c r="C17" s="100"/>
-      <c r="D17" s="100"/>
+      <c r="B17" s="106"/>
+      <c r="C17" s="104"/>
+      <c r="D17" s="104"/>
       <c r="E17" s="47" t="s">
-        <v>82</v>
+        <v>195</v>
       </c>
       <c r="F17" s="48" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="G17" s="47" t="s">
-        <v>84</v>
+        <v>196</v>
       </c>
       <c r="H17" s="47" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="102"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="48"/>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="106"/>
+      <c r="C18" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="48" t="s">
+        <v>197</v>
+      </c>
       <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
+      <c r="G18" s="48" t="s">
+        <v>198</v>
+      </c>
+      <c r="H18" s="48" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="102"/>
-      <c r="C19" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="D19" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="E19" s="48" t="s">
-        <v>87</v>
-      </c>
+      <c r="B19" s="106"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
       <c r="F19" s="48"/>
-      <c r="G19" s="48" t="s">
-        <v>90</v>
-      </c>
-      <c r="H19" s="48" t="s">
-        <v>91</v>
-      </c>
+      <c r="G19" s="66"/>
+      <c r="H19" s="48"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="102"/>
+      <c r="B20" s="106"/>
       <c r="C20" s="48"/>
       <c r="D20" s="48"/>
       <c r="E20" s="48"/>
       <c r="F20" s="48"/>
-      <c r="G20" s="71"/>
+      <c r="G20" s="66"/>
       <c r="H20" s="48"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="102"/>
+      <c r="B21" s="106"/>
       <c r="C21" s="48"/>
       <c r="D21" s="48"/>
       <c r="E21" s="48"/>
       <c r="F21" s="48"/>
-      <c r="G21" s="71"/>
+      <c r="G21" s="66"/>
       <c r="H21" s="48"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="102"/>
+      <c r="B22" s="106"/>
       <c r="C22" s="48"/>
       <c r="D22" s="48"/>
       <c r="E22" s="48"/>
       <c r="F22" s="48"/>
-      <c r="G22" s="71"/>
+      <c r="G22" s="66"/>
       <c r="H22" s="48"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="102"/>
+      <c r="B23" s="106"/>
       <c r="C23" s="48"/>
       <c r="D23" s="48"/>
       <c r="E23" s="48"/>
       <c r="F23" s="48"/>
-      <c r="G23" s="71"/>
+      <c r="G23" s="66"/>
       <c r="H23" s="48"/>
     </row>
     <row r="24" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="102"/>
-      <c r="C24" s="105" t="s">
+      <c r="B24" s="106"/>
+      <c r="C24" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="74" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="74" t="s">
+        <v>200</v>
+      </c>
+      <c r="F24" s="74" t="s">
+        <v>202</v>
+      </c>
+      <c r="G24" s="74" t="s">
+        <v>201</v>
+      </c>
+      <c r="H24" s="74" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="106"/>
+      <c r="C25" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="74" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="74" t="s">
+        <v>213</v>
+      </c>
+      <c r="F25" s="74" t="s">
+        <v>210</v>
+      </c>
+      <c r="G25" s="74" t="s">
+        <v>203</v>
+      </c>
+      <c r="H25" s="74" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="106"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75" t="s">
+        <v>207</v>
+      </c>
+      <c r="E26" s="74" t="s">
+        <v>208</v>
+      </c>
+      <c r="F26" s="74" t="s">
+        <v>209</v>
+      </c>
+      <c r="G26" s="74" t="s">
+        <v>211</v>
+      </c>
+      <c r="H26" s="74" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="106"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="74"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="106"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="75"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
+      <c r="H28" s="74"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="106"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="74"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="106"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="74"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="106"/>
+      <c r="C31" s="75"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="74"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32" s="106"/>
+      <c r="C32" s="75"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="74"/>
+      <c r="G32" s="74"/>
+      <c r="H32" s="74"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33" s="106"/>
+      <c r="C33" s="75"/>
+      <c r="D33" s="75"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74"/>
+      <c r="G33" s="74"/>
+      <c r="H33" s="74"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B34" s="106"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="74"/>
+      <c r="F34" s="74"/>
+      <c r="G34" s="74"/>
+      <c r="H34" s="74"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35" s="106"/>
+      <c r="C35" s="75"/>
+      <c r="D35" s="75"/>
+      <c r="E35" s="74"/>
+      <c r="F35" s="74"/>
+      <c r="G35" s="74"/>
+      <c r="H35" s="74"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" s="106"/>
+      <c r="C36" s="98" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="105" t="s">
+      <c r="D36" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="49" t="s">
+      <c r="E36" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="F36" s="49"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="49" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37" s="106"/>
+      <c r="C37" s="98"/>
+      <c r="D37" s="98"/>
+      <c r="E37" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="G37" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="H37" s="49"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38" s="106"/>
+      <c r="C38" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="F38" s="74"/>
+      <c r="G38" s="74" t="s">
+        <v>96</v>
+      </c>
+      <c r="H38" s="74" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B39" s="106"/>
+      <c r="C39" s="76"/>
+      <c r="D39" s="76"/>
+      <c r="E39" s="74" t="s">
+        <v>84</v>
+      </c>
+      <c r="F39" s="74" t="s">
+        <v>94</v>
+      </c>
+      <c r="G39" s="74" t="s">
+        <v>89</v>
+      </c>
+      <c r="H39" s="74" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B40" s="106"/>
+      <c r="C40" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" s="74" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="74" t="s">
+        <v>85</v>
+      </c>
+      <c r="F40" s="74" t="s">
+        <v>151</v>
+      </c>
+      <c r="G40" s="74" t="s">
+        <v>90</v>
+      </c>
+      <c r="H40" s="74" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B41" s="106"/>
+      <c r="C41" s="75"/>
+      <c r="D41" s="75"/>
+      <c r="E41" s="74"/>
+      <c r="F41" s="74"/>
+      <c r="G41" s="74"/>
+      <c r="H41" s="74"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" s="106"/>
+      <c r="C42" s="75"/>
+      <c r="D42" s="75"/>
+      <c r="E42" s="74"/>
+      <c r="F42" s="74"/>
+      <c r="G42" s="74"/>
+      <c r="H42" s="74"/>
+    </row>
+    <row r="43" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="106"/>
+      <c r="C43" s="109" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="109" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="F43" s="74" t="s">
+        <v>95</v>
+      </c>
+      <c r="G43" s="74" t="s">
+        <v>91</v>
+      </c>
+      <c r="H43" s="74" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44" s="107"/>
+      <c r="C44" s="110"/>
+      <c r="D44" s="110"/>
+      <c r="E44" s="74" t="s">
+        <v>87</v>
+      </c>
+      <c r="F44" s="74" t="s">
+        <v>93</v>
+      </c>
+      <c r="G44" s="74" t="s">
         <v>92</v>
       </c>
-      <c r="F24" s="49"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="49" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="102"/>
-      <c r="C25" s="105"/>
-      <c r="D25" s="105"/>
-      <c r="E25" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="F25" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="G25" s="49" t="s">
-        <v>102</v>
-      </c>
-      <c r="H25" s="49"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="102"/>
-      <c r="C26" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="49" t="s">
-        <v>94</v>
-      </c>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49" t="s">
+      <c r="H44" s="74" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B45" s="100" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="108" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="108" t="s">
+        <v>61</v>
+      </c>
+      <c r="E45" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="H26" s="49" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="102"/>
-      <c r="C27" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="E27" s="49" t="s">
-        <v>95</v>
-      </c>
-      <c r="F27" s="49" t="s">
-        <v>172</v>
-      </c>
-      <c r="G27" s="49" t="s">
+      <c r="F45" s="46"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="46" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B46" s="101"/>
+      <c r="C46" s="108"/>
+      <c r="D46" s="108"/>
+      <c r="E46" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="F46" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="G46" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="H46" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="H27" s="49" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="102"/>
-      <c r="C28" s="106" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="106" t="s">
-        <v>54</v>
-      </c>
-      <c r="E28" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49" t="s">
-        <v>112</v>
-      </c>
-      <c r="H28" s="49" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="102"/>
-      <c r="C29" s="107"/>
-      <c r="D29" s="107"/>
-      <c r="E29" s="49" t="s">
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B47" s="101"/>
+      <c r="C47" s="62"/>
+      <c r="D47" s="62"/>
+      <c r="E47" s="62"/>
+      <c r="F47" s="62"/>
+      <c r="G47" s="62"/>
+      <c r="H47" s="62"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B48" s="102"/>
+      <c r="C48" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="E48" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="F48" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="G48" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="H48" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="F29" s="49" t="s">
-        <v>110</v>
-      </c>
-      <c r="G29" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="H29" s="49" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="102"/>
-      <c r="C30" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="F30" s="49" t="s">
-        <v>173</v>
-      </c>
-      <c r="G30" s="49" t="s">
-        <v>106</v>
-      </c>
-      <c r="H30" s="51" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="102"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="69"/>
-      <c r="F31" s="69"/>
-      <c r="G31" s="69"/>
-      <c r="H31" s="69"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="102"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="69"/>
-      <c r="F32" s="69"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="69"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="102"/>
-      <c r="C33" s="65"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="69"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="102"/>
-      <c r="C34" s="65"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="102"/>
-      <c r="C35" s="65"/>
-      <c r="D35" s="65"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="69"/>
-      <c r="H35" s="69"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="102"/>
-      <c r="C36" s="65"/>
-      <c r="D36" s="65"/>
-      <c r="E36" s="69"/>
-      <c r="F36" s="69"/>
-      <c r="G36" s="69"/>
-      <c r="H36" s="69"/>
-    </row>
-    <row r="37" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="102"/>
-      <c r="C37" s="106" t="s">
-        <v>51</v>
-      </c>
-      <c r="D37" s="106" t="s">
-        <v>52</v>
-      </c>
-      <c r="E37" s="49" t="s">
-        <v>99</v>
-      </c>
-      <c r="F37" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="G37" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="H37" s="49" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="103"/>
-      <c r="C38" s="107"/>
-      <c r="D38" s="107"/>
-      <c r="E38" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="F38" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="G38" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="H38" s="51" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B39" s="96" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" s="104" t="s">
-        <v>59</v>
-      </c>
-      <c r="D39" s="104" t="s">
-        <v>61</v>
-      </c>
-      <c r="E39" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="F39" s="46"/>
-      <c r="G39" s="46"/>
-      <c r="H39" s="46" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="97"/>
-      <c r="C40" s="104"/>
-      <c r="D40" s="104"/>
-      <c r="E40" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="F40" s="46" t="s">
-        <v>161</v>
-      </c>
-      <c r="G40" s="46" t="s">
-        <v>121</v>
-      </c>
-      <c r="H40" s="46" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B41" s="97"/>
-      <c r="C41" s="63"/>
-      <c r="D41" s="63"/>
-      <c r="E41" s="63"/>
-      <c r="F41" s="63"/>
-      <c r="G41" s="63"/>
-      <c r="H41" s="63"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B42" s="98"/>
-      <c r="C42" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="D42" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="E42" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="F42" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="G42" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="H42" s="46" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B43" s="64"/>
-      <c r="C43" s="70"/>
-      <c r="D43" s="70" t="s">
-        <v>178</v>
-      </c>
-      <c r="E43" s="63"/>
-      <c r="F43" s="63"/>
-      <c r="G43" s="63"/>
-      <c r="H43" s="63"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B44" s="64"/>
-      <c r="C44" s="70"/>
-      <c r="D44" s="70" t="s">
-        <v>174</v>
-      </c>
-      <c r="E44" s="63"/>
-      <c r="F44" s="63"/>
-      <c r="G44" s="63"/>
-      <c r="H44" s="63"/>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B45" s="64"/>
-      <c r="C45" s="70"/>
-      <c r="D45" s="70" t="s">
-        <v>175</v>
-      </c>
-      <c r="E45" s="63"/>
-      <c r="F45" s="63"/>
-      <c r="G45" s="63"/>
-      <c r="H45" s="63"/>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B46" s="64"/>
-      <c r="C46" s="70"/>
-      <c r="D46" s="70" t="s">
-        <v>176</v>
-      </c>
-      <c r="E46" s="63"/>
-      <c r="F46" s="63"/>
-      <c r="G46" s="63"/>
-      <c r="H46" s="63"/>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B47" s="64"/>
-      <c r="C47" s="70"/>
-      <c r="D47" s="70" t="s">
-        <v>177</v>
-      </c>
-      <c r="E47" s="63"/>
-      <c r="F47" s="63"/>
-      <c r="G47" s="63"/>
-      <c r="H47" s="63"/>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B48" s="64"/>
-      <c r="C48" s="70"/>
-      <c r="D48" s="70"/>
-      <c r="E48" s="63"/>
-      <c r="F48" s="63"/>
-      <c r="G48" s="63"/>
-      <c r="H48" s="63"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B49" s="63"/>
+      <c r="C49" s="65"/>
+      <c r="D49" s="65" t="s">
+        <v>156</v>
+      </c>
+      <c r="E49" s="62"/>
+      <c r="F49" s="62"/>
+      <c r="G49" s="62"/>
+      <c r="H49" s="62"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B50" s="63"/>
+      <c r="C50" s="65"/>
+      <c r="D50" s="65" t="s">
+        <v>152</v>
+      </c>
+      <c r="E50" s="62"/>
+      <c r="F50" s="62"/>
+      <c r="G50" s="62"/>
+      <c r="H50" s="62"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B51" s="63"/>
+      <c r="C51" s="65"/>
+      <c r="D51" s="65" t="s">
+        <v>153</v>
+      </c>
+      <c r="E51" s="62"/>
+      <c r="F51" s="62"/>
+      <c r="G51" s="62"/>
+      <c r="H51" s="62"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B52" s="63"/>
+      <c r="C52" s="65"/>
+      <c r="D52" s="65" t="s">
+        <v>154</v>
+      </c>
+      <c r="E52" s="62"/>
+      <c r="F52" s="62"/>
+      <c r="G52" s="62"/>
+      <c r="H52" s="62"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B53" s="63"/>
+      <c r="C53" s="65"/>
+      <c r="D53" s="65" t="s">
+        <v>155</v>
+      </c>
+      <c r="E53" s="62"/>
+      <c r="F53" s="62"/>
+      <c r="G53" s="62"/>
+      <c r="H53" s="62"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B54" s="63"/>
+      <c r="C54" s="65"/>
+      <c r="D54" s="65"/>
+      <c r="E54" s="62"/>
+      <c r="F54" s="62"/>
+      <c r="G54" s="62"/>
+      <c r="H54" s="62"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="15">
     <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C36:C37"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="D4:D7"/>
-    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="B45:B48"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="D16:D17"/>
-    <mergeCell ref="B13:B38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="B13:B44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Auto push 2023-03-23 23:24:14.10
</commit_message>
<xml_diff>
--- a/project/CheeYoonMovie.xlsx
+++ b/project/CheeYoonMovie.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="224">
   <si>
     <t>이용자 권한과 기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -826,10 +826,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BoardContentService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>board/boardContent.jsp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -854,10 +850,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>boardNo,pageNum</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CommentWriteService.java</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -866,7 +858,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>boardContent.do</t>
+    <t>댓글 리스트 출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardContentService.java
+CommentListService</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardNo
+pageNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardNo
+commentPageNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>댓글 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>commentNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>board/boardContent.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>댓글 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>commentModifyView.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>board/commentModify.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>commentModify.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>commentNo
+commentContent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>commentModifyService.java</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1404,7 +1448,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1639,6 +1683,18 @@
     <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1688,6 +1744,12 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2106,41 +2168,41 @@
     <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="83" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="80"/>
-      <c r="O3" s="80"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
@@ -2185,32 +2247,32 @@
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20"/>
-      <c r="C6" s="81" t="s">
+      <c r="C6" s="85" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="39"/>
-      <c r="E6" s="83" t="s">
+      <c r="E6" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="83"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="85" t="s">
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="M6" s="83"/>
-      <c r="N6" s="83"/>
-      <c r="O6" s="83"/>
+      <c r="M6" s="87"/>
+      <c r="N6" s="87"/>
+      <c r="O6" s="87"/>
       <c r="P6" s="21"/>
       <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="82"/>
+      <c r="C7" s="86"/>
       <c r="D7" s="22"/>
       <c r="E7" s="13">
         <v>20</v>
@@ -2310,7 +2372,7 @@
     <row r="11" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="86" t="s">
+      <c r="C11" s="90" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="10"/>
@@ -2331,7 +2393,7 @@
     <row r="12" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="86"/>
+      <c r="C12" s="90"/>
       <c r="D12" s="10"/>
       <c r="E12" s="8"/>
       <c r="F12" s="6"/>
@@ -2369,7 +2431,7 @@
     <row r="14" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="78" t="s">
+      <c r="C14" s="82" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="10"/>
@@ -2390,7 +2452,7 @@
     <row r="15" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="78"/>
+      <c r="C15" s="82"/>
       <c r="D15" s="10"/>
       <c r="E15" s="8"/>
       <c r="F15" s="6"/>
@@ -2428,7 +2490,7 @@
     <row r="17" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="86" t="s">
+      <c r="C17" s="90" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="10"/>
@@ -2449,7 +2511,7 @@
     <row r="18" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="86"/>
+      <c r="C18" s="90"/>
       <c r="D18" s="10"/>
       <c r="E18" s="6"/>
       <c r="F18" s="8"/>
@@ -2508,7 +2570,7 @@
     <row r="21" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="88" t="s">
+      <c r="C21" s="92" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="10"/>
@@ -2529,7 +2591,7 @@
     <row r="22" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="88"/>
+      <c r="C22" s="92"/>
       <c r="D22" s="10"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -2567,7 +2629,7 @@
     <row r="24" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="88" t="s">
+      <c r="C24" s="92" t="s">
         <v>16</v>
       </c>
       <c r="D24" s="10"/>
@@ -2588,7 +2650,7 @@
     <row r="25" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="88"/>
+      <c r="C25" s="92"/>
       <c r="D25" s="10"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -2626,7 +2688,7 @@
     <row r="27" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="88" t="s">
+      <c r="C27" s="92" t="s">
         <v>111</v>
       </c>
       <c r="D27" s="10"/>
@@ -2647,7 +2709,7 @@
     <row r="28" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="88"/>
+      <c r="C28" s="92"/>
       <c r="D28" s="10"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -2685,7 +2747,7 @@
     <row r="30" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="88" t="s">
+      <c r="C30" s="92" t="s">
         <v>112</v>
       </c>
       <c r="D30" s="10"/>
@@ -2706,7 +2768,7 @@
     <row r="31" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="88"/>
+      <c r="C31" s="92"/>
       <c r="D31" s="10"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -2744,7 +2806,7 @@
     <row r="33" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="88" t="s">
+      <c r="C33" s="92" t="s">
         <v>113</v>
       </c>
       <c r="D33" s="10"/>
@@ -2765,7 +2827,7 @@
     <row r="34" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="6"/>
-      <c r="C34" s="88"/>
+      <c r="C34" s="92"/>
       <c r="D34" s="10"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -2843,7 +2905,7 @@
     <row r="38" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
       <c r="B38" s="6"/>
-      <c r="C38" s="89" t="s">
+      <c r="C38" s="93" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="10"/>
@@ -2864,7 +2926,7 @@
     <row r="39" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
       <c r="B39" s="6"/>
-      <c r="C39" s="89"/>
+      <c r="C39" s="93"/>
       <c r="D39" s="10"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
@@ -2902,7 +2964,7 @@
     <row r="41" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="89" t="s">
+      <c r="C41" s="93" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="10"/>
@@ -2923,7 +2985,7 @@
     <row r="42" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16"/>
       <c r="B42" s="6"/>
-      <c r="C42" s="89"/>
+      <c r="C42" s="93"/>
       <c r="D42" s="10"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
@@ -2961,7 +3023,7 @@
     <row r="44" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="89" t="s">
+      <c r="C44" s="93" t="s">
         <v>137</v>
       </c>
       <c r="D44" s="10"/>
@@ -2982,7 +3044,7 @@
     <row r="45" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="16"/>
       <c r="B45" s="6"/>
-      <c r="C45" s="89"/>
+      <c r="C45" s="93"/>
       <c r="D45" s="10"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
@@ -3020,7 +3082,7 @@
     <row r="47" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="89" t="s">
+      <c r="C47" s="93" t="s">
         <v>114</v>
       </c>
       <c r="D47" s="10"/>
@@ -3041,7 +3103,7 @@
     <row r="48" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="16"/>
       <c r="B48" s="6"/>
-      <c r="C48" s="89"/>
+      <c r="C48" s="93"/>
       <c r="D48" s="10"/>
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
@@ -3079,7 +3141,7 @@
     <row r="50" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="89" t="s">
+      <c r="C50" s="93" t="s">
         <v>138</v>
       </c>
       <c r="D50" s="10"/>
@@ -3100,7 +3162,7 @@
     <row r="51" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="16"/>
       <c r="B51" s="6"/>
-      <c r="C51" s="89"/>
+      <c r="C51" s="93"/>
       <c r="D51" s="10"/>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
@@ -3159,7 +3221,7 @@
     <row r="54" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16"/>
       <c r="B54" s="6"/>
-      <c r="C54" s="87" t="s">
+      <c r="C54" s="91" t="s">
         <v>115</v>
       </c>
       <c r="D54" s="10"/>
@@ -3180,7 +3242,7 @@
     <row r="55" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="87"/>
+      <c r="C55" s="91"/>
       <c r="D55" s="10"/>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
@@ -3218,7 +3280,7 @@
     <row r="57" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="16"/>
       <c r="B57" s="6"/>
-      <c r="C57" s="87" t="s">
+      <c r="C57" s="91" t="s">
         <v>116</v>
       </c>
       <c r="D57" s="10"/>
@@ -3239,7 +3301,7 @@
     <row r="58" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="87"/>
+      <c r="C58" s="91"/>
       <c r="D58" s="10"/>
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
@@ -3277,7 +3339,7 @@
     <row r="60" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="16"/>
       <c r="B60" s="6"/>
-      <c r="C60" s="87" t="s">
+      <c r="C60" s="91" t="s">
         <v>136</v>
       </c>
       <c r="D60" s="10"/>
@@ -3298,7 +3360,7 @@
     <row r="61" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="16"/>
       <c r="B61" s="6"/>
-      <c r="C61" s="87"/>
+      <c r="C61" s="91"/>
       <c r="D61" s="10"/>
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
@@ -3336,7 +3398,7 @@
     <row r="63" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="16"/>
       <c r="B63" s="6"/>
-      <c r="C63" s="87" t="s">
+      <c r="C63" s="91" t="s">
         <v>135</v>
       </c>
       <c r="D63" s="10"/>
@@ -3357,7 +3419,7 @@
     <row r="64" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="16"/>
       <c r="B64" s="6"/>
-      <c r="C64" s="87"/>
+      <c r="C64" s="91"/>
       <c r="D64" s="10"/>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
@@ -3395,7 +3457,7 @@
     <row r="66" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="16"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="87" t="s">
+      <c r="C66" s="91" t="s">
         <v>134</v>
       </c>
       <c r="D66" s="10"/>
@@ -3416,7 +3478,7 @@
     <row r="67" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="16"/>
       <c r="B67" s="6"/>
-      <c r="C67" s="87"/>
+      <c r="C67" s="91"/>
       <c r="D67" s="10"/>
       <c r="E67" s="6"/>
       <c r="F67" s="6"/>
@@ -3454,7 +3516,7 @@
     <row r="69" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="87" t="s">
+      <c r="C69" s="91" t="s">
         <v>133</v>
       </c>
       <c r="D69" s="10"/>
@@ -3475,7 +3537,7 @@
     <row r="70" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="16"/>
       <c r="B70" s="6"/>
-      <c r="C70" s="87"/>
+      <c r="C70" s="91"/>
       <c r="D70" s="10"/>
       <c r="E70" s="6"/>
       <c r="F70" s="6"/>
@@ -3513,7 +3575,7 @@
     <row r="72" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16"/>
       <c r="B72" s="6"/>
-      <c r="C72" s="91" t="s">
+      <c r="C72" s="95" t="s">
         <v>56</v>
       </c>
       <c r="D72" s="7"/>
@@ -3534,7 +3596,7 @@
     <row r="73" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="16"/>
       <c r="B73" s="6"/>
-      <c r="C73" s="91"/>
+      <c r="C73" s="95"/>
       <c r="D73" s="7"/>
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
@@ -3553,7 +3615,7 @@
     <row r="74" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16"/>
       <c r="B74" s="6"/>
-      <c r="C74" s="93" t="s">
+      <c r="C74" s="97" t="s">
         <v>109</v>
       </c>
       <c r="D74" s="7"/>
@@ -3624,7 +3686,7 @@
     <row r="75" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="16"/>
       <c r="B75" s="6"/>
-      <c r="C75" s="93"/>
+      <c r="C75" s="97"/>
       <c r="D75" s="7"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
@@ -3752,18 +3814,18 @@
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
-      <c r="F79" s="92"/>
-      <c r="G79" s="92"/>
+      <c r="F79" s="96"/>
+      <c r="G79" s="96"/>
       <c r="H79" s="6"/>
       <c r="I79" s="38" t="s">
         <v>58</v>
       </c>
       <c r="J79" s="38"/>
       <c r="K79" s="6"/>
-      <c r="L79" s="90" t="s">
+      <c r="L79" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="M79" s="90"/>
+      <c r="M79" s="94"/>
       <c r="N79" s="40"/>
       <c r="O79" s="5"/>
       <c r="P79" s="5"/>
@@ -3861,7 +3923,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="98" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3871,7 +3933,7 @@
       <c r="D3" s="58"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="94"/>
+      <c r="A4" s="98"/>
       <c r="B4" s="1" t="s">
         <v>119</v>
       </c>
@@ -3886,7 +3948,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="94"/>
+      <c r="A5" s="98"/>
       <c r="B5" s="1" t="s">
         <v>120</v>
       </c>
@@ -4165,8 +4227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4174,8 +4236,8 @@
     <col min="1" max="1" width="1.125" style="43" customWidth="1"/>
     <col min="2" max="2" width="4.5" style="43" customWidth="1"/>
     <col min="3" max="3" width="21" style="43" customWidth="1"/>
-    <col min="4" max="4" width="28.75" style="43" customWidth="1"/>
-    <col min="5" max="5" width="19.625" style="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.875" style="43" customWidth="1"/>
+    <col min="5" max="5" width="22.5" style="43" customWidth="1"/>
     <col min="6" max="6" width="19.875" style="43" customWidth="1"/>
     <col min="7" max="7" width="26.375" style="43" customWidth="1"/>
     <col min="8" max="8" width="28.25" style="43" bestFit="1" customWidth="1"/>
@@ -4204,7 +4266,7 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="101" t="s">
         <v>41</v>
       </c>
       <c r="C3" s="44" t="s">
@@ -4223,11 +4285,11 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="96"/>
-      <c r="C4" s="99" t="s">
+      <c r="B4" s="102"/>
+      <c r="C4" s="105" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="99" t="s">
+      <c r="D4" s="105" t="s">
         <v>40</v>
       </c>
       <c r="E4" s="45" t="s">
@@ -4240,9 +4302,9 @@
       </c>
     </row>
     <row r="5" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="96"/>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
+      <c r="B5" s="102"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
       <c r="E5" s="45" t="s">
         <v>144</v>
       </c>
@@ -4257,9 +4319,9 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="96"/>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
+      <c r="B6" s="102"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="102"/>
       <c r="E6" s="45" t="s">
         <v>145</v>
       </c>
@@ -4274,9 +4336,9 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="97"/>
-      <c r="C7" s="97"/>
-      <c r="D7" s="97"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="103"/>
+      <c r="D7" s="103"/>
       <c r="E7" s="45" t="s">
         <v>160</v>
       </c>
@@ -4348,13 +4410,13 @@
       <c r="H12" s="45"/>
     </row>
     <row r="13" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="105" t="s">
+      <c r="B13" s="111" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="103" t="s">
+      <c r="C13" s="109" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="103" t="s">
+      <c r="D13" s="109" t="s">
         <v>71</v>
       </c>
       <c r="E13" s="47" t="s">
@@ -4367,9 +4429,9 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="106"/>
-      <c r="C14" s="104"/>
-      <c r="D14" s="104"/>
+      <c r="B14" s="112"/>
+      <c r="C14" s="110"/>
+      <c r="D14" s="110"/>
       <c r="E14" s="47" t="s">
         <v>72</v>
       </c>
@@ -4384,7 +4446,7 @@
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="106"/>
+      <c r="B15" s="112"/>
       <c r="C15" s="47" t="s">
         <v>73</v>
       </c>
@@ -4403,11 +4465,11 @@
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="106"/>
-      <c r="C16" s="103" t="s">
+      <c r="B16" s="112"/>
+      <c r="C16" s="109" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="103" t="s">
+      <c r="D16" s="109" t="s">
         <v>76</v>
       </c>
       <c r="E16" s="47" t="s">
@@ -4420,9 +4482,9 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="106"/>
-      <c r="C17" s="104"/>
-      <c r="D17" s="104"/>
+      <c r="B17" s="112"/>
+      <c r="C17" s="110"/>
+      <c r="D17" s="110"/>
       <c r="E17" s="47" t="s">
         <v>195</v>
       </c>
@@ -4437,7 +4499,7 @@
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="106"/>
+      <c r="B18" s="112"/>
       <c r="C18" s="48" t="s">
         <v>80</v>
       </c>
@@ -4452,11 +4514,11 @@
         <v>198</v>
       </c>
       <c r="H18" s="48" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="106"/>
+      <c r="B19" s="112"/>
       <c r="C19" s="48"/>
       <c r="D19" s="48"/>
       <c r="E19" s="48"/>
@@ -4465,7 +4527,7 @@
       <c r="H19" s="48"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="106"/>
+      <c r="B20" s="112"/>
       <c r="C20" s="48"/>
       <c r="D20" s="48"/>
       <c r="E20" s="48"/>
@@ -4474,7 +4536,7 @@
       <c r="H20" s="48"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="106"/>
+      <c r="B21" s="112"/>
       <c r="C21" s="48"/>
       <c r="D21" s="48"/>
       <c r="E21" s="48"/>
@@ -4483,7 +4545,7 @@
       <c r="H21" s="48"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="106"/>
+      <c r="B22" s="112"/>
       <c r="C22" s="48"/>
       <c r="D22" s="48"/>
       <c r="E22" s="48"/>
@@ -4492,7 +4554,7 @@
       <c r="H22" s="48"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="106"/>
+      <c r="B23" s="112"/>
       <c r="C23" s="48"/>
       <c r="D23" s="48"/>
       <c r="E23" s="48"/>
@@ -4501,7 +4563,7 @@
       <c r="H23" s="48"/>
     </row>
     <row r="24" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="106"/>
+      <c r="B24" s="112"/>
       <c r="C24" s="74" t="s">
         <v>44</v>
       </c>
@@ -4518,11 +4580,11 @@
         <v>201</v>
       </c>
       <c r="H24" s="74" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="106"/>
+      <c r="B25" s="112"/>
       <c r="C25" s="74" t="s">
         <v>45</v>
       </c>
@@ -4530,93 +4592,113 @@
         <v>49</v>
       </c>
       <c r="E25" s="74" t="s">
+        <v>210</v>
+      </c>
+      <c r="F25" s="99" t="s">
         <v>213</v>
       </c>
-      <c r="F25" s="74" t="s">
-        <v>210</v>
-      </c>
-      <c r="G25" s="74" t="s">
+      <c r="G25" s="99" t="s">
+        <v>212</v>
+      </c>
+      <c r="H25" s="74" t="s">
         <v>203</v>
       </c>
-      <c r="H25" s="74" t="s">
-        <v>204</v>
-      </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="106"/>
+      <c r="B26" s="112"/>
       <c r="C26" s="75"/>
-      <c r="D26" s="75" t="s">
+      <c r="D26" s="79"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="100"/>
+      <c r="G26" s="100"/>
+      <c r="H26" s="78"/>
+    </row>
+    <row r="27" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B27" s="112"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="79" t="s">
+        <v>211</v>
+      </c>
+      <c r="E27" s="78"/>
+      <c r="F27" s="81" t="s">
+        <v>214</v>
+      </c>
+      <c r="G27" s="78"/>
+      <c r="H27" s="78"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="112"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="79"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="78"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="112"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="75" t="s">
+        <v>206</v>
+      </c>
+      <c r="E29" s="74" t="s">
         <v>207</v>
       </c>
-      <c r="E26" s="74" t="s">
+      <c r="F29" s="74" t="s">
         <v>208</v>
       </c>
-      <c r="F26" s="74" t="s">
+      <c r="G29" s="74" t="s">
         <v>209</v>
       </c>
-      <c r="G26" s="74" t="s">
-        <v>211</v>
-      </c>
-      <c r="H26" s="74" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="106"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="74"/>
-      <c r="G27" s="74"/>
-      <c r="H27" s="74"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="106"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="74"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="106"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
-      <c r="H29" s="74"/>
+      <c r="H29" s="74" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="106"/>
+      <c r="B30" s="112"/>
       <c r="C30" s="75"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
+      <c r="D30" s="75" t="s">
+        <v>218</v>
+      </c>
+      <c r="E30" s="74" t="s">
+        <v>219</v>
+      </c>
+      <c r="F30" s="74" t="s">
+        <v>216</v>
+      </c>
       <c r="G30" s="74"/>
-      <c r="H30" s="74"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="106"/>
+      <c r="H30" s="74" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B31" s="112"/>
       <c r="C31" s="75"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="74"/>
+      <c r="D31" s="80"/>
+      <c r="E31" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="F31" s="81" t="s">
+        <v>222</v>
+      </c>
+      <c r="G31" s="74" t="s">
+        <v>223</v>
+      </c>
       <c r="H31" s="74"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="106"/>
+      <c r="B32" s="112"/>
       <c r="C32" s="75"/>
-      <c r="D32" s="75"/>
+      <c r="D32" s="75" t="s">
+        <v>215</v>
+      </c>
       <c r="E32" s="74"/>
       <c r="F32" s="74"/>
       <c r="G32" s="74"/>
       <c r="H32" s="74"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="106"/>
+      <c r="B33" s="112"/>
       <c r="C33" s="75"/>
       <c r="D33" s="75"/>
       <c r="E33" s="74"/>
@@ -4625,7 +4707,7 @@
       <c r="H33" s="74"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="106"/>
+      <c r="B34" s="112"/>
       <c r="C34" s="75"/>
       <c r="D34" s="75"/>
       <c r="E34" s="74"/>
@@ -4634,7 +4716,7 @@
       <c r="H34" s="74"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="106"/>
+      <c r="B35" s="112"/>
       <c r="C35" s="75"/>
       <c r="D35" s="75"/>
       <c r="E35" s="74"/>
@@ -4643,11 +4725,11 @@
       <c r="H35" s="74"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="106"/>
-      <c r="C36" s="98" t="s">
+      <c r="B36" s="112"/>
+      <c r="C36" s="104" t="s">
         <v>43</v>
       </c>
-      <c r="D36" s="98" t="s">
+      <c r="D36" s="104" t="s">
         <v>47</v>
       </c>
       <c r="E36" s="49" t="s">
@@ -4660,9 +4742,9 @@
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="106"/>
-      <c r="C37" s="98"/>
-      <c r="D37" s="98"/>
+      <c r="B37" s="112"/>
+      <c r="C37" s="104"/>
+      <c r="D37" s="104"/>
       <c r="E37" s="49" t="s">
         <v>82</v>
       </c>
@@ -4675,7 +4757,7 @@
       <c r="H37" s="49"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="106"/>
+      <c r="B38" s="112"/>
       <c r="C38" s="75" t="s">
         <v>46</v>
       </c>
@@ -4694,7 +4776,7 @@
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B39" s="106"/>
+      <c r="B39" s="112"/>
       <c r="C39" s="76"/>
       <c r="D39" s="76"/>
       <c r="E39" s="74" t="s">
@@ -4711,7 +4793,7 @@
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="106"/>
+      <c r="B40" s="112"/>
       <c r="C40" s="74" t="s">
         <v>50</v>
       </c>
@@ -4732,7 +4814,7 @@
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B41" s="106"/>
+      <c r="B41" s="112"/>
       <c r="C41" s="75"/>
       <c r="D41" s="75"/>
       <c r="E41" s="74"/>
@@ -4741,7 +4823,7 @@
       <c r="H41" s="74"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B42" s="106"/>
+      <c r="B42" s="112"/>
       <c r="C42" s="75"/>
       <c r="D42" s="75"/>
       <c r="E42" s="74"/>
@@ -4750,11 +4832,11 @@
       <c r="H42" s="74"/>
     </row>
     <row r="43" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="106"/>
-      <c r="C43" s="109" t="s">
+      <c r="B43" s="112"/>
+      <c r="C43" s="115" t="s">
         <v>51</v>
       </c>
-      <c r="D43" s="109" t="s">
+      <c r="D43" s="115" t="s">
         <v>52</v>
       </c>
       <c r="E43" s="74" t="s">
@@ -4771,9 +4853,9 @@
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B44" s="107"/>
-      <c r="C44" s="110"/>
-      <c r="D44" s="110"/>
+      <c r="B44" s="113"/>
+      <c r="C44" s="116"/>
+      <c r="D44" s="116"/>
       <c r="E44" s="74" t="s">
         <v>87</v>
       </c>
@@ -4788,13 +4870,13 @@
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B45" s="100" t="s">
+      <c r="B45" s="106" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="108" t="s">
+      <c r="C45" s="114" t="s">
         <v>59</v>
       </c>
-      <c r="D45" s="108" t="s">
+      <c r="D45" s="114" t="s">
         <v>61</v>
       </c>
       <c r="E45" s="46" t="s">
@@ -4807,9 +4889,9 @@
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B46" s="101"/>
-      <c r="C46" s="108"/>
-      <c r="D46" s="108"/>
+      <c r="B46" s="107"/>
+      <c r="C46" s="114"/>
+      <c r="D46" s="114"/>
       <c r="E46" s="46" t="s">
         <v>60</v>
       </c>
@@ -4824,7 +4906,7 @@
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B47" s="101"/>
+      <c r="B47" s="107"/>
       <c r="C47" s="62"/>
       <c r="D47" s="62"/>
       <c r="E47" s="62"/>
@@ -4833,7 +4915,7 @@
       <c r="H47" s="62"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B48" s="102"/>
+      <c r="B48" s="108"/>
       <c r="C48" s="46" t="s">
         <v>62</v>
       </c>
@@ -4918,11 +5000,7 @@
       <c r="H54" s="62"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="D4:D7"/>
+  <mergeCells count="17">
     <mergeCell ref="B45:B48"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="D16:D17"/>
@@ -4934,6 +5012,12 @@
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="C43:C44"/>
     <mergeCell ref="D43:D44"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="D4:D7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Auto push 2023-03-24 18:01:16.45
</commit_message>
<xml_diff>
--- a/project/CheeYoonMovie.xlsx
+++ b/project/CheeYoonMovie.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="243">
   <si>
     <t>이용자 권한과 기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -343,77 +343,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>boardWrite.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boardModifyView.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boardModify.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>boardDelete.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>boardReplyView.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boardReply.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardWriteService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardModifyService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardDeleteService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardReplyViewService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardReplyService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardDto 속성들</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardDto 속성들</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardDto 속성들</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardModifyViewService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">member/mAllView.jsp </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>boardList.do</t>
-  </si>
-  <si>
-    <t>boardList.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Service</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -435,18 +372,6 @@
   </si>
   <si>
     <t>ALoginService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">fileBoard/boardWrite.jsp </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">fileBoard/boardModify.jsp </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">fileBoard/boardReply.jsp </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -619,10 +544,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>boardId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>영화 등록</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -739,10 +660,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>22수요일 메인페이지css조정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>로그인 그라데이션</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -843,10 +760,6 @@
   </si>
   <si>
     <t>commentWrite.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>commentDto속성들</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -881,14 +794,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>commentNo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>board/boardContent.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>댓글 수정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -905,12 +810,194 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>commentModifyService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>24금요일 자유게시판 댓글</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>23목요일 회원가입 로그인, 자유게시판 댓글</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22수요일 메인페이지css조정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CommentListService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CommentModifyViewService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>board/commentList.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>commentList.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardContent.do</t>
+  </si>
+  <si>
+    <t>boardContent.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>commentDelete.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CommentDeleteService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>board/boardWrite.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardWrite.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardWriteService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardModifyView.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardModifyViewService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardModify.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>board/boardModify.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardContent.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardList.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardModifyService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardNo
+pageNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardDto 속성들
+pageNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardNo
+pageNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardDto 속성들</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardDeleteService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardNo
+commentNo
+commentPageNum
+pageNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>commentNo
-commentContent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>commentModifyService.java</t>
+commentPageNum
+pageNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>commentDto속성들
+commentPageNum
+pageNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardNo
+commentDto속성들
+pageNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardReplyView.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardDto 속성들
+pageNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>board/boardReply.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardList.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardReplyViewService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pageNum
+boardNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardReply.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardReplyService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nowPlayingList.do</t>
+  </si>
+  <si>
+    <t>NowPlayingListService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movie/nowPlayingList.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nowPlayingContent.do</t>
+  </si>
+  <si>
+    <t>현재 상영작 상세보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 상영영화 리스트</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1448,7 +1535,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1677,93 +1764,108 @@
     <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1786,9 +1888,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2146,10 +2245,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BP84"/>
+  <dimension ref="A1:BP100"/>
   <sheetViews>
     <sheetView topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I90" sqref="I90"/>
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.25" defaultRowHeight="11.25" x14ac:dyDescent="0.3"/>
@@ -2168,41 +2267,41 @@
     <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="83" t="s">
-        <v>110</v>
-      </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
+      <c r="B2" s="88" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
-      <c r="M3" s="84"/>
-      <c r="N3" s="84"/>
-      <c r="O3" s="84"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
@@ -2247,32 +2346,32 @@
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20"/>
-      <c r="C6" s="85" t="s">
+      <c r="C6" s="90" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="39"/>
-      <c r="E6" s="87" t="s">
+      <c r="E6" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="87"/>
-      <c r="J6" s="87"/>
-      <c r="K6" s="88"/>
-      <c r="L6" s="89" t="s">
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="92"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="M6" s="87"/>
-      <c r="N6" s="87"/>
-      <c r="O6" s="87"/>
+      <c r="M6" s="92"/>
+      <c r="N6" s="92"/>
+      <c r="O6" s="92"/>
       <c r="P6" s="21"/>
       <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="86"/>
+      <c r="C7" s="91"/>
       <c r="D7" s="22"/>
       <c r="E7" s="13">
         <v>20</v>
@@ -2372,7 +2471,7 @@
     <row r="11" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="90" t="s">
+      <c r="C11" s="95" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="10"/>
@@ -2393,7 +2492,7 @@
     <row r="12" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="90"/>
+      <c r="C12" s="95"/>
       <c r="D12" s="10"/>
       <c r="E12" s="8"/>
       <c r="F12" s="6"/>
@@ -2431,7 +2530,7 @@
     <row r="14" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="82" t="s">
+      <c r="C14" s="87" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="10"/>
@@ -2452,7 +2551,7 @@
     <row r="15" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="82"/>
+      <c r="C15" s="87"/>
       <c r="D15" s="10"/>
       <c r="E15" s="8"/>
       <c r="F15" s="6"/>
@@ -2490,7 +2589,7 @@
     <row r="17" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="90" t="s">
+      <c r="C17" s="95" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="10"/>
@@ -2511,7 +2610,7 @@
     <row r="18" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="90"/>
+      <c r="C18" s="95"/>
       <c r="D18" s="10"/>
       <c r="E18" s="6"/>
       <c r="F18" s="8"/>
@@ -2570,7 +2669,7 @@
     <row r="21" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="92" t="s">
+      <c r="C21" s="97" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="10"/>
@@ -2591,7 +2690,7 @@
     <row r="22" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="92"/>
+      <c r="C22" s="97"/>
       <c r="D22" s="10"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -2629,7 +2728,7 @@
     <row r="24" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="92" t="s">
+      <c r="C24" s="97" t="s">
         <v>16</v>
       </c>
       <c r="D24" s="10"/>
@@ -2650,7 +2749,7 @@
     <row r="25" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="92"/>
+      <c r="C25" s="97"/>
       <c r="D25" s="10"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -2688,8 +2787,8 @@
     <row r="27" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="92" t="s">
-        <v>111</v>
+      <c r="C27" s="97" t="s">
+        <v>92</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="6"/>
@@ -2709,7 +2808,7 @@
     <row r="28" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="92"/>
+      <c r="C28" s="97"/>
       <c r="D28" s="10"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -2747,8 +2846,8 @@
     <row r="30" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="92" t="s">
-        <v>112</v>
+      <c r="C30" s="97" t="s">
+        <v>93</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="6"/>
@@ -2768,7 +2867,7 @@
     <row r="31" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="92"/>
+      <c r="C31" s="97"/>
       <c r="D31" s="10"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -2806,8 +2905,8 @@
     <row r="33" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="92" t="s">
-        <v>113</v>
+      <c r="C33" s="97" t="s">
+        <v>94</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="6"/>
@@ -2827,7 +2926,7 @@
     <row r="34" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="6"/>
-      <c r="C34" s="92"/>
+      <c r="C34" s="97"/>
       <c r="D34" s="10"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -2905,7 +3004,7 @@
     <row r="38" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
       <c r="B38" s="6"/>
-      <c r="C38" s="93" t="s">
+      <c r="C38" s="98" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="10"/>
@@ -2926,7 +3025,7 @@
     <row r="39" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
       <c r="B39" s="6"/>
-      <c r="C39" s="93"/>
+      <c r="C39" s="98"/>
       <c r="D39" s="10"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
@@ -2964,7 +3063,7 @@
     <row r="41" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="93" t="s">
+      <c r="C41" s="98" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="10"/>
@@ -2985,7 +3084,7 @@
     <row r="42" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16"/>
       <c r="B42" s="6"/>
-      <c r="C42" s="93"/>
+      <c r="C42" s="98"/>
       <c r="D42" s="10"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
@@ -3023,8 +3122,8 @@
     <row r="44" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="93" t="s">
-        <v>137</v>
+      <c r="C44" s="98" t="s">
+        <v>118</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="6"/>
@@ -3044,7 +3143,7 @@
     <row r="45" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="16"/>
       <c r="B45" s="6"/>
-      <c r="C45" s="93"/>
+      <c r="C45" s="98"/>
       <c r="D45" s="10"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
@@ -3082,8 +3181,8 @@
     <row r="47" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="93" t="s">
-        <v>114</v>
+      <c r="C47" s="98" t="s">
+        <v>95</v>
       </c>
       <c r="D47" s="10"/>
       <c r="E47" s="6"/>
@@ -3103,7 +3202,7 @@
     <row r="48" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="16"/>
       <c r="B48" s="6"/>
-      <c r="C48" s="93"/>
+      <c r="C48" s="98"/>
       <c r="D48" s="10"/>
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
@@ -3141,8 +3240,8 @@
     <row r="50" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="93" t="s">
-        <v>138</v>
+      <c r="C50" s="98" t="s">
+        <v>119</v>
       </c>
       <c r="D50" s="10"/>
       <c r="E50" s="6"/>
@@ -3162,7 +3261,7 @@
     <row r="51" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="16"/>
       <c r="B51" s="6"/>
-      <c r="C51" s="93"/>
+      <c r="C51" s="98"/>
       <c r="D51" s="10"/>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
@@ -3221,8 +3320,8 @@
     <row r="54" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16"/>
       <c r="B54" s="6"/>
-      <c r="C54" s="91" t="s">
-        <v>115</v>
+      <c r="C54" s="96" t="s">
+        <v>96</v>
       </c>
       <c r="D54" s="10"/>
       <c r="E54" s="6"/>
@@ -3242,7 +3341,7 @@
     <row r="55" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="91"/>
+      <c r="C55" s="96"/>
       <c r="D55" s="10"/>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
@@ -3280,8 +3379,8 @@
     <row r="57" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="16"/>
       <c r="B57" s="6"/>
-      <c r="C57" s="91" t="s">
-        <v>116</v>
+      <c r="C57" s="96" t="s">
+        <v>97</v>
       </c>
       <c r="D57" s="10"/>
       <c r="E57" s="6"/>
@@ -3301,7 +3400,7 @@
     <row r="58" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="91"/>
+      <c r="C58" s="96"/>
       <c r="D58" s="10"/>
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
@@ -3339,8 +3438,8 @@
     <row r="60" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="16"/>
       <c r="B60" s="6"/>
-      <c r="C60" s="91" t="s">
-        <v>136</v>
+      <c r="C60" s="96" t="s">
+        <v>117</v>
       </c>
       <c r="D60" s="10"/>
       <c r="E60" s="6"/>
@@ -3360,7 +3459,7 @@
     <row r="61" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="16"/>
       <c r="B61" s="6"/>
-      <c r="C61" s="91"/>
+      <c r="C61" s="96"/>
       <c r="D61" s="10"/>
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
@@ -3398,8 +3497,8 @@
     <row r="63" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="16"/>
       <c r="B63" s="6"/>
-      <c r="C63" s="91" t="s">
-        <v>135</v>
+      <c r="C63" s="96" t="s">
+        <v>116</v>
       </c>
       <c r="D63" s="10"/>
       <c r="E63" s="6"/>
@@ -3419,7 +3518,7 @@
     <row r="64" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="16"/>
       <c r="B64" s="6"/>
-      <c r="C64" s="91"/>
+      <c r="C64" s="96"/>
       <c r="D64" s="10"/>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
@@ -3457,8 +3556,8 @@
     <row r="66" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="16"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="91" t="s">
-        <v>134</v>
+      <c r="C66" s="96" t="s">
+        <v>115</v>
       </c>
       <c r="D66" s="10"/>
       <c r="E66" s="6"/>
@@ -3478,7 +3577,7 @@
     <row r="67" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="16"/>
       <c r="B67" s="6"/>
-      <c r="C67" s="91"/>
+      <c r="C67" s="96"/>
       <c r="D67" s="10"/>
       <c r="E67" s="6"/>
       <c r="F67" s="6"/>
@@ -3516,8 +3615,8 @@
     <row r="69" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="91" t="s">
-        <v>133</v>
+      <c r="C69" s="96" t="s">
+        <v>114</v>
       </c>
       <c r="D69" s="10"/>
       <c r="E69" s="6"/>
@@ -3537,7 +3636,7 @@
     <row r="70" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="16"/>
       <c r="B70" s="6"/>
-      <c r="C70" s="91"/>
+      <c r="C70" s="96"/>
       <c r="D70" s="10"/>
       <c r="E70" s="6"/>
       <c r="F70" s="6"/>
@@ -3575,7 +3674,7 @@
     <row r="72" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16"/>
       <c r="B72" s="6"/>
-      <c r="C72" s="95" t="s">
+      <c r="C72" s="100" t="s">
         <v>56</v>
       </c>
       <c r="D72" s="7"/>
@@ -3596,7 +3695,7 @@
     <row r="73" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="16"/>
       <c r="B73" s="6"/>
-      <c r="C73" s="95"/>
+      <c r="C73" s="100"/>
       <c r="D73" s="7"/>
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
@@ -3615,8 +3714,8 @@
     <row r="74" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16"/>
       <c r="B74" s="6"/>
-      <c r="C74" s="97" t="s">
-        <v>109</v>
+      <c r="C74" s="102" t="s">
+        <v>90</v>
       </c>
       <c r="D74" s="7"/>
       <c r="E74" s="6"/>
@@ -3686,7 +3785,7 @@
     <row r="75" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="16"/>
       <c r="B75" s="6"/>
-      <c r="C75" s="97"/>
+      <c r="C75" s="102"/>
       <c r="D75" s="7"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
@@ -3814,18 +3913,18 @@
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
-      <c r="F79" s="96"/>
-      <c r="G79" s="96"/>
+      <c r="F79" s="101"/>
+      <c r="G79" s="101"/>
       <c r="H79" s="6"/>
       <c r="I79" s="38" t="s">
         <v>58</v>
       </c>
       <c r="J79" s="38"/>
       <c r="K79" s="6"/>
-      <c r="L79" s="94" t="s">
+      <c r="L79" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="M79" s="94"/>
+      <c r="M79" s="99"/>
       <c r="N79" s="40"/>
       <c r="O79" s="5"/>
       <c r="P79" s="5"/>
@@ -3851,18 +3950,70 @@
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C82" s="4" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C83" s="4" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C84" s="4" t="s">
-        <v>181</v>
-      </c>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C85" s="86" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C86" s="86" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C87" s="86"/>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C88" s="86"/>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C89" s="86"/>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C90" s="86"/>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C91" s="86"/>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C92" s="86"/>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C93" s="86"/>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C94" s="86"/>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C95" s="86"/>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C96" s="86"/>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C97" s="86"/>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C98" s="86"/>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C99" s="85"/>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C100" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="27">
@@ -3923,46 +4074,46 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="98" t="s">
+      <c r="A3" s="103" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="C3" s="58"/>
       <c r="D3" s="58"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="98"/>
+      <c r="A4" s="103"/>
       <c r="B4" s="1" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="98"/>
+      <c r="A5" s="103"/>
       <c r="B5" s="1" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -3976,19 +4127,19 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" s="61" t="s">
         <v>122</v>
       </c>
-      <c r="F6" s="61" t="s">
-        <v>141</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -4021,65 +4172,65 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="C1" s="70"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="C2" s="60"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="C3" s="59"/>
       <c r="E3" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="C5" s="67"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="C6" s="68"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="C7" s="69"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="C10" s="71"/>
       <c r="D10" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="C11" s="72"/>
       <c r="D11">
@@ -4088,7 +4239,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="C12" s="73"/>
       <c r="D12">
@@ -4097,7 +4248,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="C13" s="69"/>
       <c r="D13">
@@ -4106,7 +4257,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -4114,12 +4265,12 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="C40" s="55"/>
     </row>
@@ -4225,10 +4376,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H54"/>
+  <dimension ref="B2:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4239,7 +4390,7 @@
     <col min="4" max="4" width="27.875" style="43" customWidth="1"/>
     <col min="5" max="5" width="22.5" style="43" customWidth="1"/>
     <col min="6" max="6" width="19.875" style="43" customWidth="1"/>
-    <col min="7" max="7" width="26.375" style="43" customWidth="1"/>
+    <col min="7" max="7" width="27.25" style="43" customWidth="1"/>
     <col min="8" max="8" width="28.25" style="43" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="8.75" style="43"/>
   </cols>
@@ -4247,26 +4398,26 @@
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="41"/>
       <c r="C2" s="42" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="D2" s="42" t="s">
         <v>36</v>
       </c>
       <c r="E2" s="42" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="F2" s="42" t="s">
         <v>37</v>
       </c>
       <c r="G2" s="42" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="H2" s="42" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="101" t="s">
+      <c r="B3" s="106" t="s">
         <v>41</v>
       </c>
       <c r="C3" s="44" t="s">
@@ -4285,451 +4436,471 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="102"/>
-      <c r="C4" s="105" t="s">
+      <c r="B4" s="107"/>
+      <c r="C4" s="110" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="105" t="s">
+      <c r="D4" s="110" t="s">
         <v>40</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="F4" s="45"/>
       <c r="G4" s="45"/>
       <c r="H4" s="45" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="102"/>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
       <c r="E5" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5" s="45" t="s">
         <v>144</v>
       </c>
-      <c r="F5" s="45" t="s">
-        <v>164</v>
-      </c>
       <c r="G5" s="45" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="H5" s="45" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="F6" s="45" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="102"/>
-      <c r="C6" s="102"/>
-      <c r="D6" s="102"/>
-      <c r="E6" s="45" t="s">
-        <v>145</v>
-      </c>
-      <c r="F6" s="45" t="s">
-        <v>166</v>
-      </c>
       <c r="G6" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="H6" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="H6" s="45" t="s">
-        <v>167</v>
-      </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
+      <c r="B7" s="108"/>
+      <c r="C7" s="108"/>
+      <c r="D7" s="108"/>
       <c r="E7" s="45" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="F7" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="G7" s="45" t="s">
         <v>142</v>
       </c>
-      <c r="G7" s="45" t="s">
-        <v>162</v>
-      </c>
       <c r="H7" s="45" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="56"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
       <c r="E8" s="45"/>
       <c r="F8" s="45"/>
       <c r="G8" s="45"/>
       <c r="H8" s="45"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="56"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="45"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="84"/>
+      <c r="D9" s="84" t="s">
+        <v>242</v>
+      </c>
+      <c r="E9" s="45" t="s">
+        <v>237</v>
+      </c>
       <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
+      <c r="G9" s="45" t="s">
+        <v>238</v>
+      </c>
+      <c r="H9" s="45" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="64"/>
-      <c r="C10" s="57" t="s">
-        <v>148</v>
-      </c>
-      <c r="D10" s="57" t="s">
-        <v>149</v>
+      <c r="B10" s="83"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84" t="s">
+        <v>241</v>
       </c>
       <c r="E10" s="45" t="s">
-        <v>184</v>
-      </c>
-      <c r="F10" s="45" t="s">
-        <v>185</v>
-      </c>
-      <c r="G10" s="45" t="s">
-        <v>186</v>
-      </c>
-      <c r="H10" s="45" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="56"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
+        <v>240</v>
+      </c>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="83"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="84"/>
       <c r="E11" s="45"/>
       <c r="F11" s="45"/>
       <c r="G11" s="45"/>
       <c r="H11" s="45"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="56"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="84"/>
       <c r="E12" s="45"/>
       <c r="F12" s="45"/>
       <c r="G12" s="45"/>
       <c r="H12" s="45"/>
     </row>
-    <row r="13" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="111" t="s">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="83"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="83"/>
+      <c r="C14" s="84"/>
+      <c r="D14" s="84"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="83"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="83"/>
+      <c r="C16" s="84"/>
+      <c r="D16" s="84"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="83"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="84"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="83"/>
+      <c r="C18" s="84"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="83"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="84"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="56"/>
+      <c r="C20" s="57" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="F20" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="G20" s="45" t="s">
+        <v>165</v>
+      </c>
+      <c r="H20" s="45" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="116" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="109" t="s">
+      <c r="C21" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="109" t="s">
+      <c r="D21" s="114" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="47" t="s">
-        <v>157</v>
-      </c>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="112"/>
-      <c r="C14" s="110"/>
-      <c r="D14" s="110"/>
-      <c r="E14" s="47" t="s">
+      <c r="E21" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="117"/>
+      <c r="C22" s="115"/>
+      <c r="D22" s="115"/>
+      <c r="E22" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="47" t="s">
-        <v>150</v>
-      </c>
-      <c r="G14" s="47" t="s">
+      <c r="F22" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="G22" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="H22" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="117"/>
+      <c r="C23" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="47" t="s">
+        <v>171</v>
+      </c>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47" t="s">
+        <v>167</v>
+      </c>
+      <c r="H23" s="48" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="117"/>
+      <c r="C24" s="114" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="114" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="47" t="s">
+        <v>172</v>
+      </c>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="117"/>
+      <c r="C25" s="115"/>
+      <c r="D25" s="115"/>
+      <c r="E25" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="F25" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="G25" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="H25" s="47" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="117"/>
+      <c r="C26" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="H26" s="48" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="117"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="48"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="117"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="48"/>
+    </row>
+    <row r="29" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="117"/>
+      <c r="C29" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="74" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="74" t="s">
+        <v>179</v>
+      </c>
+      <c r="F29" s="74" t="s">
+        <v>181</v>
+      </c>
+      <c r="G29" s="74" t="s">
+        <v>180</v>
+      </c>
+      <c r="H29" s="74" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="117"/>
+      <c r="C30" s="119" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="119" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="119" t="s">
+        <v>188</v>
+      </c>
+      <c r="F30" s="104" t="s">
+        <v>191</v>
+      </c>
+      <c r="G30" s="104" t="s">
         <v>190</v>
       </c>
-      <c r="H14" s="48" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="112"/>
-      <c r="C15" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="47" t="s">
-        <v>192</v>
-      </c>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47" t="s">
+      <c r="H30" s="119" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="117"/>
+      <c r="C31" s="120"/>
+      <c r="D31" s="120"/>
+      <c r="E31" s="120"/>
+      <c r="F31" s="105"/>
+      <c r="G31" s="105"/>
+      <c r="H31" s="120"/>
+    </row>
+    <row r="32" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B32" s="117"/>
+      <c r="C32" s="82"/>
+      <c r="D32" s="80" t="s">
+        <v>185</v>
+      </c>
+      <c r="E32" s="79" t="s">
+        <v>186</v>
+      </c>
+      <c r="F32" s="78" t="s">
+        <v>228</v>
+      </c>
+      <c r="G32" s="79" t="s">
+        <v>187</v>
+      </c>
+      <c r="H32" s="79" t="s">
         <v>188</v>
       </c>
-      <c r="H15" s="48" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="112"/>
-      <c r="C16" s="109" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="109" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="47" t="s">
+    </row>
+    <row r="33" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B33" s="117"/>
+      <c r="C33" s="119"/>
+      <c r="D33" s="119" t="s">
+        <v>194</v>
+      </c>
+      <c r="E33" s="81" t="s">
+        <v>195</v>
+      </c>
+      <c r="F33" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="G33" s="79" t="s">
+        <v>203</v>
+      </c>
+      <c r="H33" s="74" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B34" s="117"/>
+      <c r="C34" s="120"/>
+      <c r="D34" s="120"/>
+      <c r="E34" s="81" t="s">
+        <v>197</v>
+      </c>
+      <c r="F34" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="G34" s="79" t="s">
+        <v>198</v>
+      </c>
+      <c r="H34" s="79" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="B35" s="117"/>
+      <c r="C35" s="75"/>
+      <c r="D35" s="82" t="s">
         <v>193</v>
       </c>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="112"/>
-      <c r="C17" s="110"/>
-      <c r="D17" s="110"/>
-      <c r="E17" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="F17" s="48" t="s">
-        <v>189</v>
-      </c>
-      <c r="G17" s="47" t="s">
-        <v>196</v>
-      </c>
-      <c r="H17" s="47" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="112"/>
-      <c r="C18" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="E18" s="48" t="s">
-        <v>197</v>
-      </c>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48" t="s">
-        <v>198</v>
-      </c>
-      <c r="H18" s="48" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="112"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="66"/>
-      <c r="H19" s="48"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="112"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="66"/>
-      <c r="H20" s="48"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="112"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="48"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="112"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="48"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="112"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="48"/>
-    </row>
-    <row r="24" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="112"/>
-      <c r="C24" s="74" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="74" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="74" t="s">
-        <v>200</v>
-      </c>
-      <c r="F24" s="74" t="s">
-        <v>202</v>
-      </c>
-      <c r="G24" s="74" t="s">
-        <v>201</v>
-      </c>
-      <c r="H24" s="74" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="112"/>
-      <c r="C25" s="74" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" s="74" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="74" t="s">
-        <v>210</v>
-      </c>
-      <c r="F25" s="99" t="s">
-        <v>213</v>
-      </c>
-      <c r="G25" s="99" t="s">
-        <v>212</v>
-      </c>
-      <c r="H25" s="74" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="112"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="79"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="100"/>
-      <c r="G26" s="100"/>
-      <c r="H26" s="78"/>
-    </row>
-    <row r="27" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B27" s="112"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="79" t="s">
-        <v>211</v>
-      </c>
-      <c r="E27" s="78"/>
-      <c r="F27" s="81" t="s">
-        <v>214</v>
-      </c>
-      <c r="G27" s="78"/>
-      <c r="H27" s="78"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="112"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="79"/>
-      <c r="E28" s="78"/>
-      <c r="F28" s="78"/>
-      <c r="G28" s="78"/>
-      <c r="H28" s="78"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="112"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="75" t="s">
+      <c r="E35" s="81" t="s">
+        <v>208</v>
+      </c>
+      <c r="F35" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="G35" s="81" t="s">
+        <v>209</v>
+      </c>
+      <c r="H35" s="81" t="s">
         <v>206</v>
       </c>
-      <c r="E29" s="74" t="s">
-        <v>207</v>
-      </c>
-      <c r="F29" s="74" t="s">
-        <v>208</v>
-      </c>
-      <c r="G29" s="74" t="s">
-        <v>209</v>
-      </c>
-      <c r="H29" s="74" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="112"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="75" t="s">
-        <v>218</v>
-      </c>
-      <c r="E30" s="74" t="s">
-        <v>219</v>
-      </c>
-      <c r="F30" s="74" t="s">
-        <v>216</v>
-      </c>
-      <c r="G30" s="74"/>
-      <c r="H30" s="74" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B31" s="112"/>
-      <c r="C31" s="75"/>
-      <c r="D31" s="80"/>
-      <c r="E31" s="74" t="s">
-        <v>221</v>
-      </c>
-      <c r="F31" s="81" t="s">
-        <v>222</v>
-      </c>
-      <c r="G31" s="74" t="s">
-        <v>223</v>
-      </c>
-      <c r="H31" s="74"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="112"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="75" t="s">
-        <v>215</v>
-      </c>
-      <c r="E32" s="74"/>
-      <c r="F32" s="74"/>
-      <c r="G32" s="74"/>
-      <c r="H32" s="74"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="112"/>
-      <c r="C33" s="75"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="74"/>
-      <c r="G33" s="74"/>
-      <c r="H33" s="74"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="112"/>
-      <c r="C34" s="75"/>
-      <c r="D34" s="75"/>
-      <c r="E34" s="74"/>
-      <c r="F34" s="74"/>
-      <c r="G34" s="74"/>
-      <c r="H34" s="74"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="112"/>
-      <c r="C35" s="75"/>
-      <c r="D35" s="75"/>
-      <c r="E35" s="74"/>
-      <c r="F35" s="74"/>
-      <c r="G35" s="74"/>
-      <c r="H35" s="74"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="112"/>
-      <c r="C36" s="104" t="s">
+      <c r="B36" s="117"/>
+      <c r="C36" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="D36" s="104" t="s">
+      <c r="D36" s="109" t="s">
         <v>47</v>
       </c>
       <c r="E36" s="49" t="s">
@@ -4738,286 +4909,344 @@
       <c r="F36" s="49"/>
       <c r="G36" s="50"/>
       <c r="H36" s="49" t="s">
-        <v>106</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="112"/>
-      <c r="C37" s="104"/>
-      <c r="D37" s="104"/>
+      <c r="B37" s="117"/>
+      <c r="C37" s="109"/>
+      <c r="D37" s="109"/>
       <c r="E37" s="49" t="s">
+        <v>211</v>
+      </c>
+      <c r="F37" s="78" t="s">
+        <v>223</v>
+      </c>
+      <c r="G37" s="49" t="s">
+        <v>212</v>
+      </c>
+      <c r="H37" s="49" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B38" s="117"/>
+      <c r="C38" s="119" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="119" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38" s="74" t="s">
+        <v>213</v>
+      </c>
+      <c r="F38" s="78" t="s">
+        <v>220</v>
+      </c>
+      <c r="G38" s="74" t="s">
+        <v>214</v>
+      </c>
+      <c r="H38" s="74" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B39" s="117"/>
+      <c r="C39" s="120"/>
+      <c r="D39" s="120"/>
+      <c r="E39" s="74" t="s">
+        <v>215</v>
+      </c>
+      <c r="F39" s="78" t="s">
+        <v>221</v>
+      </c>
+      <c r="G39" s="74" t="s">
+        <v>219</v>
+      </c>
+      <c r="H39" s="74" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B40" s="117"/>
+      <c r="C40" s="81" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="F37" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="G37" s="49" t="s">
-        <v>88</v>
-      </c>
-      <c r="H37" s="49"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="112"/>
-      <c r="C38" s="75" t="s">
-        <v>46</v>
-      </c>
-      <c r="D38" s="75" t="s">
-        <v>54</v>
-      </c>
-      <c r="E38" s="74" t="s">
-        <v>83</v>
-      </c>
-      <c r="F38" s="74"/>
-      <c r="G38" s="74" t="s">
-        <v>96</v>
-      </c>
-      <c r="H38" s="74" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B39" s="112"/>
-      <c r="C39" s="76"/>
-      <c r="D39" s="76"/>
-      <c r="E39" s="74" t="s">
-        <v>84</v>
-      </c>
-      <c r="F39" s="74" t="s">
-        <v>94</v>
-      </c>
-      <c r="G39" s="74" t="s">
-        <v>89</v>
-      </c>
-      <c r="H39" s="74" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="112"/>
-      <c r="C40" s="74" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" s="74" t="s">
-        <v>53</v>
-      </c>
-      <c r="E40" s="74" t="s">
-        <v>85</v>
-      </c>
-      <c r="F40" s="74" t="s">
-        <v>151</v>
-      </c>
-      <c r="G40" s="74" t="s">
-        <v>90</v>
-      </c>
-      <c r="H40" s="74" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B41" s="112"/>
-      <c r="C41" s="75"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="74"/>
-      <c r="F41" s="74"/>
-      <c r="G41" s="74"/>
-      <c r="H41" s="74"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B42" s="112"/>
-      <c r="C42" s="75"/>
-      <c r="D42" s="75"/>
-      <c r="E42" s="74"/>
-      <c r="F42" s="74"/>
-      <c r="G42" s="74"/>
-      <c r="H42" s="74"/>
-    </row>
-    <row r="43" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="112"/>
-      <c r="C43" s="115" t="s">
+      <c r="F40" s="78" t="s">
+        <v>222</v>
+      </c>
+      <c r="G40" s="81" t="s">
+        <v>224</v>
+      </c>
+      <c r="H40" s="81" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B41" s="117"/>
+      <c r="C41" s="119" t="s">
         <v>51</v>
       </c>
-      <c r="D43" s="115" t="s">
+      <c r="D41" s="119" t="s">
         <v>52</v>
       </c>
-      <c r="E43" s="74" t="s">
-        <v>86</v>
-      </c>
-      <c r="F43" s="74" t="s">
-        <v>95</v>
-      </c>
-      <c r="G43" s="74" t="s">
-        <v>91</v>
-      </c>
-      <c r="H43" s="74" t="s">
-        <v>108</v>
-      </c>
+      <c r="E41" s="74" t="s">
+        <v>229</v>
+      </c>
+      <c r="F41" s="78" t="s">
+        <v>234</v>
+      </c>
+      <c r="G41" s="74" t="s">
+        <v>233</v>
+      </c>
+      <c r="H41" s="74" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B42" s="117"/>
+      <c r="C42" s="120"/>
+      <c r="D42" s="120"/>
+      <c r="E42" s="74" t="s">
+        <v>235</v>
+      </c>
+      <c r="F42" s="78" t="s">
+        <v>230</v>
+      </c>
+      <c r="G42" s="74" t="s">
+        <v>236</v>
+      </c>
+      <c r="H42" s="74" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" s="117"/>
+      <c r="C43" s="82"/>
+      <c r="D43" s="82"/>
+      <c r="E43" s="81"/>
+      <c r="F43" s="81"/>
+      <c r="G43" s="81"/>
+      <c r="H43" s="81"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B44" s="113"/>
-      <c r="C44" s="116"/>
-      <c r="D44" s="116"/>
-      <c r="E44" s="74" t="s">
-        <v>87</v>
-      </c>
-      <c r="F44" s="74" t="s">
-        <v>93</v>
-      </c>
-      <c r="G44" s="74" t="s">
-        <v>92</v>
-      </c>
-      <c r="H44" s="74" t="s">
-        <v>98</v>
-      </c>
+      <c r="B44" s="117"/>
+      <c r="C44" s="82"/>
+      <c r="D44" s="82"/>
+      <c r="E44" s="81"/>
+      <c r="F44" s="81"/>
+      <c r="G44" s="81"/>
+      <c r="H44" s="81"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B45" s="106" t="s">
+      <c r="B45" s="117"/>
+      <c r="C45" s="82"/>
+      <c r="D45" s="82"/>
+      <c r="E45" s="81"/>
+      <c r="F45" s="81"/>
+      <c r="G45" s="81"/>
+      <c r="H45" s="81"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B46" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="114" t="s">
-        <v>59</v>
-      </c>
-      <c r="D45" s="114" t="s">
-        <v>61</v>
-      </c>
-      <c r="E45" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="F45" s="46"/>
-      <c r="G45" s="46"/>
-      <c r="H45" s="46" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B46" s="107"/>
-      <c r="C46" s="114"/>
-      <c r="D46" s="114"/>
-      <c r="E46" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="F46" s="46" t="s">
-        <v>143</v>
-      </c>
-      <c r="G46" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="H46" s="46" t="s">
-        <v>104</v>
-      </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B47" s="107"/>
-      <c r="C47" s="62"/>
-      <c r="D47" s="62"/>
-      <c r="E47" s="62"/>
-      <c r="F47" s="62"/>
-      <c r="G47" s="62"/>
-      <c r="H47" s="62"/>
+      <c r="B47" s="112"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B48" s="108"/>
-      <c r="C48" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="D48" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="E48" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="F48" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="G48" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="H48" s="46" t="s">
-        <v>97</v>
-      </c>
+      <c r="B48" s="112"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B49" s="63"/>
-      <c r="C49" s="65"/>
-      <c r="D49" s="65" t="s">
-        <v>156</v>
-      </c>
-      <c r="E49" s="62"/>
-      <c r="F49" s="62"/>
-      <c r="G49" s="62"/>
-      <c r="H49" s="62"/>
+      <c r="B49" s="113"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B50" s="63"/>
-      <c r="C50" s="65"/>
-      <c r="D50" s="65" t="s">
-        <v>152</v>
-      </c>
-      <c r="E50" s="62"/>
-      <c r="F50" s="62"/>
-      <c r="G50" s="62"/>
-      <c r="H50" s="62"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B51" s="63"/>
-      <c r="C51" s="65"/>
-      <c r="D51" s="65" t="s">
-        <v>153</v>
-      </c>
-      <c r="E51" s="62"/>
-      <c r="F51" s="62"/>
-      <c r="G51" s="62"/>
-      <c r="H51" s="62"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B52" s="63"/>
-      <c r="C52" s="65"/>
-      <c r="D52" s="65" t="s">
-        <v>154</v>
-      </c>
-      <c r="E52" s="62"/>
-      <c r="F52" s="62"/>
-      <c r="G52" s="62"/>
-      <c r="H52" s="62"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B53" s="63"/>
-      <c r="C53" s="65"/>
-      <c r="D53" s="65" t="s">
-        <v>155</v>
-      </c>
-      <c r="E53" s="62"/>
-      <c r="F53" s="62"/>
-      <c r="G53" s="62"/>
-      <c r="H53" s="62"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B54" s="63"/>
-      <c r="C54" s="65"/>
-      <c r="D54" s="65"/>
-      <c r="E54" s="62"/>
-      <c r="F54" s="62"/>
-      <c r="G54" s="62"/>
-      <c r="H54" s="62"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B55" s="63"/>
+    </row>
+    <row r="63" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="D63" s="77" t="s">
+        <v>189</v>
+      </c>
+      <c r="E63" s="79" t="s">
+        <v>205</v>
+      </c>
+      <c r="F63" s="78" t="s">
+        <v>192</v>
+      </c>
+      <c r="G63" s="79" t="s">
+        <v>202</v>
+      </c>
+      <c r="H63" s="76" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="70" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C70" s="118" t="s">
+        <v>59</v>
+      </c>
+      <c r="D70" s="118" t="s">
+        <v>61</v>
+      </c>
+      <c r="E70" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="F70" s="46"/>
+      <c r="G70" s="46"/>
+      <c r="H70" s="46" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="71" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C71" s="118"/>
+      <c r="D71" s="118"/>
+      <c r="E71" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="F71" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="G71" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="H71" s="46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C72" s="62"/>
+      <c r="D72" s="62"/>
+      <c r="E72" s="62"/>
+      <c r="F72" s="62"/>
+      <c r="G72" s="62"/>
+      <c r="H72" s="62"/>
+    </row>
+    <row r="73" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C73" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="D73" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="E73" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="F73" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="G73" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="H73" s="46" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="74" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C74" s="65"/>
+      <c r="D74" s="65" t="s">
+        <v>136</v>
+      </c>
+      <c r="E74" s="62"/>
+      <c r="F74" s="62"/>
+      <c r="G74" s="62"/>
+      <c r="H74" s="62"/>
+    </row>
+    <row r="75" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C75" s="65"/>
+      <c r="D75" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="E75" s="62"/>
+      <c r="F75" s="62"/>
+      <c r="G75" s="62"/>
+      <c r="H75" s="62"/>
+    </row>
+    <row r="76" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C76" s="65"/>
+      <c r="D76" s="65" t="s">
+        <v>133</v>
+      </c>
+      <c r="E76" s="62"/>
+      <c r="F76" s="62"/>
+      <c r="G76" s="62"/>
+      <c r="H76" s="62"/>
+    </row>
+    <row r="77" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C77" s="65"/>
+      <c r="D77" s="65" t="s">
+        <v>134</v>
+      </c>
+      <c r="E77" s="62"/>
+      <c r="F77" s="62"/>
+      <c r="G77" s="62"/>
+      <c r="H77" s="62"/>
+    </row>
+    <row r="78" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C78" s="65"/>
+      <c r="D78" s="65" t="s">
+        <v>135</v>
+      </c>
+      <c r="E78" s="62"/>
+      <c r="F78" s="62"/>
+      <c r="G78" s="62"/>
+      <c r="H78" s="62"/>
+    </row>
+    <row r="79" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C79" s="65"/>
+      <c r="D79" s="65"/>
+      <c r="E79" s="62"/>
+      <c r="F79" s="62"/>
+      <c r="G79" s="62"/>
+      <c r="H79" s="62"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="B13:B44"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
+  <mergeCells count="25">
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B21:B45"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
     <mergeCell ref="D36:D37"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="F30:F31"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="C36:C37"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="D4:D7"/>
+    <mergeCell ref="E30:E31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Auto push 2023-03-25 23:46:25.55
</commit_message>
<xml_diff>
--- a/project/CheeYoonMovie.xlsx
+++ b/project/CheeYoonMovie.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="254">
   <si>
     <t>이용자 권한과 기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,15 +72,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>메인화면(해더, 풋터)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>공통 모듈 구현</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자유게시판(답변, 페이징)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -396,18 +388,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>영화 목록 (상영작, 예고작)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>관리자 등록, 삭제</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>영화 등록, 수정, 보기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>영화 검색, 조회</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -480,18 +464,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>회원 제재 (회원 목록)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>배우 등록, 수정, 보기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화 검색 (이름,태그), 배우 검색</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>영화 상세보기, 배우 상세보기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -656,10 +628,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>21화요일 회원가입,로그인페이지생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>로그인 그라데이션</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -772,11 +740,6 @@
   </si>
   <si>
     <t>댓글 리스트 출력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardContentService.java
-CommentListService</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -814,15 +777,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>24금요일 자유게시판 댓글</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>23목요일 회원가입 로그인, 자유게시판 댓글</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>22수요일 메인페이지css조정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -990,14 +945,103 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>nowPlayingContent.do</t>
-  </si>
-  <si>
-    <t>현재 상영작 상세보기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>현재 상영영화 리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인화면(header,footer,sidebar)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>24금요일 자유게시판, 댓글, 현재상영작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자유게시판 조회 (답변, 페이징)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 검색 (이름,태그), 배우 검색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 상영작 리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상영 예고작 리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 랭킹 리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 제재 (회원 목록)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화,인물 등록, 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자유게시판 답변글 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21화요일 메인페이지틀,회원가입,로그인페이지틀 , css</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22수요일 메인페이지css조정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movieId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 상세보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상영 예고작 리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>upComingList.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movie/upComingList.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>25토요일 현재상영작,상영예고작, 영화상세보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>26일요일 영화 상세보기 , 영화랭킹리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardContentService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MovieContentService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UpComingListService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movieContent.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movie/movieContent.jsp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1535,7 +1579,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1605,9 +1649,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1797,6 +1838,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1848,55 +1898,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2245,10 +2295,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BP100"/>
+  <dimension ref="A1:BP105"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView topLeftCell="A34" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.25" defaultRowHeight="11.25" x14ac:dyDescent="0.3"/>
@@ -2267,41 +2317,41 @@
     <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="88" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
+      <c r="B2" s="90" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="91"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
+      <c r="O3" s="91"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
@@ -2346,67 +2396,67 @@
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20"/>
-      <c r="C6" s="90" t="s">
+      <c r="C6" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="92" t="s">
+      <c r="D6" s="38"/>
+      <c r="E6" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="94" t="s">
-        <v>35</v>
-      </c>
-      <c r="M6" s="92"/>
-      <c r="N6" s="92"/>
-      <c r="O6" s="92"/>
+      <c r="F6" s="94"/>
+      <c r="G6" s="94"/>
+      <c r="H6" s="94"/>
+      <c r="I6" s="94"/>
+      <c r="J6" s="94"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="96" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="94"/>
+      <c r="N6" s="94"/>
+      <c r="O6" s="94"/>
       <c r="P6" s="21"/>
       <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="91"/>
+      <c r="C7" s="93"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="13">
+      <c r="E7" s="87">
         <v>20</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="87">
         <v>21</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="87">
         <v>22</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="87">
         <v>23</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="87">
         <v>24</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="87">
         <v>25</v>
       </c>
-      <c r="K7" s="23">
+      <c r="K7" s="88">
         <v>26</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="87">
         <v>27</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="87">
         <v>28</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="87">
         <v>29</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="87">
         <v>30</v>
       </c>
-      <c r="P7" s="24"/>
+      <c r="P7" s="23"/>
       <c r="Q7" s="5"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -2471,11 +2521,11 @@
     <row r="11" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="95" t="s">
-        <v>33</v>
+      <c r="C11" s="97" t="s">
+        <v>31</v>
       </c>
       <c r="D11" s="10"/>
-      <c r="E11" s="38"/>
+      <c r="E11" s="37"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -2492,7 +2542,7 @@
     <row r="12" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="95"/>
+      <c r="C12" s="97"/>
       <c r="D12" s="10"/>
       <c r="E12" s="8"/>
       <c r="F12" s="6"/>
@@ -2530,11 +2580,11 @@
     <row r="14" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="87" t="s">
-        <v>34</v>
+      <c r="C14" s="89" t="s">
+        <v>32</v>
       </c>
       <c r="D14" s="10"/>
-      <c r="E14" s="38"/>
+      <c r="E14" s="37"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
@@ -2551,7 +2601,7 @@
     <row r="15" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="87"/>
+      <c r="C15" s="89"/>
       <c r="D15" s="10"/>
       <c r="E15" s="8"/>
       <c r="F15" s="6"/>
@@ -2589,12 +2639,12 @@
     <row r="17" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="95" t="s">
+      <c r="C17" s="97" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="10"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="38"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -2610,10 +2660,10 @@
     <row r="18" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="95"/>
+      <c r="C18" s="97"/>
       <c r="D18" s="10"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -2669,16 +2719,16 @@
     <row r="21" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="97" t="s">
-        <v>12</v>
+      <c r="C21" s="99" t="s">
+        <v>230</v>
       </c>
       <c r="D21" s="10"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
@@ -2690,10 +2740,10 @@
     <row r="22" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="97"/>
+      <c r="C22" s="99"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
@@ -2728,16 +2778,16 @@
     <row r="24" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="97" t="s">
-        <v>16</v>
+      <c r="C24" s="99" t="s">
+        <v>14</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
@@ -2749,14 +2799,14 @@
     <row r="25" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="97"/>
+      <c r="C25" s="99"/>
       <c r="D25" s="10"/>
       <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
@@ -2787,16 +2837,16 @@
     <row r="27" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="97" t="s">
-        <v>92</v>
+      <c r="C27" s="99" t="s">
+        <v>90</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
@@ -2808,14 +2858,14 @@
     <row r="28" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="97"/>
+      <c r="C28" s="99"/>
       <c r="D28" s="10"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
+      <c r="J28" s="6"/>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
       <c r="M28" s="11"/>
@@ -2846,16 +2896,16 @@
     <row r="30" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="97" t="s">
-        <v>93</v>
+      <c r="C30" s="99" t="s">
+        <v>91</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
@@ -2867,14 +2917,14 @@
     <row r="31" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="97"/>
+      <c r="C31" s="99"/>
       <c r="D31" s="10"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
+      <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
@@ -2886,7 +2936,7 @@
     <row r="32" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="16"/>
       <c r="B32" s="6"/>
-      <c r="C32" s="10"/>
+      <c r="C32" s="6"/>
       <c r="D32" s="10"/>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
@@ -2905,17 +2955,17 @@
     <row r="33" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="97" t="s">
-        <v>94</v>
+      <c r="C33" s="99" t="s">
+        <v>239</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
-      <c r="I33" s="38"/>
-      <c r="J33" s="38"/>
-      <c r="K33" s="5"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
       <c r="N33" s="6"/>
@@ -2926,14 +2976,14 @@
     <row r="34" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="6"/>
-      <c r="C34" s="97"/>
+      <c r="C34" s="99"/>
       <c r="D34" s="10"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
       <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
+      <c r="J34" s="6"/>
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
@@ -2964,7 +3014,9 @@
     <row r="36" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="16"/>
       <c r="B36" s="6"/>
-      <c r="C36" s="10"/>
+      <c r="C36" s="99" t="s">
+        <v>92</v>
+      </c>
       <c r="D36" s="10"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
@@ -2972,7 +3024,7 @@
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
+      <c r="K36" s="5"/>
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
@@ -2980,13 +3032,11 @@
       <c r="P36" s="16"/>
       <c r="Q36" s="5"/>
     </row>
-    <row r="37" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
       <c r="B37" s="6"/>
-      <c r="C37" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="6"/>
+      <c r="C37" s="99"/>
+      <c r="D37" s="10"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
@@ -3004,17 +3054,15 @@
     <row r="38" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
       <c r="B38" s="6"/>
-      <c r="C38" s="98" t="s">
-        <v>15</v>
-      </c>
+      <c r="C38" s="10"/>
       <c r="D38" s="10"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="38"/>
-      <c r="I38" s="38"/>
-      <c r="J38" s="38"/>
-      <c r="K38" s="25"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
       <c r="L38" s="6"/>
       <c r="M38" s="6"/>
       <c r="N38" s="6"/>
@@ -3022,14 +3070,16 @@
       <c r="P38" s="16"/>
       <c r="Q38" s="5"/>
     </row>
-    <row r="39" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
       <c r="B39" s="6"/>
-      <c r="C39" s="98"/>
-      <c r="D39" s="10"/>
+      <c r="C39" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
-      <c r="G39" s="8"/>
+      <c r="G39" s="6"/>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
@@ -3044,15 +3094,17 @@
     <row r="40" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="6"/>
-      <c r="C40" s="10"/>
+      <c r="C40" s="100" t="s">
+        <v>13</v>
+      </c>
       <c r="D40" s="10"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
+      <c r="K40" s="24"/>
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
       <c r="N40" s="6"/>
@@ -3063,19 +3115,17 @@
     <row r="41" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="98" t="s">
-        <v>14</v>
-      </c>
+      <c r="C41" s="100"/>
       <c r="D41" s="10"/>
       <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
       <c r="K41" s="6"/>
-      <c r="L41" s="38"/>
-      <c r="M41" s="38"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
       <c r="N41" s="6"/>
       <c r="O41" s="6"/>
       <c r="P41" s="16"/>
@@ -3084,7 +3134,7 @@
     <row r="42" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16"/>
       <c r="B42" s="6"/>
-      <c r="C42" s="98"/>
+      <c r="C42" s="10"/>
       <c r="D42" s="10"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
@@ -3093,8 +3143,8 @@
       <c r="I42" s="6"/>
       <c r="J42" s="6"/>
       <c r="K42" s="6"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
       <c r="N42" s="6"/>
       <c r="O42" s="6"/>
       <c r="P42" s="16"/>
@@ -3103,12 +3153,14 @@
     <row r="43" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="16"/>
       <c r="B43" s="6"/>
-      <c r="C43" s="10"/>
+      <c r="C43" s="100" t="s">
+        <v>232</v>
+      </c>
       <c r="D43" s="10"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
+      <c r="H43" s="37"/>
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
       <c r="K43" s="6"/>
@@ -3122,28 +3174,26 @@
     <row r="44" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="98" t="s">
-        <v>118</v>
-      </c>
+      <c r="C44" s="100"/>
       <c r="D44" s="10"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
+      <c r="H44" s="8"/>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
-      <c r="L44" s="38"/>
-      <c r="M44" s="38"/>
-      <c r="N44" s="38"/>
-      <c r="O44" s="38"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="6"/>
+      <c r="N44" s="6"/>
+      <c r="O44" s="6"/>
       <c r="P44" s="16"/>
       <c r="Q44" s="5"/>
     </row>
     <row r="45" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="16"/>
       <c r="B45" s="6"/>
-      <c r="C45" s="98"/>
+      <c r="C45" s="10"/>
       <c r="D45" s="10"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
@@ -3153,8 +3203,8 @@
       <c r="J45" s="6"/>
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
-      <c r="M45" s="11"/>
-      <c r="N45" s="8"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
       <c r="O45" s="6"/>
       <c r="P45" s="16"/>
       <c r="Q45" s="5"/>
@@ -3162,39 +3212,38 @@
     <row r="46" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16"/>
       <c r="B46" s="6"/>
-      <c r="C46" s="10"/>
+      <c r="C46" s="100" t="s">
+        <v>234</v>
+      </c>
       <c r="D46" s="10"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
       <c r="K46" s="6"/>
       <c r="L46" s="6"/>
-      <c r="M46" s="11"/>
-      <c r="N46" s="11"/>
-      <c r="O46" s="6"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="6"/>
       <c r="P46" s="16"/>
       <c r="Q46" s="5"/>
     </row>
     <row r="47" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="98" t="s">
-        <v>95</v>
-      </c>
+      <c r="C47" s="100"/>
       <c r="D47" s="10"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
       <c r="K47" s="6"/>
-      <c r="L47" s="38"/>
-      <c r="M47" s="38"/>
-      <c r="N47" s="11"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="6"/>
       <c r="O47" s="6"/>
       <c r="P47" s="16"/>
       <c r="Q47" s="5"/>
@@ -3202,7 +3251,7 @@
     <row r="48" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="16"/>
       <c r="B48" s="6"/>
-      <c r="C48" s="98"/>
+      <c r="C48" s="10"/>
       <c r="D48" s="10"/>
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
@@ -3211,28 +3260,30 @@
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="8"/>
+      <c r="L48" s="6"/>
+      <c r="M48" s="11"/>
       <c r="N48" s="11"/>
       <c r="O48" s="6"/>
       <c r="P48" s="16"/>
       <c r="Q48" s="5"/>
     </row>
-    <row r="49" spans="1:17" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="16"/>
       <c r="B49" s="6"/>
-      <c r="C49" s="10"/>
+      <c r="C49" s="100" t="s">
+        <v>235</v>
+      </c>
       <c r="D49" s="10"/>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="6"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="37"/>
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
       <c r="M49" s="6"/>
-      <c r="N49" s="6"/>
+      <c r="N49" s="11"/>
       <c r="O49" s="6"/>
       <c r="P49" s="16"/>
       <c r="Q49" s="5"/>
@@ -3240,28 +3291,26 @@
     <row r="50" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="98" t="s">
-        <v>119</v>
-      </c>
+      <c r="C50" s="100"/>
       <c r="D50" s="10"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
-      <c r="J50" s="6"/>
+      <c r="J50" s="8"/>
       <c r="K50" s="6"/>
-      <c r="L50" s="38"/>
-      <c r="M50" s="38"/>
-      <c r="N50" s="6"/>
+      <c r="L50" s="6"/>
+      <c r="M50" s="6"/>
+      <c r="N50" s="11"/>
       <c r="O50" s="6"/>
       <c r="P50" s="16"/>
       <c r="Q50" s="5"/>
     </row>
-    <row r="51" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="16"/>
       <c r="B51" s="6"/>
-      <c r="C51" s="98"/>
+      <c r="C51" s="10"/>
       <c r="D51" s="10"/>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
@@ -3271,7 +3320,7 @@
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
-      <c r="M51" s="8"/>
+      <c r="M51" s="6"/>
       <c r="N51" s="6"/>
       <c r="O51" s="6"/>
       <c r="P51" s="16"/>
@@ -3280,15 +3329,17 @@
     <row r="52" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="16"/>
       <c r="B52" s="6"/>
-      <c r="C52" s="10"/>
+      <c r="C52" s="100" t="s">
+        <v>112</v>
+      </c>
       <c r="D52" s="10"/>
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
-      <c r="K52" s="6"/>
+      <c r="J52" s="37"/>
+      <c r="K52" s="37"/>
       <c r="L52" s="6"/>
       <c r="M52" s="6"/>
       <c r="N52" s="6"/>
@@ -3296,13 +3347,11 @@
       <c r="P52" s="16"/>
       <c r="Q52" s="5"/>
     </row>
-    <row r="53" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16"/>
       <c r="B53" s="6"/>
-      <c r="C53" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D53" s="6"/>
+      <c r="C53" s="100"/>
+      <c r="D53" s="10"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
@@ -3320,9 +3369,7 @@
     <row r="54" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16"/>
       <c r="B54" s="6"/>
-      <c r="C54" s="96" t="s">
-        <v>96</v>
-      </c>
+      <c r="C54" s="10"/>
       <c r="D54" s="10"/>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
@@ -3331,8 +3378,8 @@
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
-      <c r="L54" s="38"/>
-      <c r="M54" s="38"/>
+      <c r="L54" s="6"/>
+      <c r="M54" s="6"/>
       <c r="N54" s="6"/>
       <c r="O54" s="6"/>
       <c r="P54" s="16"/>
@@ -3341,7 +3388,9 @@
     <row r="55" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="96"/>
+      <c r="C55" s="100" t="s">
+        <v>236</v>
+      </c>
       <c r="D55" s="10"/>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
@@ -3349,8 +3398,8 @@
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
-      <c r="K55" s="6"/>
-      <c r="L55" s="8"/>
+      <c r="K55" s="37"/>
+      <c r="L55" s="6"/>
       <c r="M55" s="6"/>
       <c r="N55" s="6"/>
       <c r="O55" s="6"/>
@@ -3360,7 +3409,7 @@
     <row r="56" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="16"/>
       <c r="B56" s="6"/>
-      <c r="C56" s="10"/>
+      <c r="C56" s="100"/>
       <c r="D56" s="10"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
@@ -3379,9 +3428,7 @@
     <row r="57" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="16"/>
       <c r="B57" s="6"/>
-      <c r="C57" s="96" t="s">
-        <v>97</v>
-      </c>
+      <c r="C57" s="10"/>
       <c r="D57" s="10"/>
       <c r="E57" s="6"/>
       <c r="F57" s="6"/>
@@ -3390,8 +3437,8 @@
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
       <c r="K57" s="6"/>
-      <c r="L57" s="38"/>
-      <c r="M57" s="38"/>
+      <c r="L57" s="6"/>
+      <c r="M57" s="6"/>
       <c r="N57" s="6"/>
       <c r="O57" s="6"/>
       <c r="P57" s="16"/>
@@ -3400,7 +3447,9 @@
     <row r="58" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="96"/>
+      <c r="C58" s="100" t="s">
+        <v>233</v>
+      </c>
       <c r="D58" s="10"/>
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
@@ -3409,7 +3458,7 @@
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
       <c r="K58" s="6"/>
-      <c r="L58" s="8"/>
+      <c r="L58" s="6"/>
       <c r="M58" s="6"/>
       <c r="N58" s="6"/>
       <c r="O58" s="6"/>
@@ -3419,7 +3468,7 @@
     <row r="59" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="16"/>
       <c r="B59" s="6"/>
-      <c r="C59" s="10"/>
+      <c r="C59" s="100"/>
       <c r="D59" s="10"/>
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
@@ -3438,9 +3487,7 @@
     <row r="60" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="16"/>
       <c r="B60" s="6"/>
-      <c r="C60" s="96" t="s">
-        <v>117</v>
-      </c>
+      <c r="C60" s="10"/>
       <c r="D60" s="10"/>
       <c r="E60" s="6"/>
       <c r="F60" s="6"/>
@@ -3449,18 +3496,20 @@
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>
-      <c r="L60" s="38"/>
-      <c r="M60" s="38"/>
+      <c r="L60" s="6"/>
+      <c r="M60" s="6"/>
       <c r="N60" s="6"/>
       <c r="O60" s="6"/>
       <c r="P60" s="16"/>
       <c r="Q60" s="5"/>
     </row>
-    <row r="61" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="16"/>
       <c r="B61" s="6"/>
-      <c r="C61" s="96"/>
-      <c r="D61" s="10"/>
+      <c r="C61" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" s="6"/>
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
@@ -3469,8 +3518,8 @@
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
       <c r="L61" s="6"/>
-      <c r="M61" s="11"/>
-      <c r="N61" s="8"/>
+      <c r="M61" s="6"/>
+      <c r="N61" s="6"/>
       <c r="O61" s="6"/>
       <c r="P61" s="16"/>
       <c r="Q61" s="5"/>
@@ -3478,7 +3527,9 @@
     <row r="62" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="16"/>
       <c r="B62" s="6"/>
-      <c r="C62" s="10"/>
+      <c r="C62" s="98" t="s">
+        <v>93</v>
+      </c>
       <c r="D62" s="10"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
@@ -3497,16 +3548,14 @@
     <row r="63" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="16"/>
       <c r="B63" s="6"/>
-      <c r="C63" s="96" t="s">
-        <v>116</v>
-      </c>
+      <c r="C63" s="98"/>
       <c r="D63" s="10"/>
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
-      <c r="H63" s="38"/>
-      <c r="I63" s="38"/>
-      <c r="J63" s="38"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="6"/>
       <c r="K63" s="6"/>
       <c r="L63" s="6"/>
       <c r="M63" s="6"/>
@@ -3518,14 +3567,14 @@
     <row r="64" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="16"/>
       <c r="B64" s="6"/>
-      <c r="C64" s="96"/>
+      <c r="C64" s="10"/>
       <c r="D64" s="10"/>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
-      <c r="H64" s="8"/>
-      <c r="I64" s="8"/>
-      <c r="J64" s="8"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="6"/>
       <c r="K64" s="6"/>
       <c r="L64" s="6"/>
       <c r="M64" s="6"/>
@@ -3537,7 +3586,9 @@
     <row r="65" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="16"/>
       <c r="B65" s="6"/>
-      <c r="C65" s="10"/>
+      <c r="C65" s="98" t="s">
+        <v>111</v>
+      </c>
       <c r="D65" s="10"/>
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
@@ -3556,16 +3607,14 @@
     <row r="66" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="16"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="96" t="s">
-        <v>115</v>
-      </c>
+      <c r="C66" s="98"/>
       <c r="D66" s="10"/>
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
-      <c r="H66" s="38"/>
-      <c r="I66" s="38"/>
-      <c r="J66" s="38"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="6"/>
       <c r="K66" s="6"/>
       <c r="L66" s="6"/>
       <c r="M66" s="6"/>
@@ -3577,14 +3626,14 @@
     <row r="67" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="16"/>
       <c r="B67" s="6"/>
-      <c r="C67" s="96"/>
+      <c r="C67" s="10"/>
       <c r="D67" s="10"/>
       <c r="E67" s="6"/>
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
-      <c r="H67" s="8"/>
-      <c r="I67" s="8"/>
-      <c r="J67" s="8"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="6"/>
       <c r="K67" s="6"/>
       <c r="L67" s="6"/>
       <c r="M67" s="6"/>
@@ -3596,7 +3645,9 @@
     <row r="68" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="16"/>
       <c r="B68" s="6"/>
-      <c r="C68" s="10"/>
+      <c r="C68" s="98" t="s">
+        <v>237</v>
+      </c>
       <c r="D68" s="10"/>
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
@@ -3615,9 +3666,7 @@
     <row r="69" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="96" t="s">
-        <v>114</v>
-      </c>
+      <c r="C69" s="98"/>
       <c r="D69" s="10"/>
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
@@ -3626,8 +3675,8 @@
       <c r="I69" s="6"/>
       <c r="J69" s="6"/>
       <c r="K69" s="6"/>
-      <c r="L69" s="38"/>
-      <c r="M69" s="38"/>
+      <c r="L69" s="6"/>
+      <c r="M69" s="11"/>
       <c r="N69" s="6"/>
       <c r="O69" s="6"/>
       <c r="P69" s="16"/>
@@ -3636,7 +3685,7 @@
     <row r="70" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="16"/>
       <c r="B70" s="6"/>
-      <c r="C70" s="96"/>
+      <c r="C70" s="10"/>
       <c r="D70" s="10"/>
       <c r="E70" s="6"/>
       <c r="F70" s="6"/>
@@ -3646,7 +3695,7 @@
       <c r="J70" s="6"/>
       <c r="K70" s="6"/>
       <c r="L70" s="6"/>
-      <c r="M70" s="8"/>
+      <c r="M70" s="6"/>
       <c r="N70" s="6"/>
       <c r="O70" s="6"/>
       <c r="P70" s="16"/>
@@ -3655,7 +3704,9 @@
     <row r="71" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="16"/>
       <c r="B71" s="6"/>
-      <c r="C71" s="10"/>
+      <c r="C71" s="98" t="s">
+        <v>238</v>
+      </c>
       <c r="D71" s="10"/>
       <c r="E71" s="6"/>
       <c r="F71" s="6"/>
@@ -3671,13 +3722,11 @@
       <c r="P71" s="16"/>
       <c r="Q71" s="5"/>
     </row>
-    <row r="72" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16"/>
       <c r="B72" s="6"/>
-      <c r="C72" s="100" t="s">
-        <v>56</v>
-      </c>
-      <c r="D72" s="7"/>
+      <c r="C72" s="98"/>
+      <c r="D72" s="10"/>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
@@ -3688,15 +3737,15 @@
       <c r="L72" s="6"/>
       <c r="M72" s="6"/>
       <c r="N72" s="6"/>
-      <c r="O72" s="5"/>
+      <c r="O72" s="6"/>
       <c r="P72" s="16"/>
       <c r="Q72" s="5"/>
     </row>
-    <row r="73" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="16"/>
       <c r="B73" s="6"/>
-      <c r="C73" s="100"/>
-      <c r="D73" s="7"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
@@ -3707,17 +3756,17 @@
       <c r="L73" s="6"/>
       <c r="M73" s="6"/>
       <c r="N73" s="6"/>
-      <c r="O73" s="5"/>
+      <c r="O73" s="6"/>
       <c r="P73" s="16"/>
       <c r="Q73" s="5"/>
     </row>
-    <row r="74" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16"/>
       <c r="B74" s="6"/>
-      <c r="C74" s="102" t="s">
-        <v>90</v>
-      </c>
-      <c r="D74" s="7"/>
+      <c r="C74" s="98" t="s">
+        <v>110</v>
+      </c>
+      <c r="D74" s="10"/>
       <c r="E74" s="6"/>
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
@@ -3728,65 +3777,15 @@
       <c r="L74" s="6"/>
       <c r="M74" s="6"/>
       <c r="N74" s="6"/>
-      <c r="O74" s="38"/>
+      <c r="O74" s="6"/>
       <c r="P74" s="16"/>
-      <c r="R74" s="53"/>
-      <c r="S74" s="53"/>
-      <c r="T74" s="53"/>
-      <c r="U74" s="53"/>
-      <c r="V74" s="53"/>
-      <c r="W74" s="53"/>
-      <c r="X74" s="53"/>
-      <c r="Y74" s="53"/>
-      <c r="Z74" s="53"/>
-      <c r="AA74" s="53"/>
-      <c r="AB74" s="53"/>
-      <c r="AC74" s="53"/>
-      <c r="AD74" s="53"/>
-      <c r="AE74" s="53"/>
-      <c r="AF74" s="53"/>
-      <c r="AG74" s="53"/>
-      <c r="AH74" s="53"/>
-      <c r="AI74" s="53"/>
-      <c r="AJ74" s="53"/>
-      <c r="AK74" s="53"/>
-      <c r="AL74" s="53"/>
-      <c r="AM74" s="53"/>
-      <c r="AN74" s="53"/>
-      <c r="AO74" s="53"/>
-      <c r="AP74" s="53"/>
-      <c r="AQ74" s="53"/>
-      <c r="AR74" s="53"/>
-      <c r="AS74" s="53"/>
-      <c r="AT74" s="53"/>
-      <c r="AU74" s="53"/>
-      <c r="AV74" s="53"/>
-      <c r="AW74" s="53"/>
-      <c r="AX74" s="53"/>
-      <c r="AY74" s="53"/>
-      <c r="AZ74" s="53"/>
-      <c r="BA74" s="53"/>
-      <c r="BB74" s="53"/>
-      <c r="BC74" s="53"/>
-      <c r="BD74" s="53"/>
-      <c r="BE74" s="53"/>
-      <c r="BF74" s="53"/>
-      <c r="BG74" s="53"/>
-      <c r="BH74" s="53"/>
-      <c r="BI74" s="53"/>
-      <c r="BJ74" s="53"/>
-      <c r="BK74" s="53"/>
-      <c r="BL74" s="53"/>
-      <c r="BM74" s="53"/>
-      <c r="BN74" s="53"/>
-      <c r="BO74" s="53"/>
-      <c r="BP74" s="53"/>
-    </row>
-    <row r="75" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q74" s="5"/>
+    </row>
+    <row r="75" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="16"/>
       <c r="B75" s="6"/>
-      <c r="C75" s="102"/>
-      <c r="D75" s="7"/>
+      <c r="C75" s="98"/>
+      <c r="D75" s="10"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
       <c r="G75" s="6"/>
@@ -3797,65 +3796,15 @@
       <c r="L75" s="6"/>
       <c r="M75" s="6"/>
       <c r="N75" s="6"/>
-      <c r="O75" s="8"/>
+      <c r="O75" s="6"/>
       <c r="P75" s="16"/>
-      <c r="R75" s="53"/>
-      <c r="S75" s="53"/>
-      <c r="T75" s="53"/>
-      <c r="U75" s="53"/>
-      <c r="V75" s="53"/>
-      <c r="W75" s="53"/>
-      <c r="X75" s="53"/>
-      <c r="Y75" s="53"/>
-      <c r="Z75" s="53"/>
-      <c r="AA75" s="53"/>
-      <c r="AB75" s="53"/>
-      <c r="AC75" s="53"/>
-      <c r="AD75" s="53"/>
-      <c r="AE75" s="53"/>
-      <c r="AF75" s="53"/>
-      <c r="AG75" s="53"/>
-      <c r="AH75" s="53"/>
-      <c r="AI75" s="53"/>
-      <c r="AJ75" s="53"/>
-      <c r="AK75" s="53"/>
-      <c r="AL75" s="53"/>
-      <c r="AM75" s="53"/>
-      <c r="AN75" s="53"/>
-      <c r="AO75" s="53"/>
-      <c r="AP75" s="53"/>
-      <c r="AQ75" s="53"/>
-      <c r="AR75" s="53"/>
-      <c r="AS75" s="53"/>
-      <c r="AT75" s="53"/>
-      <c r="AU75" s="53"/>
-      <c r="AV75" s="53"/>
-      <c r="AW75" s="53"/>
-      <c r="AX75" s="53"/>
-      <c r="AY75" s="53"/>
-      <c r="AZ75" s="53"/>
-      <c r="BA75" s="53"/>
-      <c r="BB75" s="53"/>
-      <c r="BC75" s="53"/>
-      <c r="BD75" s="53"/>
-      <c r="BE75" s="53"/>
-      <c r="BF75" s="53"/>
-      <c r="BG75" s="53"/>
-      <c r="BH75" s="53"/>
-      <c r="BI75" s="53"/>
-      <c r="BJ75" s="53"/>
-      <c r="BK75" s="53"/>
-      <c r="BL75" s="53"/>
-      <c r="BM75" s="53"/>
-      <c r="BN75" s="53"/>
-      <c r="BO75" s="53"/>
-      <c r="BP75" s="53"/>
-    </row>
-    <row r="76" spans="1:68" s="53" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="51"/>
-      <c r="B76" s="52"/>
-      <c r="C76" s="54"/>
-      <c r="D76" s="7"/>
+      <c r="Q75" s="5"/>
+    </row>
+    <row r="76" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="16"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
@@ -3867,147 +3816,335 @@
       <c r="M76" s="6"/>
       <c r="N76" s="6"/>
       <c r="O76" s="6"/>
-      <c r="P76" s="51"/>
-    </row>
-    <row r="77" spans="1:68" ht="3" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P76" s="16"/>
+      <c r="Q76" s="5"/>
+    </row>
+    <row r="77" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="16"/>
-      <c r="B77" s="17"/>
-      <c r="C77" s="15"/>
-      <c r="D77" s="15"/>
-      <c r="E77" s="15"/>
-      <c r="F77" s="15"/>
-      <c r="G77" s="15"/>
-      <c r="H77" s="15"/>
-      <c r="I77" s="15"/>
-      <c r="J77" s="15"/>
-      <c r="K77" s="15"/>
-      <c r="L77" s="15"/>
-      <c r="M77" s="15"/>
-      <c r="N77" s="15"/>
-      <c r="O77" s="15"/>
-      <c r="P77" s="18"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="102" t="s">
+        <v>54</v>
+      </c>
+      <c r="D77" s="7"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="6"/>
+      <c r="M77" s="6"/>
+      <c r="N77" s="6"/>
+      <c r="O77" s="5"/>
+      <c r="P77" s="16"/>
       <c r="Q77" s="5"/>
     </row>
-    <row r="78" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="5"/>
-      <c r="B78" s="5"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="5"/>
-      <c r="G78" s="5"/>
-      <c r="H78" s="5"/>
-      <c r="I78" s="5"/>
-      <c r="J78" s="5"/>
-      <c r="K78" s="5"/>
-      <c r="L78" s="5"/>
-      <c r="M78" s="5"/>
-      <c r="N78" s="5"/>
+    <row r="78" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="16"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="102"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="6"/>
+      <c r="K78" s="6"/>
+      <c r="L78" s="6"/>
+      <c r="M78" s="6"/>
+      <c r="N78" s="6"/>
       <c r="O78" s="5"/>
-      <c r="P78" s="5"/>
+      <c r="P78" s="16"/>
       <c r="Q78" s="5"/>
     </row>
-    <row r="79" spans="1:68" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="5"/>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5"/>
-      <c r="F79" s="101"/>
-      <c r="G79" s="101"/>
+    <row r="79" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="16"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="104" t="s">
+        <v>88</v>
+      </c>
+      <c r="D79" s="7"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
       <c r="H79" s="6"/>
-      <c r="I79" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="J79" s="38"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="6"/>
       <c r="K79" s="6"/>
-      <c r="L79" s="99" t="s">
-        <v>57</v>
-      </c>
-      <c r="M79" s="99"/>
-      <c r="N79" s="40"/>
-      <c r="O79" s="5"/>
-      <c r="P79" s="5"/>
-      <c r="Q79" s="5"/>
-    </row>
-    <row r="80" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5"/>
-      <c r="F80" s="5"/>
-      <c r="G80" s="5"/>
-      <c r="H80" s="5"/>
-      <c r="I80" s="5"/>
-      <c r="J80" s="5"/>
-      <c r="K80" s="5"/>
-      <c r="L80" s="5"/>
-      <c r="M80" s="5"/>
-      <c r="N80" s="5"/>
-      <c r="O80" s="5"/>
-      <c r="P80" s="5"/>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C82" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C83" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C84" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C85" s="86" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C86" s="86" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C87" s="86"/>
-    </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C88" s="86"/>
-    </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C89" s="86"/>
-    </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C90" s="86"/>
-    </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C91" s="86"/>
-    </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C92" s="86"/>
-    </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C93" s="86"/>
-    </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C94" s="86"/>
-    </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C95" s="86"/>
-    </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C96" s="86"/>
+      <c r="L79" s="6"/>
+      <c r="M79" s="6"/>
+      <c r="N79" s="6"/>
+      <c r="O79" s="37"/>
+      <c r="P79" s="16"/>
+      <c r="R79" s="52"/>
+      <c r="S79" s="52"/>
+      <c r="T79" s="52"/>
+      <c r="U79" s="52"/>
+      <c r="V79" s="52"/>
+      <c r="W79" s="52"/>
+      <c r="X79" s="52"/>
+      <c r="Y79" s="52"/>
+      <c r="Z79" s="52"/>
+      <c r="AA79" s="52"/>
+      <c r="AB79" s="52"/>
+      <c r="AC79" s="52"/>
+      <c r="AD79" s="52"/>
+      <c r="AE79" s="52"/>
+      <c r="AF79" s="52"/>
+      <c r="AG79" s="52"/>
+      <c r="AH79" s="52"/>
+      <c r="AI79" s="52"/>
+      <c r="AJ79" s="52"/>
+      <c r="AK79" s="52"/>
+      <c r="AL79" s="52"/>
+      <c r="AM79" s="52"/>
+      <c r="AN79" s="52"/>
+      <c r="AO79" s="52"/>
+      <c r="AP79" s="52"/>
+      <c r="AQ79" s="52"/>
+      <c r="AR79" s="52"/>
+      <c r="AS79" s="52"/>
+      <c r="AT79" s="52"/>
+      <c r="AU79" s="52"/>
+      <c r="AV79" s="52"/>
+      <c r="AW79" s="52"/>
+      <c r="AX79" s="52"/>
+      <c r="AY79" s="52"/>
+      <c r="AZ79" s="52"/>
+      <c r="BA79" s="52"/>
+      <c r="BB79" s="52"/>
+      <c r="BC79" s="52"/>
+      <c r="BD79" s="52"/>
+      <c r="BE79" s="52"/>
+      <c r="BF79" s="52"/>
+      <c r="BG79" s="52"/>
+      <c r="BH79" s="52"/>
+      <c r="BI79" s="52"/>
+      <c r="BJ79" s="52"/>
+      <c r="BK79" s="52"/>
+      <c r="BL79" s="52"/>
+      <c r="BM79" s="52"/>
+      <c r="BN79" s="52"/>
+      <c r="BO79" s="52"/>
+      <c r="BP79" s="52"/>
+    </row>
+    <row r="80" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="16"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="104"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="6"/>
+      <c r="K80" s="6"/>
+      <c r="L80" s="6"/>
+      <c r="M80" s="6"/>
+      <c r="N80" s="6"/>
+      <c r="O80" s="8"/>
+      <c r="P80" s="16"/>
+      <c r="R80" s="52"/>
+      <c r="S80" s="52"/>
+      <c r="T80" s="52"/>
+      <c r="U80" s="52"/>
+      <c r="V80" s="52"/>
+      <c r="W80" s="52"/>
+      <c r="X80" s="52"/>
+      <c r="Y80" s="52"/>
+      <c r="Z80" s="52"/>
+      <c r="AA80" s="52"/>
+      <c r="AB80" s="52"/>
+      <c r="AC80" s="52"/>
+      <c r="AD80" s="52"/>
+      <c r="AE80" s="52"/>
+      <c r="AF80" s="52"/>
+      <c r="AG80" s="52"/>
+      <c r="AH80" s="52"/>
+      <c r="AI80" s="52"/>
+      <c r="AJ80" s="52"/>
+      <c r="AK80" s="52"/>
+      <c r="AL80" s="52"/>
+      <c r="AM80" s="52"/>
+      <c r="AN80" s="52"/>
+      <c r="AO80" s="52"/>
+      <c r="AP80" s="52"/>
+      <c r="AQ80" s="52"/>
+      <c r="AR80" s="52"/>
+      <c r="AS80" s="52"/>
+      <c r="AT80" s="52"/>
+      <c r="AU80" s="52"/>
+      <c r="AV80" s="52"/>
+      <c r="AW80" s="52"/>
+      <c r="AX80" s="52"/>
+      <c r="AY80" s="52"/>
+      <c r="AZ80" s="52"/>
+      <c r="BA80" s="52"/>
+      <c r="BB80" s="52"/>
+      <c r="BC80" s="52"/>
+      <c r="BD80" s="52"/>
+      <c r="BE80" s="52"/>
+      <c r="BF80" s="52"/>
+      <c r="BG80" s="52"/>
+      <c r="BH80" s="52"/>
+      <c r="BI80" s="52"/>
+      <c r="BJ80" s="52"/>
+      <c r="BK80" s="52"/>
+      <c r="BL80" s="52"/>
+      <c r="BM80" s="52"/>
+      <c r="BN80" s="52"/>
+      <c r="BO80" s="52"/>
+      <c r="BP80" s="52"/>
+    </row>
+    <row r="81" spans="1:17" s="52" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="50"/>
+      <c r="B81" s="51"/>
+      <c r="C81" s="53"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="L81" s="6"/>
+      <c r="M81" s="6"/>
+      <c r="N81" s="6"/>
+      <c r="O81" s="6"/>
+      <c r="P81" s="50"/>
+    </row>
+    <row r="82" spans="1:17" ht="3" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="16"/>
+      <c r="B82" s="17"/>
+      <c r="C82" s="15"/>
+      <c r="D82" s="15"/>
+      <c r="E82" s="15"/>
+      <c r="F82" s="15"/>
+      <c r="G82" s="15"/>
+      <c r="H82" s="15"/>
+      <c r="I82" s="15"/>
+      <c r="J82" s="15"/>
+      <c r="K82" s="15"/>
+      <c r="L82" s="15"/>
+      <c r="M82" s="15"/>
+      <c r="N82" s="15"/>
+      <c r="O82" s="15"/>
+      <c r="P82" s="18"/>
+      <c r="Q82" s="5"/>
+    </row>
+    <row r="83" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="5"/>
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+      <c r="H83" s="5"/>
+      <c r="I83" s="5"/>
+      <c r="J83" s="5"/>
+      <c r="K83" s="5"/>
+      <c r="L83" s="5"/>
+      <c r="M83" s="5"/>
+      <c r="N83" s="5"/>
+      <c r="O83" s="5"/>
+      <c r="P83" s="5"/>
+      <c r="Q83" s="5"/>
+    </row>
+    <row r="84" spans="1:17" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="5"/>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5"/>
+      <c r="F84" s="103"/>
+      <c r="G84" s="103"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="J84" s="37"/>
+      <c r="K84" s="6"/>
+      <c r="L84" s="101" t="s">
+        <v>55</v>
+      </c>
+      <c r="M84" s="101"/>
+      <c r="N84" s="39"/>
+      <c r="O84" s="5"/>
+      <c r="P84" s="5"/>
+      <c r="Q84" s="5"/>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A85" s="5"/>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="5"/>
+      <c r="I85" s="5"/>
+      <c r="J85" s="5"/>
+      <c r="K85" s="5"/>
+      <c r="L85" s="5"/>
+      <c r="M85" s="5"/>
+      <c r="N85" s="5"/>
+      <c r="O85" s="5"/>
+      <c r="P85" s="5"/>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C87" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C88" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C89" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C90" s="85" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C91" s="85" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C92" s="85" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C93" s="85" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C94" s="85"/>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C95" s="85"/>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C96" s="85"/>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C97" s="86"/>
+      <c r="C97" s="85"/>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C98" s="86"/>
+      <c r="C98" s="85"/>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C99" s="85"/>
@@ -4015,29 +4152,46 @@
     <row r="100" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C100" s="85"/>
     </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C101" s="85"/>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C102" s="85"/>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C103" s="85"/>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C104" s="84"/>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C105" s="84"/>
+    </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="L79:M79"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="F79:G79"/>
+  <mergeCells count="29">
+    <mergeCell ref="L84:M84"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="C79:C80"/>
     <mergeCell ref="C74:C75"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C62:C63"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="C58:C59"/>
     <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C47:C48"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="B2:O3"/>
     <mergeCell ref="C6:C7"/>
@@ -4074,46 +4228,46 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="105" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+        <v>102</v>
+      </c>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="103"/>
+      <c r="A4" s="105"/>
       <c r="B4" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="103"/>
+      <c r="A5" s="105"/>
       <c r="B5" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -4127,19 +4281,19 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F6" s="61" t="s">
-        <v>122</v>
+        <v>99</v>
+      </c>
+      <c r="F6" s="60" t="s">
+        <v>115</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -4172,92 +4326,92 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C1" s="70"/>
+        <v>145</v>
+      </c>
+      <c r="C1" s="69"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2" s="60"/>
+        <v>108</v>
+      </c>
+      <c r="C2" s="59"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" s="59"/>
+        <v>107</v>
+      </c>
+      <c r="C3" s="58"/>
       <c r="E3" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C5" s="67"/>
+        <v>142</v>
+      </c>
+      <c r="C5" s="66"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C6" s="68"/>
+        <v>144</v>
+      </c>
+      <c r="C6" s="67"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C7" s="69"/>
+        <v>143</v>
+      </c>
+      <c r="C7" s="68"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>157</v>
-      </c>
-      <c r="C10" s="71"/>
+        <v>150</v>
+      </c>
+      <c r="C10" s="70"/>
       <c r="D10" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>153</v>
-      </c>
-      <c r="C11" s="72"/>
+        <v>146</v>
+      </c>
+      <c r="C11" s="71"/>
       <c r="D11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>155</v>
-      </c>
-      <c r="C12" s="73"/>
+        <v>148</v>
+      </c>
+      <c r="C12" s="72"/>
       <c r="D12">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>156</v>
-      </c>
-      <c r="C13" s="69"/>
+        <v>149</v>
+      </c>
+      <c r="C13" s="68"/>
       <c r="D13">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -4265,107 +4419,107 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>110</v>
-      </c>
-      <c r="C40" s="55"/>
+        <v>106</v>
+      </c>
+      <c r="C40" s="54"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" s="27"/>
+        <v>15</v>
+      </c>
+      <c r="C45" s="26"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>18</v>
-      </c>
-      <c r="C46" s="28"/>
+        <v>16</v>
+      </c>
+      <c r="C46" s="27"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>19</v>
-      </c>
-      <c r="C47" s="29"/>
+        <v>17</v>
+      </c>
+      <c r="C47" s="28"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>32</v>
-      </c>
-      <c r="C48" s="30"/>
+        <v>30</v>
+      </c>
+      <c r="C48" s="29"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>20</v>
-      </c>
-      <c r="C49" s="31"/>
+        <v>18</v>
+      </c>
+      <c r="C49" s="30"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>21</v>
-      </c>
-      <c r="C50" s="32"/>
+        <v>19</v>
+      </c>
+      <c r="C50" s="31"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>22</v>
-      </c>
-      <c r="C51" s="33"/>
+        <v>20</v>
+      </c>
+      <c r="C51" s="32"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>24</v>
-      </c>
-      <c r="C53" s="34"/>
+        <v>22</v>
+      </c>
+      <c r="C53" s="33"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C54" s="31"/>
+      <c r="A54" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" s="30"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>26</v>
-      </c>
-      <c r="C55" s="35"/>
+        <v>24</v>
+      </c>
+      <c r="C55" s="34"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>28</v>
-      </c>
-      <c r="C57" s="36"/>
+        <v>26</v>
+      </c>
+      <c r="C57" s="35"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>30</v>
-      </c>
-      <c r="C59" s="30"/>
+        <v>28</v>
+      </c>
+      <c r="C59" s="29"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>31</v>
-      </c>
-      <c r="C60" s="37"/>
+        <v>29</v>
+      </c>
+      <c r="C60" s="36"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4379,846 +4533,860 @@
   <dimension ref="B2:H79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.125" style="43" customWidth="1"/>
-    <col min="2" max="2" width="4.5" style="43" customWidth="1"/>
-    <col min="3" max="3" width="21" style="43" customWidth="1"/>
-    <col min="4" max="4" width="27.875" style="43" customWidth="1"/>
-    <col min="5" max="5" width="22.5" style="43" customWidth="1"/>
-    <col min="6" max="6" width="19.875" style="43" customWidth="1"/>
-    <col min="7" max="7" width="27.25" style="43" customWidth="1"/>
-    <col min="8" max="8" width="28.25" style="43" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.75" style="43"/>
+    <col min="1" max="1" width="1.125" style="42" customWidth="1"/>
+    <col min="2" max="2" width="4.5" style="42" customWidth="1"/>
+    <col min="3" max="3" width="21" style="42" customWidth="1"/>
+    <col min="4" max="4" width="27.875" style="42" customWidth="1"/>
+    <col min="5" max="5" width="22.5" style="42" customWidth="1"/>
+    <col min="6" max="6" width="19.875" style="42" customWidth="1"/>
+    <col min="7" max="7" width="27.25" style="42" customWidth="1"/>
+    <col min="8" max="8" width="28.25" style="42" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.75" style="42"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="41"/>
-      <c r="C2" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="42" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" s="41" t="s">
         <v>36</v>
-      </c>
-      <c r="E2" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" s="42" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="106" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44" t="s">
         <v>67</v>
-      </c>
-      <c r="E3" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="107"/>
       <c r="C4" s="110" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" s="110" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="45" t="s">
-        <v>138</v>
-      </c>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45" t="s">
-        <v>139</v>
+        <v>38</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="107"/>
       <c r="C5" s="107"/>
       <c r="D5" s="107"/>
-      <c r="E5" s="45" t="s">
-        <v>125</v>
-      </c>
-      <c r="F5" s="45" t="s">
-        <v>144</v>
-      </c>
-      <c r="G5" s="45" t="s">
-        <v>145</v>
-      </c>
-      <c r="H5" s="45" t="s">
-        <v>127</v>
+      <c r="E5" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="G5" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="107"/>
       <c r="C6" s="107"/>
       <c r="D6" s="107"/>
-      <c r="E6" s="45" t="s">
-        <v>126</v>
-      </c>
-      <c r="F6" s="45" t="s">
-        <v>146</v>
-      </c>
-      <c r="G6" s="45" t="s">
-        <v>128</v>
-      </c>
-      <c r="H6" s="45" t="s">
-        <v>147</v>
+      <c r="E6" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="F6" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="G6" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="H6" s="44" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="108"/>
       <c r="C7" s="108"/>
       <c r="D7" s="108"/>
-      <c r="E7" s="45" t="s">
-        <v>140</v>
-      </c>
-      <c r="F7" s="45" t="s">
+      <c r="E7" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="H7" s="44" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="55"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="63"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="83" t="s">
+        <v>229</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44" t="s">
+        <v>227</v>
+      </c>
+      <c r="H9" s="44" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="82"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="86" t="s">
+        <v>244</v>
+      </c>
+      <c r="E10" s="44" t="s">
+        <v>245</v>
+      </c>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44" t="s">
+        <v>251</v>
+      </c>
+      <c r="H10" s="44" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="82"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="83" t="s">
+        <v>243</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>252</v>
+      </c>
+      <c r="F11" s="44" t="s">
+        <v>242</v>
+      </c>
+      <c r="G11" s="44" t="s">
+        <v>250</v>
+      </c>
+      <c r="H11" s="44" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="82"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="82"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="82"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="83"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="82"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="82"/>
+      <c r="C16" s="83"/>
+      <c r="D16" s="83"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="82"/>
+      <c r="C17" s="83"/>
+      <c r="D17" s="83"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="82"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="83"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="82"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="83"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="55"/>
+      <c r="C20" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="56" t="s">
         <v>123</v>
       </c>
-      <c r="G7" s="45" t="s">
-        <v>142</v>
-      </c>
-      <c r="H7" s="45" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="56"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="64"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84" t="s">
-        <v>242</v>
-      </c>
-      <c r="E9" s="45" t="s">
-        <v>237</v>
-      </c>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45" t="s">
-        <v>238</v>
-      </c>
-      <c r="H9" s="45" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="83"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84" t="s">
-        <v>241</v>
-      </c>
-      <c r="E10" s="45" t="s">
-        <v>240</v>
-      </c>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="83"/>
-      <c r="C11" s="84"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="83"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="83"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="83"/>
-      <c r="C14" s="84"/>
-      <c r="D14" s="84"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="83"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="83"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="84"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="83"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="83"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="84"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="83"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="84"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="56"/>
-      <c r="C20" s="57" t="s">
-        <v>129</v>
-      </c>
-      <c r="D20" s="57" t="s">
+      <c r="E20" s="44" t="s">
+        <v>155</v>
+      </c>
+      <c r="F20" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="G20" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="H20" s="44" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="119" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="114" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="114" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="E20" s="45" t="s">
-        <v>163</v>
-      </c>
-      <c r="F20" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="G20" s="45" t="s">
-        <v>165</v>
-      </c>
-      <c r="H20" s="45" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="116" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="114" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="114" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47" t="s">
-        <v>141</v>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="117"/>
+      <c r="B22" s="120"/>
       <c r="C22" s="115"/>
       <c r="D22" s="115"/>
-      <c r="E22" s="47" t="s">
+      <c r="E22" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="G22" s="46" t="s">
+        <v>161</v>
+      </c>
+      <c r="H22" s="47" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="120"/>
+      <c r="C23" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="F22" s="47" t="s">
-        <v>131</v>
-      </c>
-      <c r="G22" s="47" t="s">
-        <v>169</v>
-      </c>
-      <c r="H22" s="48" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="117"/>
-      <c r="C23" s="47" t="s">
+      <c r="E23" s="46" t="s">
+        <v>163</v>
+      </c>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46" t="s">
+        <v>159</v>
+      </c>
+      <c r="H23" s="47" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="120"/>
+      <c r="C24" s="114" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="47" t="s">
+      <c r="D24" s="114" t="s">
         <v>74</v>
       </c>
-      <c r="E23" s="47" t="s">
-        <v>171</v>
-      </c>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47" t="s">
-        <v>167</v>
-      </c>
-      <c r="H23" s="48" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="117"/>
-      <c r="C24" s="114" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" s="114" t="s">
-        <v>76</v>
-      </c>
-      <c r="E24" s="47" t="s">
-        <v>172</v>
-      </c>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47" t="s">
-        <v>173</v>
+      <c r="E24" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="117"/>
+      <c r="B25" s="120"/>
       <c r="C25" s="115"/>
       <c r="D25" s="115"/>
-      <c r="E25" s="47" t="s">
+      <c r="E25" s="46" t="s">
+        <v>166</v>
+      </c>
+      <c r="F25" s="47" t="s">
+        <v>160</v>
+      </c>
+      <c r="G25" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="H25" s="46" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="120"/>
+      <c r="C26" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="47" t="s">
+        <v>168</v>
+      </c>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="H26" s="47" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="120"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="47"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="120"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="47"/>
+    </row>
+    <row r="29" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="120"/>
+      <c r="C29" s="73" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="73" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="73" t="s">
+        <v>171</v>
+      </c>
+      <c r="F29" s="73" t="s">
+        <v>173</v>
+      </c>
+      <c r="G29" s="73" t="s">
+        <v>172</v>
+      </c>
+      <c r="H29" s="73" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="120"/>
+      <c r="C30" s="111" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="111" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="111" t="s">
+        <v>180</v>
+      </c>
+      <c r="F30" s="121" t="s">
+        <v>182</v>
+      </c>
+      <c r="G30" s="121" t="s">
+        <v>249</v>
+      </c>
+      <c r="H30" s="111" t="s">
         <v>174</v>
       </c>
-      <c r="F25" s="48" t="s">
-        <v>168</v>
-      </c>
-      <c r="G25" s="47" t="s">
-        <v>175</v>
-      </c>
-      <c r="H25" s="47" t="s">
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="120"/>
+      <c r="C31" s="112"/>
+      <c r="D31" s="112"/>
+      <c r="E31" s="112"/>
+      <c r="F31" s="122"/>
+      <c r="G31" s="122"/>
+      <c r="H31" s="112"/>
+    </row>
+    <row r="32" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B32" s="120"/>
+      <c r="C32" s="81"/>
+      <c r="D32" s="79" t="s">
+        <v>177</v>
+      </c>
+      <c r="E32" s="78" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="117"/>
-      <c r="C26" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="D26" s="48" t="s">
+      <c r="F32" s="77" t="s">
+        <v>217</v>
+      </c>
+      <c r="G32" s="78" t="s">
+        <v>179</v>
+      </c>
+      <c r="H32" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B33" s="120"/>
+      <c r="C33" s="111"/>
+      <c r="D33" s="111" t="s">
+        <v>185</v>
+      </c>
+      <c r="E33" s="80" t="s">
+        <v>186</v>
+      </c>
+      <c r="F33" s="77" t="s">
+        <v>215</v>
+      </c>
+      <c r="G33" s="78" t="s">
+        <v>192</v>
+      </c>
+      <c r="H33" s="73" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B34" s="120"/>
+      <c r="C34" s="112"/>
+      <c r="D34" s="112"/>
+      <c r="E34" s="80" t="s">
+        <v>188</v>
+      </c>
+      <c r="F34" s="77" t="s">
+        <v>216</v>
+      </c>
+      <c r="G34" s="78" t="s">
+        <v>189</v>
+      </c>
+      <c r="H34" s="78" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="B35" s="120"/>
+      <c r="C35" s="74"/>
+      <c r="D35" s="81" t="s">
+        <v>184</v>
+      </c>
+      <c r="E35" s="80" t="s">
+        <v>197</v>
+      </c>
+      <c r="F35" s="77" t="s">
+        <v>214</v>
+      </c>
+      <c r="G35" s="80" t="s">
+        <v>198</v>
+      </c>
+      <c r="H35" s="80" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" s="120"/>
+      <c r="C36" s="109" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="109" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="48" t="s">
-        <v>176</v>
-      </c>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48" t="s">
-        <v>177</v>
-      </c>
-      <c r="H26" s="48" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="117"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="48"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="117"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="48"/>
-    </row>
-    <row r="29" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="117"/>
-      <c r="C29" s="74" t="s">
-        <v>44</v>
-      </c>
-      <c r="D29" s="74" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" s="74" t="s">
-        <v>179</v>
-      </c>
-      <c r="F29" s="74" t="s">
-        <v>181</v>
-      </c>
-      <c r="G29" s="74" t="s">
-        <v>180</v>
-      </c>
-      <c r="H29" s="74" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="117"/>
-      <c r="C30" s="119" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" s="119" t="s">
-        <v>49</v>
-      </c>
-      <c r="E30" s="119" t="s">
-        <v>188</v>
-      </c>
-      <c r="F30" s="104" t="s">
-        <v>191</v>
-      </c>
-      <c r="G30" s="104" t="s">
-        <v>190</v>
-      </c>
-      <c r="H30" s="119" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="117"/>
-      <c r="C31" s="120"/>
-      <c r="D31" s="120"/>
-      <c r="E31" s="120"/>
-      <c r="F31" s="105"/>
-      <c r="G31" s="105"/>
-      <c r="H31" s="120"/>
-    </row>
-    <row r="32" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B32" s="117"/>
-      <c r="C32" s="82"/>
-      <c r="D32" s="80" t="s">
-        <v>185</v>
-      </c>
-      <c r="E32" s="79" t="s">
-        <v>186</v>
-      </c>
-      <c r="F32" s="78" t="s">
-        <v>228</v>
-      </c>
-      <c r="G32" s="79" t="s">
-        <v>187</v>
-      </c>
-      <c r="H32" s="79" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B33" s="117"/>
-      <c r="C33" s="119"/>
-      <c r="D33" s="119" t="s">
-        <v>194</v>
-      </c>
-      <c r="E33" s="81" t="s">
-        <v>195</v>
-      </c>
-      <c r="F33" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="G33" s="79" t="s">
-        <v>203</v>
-      </c>
-      <c r="H33" s="74" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B34" s="117"/>
-      <c r="C34" s="120"/>
-      <c r="D34" s="120"/>
-      <c r="E34" s="81" t="s">
-        <v>197</v>
-      </c>
-      <c r="F34" s="78" t="s">
-        <v>227</v>
-      </c>
-      <c r="G34" s="79" t="s">
-        <v>198</v>
-      </c>
-      <c r="H34" s="79" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" ht="66" x14ac:dyDescent="0.3">
-      <c r="B35" s="117"/>
-      <c r="C35" s="75"/>
-      <c r="D35" s="82" t="s">
-        <v>193</v>
-      </c>
-      <c r="E35" s="81" t="s">
-        <v>208</v>
-      </c>
-      <c r="F35" s="78" t="s">
-        <v>225</v>
-      </c>
-      <c r="G35" s="81" t="s">
-        <v>209</v>
-      </c>
-      <c r="H35" s="81" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="117"/>
-      <c r="C36" s="109" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" s="109" t="s">
-        <v>47</v>
-      </c>
-      <c r="E36" s="49" t="s">
-        <v>81</v>
-      </c>
-      <c r="F36" s="49"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="49" t="s">
-        <v>210</v>
+      <c r="F36" s="48"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="48" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="117"/>
+      <c r="B37" s="120"/>
       <c r="C37" s="109"/>
       <c r="D37" s="109"/>
-      <c r="E37" s="49" t="s">
+      <c r="E37" s="48" t="s">
+        <v>200</v>
+      </c>
+      <c r="F37" s="77" t="s">
+        <v>212</v>
+      </c>
+      <c r="G37" s="48" t="s">
+        <v>201</v>
+      </c>
+      <c r="H37" s="48" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B38" s="120"/>
+      <c r="C38" s="111" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="111" t="s">
+        <v>52</v>
+      </c>
+      <c r="E38" s="73" t="s">
+        <v>202</v>
+      </c>
+      <c r="F38" s="77" t="s">
+        <v>209</v>
+      </c>
+      <c r="G38" s="73" t="s">
+        <v>203</v>
+      </c>
+      <c r="H38" s="73" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B39" s="120"/>
+      <c r="C39" s="112"/>
+      <c r="D39" s="112"/>
+      <c r="E39" s="73" t="s">
+        <v>204</v>
+      </c>
+      <c r="F39" s="77" t="s">
+        <v>210</v>
+      </c>
+      <c r="G39" s="73" t="s">
+        <v>208</v>
+      </c>
+      <c r="H39" s="73" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B40" s="120"/>
+      <c r="C40" s="80" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="80" t="s">
+        <v>51</v>
+      </c>
+      <c r="E40" s="80" t="s">
+        <v>80</v>
+      </c>
+      <c r="F40" s="77" t="s">
         <v>211</v>
       </c>
-      <c r="F37" s="78" t="s">
+      <c r="G40" s="80" t="s">
+        <v>213</v>
+      </c>
+      <c r="H40" s="80" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B41" s="120"/>
+      <c r="C41" s="111" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="111" t="s">
+        <v>50</v>
+      </c>
+      <c r="E41" s="73" t="s">
+        <v>218</v>
+      </c>
+      <c r="F41" s="77" t="s">
         <v>223</v>
       </c>
-      <c r="G37" s="49" t="s">
-        <v>212</v>
-      </c>
-      <c r="H37" s="49" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B38" s="117"/>
-      <c r="C38" s="119" t="s">
-        <v>46</v>
-      </c>
-      <c r="D38" s="119" t="s">
-        <v>54</v>
-      </c>
-      <c r="E38" s="74" t="s">
-        <v>213</v>
-      </c>
-      <c r="F38" s="78" t="s">
+      <c r="G41" s="73" t="s">
+        <v>222</v>
+      </c>
+      <c r="H41" s="73" t="s">
         <v>220</v>
       </c>
-      <c r="G38" s="74" t="s">
-        <v>214</v>
-      </c>
-      <c r="H38" s="74" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B39" s="117"/>
-      <c r="C39" s="120"/>
-      <c r="D39" s="120"/>
-      <c r="E39" s="74" t="s">
-        <v>215</v>
-      </c>
-      <c r="F39" s="78" t="s">
+    </row>
+    <row r="42" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B42" s="120"/>
+      <c r="C42" s="112"/>
+      <c r="D42" s="112"/>
+      <c r="E42" s="73" t="s">
+        <v>224</v>
+      </c>
+      <c r="F42" s="77" t="s">
+        <v>219</v>
+      </c>
+      <c r="G42" s="73" t="s">
+        <v>225</v>
+      </c>
+      <c r="H42" s="73" t="s">
         <v>221</v>
       </c>
-      <c r="G39" s="74" t="s">
-        <v>219</v>
-      </c>
-      <c r="H39" s="74" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B40" s="117"/>
-      <c r="C40" s="81" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" s="81" t="s">
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" s="120"/>
+      <c r="C43" s="81"/>
+      <c r="D43" s="81"/>
+      <c r="E43" s="80"/>
+      <c r="F43" s="80"/>
+      <c r="G43" s="80"/>
+      <c r="H43" s="80"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44" s="120"/>
+      <c r="C44" s="81"/>
+      <c r="D44" s="81"/>
+      <c r="E44" s="80"/>
+      <c r="F44" s="80"/>
+      <c r="G44" s="80"/>
+      <c r="H44" s="80"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B45" s="120"/>
+      <c r="C45" s="81"/>
+      <c r="D45" s="81"/>
+      <c r="E45" s="80"/>
+      <c r="F45" s="80"/>
+      <c r="G45" s="80"/>
+      <c r="H45" s="80"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B46" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="E40" s="81" t="s">
-        <v>82</v>
-      </c>
-      <c r="F40" s="78" t="s">
-        <v>222</v>
-      </c>
-      <c r="G40" s="81" t="s">
-        <v>224</v>
-      </c>
-      <c r="H40" s="81" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B41" s="117"/>
-      <c r="C41" s="119" t="s">
-        <v>51</v>
-      </c>
-      <c r="D41" s="119" t="s">
-        <v>52</v>
-      </c>
-      <c r="E41" s="74" t="s">
-        <v>229</v>
-      </c>
-      <c r="F41" s="78" t="s">
-        <v>234</v>
-      </c>
-      <c r="G41" s="74" t="s">
-        <v>233</v>
-      </c>
-      <c r="H41" s="74" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B42" s="117"/>
-      <c r="C42" s="120"/>
-      <c r="D42" s="120"/>
-      <c r="E42" s="74" t="s">
-        <v>235</v>
-      </c>
-      <c r="F42" s="78" t="s">
-        <v>230</v>
-      </c>
-      <c r="G42" s="74" t="s">
-        <v>236</v>
-      </c>
-      <c r="H42" s="74" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B43" s="117"/>
-      <c r="C43" s="82"/>
-      <c r="D43" s="82"/>
-      <c r="E43" s="81"/>
-      <c r="F43" s="81"/>
-      <c r="G43" s="81"/>
-      <c r="H43" s="81"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B44" s="117"/>
-      <c r="C44" s="82"/>
-      <c r="D44" s="82"/>
-      <c r="E44" s="81"/>
-      <c r="F44" s="81"/>
-      <c r="G44" s="81"/>
-      <c r="H44" s="81"/>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B45" s="117"/>
-      <c r="C45" s="82"/>
-      <c r="D45" s="82"/>
-      <c r="E45" s="81"/>
-      <c r="F45" s="81"/>
-      <c r="G45" s="81"/>
-      <c r="H45" s="81"/>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B46" s="111" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B47" s="112"/>
+      <c r="B47" s="117"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B48" s="112"/>
+      <c r="B48" s="117"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B49" s="113"/>
+      <c r="B49" s="118"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B50" s="63"/>
+      <c r="B50" s="62"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B51" s="63"/>
+      <c r="B51" s="62"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B52" s="63"/>
+      <c r="B52" s="62"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B53" s="63"/>
+      <c r="B53" s="62"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B54" s="63"/>
+      <c r="B54" s="62"/>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B55" s="63"/>
+      <c r="B55" s="62"/>
     </row>
     <row r="63" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="D63" s="77" t="s">
-        <v>189</v>
-      </c>
-      <c r="E63" s="79" t="s">
-        <v>205</v>
-      </c>
-      <c r="F63" s="78" t="s">
-        <v>192</v>
-      </c>
-      <c r="G63" s="79" t="s">
-        <v>202</v>
-      </c>
-      <c r="H63" s="76" t="s">
-        <v>204</v>
+      <c r="D63" s="76" t="s">
+        <v>181</v>
+      </c>
+      <c r="E63" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="F63" s="77" t="s">
+        <v>183</v>
+      </c>
+      <c r="G63" s="78" t="s">
+        <v>191</v>
+      </c>
+      <c r="H63" s="75" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="70" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C70" s="118" t="s">
+      <c r="C70" s="113" t="s">
+        <v>57</v>
+      </c>
+      <c r="D70" s="113" t="s">
         <v>59</v>
       </c>
-      <c r="D70" s="118" t="s">
+      <c r="E70" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="F70" s="45"/>
+      <c r="G70" s="45"/>
+      <c r="H70" s="45" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C71" s="113"/>
+      <c r="D71" s="113"/>
+      <c r="E71" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="F71" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="G71" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="H71" s="45" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="72" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C72" s="61"/>
+      <c r="D72" s="61"/>
+      <c r="E72" s="61"/>
+      <c r="F72" s="61"/>
+      <c r="G72" s="61"/>
+      <c r="H72" s="61"/>
+    </row>
+    <row r="73" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C73" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="D73" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="E70" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="F70" s="46"/>
-      <c r="G70" s="46"/>
-      <c r="H70" s="46" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="71" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C71" s="118"/>
-      <c r="D71" s="118"/>
-      <c r="E71" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="F71" s="46" t="s">
-        <v>124</v>
-      </c>
-      <c r="G71" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="H71" s="46" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="72" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C72" s="62"/>
-      <c r="D72" s="62"/>
-      <c r="E72" s="62"/>
-      <c r="F72" s="62"/>
-      <c r="G72" s="62"/>
-      <c r="H72" s="62"/>
-    </row>
-    <row r="73" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C73" s="46" t="s">
+      <c r="E73" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="D73" s="46" t="s">
+      <c r="F73" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="E73" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="F73" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="G73" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="H73" s="46" t="s">
-        <v>83</v>
+      <c r="G73" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="H73" s="45" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C74" s="65"/>
-      <c r="D74" s="65" t="s">
-        <v>136</v>
-      </c>
-      <c r="E74" s="62"/>
-      <c r="F74" s="62"/>
-      <c r="G74" s="62"/>
-      <c r="H74" s="62"/>
+      <c r="C74" s="64"/>
+      <c r="D74" s="64" t="s">
+        <v>129</v>
+      </c>
+      <c r="E74" s="61"/>
+      <c r="F74" s="61"/>
+      <c r="G74" s="61"/>
+      <c r="H74" s="61"/>
     </row>
     <row r="75" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C75" s="65"/>
-      <c r="D75" s="65" t="s">
-        <v>132</v>
-      </c>
-      <c r="E75" s="62"/>
-      <c r="F75" s="62"/>
-      <c r="G75" s="62"/>
-      <c r="H75" s="62"/>
+      <c r="C75" s="64"/>
+      <c r="D75" s="64" t="s">
+        <v>125</v>
+      </c>
+      <c r="E75" s="61"/>
+      <c r="F75" s="61"/>
+      <c r="G75" s="61"/>
+      <c r="H75" s="61"/>
     </row>
     <row r="76" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C76" s="65"/>
-      <c r="D76" s="65" t="s">
-        <v>133</v>
-      </c>
-      <c r="E76" s="62"/>
-      <c r="F76" s="62"/>
-      <c r="G76" s="62"/>
-      <c r="H76" s="62"/>
+      <c r="C76" s="64"/>
+      <c r="D76" s="64" t="s">
+        <v>126</v>
+      </c>
+      <c r="E76" s="61"/>
+      <c r="F76" s="61"/>
+      <c r="G76" s="61"/>
+      <c r="H76" s="61"/>
     </row>
     <row r="77" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C77" s="65"/>
-      <c r="D77" s="65" t="s">
-        <v>134</v>
-      </c>
-      <c r="E77" s="62"/>
-      <c r="F77" s="62"/>
-      <c r="G77" s="62"/>
-      <c r="H77" s="62"/>
+      <c r="C77" s="64"/>
+      <c r="D77" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="E77" s="61"/>
+      <c r="F77" s="61"/>
+      <c r="G77" s="61"/>
+      <c r="H77" s="61"/>
     </row>
     <row r="78" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C78" s="65"/>
-      <c r="D78" s="65" t="s">
-        <v>135</v>
-      </c>
-      <c r="E78" s="62"/>
-      <c r="F78" s="62"/>
-      <c r="G78" s="62"/>
-      <c r="H78" s="62"/>
+      <c r="C78" s="64"/>
+      <c r="D78" s="64" t="s">
+        <v>128</v>
+      </c>
+      <c r="E78" s="61"/>
+      <c r="F78" s="61"/>
+      <c r="G78" s="61"/>
+      <c r="H78" s="61"/>
     </row>
     <row r="79" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C79" s="65"/>
-      <c r="D79" s="65"/>
-      <c r="E79" s="62"/>
-      <c r="F79" s="62"/>
-      <c r="G79" s="62"/>
-      <c r="H79" s="62"/>
+      <c r="C79" s="64"/>
+      <c r="D79" s="64"/>
+      <c r="E79" s="61"/>
+      <c r="F79" s="61"/>
+      <c r="G79" s="61"/>
+      <c r="H79" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -5229,6 +5397,8 @@
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="B21:B45"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="F30:F31"/>
     <mergeCell ref="C70:C71"/>
     <mergeCell ref="D70:D71"/>
     <mergeCell ref="C21:C22"/>
@@ -5240,8 +5410,6 @@
     <mergeCell ref="C33:C34"/>
     <mergeCell ref="D30:D31"/>
     <mergeCell ref="C30:C31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="F30:F31"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="C36:C37"/>
     <mergeCell ref="C4:C7"/>

</xml_diff>

<commit_message>
Auto push 2023-03-26 22:07:52.67
</commit_message>
<xml_diff>
--- a/project/CheeYoonMovie.xlsx
+++ b/project/CheeYoonMovie.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12240" activeTab="3"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="8" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="279">
   <si>
     <t>이용자 권한과 기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -540,10 +540,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>registerView.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">user/register.jsp </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -637,18 +633,6 @@
   </si>
   <si>
     <t>search.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>searchName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Search.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>main/search.jsp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -934,114 +918,231 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>NowPlayingListService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movie/nowPlayingList.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 상영영화 리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인화면(header,footer,sidebar)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>24금요일 자유게시판, 댓글, 현재상영작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자유게시판 조회 (답변, 페이징)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 검색 (이름,태그), 배우 검색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 상영작 리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상영 예고작 리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 랭킹 리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 제재 (회원 목록)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화,인물 등록, 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자유게시판 답변글 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21화요일 메인페이지틀,회원가입,로그인페이지틀 , css</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22수요일 메인페이지css조정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movieId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 상세보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상영 예고작 리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>upComingList.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movie/upComingList.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>25토요일 현재상영작,상영예고작, 영화상세보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardContentService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MovieContentService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UpComingListService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movie/movieContent.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>목요일 마지막 css 조정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금요일 포트폴리오</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>nowPlayingList.do</t>
-  </si>
-  <si>
-    <t>NowPlayingListService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>movie/nowPlayingList.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>현재 상영영화 리스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메인화면(header,footer,sidebar)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>24금요일 자유게시판, 댓글, 현재상영작</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자유게시판 조회 (답변, 페이징)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화 검색 (이름,태그), 배우 검색</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>현재 상영작 리스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상영 예고작 리스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화 랭킹 리스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원 제재 (회원 목록)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화,인물 등록, 수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자유게시판 답변글 기능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>21화요일 메인페이지틀,회원가입,로그인페이지틀 , css</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>22수요일 메인페이지css조정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>movieId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화 상세보기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상영 예고작 리스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>upComingList.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>movie/upComingList.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>25토요일 현재상영작,상영예고작, 영화상세보기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>26일요일 영화 상세보기 , 영화랭킹리스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BoardContentService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MovieContentService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UpComingListService.java</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>movieContent.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>movie/movieContent.jsp</t>
+  </si>
+  <si>
+    <t>registerView.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movieContent.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MainService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평점 중복확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movieId,userId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ratingConfirm.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RatingConfirmService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movie/ratingConfirm.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ratingWrite.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RatingWriteService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movieContent.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평점 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평점 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RatingDto속성들</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ratingModify.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RatingModifyService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RatingDto속성들
+pageNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ratingDelete.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userId,movieId,pageNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RatingDeleteService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movieContent.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화요일 관리자모드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>26일요일 영화 상세보기, 평점 등록,수정,삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수요일 평점 리스트? 영화랭킹?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>q(검색어)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SearchMovieService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main/search.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>월요일 검색사이트, 관리자모드</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1579,7 +1680,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1846,6 +1947,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2297,8 +2404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BP105"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="O50" sqref="O50"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J96" sqref="J96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.25" defaultRowHeight="11.25" x14ac:dyDescent="0.3"/>
@@ -2317,41 +2424,41 @@
     <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="92" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="91"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
@@ -2396,32 +2503,32 @@
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20"/>
-      <c r="C6" s="92" t="s">
+      <c r="C6" s="94" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="38"/>
-      <c r="E6" s="94" t="s">
+      <c r="E6" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="94"/>
-      <c r="G6" s="94"/>
-      <c r="H6" s="94"/>
-      <c r="I6" s="94"/>
-      <c r="J6" s="94"/>
-      <c r="K6" s="95"/>
-      <c r="L6" s="96" t="s">
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="96"/>
+      <c r="J6" s="96"/>
+      <c r="K6" s="97"/>
+      <c r="L6" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="94"/>
-      <c r="N6" s="94"/>
-      <c r="O6" s="94"/>
+      <c r="M6" s="96"/>
+      <c r="N6" s="96"/>
+      <c r="O6" s="96"/>
       <c r="P6" s="21"/>
       <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="93"/>
+      <c r="C7" s="95"/>
       <c r="D7" s="22"/>
       <c r="E7" s="87">
         <v>20</v>
@@ -2521,7 +2628,7 @@
     <row r="11" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="97" t="s">
+      <c r="C11" s="99" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="10"/>
@@ -2542,7 +2649,7 @@
     <row r="12" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="97"/>
+      <c r="C12" s="99"/>
       <c r="D12" s="10"/>
       <c r="E12" s="8"/>
       <c r="F12" s="6"/>
@@ -2580,7 +2687,7 @@
     <row r="14" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="89" t="s">
+      <c r="C14" s="91" t="s">
         <v>32</v>
       </c>
       <c r="D14" s="10"/>
@@ -2601,7 +2708,7 @@
     <row r="15" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="89"/>
+      <c r="C15" s="91"/>
       <c r="D15" s="10"/>
       <c r="E15" s="8"/>
       <c r="F15" s="6"/>
@@ -2639,7 +2746,7 @@
     <row r="17" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="97" t="s">
+      <c r="C17" s="99" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="10"/>
@@ -2660,7 +2767,7 @@
     <row r="18" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="97"/>
+      <c r="C18" s="99"/>
       <c r="D18" s="10"/>
       <c r="E18" s="8"/>
       <c r="F18" s="6"/>
@@ -2719,8 +2826,8 @@
     <row r="21" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="99" t="s">
-        <v>230</v>
+      <c r="C21" s="101" t="s">
+        <v>225</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="37"/>
@@ -2740,7 +2847,7 @@
     <row r="22" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="99"/>
+      <c r="C22" s="101"/>
       <c r="D22" s="10"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
@@ -2778,7 +2885,7 @@
     <row r="24" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="99" t="s">
+      <c r="C24" s="101" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="10"/>
@@ -2799,7 +2906,7 @@
     <row r="25" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="99"/>
+      <c r="C25" s="101"/>
       <c r="D25" s="10"/>
       <c r="E25" s="6"/>
       <c r="F25" s="8"/>
@@ -2837,7 +2944,7 @@
     <row r="27" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="99" t="s">
+      <c r="C27" s="101" t="s">
         <v>90</v>
       </c>
       <c r="D27" s="10"/>
@@ -2858,7 +2965,7 @@
     <row r="28" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="99"/>
+      <c r="C28" s="101"/>
       <c r="D28" s="10"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -2896,7 +3003,7 @@
     <row r="30" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="99" t="s">
+      <c r="C30" s="101" t="s">
         <v>91</v>
       </c>
       <c r="D30" s="10"/>
@@ -2917,7 +3024,7 @@
     <row r="31" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="99"/>
+      <c r="C31" s="101"/>
       <c r="D31" s="10"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -2955,8 +3062,8 @@
     <row r="33" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="99" t="s">
-        <v>239</v>
+      <c r="C33" s="101" t="s">
+        <v>234</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="6"/>
@@ -2976,7 +3083,7 @@
     <row r="34" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="6"/>
-      <c r="C34" s="99"/>
+      <c r="C34" s="101"/>
       <c r="D34" s="10"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -3014,7 +3121,7 @@
     <row r="36" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="16"/>
       <c r="B36" s="6"/>
-      <c r="C36" s="99" t="s">
+      <c r="C36" s="101" t="s">
         <v>92</v>
       </c>
       <c r="D36" s="10"/>
@@ -3025,7 +3132,7 @@
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
       <c r="K36" s="5"/>
-      <c r="L36" s="6"/>
+      <c r="L36" s="37"/>
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
       <c r="O36" s="6"/>
@@ -3035,7 +3142,7 @@
     <row r="37" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
       <c r="B37" s="6"/>
-      <c r="C37" s="99"/>
+      <c r="C37" s="101"/>
       <c r="D37" s="10"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
@@ -3043,7 +3150,7 @@
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
+      <c r="K37" s="8"/>
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
       <c r="N37" s="6"/>
@@ -3094,7 +3201,7 @@
     <row r="40" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="6"/>
-      <c r="C40" s="100" t="s">
+      <c r="C40" s="102" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="10"/>
@@ -3115,7 +3222,7 @@
     <row r="41" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="100"/>
+      <c r="C41" s="102"/>
       <c r="D41" s="10"/>
       <c r="E41" s="6"/>
       <c r="F41" s="8"/>
@@ -3153,8 +3260,8 @@
     <row r="43" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="16"/>
       <c r="B43" s="6"/>
-      <c r="C43" s="100" t="s">
-        <v>232</v>
+      <c r="C43" s="102" t="s">
+        <v>227</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="6"/>
@@ -3174,7 +3281,7 @@
     <row r="44" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="100"/>
+      <c r="C44" s="102"/>
       <c r="D44" s="10"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
@@ -3212,8 +3319,8 @@
     <row r="46" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16"/>
       <c r="B46" s="6"/>
-      <c r="C46" s="100" t="s">
-        <v>234</v>
+      <c r="C46" s="102" t="s">
+        <v>229</v>
       </c>
       <c r="D46" s="10"/>
       <c r="E46" s="6"/>
@@ -3232,7 +3339,7 @@
     <row r="47" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="100"/>
+      <c r="C47" s="102"/>
       <c r="D47" s="10"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
@@ -3270,8 +3377,8 @@
     <row r="49" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="16"/>
       <c r="B49" s="6"/>
-      <c r="C49" s="100" t="s">
-        <v>235</v>
+      <c r="C49" s="102" t="s">
+        <v>230</v>
       </c>
       <c r="D49" s="10"/>
       <c r="E49" s="6"/>
@@ -3291,7 +3398,7 @@
     <row r="50" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="100"/>
+      <c r="C50" s="102"/>
       <c r="D50" s="10"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
@@ -3329,7 +3436,7 @@
     <row r="52" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="16"/>
       <c r="B52" s="6"/>
-      <c r="C52" s="100" t="s">
+      <c r="C52" s="102" t="s">
         <v>112</v>
       </c>
       <c r="D52" s="10"/>
@@ -3350,15 +3457,15 @@
     <row r="53" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16"/>
       <c r="B53" s="6"/>
-      <c r="C53" s="100"/>
+      <c r="C53" s="102"/>
       <c r="D53" s="10"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
-      <c r="J53" s="6"/>
-      <c r="K53" s="6"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="8"/>
       <c r="L53" s="6"/>
       <c r="M53" s="6"/>
       <c r="N53" s="6"/>
@@ -3388,8 +3495,8 @@
     <row r="55" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="100" t="s">
-        <v>236</v>
+      <c r="C55" s="102" t="s">
+        <v>231</v>
       </c>
       <c r="D55" s="10"/>
       <c r="E55" s="6"/>
@@ -3398,18 +3505,17 @@
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
-      <c r="K55" s="37"/>
       <c r="L55" s="6"/>
       <c r="M55" s="6"/>
       <c r="N55" s="6"/>
-      <c r="O55" s="6"/>
+      <c r="O55" s="37"/>
       <c r="P55" s="16"/>
       <c r="Q55" s="5"/>
     </row>
     <row r="56" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="16"/>
       <c r="B56" s="6"/>
-      <c r="C56" s="100"/>
+      <c r="C56" s="102"/>
       <c r="D56" s="10"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
@@ -3447,8 +3553,8 @@
     <row r="58" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="100" t="s">
-        <v>233</v>
+      <c r="C58" s="102" t="s">
+        <v>228</v>
       </c>
       <c r="D58" s="10"/>
       <c r="E58" s="6"/>
@@ -3458,8 +3564,8 @@
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
       <c r="K58" s="6"/>
-      <c r="L58" s="6"/>
-      <c r="M58" s="6"/>
+      <c r="L58" s="37"/>
+      <c r="M58" s="37"/>
       <c r="N58" s="6"/>
       <c r="O58" s="6"/>
       <c r="P58" s="16"/>
@@ -3468,7 +3574,7 @@
     <row r="59" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="16"/>
       <c r="B59" s="6"/>
-      <c r="C59" s="100"/>
+      <c r="C59" s="102"/>
       <c r="D59" s="10"/>
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
@@ -3527,7 +3633,7 @@
     <row r="62" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="16"/>
       <c r="B62" s="6"/>
-      <c r="C62" s="98" t="s">
+      <c r="C62" s="100" t="s">
         <v>93</v>
       </c>
       <c r="D62" s="10"/>
@@ -3548,7 +3654,7 @@
     <row r="63" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="16"/>
       <c r="B63" s="6"/>
-      <c r="C63" s="98"/>
+      <c r="C63" s="100"/>
       <c r="D63" s="10"/>
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
@@ -3586,7 +3692,7 @@
     <row r="65" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="16"/>
       <c r="B65" s="6"/>
-      <c r="C65" s="98" t="s">
+      <c r="C65" s="100" t="s">
         <v>111</v>
       </c>
       <c r="D65" s="10"/>
@@ -3607,7 +3713,7 @@
     <row r="66" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="16"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="98"/>
+      <c r="C66" s="100"/>
       <c r="D66" s="10"/>
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
@@ -3645,8 +3751,8 @@
     <row r="68" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="16"/>
       <c r="B68" s="6"/>
-      <c r="C68" s="98" t="s">
-        <v>237</v>
+      <c r="C68" s="100" t="s">
+        <v>232</v>
       </c>
       <c r="D68" s="10"/>
       <c r="E68" s="6"/>
@@ -3666,7 +3772,7 @@
     <row r="69" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="98"/>
+      <c r="C69" s="100"/>
       <c r="D69" s="10"/>
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
@@ -3704,8 +3810,8 @@
     <row r="71" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="16"/>
       <c r="B71" s="6"/>
-      <c r="C71" s="98" t="s">
-        <v>238</v>
+      <c r="C71" s="100" t="s">
+        <v>233</v>
       </c>
       <c r="D71" s="10"/>
       <c r="E71" s="6"/>
@@ -3725,7 +3831,7 @@
     <row r="72" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16"/>
       <c r="B72" s="6"/>
-      <c r="C72" s="98"/>
+      <c r="C72" s="100"/>
       <c r="D72" s="10"/>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
@@ -3763,7 +3869,7 @@
     <row r="74" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16"/>
       <c r="B74" s="6"/>
-      <c r="C74" s="98" t="s">
+      <c r="C74" s="100" t="s">
         <v>110</v>
       </c>
       <c r="D74" s="10"/>
@@ -3784,7 +3890,7 @@
     <row r="75" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="16"/>
       <c r="B75" s="6"/>
-      <c r="C75" s="98"/>
+      <c r="C75" s="100"/>
       <c r="D75" s="10"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
@@ -3822,7 +3928,7 @@
     <row r="77" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="16"/>
       <c r="B77" s="6"/>
-      <c r="C77" s="102" t="s">
+      <c r="C77" s="104" t="s">
         <v>54</v>
       </c>
       <c r="D77" s="7"/>
@@ -3843,7 +3949,7 @@
     <row r="78" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="16"/>
       <c r="B78" s="6"/>
-      <c r="C78" s="102"/>
+      <c r="C78" s="104"/>
       <c r="D78" s="7"/>
       <c r="E78" s="6"/>
       <c r="F78" s="6"/>
@@ -3862,7 +3968,7 @@
     <row r="79" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="16"/>
       <c r="B79" s="6"/>
-      <c r="C79" s="104" t="s">
+      <c r="C79" s="106" t="s">
         <v>88</v>
       </c>
       <c r="D79" s="7"/>
@@ -3933,7 +4039,7 @@
     <row r="80" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="16"/>
       <c r="B80" s="6"/>
-      <c r="C80" s="104"/>
+      <c r="C80" s="106"/>
       <c r="D80" s="7"/>
       <c r="E80" s="6"/>
       <c r="F80" s="6"/>
@@ -4061,18 +4167,18 @@
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5"/>
-      <c r="F84" s="103"/>
-      <c r="G84" s="103"/>
+      <c r="F84" s="105"/>
+      <c r="G84" s="105"/>
       <c r="H84" s="6"/>
       <c r="I84" s="37" t="s">
         <v>56</v>
       </c>
       <c r="J84" s="37"/>
       <c r="K84" s="6"/>
-      <c r="L84" s="101" t="s">
+      <c r="L84" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="M84" s="101"/>
+      <c r="M84" s="103"/>
       <c r="N84" s="39"/>
       <c r="O84" s="5"/>
       <c r="P84" s="5"/>
@@ -4098,53 +4204,63 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C87" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C88" s="4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C89" s="4" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C90" s="85" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C91" s="85" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C92" s="85" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C93" s="85" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C94" s="85" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C95" s="85" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C96" s="85" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C97" s="85" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C98" s="85" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C94" s="85"/>
-    </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C95" s="85"/>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C96" s="85"/>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C97" s="85"/>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C98" s="85"/>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C99" s="85"/>
@@ -4228,7 +4344,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="107" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -4238,7 +4354,7 @@
       <c r="D3" s="57"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="105"/>
+      <c r="A4" s="107"/>
       <c r="B4" s="1" t="s">
         <v>96</v>
       </c>
@@ -4253,7 +4369,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="105"/>
+      <c r="A5" s="107"/>
       <c r="B5" s="1" t="s">
         <v>97</v>
       </c>
@@ -4326,7 +4442,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C1" s="69"/>
     </row>
@@ -4342,7 +4458,7 @@
       </c>
       <c r="C3" s="58"/>
       <c r="E3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -4352,39 +4468,39 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C5" s="66"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C6" s="67"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" s="68"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C10" s="70"/>
       <c r="D10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C11" s="71"/>
       <c r="D11">
@@ -4393,7 +4509,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C12" s="72"/>
       <c r="D12">
@@ -4402,7 +4518,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C13" s="68"/>
       <c r="D13">
@@ -4411,7 +4527,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -4419,7 +4535,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -4532,8 +4648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="D40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4571,7 +4687,7 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="108" t="s">
         <v>39</v>
       </c>
       <c r="C3" s="43" t="s">
@@ -4584,77 +4700,79 @@
         <v>66</v>
       </c>
       <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
+      <c r="G3" s="44" t="s">
+        <v>253</v>
+      </c>
       <c r="H3" s="44" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="107"/>
-      <c r="C4" s="110" t="s">
+      <c r="B4" s="109"/>
+      <c r="C4" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="110" t="s">
+      <c r="D4" s="112" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="44" t="s">
-        <v>131</v>
+        <v>251</v>
       </c>
       <c r="F4" s="44"/>
       <c r="G4" s="44"/>
       <c r="H4" s="44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="107"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="107"/>
+      <c r="B5" s="109"/>
+      <c r="C5" s="109"/>
+      <c r="D5" s="109"/>
       <c r="E5" s="44" t="s">
         <v>118</v>
       </c>
       <c r="F5" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="G5" s="44" t="s">
         <v>137</v>
-      </c>
-      <c r="G5" s="44" t="s">
-        <v>138</v>
       </c>
       <c r="H5" s="44" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="107"/>
-      <c r="C6" s="107"/>
-      <c r="D6" s="107"/>
+      <c r="B6" s="109"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="109"/>
       <c r="E6" s="44" t="s">
         <v>119</v>
       </c>
       <c r="F6" s="44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G6" s="44" t="s">
         <v>121</v>
       </c>
       <c r="H6" s="44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="108"/>
-      <c r="C7" s="108"/>
-      <c r="D7" s="108"/>
+      <c r="B7" s="110"/>
+      <c r="C7" s="110"/>
+      <c r="D7" s="110"/>
       <c r="E7" s="44" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F7" s="44" t="s">
         <v>116</v>
       </c>
       <c r="G7" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="H7" s="44" t="s">
         <v>135</v>
-      </c>
-      <c r="H7" s="44" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
@@ -4670,59 +4788,59 @@
       <c r="B9" s="63"/>
       <c r="C9" s="83"/>
       <c r="D9" s="83" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>226</v>
+        <v>249</v>
       </c>
       <c r="F9" s="44"/>
       <c r="G9" s="44" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="H9" s="44" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="82"/>
       <c r="C10" s="83"/>
       <c r="D10" s="86" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="E10" s="44" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="F10" s="44"/>
       <c r="G10" s="44" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="H10" s="44" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="82"/>
       <c r="C11" s="83"/>
       <c r="D11" s="83" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E11" s="44" t="s">
         <v>252</v>
       </c>
       <c r="F11" s="44" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G11" s="44" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="H11" s="44" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="82"/>
       <c r="C12" s="83"/>
-      <c r="D12" s="83"/>
+      <c r="D12" s="89"/>
       <c r="E12" s="44"/>
       <c r="F12" s="44"/>
       <c r="G12" s="44"/>
@@ -4731,11 +4849,21 @@
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="82"/>
       <c r="C13" s="83"/>
-      <c r="D13" s="83"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
+      <c r="D13" s="89" t="s">
+        <v>254</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>256</v>
+      </c>
+      <c r="F13" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="G13" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="H13" s="44" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="82"/>
@@ -4749,29 +4877,57 @@
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="82"/>
       <c r="C15" s="83"/>
-      <c r="D15" s="83"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D15" s="83" t="s">
+        <v>263</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>259</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>264</v>
+      </c>
+      <c r="G15" s="44" t="s">
+        <v>260</v>
+      </c>
+      <c r="H15" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="33" x14ac:dyDescent="0.3">
       <c r="B16" s="82"/>
       <c r="C16" s="83"/>
-      <c r="D16" s="83"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
+      <c r="D16" s="83" t="s">
+        <v>262</v>
+      </c>
+      <c r="E16" s="44" t="s">
+        <v>265</v>
+      </c>
+      <c r="F16" s="90" t="s">
+        <v>267</v>
+      </c>
+      <c r="G16" s="44" t="s">
+        <v>266</v>
+      </c>
+      <c r="H16" s="44" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="82"/>
       <c r="C17" s="83"/>
       <c r="D17" s="83"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
+      <c r="E17" s="44" t="s">
+        <v>268</v>
+      </c>
+      <c r="F17" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="G17" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="H17" s="44" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="82"/>
@@ -4800,26 +4956,26 @@
         <v>123</v>
       </c>
       <c r="E20" s="44" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F20" s="44" t="s">
-        <v>156</v>
+        <v>275</v>
       </c>
       <c r="G20" s="44" t="s">
-        <v>157</v>
+        <v>276</v>
       </c>
       <c r="H20" s="44" t="s">
-        <v>158</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="119" t="s">
+      <c r="B21" s="121" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="114" t="s">
+      <c r="C21" s="116" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="114" t="s">
+      <c r="D21" s="116" t="s">
         <v>69</v>
       </c>
       <c r="E21" s="46" t="s">
@@ -4828,13 +4984,13 @@
       <c r="F21" s="46"/>
       <c r="G21" s="46"/>
       <c r="H21" s="46" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="120"/>
-      <c r="C22" s="115"/>
-      <c r="D22" s="115"/>
+      <c r="B22" s="122"/>
+      <c r="C22" s="117"/>
+      <c r="D22" s="117"/>
       <c r="E22" s="46" t="s">
         <v>70</v>
       </c>
@@ -4842,14 +4998,14 @@
         <v>124</v>
       </c>
       <c r="G22" s="46" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H22" s="47" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="120"/>
+      <c r="B23" s="122"/>
       <c r="C23" s="46" t="s">
         <v>71</v>
       </c>
@@ -4857,52 +5013,52 @@
         <v>72</v>
       </c>
       <c r="E23" s="46" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F23" s="46"/>
       <c r="G23" s="46" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H23" s="47" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="120"/>
-      <c r="C24" s="114" t="s">
+      <c r="B24" s="122"/>
+      <c r="C24" s="116" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="114" t="s">
+      <c r="D24" s="116" t="s">
         <v>74</v>
       </c>
       <c r="E24" s="46" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F24" s="46"/>
       <c r="G24" s="46"/>
       <c r="H24" s="46" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="120"/>
-      <c r="C25" s="115"/>
-      <c r="D25" s="115"/>
+      <c r="B25" s="122"/>
+      <c r="C25" s="117"/>
+      <c r="D25" s="117"/>
       <c r="E25" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="F25" s="47" t="s">
+        <v>156</v>
+      </c>
+      <c r="G25" s="46" t="s">
+        <v>163</v>
+      </c>
+      <c r="H25" s="46" t="s">
         <v>166</v>
       </c>
-      <c r="F25" s="47" t="s">
-        <v>160</v>
-      </c>
-      <c r="G25" s="46" t="s">
-        <v>167</v>
-      </c>
-      <c r="H25" s="46" t="s">
-        <v>170</v>
-      </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="120"/>
+      <c r="B26" s="122"/>
       <c r="C26" s="47" t="s">
         <v>78</v>
       </c>
@@ -4910,18 +5066,18 @@
         <v>77</v>
       </c>
       <c r="E26" s="47" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F26" s="47"/>
       <c r="G26" s="47" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H26" s="47" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="120"/>
+      <c r="B27" s="122"/>
       <c r="C27" s="47"/>
       <c r="D27" s="47"/>
       <c r="E27" s="47"/>
@@ -4930,7 +5086,7 @@
       <c r="H27" s="47"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="120"/>
+      <c r="B28" s="122"/>
       <c r="C28" s="47"/>
       <c r="D28" s="47"/>
       <c r="E28" s="47"/>
@@ -4939,7 +5095,7 @@
       <c r="H28" s="47"/>
     </row>
     <row r="29" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="120"/>
+      <c r="B29" s="122"/>
       <c r="C29" s="73" t="s">
         <v>42</v>
       </c>
@@ -4947,128 +5103,128 @@
         <v>46</v>
       </c>
       <c r="E29" s="73" t="s">
+        <v>167</v>
+      </c>
+      <c r="F29" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="G29" s="73" t="s">
+        <v>168</v>
+      </c>
+      <c r="H29" s="73" t="s">
         <v>171</v>
       </c>
-      <c r="F29" s="73" t="s">
-        <v>173</v>
-      </c>
-      <c r="G29" s="73" t="s">
-        <v>172</v>
-      </c>
-      <c r="H29" s="73" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="30" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="120"/>
-      <c r="C30" s="111" t="s">
+      <c r="B30" s="122"/>
+      <c r="C30" s="113" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="111" t="s">
+      <c r="D30" s="113" t="s">
         <v>47</v>
       </c>
-      <c r="E30" s="111" t="s">
-        <v>180</v>
-      </c>
-      <c r="F30" s="121" t="s">
-        <v>182</v>
-      </c>
-      <c r="G30" s="121" t="s">
-        <v>249</v>
-      </c>
-      <c r="H30" s="111" t="s">
-        <v>174</v>
+      <c r="E30" s="113" t="s">
+        <v>176</v>
+      </c>
+      <c r="F30" s="123" t="s">
+        <v>178</v>
+      </c>
+      <c r="G30" s="123" t="s">
+        <v>243</v>
+      </c>
+      <c r="H30" s="113" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="120"/>
-      <c r="C31" s="112"/>
-      <c r="D31" s="112"/>
-      <c r="E31" s="112"/>
-      <c r="F31" s="122"/>
-      <c r="G31" s="122"/>
-      <c r="H31" s="112"/>
+      <c r="B31" s="122"/>
+      <c r="C31" s="114"/>
+      <c r="D31" s="114"/>
+      <c r="E31" s="114"/>
+      <c r="F31" s="124"/>
+      <c r="G31" s="124"/>
+      <c r="H31" s="114"/>
     </row>
     <row r="32" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B32" s="120"/>
+      <c r="B32" s="122"/>
       <c r="C32" s="81"/>
       <c r="D32" s="79" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E32" s="78" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F32" s="77" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G32" s="78" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="H32" s="78" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B33" s="120"/>
-      <c r="C33" s="111"/>
-      <c r="D33" s="111" t="s">
+      <c r="B33" s="122"/>
+      <c r="C33" s="113"/>
+      <c r="D33" s="113" t="s">
+        <v>181</v>
+      </c>
+      <c r="E33" s="80" t="s">
+        <v>182</v>
+      </c>
+      <c r="F33" s="77" t="s">
+        <v>211</v>
+      </c>
+      <c r="G33" s="78" t="s">
+        <v>188</v>
+      </c>
+      <c r="H33" s="73" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B34" s="122"/>
+      <c r="C34" s="114"/>
+      <c r="D34" s="114"/>
+      <c r="E34" s="80" t="s">
+        <v>184</v>
+      </c>
+      <c r="F34" s="77" t="s">
+        <v>212</v>
+      </c>
+      <c r="G34" s="78" t="s">
         <v>185</v>
       </c>
-      <c r="E33" s="80" t="s">
-        <v>186</v>
-      </c>
-      <c r="F33" s="77" t="s">
-        <v>215</v>
-      </c>
-      <c r="G33" s="78" t="s">
+      <c r="H34" s="78" t="s">
         <v>192</v>
       </c>
-      <c r="H33" s="73" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B34" s="120"/>
-      <c r="C34" s="112"/>
-      <c r="D34" s="112"/>
-      <c r="E34" s="80" t="s">
-        <v>188</v>
-      </c>
-      <c r="F34" s="77" t="s">
-        <v>216</v>
-      </c>
-      <c r="G34" s="78" t="s">
-        <v>189</v>
-      </c>
-      <c r="H34" s="78" t="s">
-        <v>196</v>
-      </c>
     </row>
     <row r="35" spans="2:8" ht="66" x14ac:dyDescent="0.3">
-      <c r="B35" s="120"/>
+      <c r="B35" s="122"/>
       <c r="C35" s="74"/>
       <c r="D35" s="81" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E35" s="80" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F35" s="77" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G35" s="80" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H35" s="80" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="120"/>
-      <c r="C36" s="109" t="s">
+      <c r="B36" s="122"/>
+      <c r="C36" s="111" t="s">
         <v>41</v>
       </c>
-      <c r="D36" s="109" t="s">
+      <c r="D36" s="111" t="s">
         <v>45</v>
       </c>
       <c r="E36" s="48" t="s">
@@ -5077,66 +5233,66 @@
       <c r="F36" s="48"/>
       <c r="G36" s="49"/>
       <c r="H36" s="48" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37" s="122"/>
+      <c r="C37" s="111"/>
+      <c r="D37" s="111"/>
+      <c r="E37" s="48" t="s">
+        <v>196</v>
+      </c>
+      <c r="F37" s="77" t="s">
+        <v>208</v>
+      </c>
+      <c r="G37" s="48" t="s">
+        <v>197</v>
+      </c>
+      <c r="H37" s="48" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B38" s="122"/>
+      <c r="C38" s="113" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="113" t="s">
+        <v>52</v>
+      </c>
+      <c r="E38" s="73" t="s">
+        <v>198</v>
+      </c>
+      <c r="F38" s="77" t="s">
+        <v>205</v>
+      </c>
+      <c r="G38" s="73" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="120"/>
-      <c r="C37" s="109"/>
-      <c r="D37" s="109"/>
-      <c r="E37" s="48" t="s">
+      <c r="H38" s="73" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B39" s="122"/>
+      <c r="C39" s="114"/>
+      <c r="D39" s="114"/>
+      <c r="E39" s="73" t="s">
         <v>200</v>
       </c>
-      <c r="F37" s="77" t="s">
-        <v>212</v>
-      </c>
-      <c r="G37" s="48" t="s">
-        <v>201</v>
-      </c>
-      <c r="H37" s="48" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B38" s="120"/>
-      <c r="C38" s="111" t="s">
-        <v>44</v>
-      </c>
-      <c r="D38" s="111" t="s">
-        <v>52</v>
-      </c>
-      <c r="E38" s="73" t="s">
+      <c r="F39" s="77" t="s">
+        <v>206</v>
+      </c>
+      <c r="G39" s="73" t="s">
+        <v>204</v>
+      </c>
+      <c r="H39" s="73" t="s">
         <v>202</v>
       </c>
-      <c r="F38" s="77" t="s">
-        <v>209</v>
-      </c>
-      <c r="G38" s="73" t="s">
-        <v>203</v>
-      </c>
-      <c r="H38" s="73" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B39" s="120"/>
-      <c r="C39" s="112"/>
-      <c r="D39" s="112"/>
-      <c r="E39" s="73" t="s">
-        <v>204</v>
-      </c>
-      <c r="F39" s="77" t="s">
-        <v>210</v>
-      </c>
-      <c r="G39" s="73" t="s">
-        <v>208</v>
-      </c>
-      <c r="H39" s="73" t="s">
-        <v>206</v>
-      </c>
     </row>
     <row r="40" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B40" s="120"/>
+      <c r="B40" s="122"/>
       <c r="C40" s="80" t="s">
         <v>48</v>
       </c>
@@ -5147,55 +5303,55 @@
         <v>80</v>
       </c>
       <c r="F40" s="77" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G40" s="80" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H40" s="80" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B41" s="120"/>
-      <c r="C41" s="111" t="s">
+      <c r="B41" s="122"/>
+      <c r="C41" s="113" t="s">
         <v>49</v>
       </c>
-      <c r="D41" s="111" t="s">
+      <c r="D41" s="113" t="s">
         <v>50</v>
       </c>
       <c r="E41" s="73" t="s">
+        <v>214</v>
+      </c>
+      <c r="F41" s="77" t="s">
+        <v>219</v>
+      </c>
+      <c r="G41" s="73" t="s">
         <v>218</v>
       </c>
-      <c r="F41" s="77" t="s">
-        <v>223</v>
-      </c>
-      <c r="G41" s="73" t="s">
-        <v>222</v>
-      </c>
       <c r="H41" s="73" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B42" s="122"/>
+      <c r="C42" s="114"/>
+      <c r="D42" s="114"/>
+      <c r="E42" s="73" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B42" s="120"/>
-      <c r="C42" s="112"/>
-      <c r="D42" s="112"/>
-      <c r="E42" s="73" t="s">
-        <v>224</v>
-      </c>
       <c r="F42" s="77" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G42" s="73" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="H42" s="73" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B43" s="120"/>
+      <c r="B43" s="122"/>
       <c r="C43" s="81"/>
       <c r="D43" s="81"/>
       <c r="E43" s="80"/>
@@ -5204,7 +5360,7 @@
       <c r="H43" s="80"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B44" s="120"/>
+      <c r="B44" s="122"/>
       <c r="C44" s="81"/>
       <c r="D44" s="81"/>
       <c r="E44" s="80"/>
@@ -5213,7 +5369,7 @@
       <c r="H44" s="80"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B45" s="120"/>
+      <c r="B45" s="122"/>
       <c r="C45" s="81"/>
       <c r="D45" s="81"/>
       <c r="E45" s="80"/>
@@ -5222,18 +5378,18 @@
       <c r="H45" s="80"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B46" s="116" t="s">
+      <c r="B46" s="118" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B47" s="117"/>
+      <c r="B47" s="119"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B48" s="117"/>
+      <c r="B48" s="119"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B49" s="118"/>
+      <c r="B49" s="120"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B50" s="62"/>
@@ -5255,26 +5411,26 @@
     </row>
     <row r="63" spans="2:8" ht="33" x14ac:dyDescent="0.3">
       <c r="D63" s="76" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E63" s="78" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F63" s="77" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G63" s="78" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H63" s="75" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="70" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C70" s="113" t="s">
+      <c r="C70" s="115" t="s">
         <v>57</v>
       </c>
-      <c r="D70" s="113" t="s">
+      <c r="D70" s="115" t="s">
         <v>59</v>
       </c>
       <c r="E70" s="45" t="s">
@@ -5287,8 +5443,8 @@
       </c>
     </row>
     <row r="71" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C71" s="113"/>
-      <c r="D71" s="113"/>
+      <c r="C71" s="115"/>
+      <c r="D71" s="115"/>
       <c r="E71" s="45" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Auto push 2023-03-27 13:11:15.14
</commit_message>
<xml_diff>
--- a/project/CheeYoonMovie.xlsx
+++ b/project/CheeYoonMovie.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12240"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12240" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="8" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="287">
   <si>
     <t>이용자 권한과 기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -247,10 +247,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>adminLogin.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>관리자모드 로그인</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -319,10 +315,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>admin/adminLogin.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>회원탈퇴</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -352,10 +344,6 @@
   </si>
   <si>
     <t>Controller 요청 경로</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>adminLoginView.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -668,10 +656,6 @@
   </si>
   <si>
     <t>UserModifyService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>withdrawal.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -962,10 +946,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>영화,인물 등록, 수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>자유게시판 답변글 기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1126,10 +1106,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>수요일 평점 리스트? 영화랭킹?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>q(검색어)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1143,6 +1119,62 @@
   </si>
   <si>
     <t>월요일 검색사이트, 관리자모드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수요일 평점 리스트? 영화랭킹? 마이메뉴?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평점 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 등록, 수정 (인물)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자유게시판 댓글 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자유게시판 댓글 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자유게시판 댓글 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 평점 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평점 중복 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 평점 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 평점 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin/adminLogin.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adminLoginView.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>withdrawal.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adminLogin.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1680,7 +1712,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1876,9 +1908,6 @@
     <xf numFmtId="0" fontId="11" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -1948,11 +1977,38 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1978,33 +2034,48 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2014,47 +2085,11 @@
     <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2092,6 +2127,7 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFFFFFCC"/>
       <color rgb="FF2C2C2C"/>
       <color rgb="FF4B4B4B"/>
       <color rgb="FF646464"/>
@@ -2101,7 +2137,6 @@
       <color rgb="FF0A0A0A"/>
       <color rgb="FF373737"/>
       <color rgb="FF3FFFDA"/>
-      <color rgb="FFFFFFCC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2404,8 +2439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BP105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J96" sqref="J96"/>
+    <sheetView topLeftCell="A58" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J73" sqref="J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.25" defaultRowHeight="11.25" x14ac:dyDescent="0.3"/>
@@ -2424,41 +2459,41 @@
     <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="92" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="93"/>
-      <c r="M2" s="93"/>
-      <c r="N2" s="93"/>
-      <c r="O2" s="93"/>
+      <c r="B2" s="100" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
+      <c r="O2" s="101"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
+      <c r="O3" s="101"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
@@ -2503,64 +2538,64 @@
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20"/>
-      <c r="C6" s="94" t="s">
+      <c r="C6" s="102" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="38"/>
-      <c r="E6" s="96" t="s">
+      <c r="E6" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="96"/>
-      <c r="G6" s="96"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="96"/>
-      <c r="J6" s="96"/>
-      <c r="K6" s="97"/>
-      <c r="L6" s="98" t="s">
+      <c r="F6" s="104"/>
+      <c r="G6" s="104"/>
+      <c r="H6" s="104"/>
+      <c r="I6" s="104"/>
+      <c r="J6" s="104"/>
+      <c r="K6" s="105"/>
+      <c r="L6" s="106" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="96"/>
-      <c r="N6" s="96"/>
-      <c r="O6" s="96"/>
+      <c r="M6" s="104"/>
+      <c r="N6" s="104"/>
+      <c r="O6" s="104"/>
       <c r="P6" s="21"/>
       <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="95"/>
+      <c r="C7" s="103"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="87">
+      <c r="E7" s="86">
         <v>20</v>
       </c>
-      <c r="F7" s="87">
+      <c r="F7" s="86">
         <v>21</v>
       </c>
-      <c r="G7" s="87">
+      <c r="G7" s="86">
         <v>22</v>
       </c>
-      <c r="H7" s="87">
+      <c r="H7" s="86">
         <v>23</v>
       </c>
-      <c r="I7" s="87">
+      <c r="I7" s="86">
         <v>24</v>
       </c>
-      <c r="J7" s="87">
+      <c r="J7" s="86">
         <v>25</v>
       </c>
-      <c r="K7" s="88">
+      <c r="K7" s="87">
         <v>26</v>
       </c>
-      <c r="L7" s="87">
+      <c r="L7" s="86">
         <v>27</v>
       </c>
-      <c r="M7" s="87">
+      <c r="M7" s="86">
         <v>28</v>
       </c>
-      <c r="N7" s="87">
+      <c r="N7" s="86">
         <v>29</v>
       </c>
-      <c r="O7" s="87">
+      <c r="O7" s="86">
         <v>30</v>
       </c>
       <c r="P7" s="23"/>
@@ -2628,7 +2663,7 @@
     <row r="11" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="99" t="s">
+      <c r="C11" s="96" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="10"/>
@@ -2649,7 +2684,7 @@
     <row r="12" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="99"/>
+      <c r="C12" s="96"/>
       <c r="D12" s="10"/>
       <c r="E12" s="8"/>
       <c r="F12" s="6"/>
@@ -2687,7 +2722,7 @@
     <row r="14" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="91" t="s">
+      <c r="C14" s="99" t="s">
         <v>32</v>
       </c>
       <c r="D14" s="10"/>
@@ -2708,7 +2743,7 @@
     <row r="15" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="91"/>
+      <c r="C15" s="99"/>
       <c r="D15" s="10"/>
       <c r="E15" s="8"/>
       <c r="F15" s="6"/>
@@ -2746,7 +2781,7 @@
     <row r="17" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="99" t="s">
+      <c r="C17" s="96" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="10"/>
@@ -2767,7 +2802,7 @@
     <row r="18" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="99"/>
+      <c r="C18" s="96"/>
       <c r="D18" s="10"/>
       <c r="E18" s="8"/>
       <c r="F18" s="6"/>
@@ -2826,8 +2861,8 @@
     <row r="21" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="101" t="s">
-        <v>225</v>
+      <c r="C21" s="97" t="s">
+        <v>221</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="37"/>
@@ -2847,7 +2882,7 @@
     <row r="22" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="101"/>
+      <c r="C22" s="97"/>
       <c r="D22" s="10"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
@@ -2885,7 +2920,7 @@
     <row r="24" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="101" t="s">
+      <c r="C24" s="97" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="10"/>
@@ -2906,7 +2941,7 @@
     <row r="25" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="101"/>
+      <c r="C25" s="97"/>
       <c r="D25" s="10"/>
       <c r="E25" s="6"/>
       <c r="F25" s="8"/>
@@ -2944,8 +2979,8 @@
     <row r="27" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="101" t="s">
-        <v>90</v>
+      <c r="C27" s="97" t="s">
+        <v>87</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="6"/>
@@ -2965,7 +3000,7 @@
     <row r="28" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="101"/>
+      <c r="C28" s="97"/>
       <c r="D28" s="10"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -3003,8 +3038,8 @@
     <row r="30" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="101" t="s">
-        <v>91</v>
+      <c r="C30" s="97" t="s">
+        <v>88</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="6"/>
@@ -3024,7 +3059,7 @@
     <row r="31" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="101"/>
+      <c r="C31" s="97"/>
       <c r="D31" s="10"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -3062,8 +3097,8 @@
     <row r="33" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="101" t="s">
-        <v>234</v>
+      <c r="C33" s="97" t="s">
+        <v>229</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="6"/>
@@ -3083,7 +3118,7 @@
     <row r="34" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="6"/>
-      <c r="C34" s="101"/>
+      <c r="C34" s="97"/>
       <c r="D34" s="10"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -3121,8 +3156,8 @@
     <row r="36" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="16"/>
       <c r="B36" s="6"/>
-      <c r="C36" s="101" t="s">
-        <v>92</v>
+      <c r="C36" s="97" t="s">
+        <v>89</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="6"/>
@@ -3142,7 +3177,7 @@
     <row r="37" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
       <c r="B37" s="6"/>
-      <c r="C37" s="101"/>
+      <c r="C37" s="97"/>
       <c r="D37" s="10"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
@@ -3201,7 +3236,7 @@
     <row r="40" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="6"/>
-      <c r="C40" s="102" t="s">
+      <c r="C40" s="98" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="10"/>
@@ -3222,7 +3257,7 @@
     <row r="41" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="102"/>
+      <c r="C41" s="98"/>
       <c r="D41" s="10"/>
       <c r="E41" s="6"/>
       <c r="F41" s="8"/>
@@ -3260,8 +3295,8 @@
     <row r="43" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="16"/>
       <c r="B43" s="6"/>
-      <c r="C43" s="102" t="s">
-        <v>227</v>
+      <c r="C43" s="98" t="s">
+        <v>223</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="6"/>
@@ -3281,7 +3316,7 @@
     <row r="44" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="102"/>
+      <c r="C44" s="98"/>
       <c r="D44" s="10"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
@@ -3319,8 +3354,8 @@
     <row r="46" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16"/>
       <c r="B46" s="6"/>
-      <c r="C46" s="102" t="s">
-        <v>229</v>
+      <c r="C46" s="98" t="s">
+        <v>225</v>
       </c>
       <c r="D46" s="10"/>
       <c r="E46" s="6"/>
@@ -3339,7 +3374,7 @@
     <row r="47" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="102"/>
+      <c r="C47" s="98"/>
       <c r="D47" s="10"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
@@ -3377,8 +3412,8 @@
     <row r="49" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="16"/>
       <c r="B49" s="6"/>
-      <c r="C49" s="102" t="s">
-        <v>230</v>
+      <c r="C49" s="98" t="s">
+        <v>226</v>
       </c>
       <c r="D49" s="10"/>
       <c r="E49" s="6"/>
@@ -3398,7 +3433,7 @@
     <row r="50" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="102"/>
+      <c r="C50" s="98"/>
       <c r="D50" s="10"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
@@ -3436,8 +3471,8 @@
     <row r="52" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="16"/>
       <c r="B52" s="6"/>
-      <c r="C52" s="102" t="s">
-        <v>112</v>
+      <c r="C52" s="98" t="s">
+        <v>109</v>
       </c>
       <c r="D52" s="10"/>
       <c r="E52" s="6"/>
@@ -3457,7 +3492,7 @@
     <row r="53" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16"/>
       <c r="B53" s="6"/>
-      <c r="C53" s="102"/>
+      <c r="C53" s="98"/>
       <c r="D53" s="10"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
@@ -3495,8 +3530,8 @@
     <row r="55" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="102" t="s">
-        <v>231</v>
+      <c r="C55" s="98" t="s">
+        <v>227</v>
       </c>
       <c r="D55" s="10"/>
       <c r="E55" s="6"/>
@@ -3515,7 +3550,7 @@
     <row r="56" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="16"/>
       <c r="B56" s="6"/>
-      <c r="C56" s="102"/>
+      <c r="C56" s="98"/>
       <c r="D56" s="10"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
@@ -3553,8 +3588,8 @@
     <row r="58" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="102" t="s">
-        <v>228</v>
+      <c r="C58" s="98" t="s">
+        <v>224</v>
       </c>
       <c r="D58" s="10"/>
       <c r="E58" s="6"/>
@@ -3574,7 +3609,7 @@
     <row r="59" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="16"/>
       <c r="B59" s="6"/>
-      <c r="C59" s="102"/>
+      <c r="C59" s="98"/>
       <c r="D59" s="10"/>
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
@@ -3583,7 +3618,7 @@
       <c r="I59" s="6"/>
       <c r="J59" s="6"/>
       <c r="K59" s="6"/>
-      <c r="L59" s="6"/>
+      <c r="L59" s="8"/>
       <c r="M59" s="6"/>
       <c r="N59" s="6"/>
       <c r="O59" s="6"/>
@@ -3633,8 +3668,8 @@
     <row r="62" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="16"/>
       <c r="B62" s="6"/>
-      <c r="C62" s="100" t="s">
-        <v>93</v>
+      <c r="C62" s="92" t="s">
+        <v>90</v>
       </c>
       <c r="D62" s="10"/>
       <c r="E62" s="6"/>
@@ -3654,7 +3689,7 @@
     <row r="63" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="16"/>
       <c r="B63" s="6"/>
-      <c r="C63" s="100"/>
+      <c r="C63" s="92"/>
       <c r="D63" s="10"/>
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
@@ -3692,8 +3727,8 @@
     <row r="65" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="16"/>
       <c r="B65" s="6"/>
-      <c r="C65" s="100" t="s">
-        <v>111</v>
+      <c r="C65" s="92" t="s">
+        <v>108</v>
       </c>
       <c r="D65" s="10"/>
       <c r="E65" s="6"/>
@@ -3713,7 +3748,7 @@
     <row r="66" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="16"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="100"/>
+      <c r="C66" s="92"/>
       <c r="D66" s="10"/>
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
@@ -3751,8 +3786,8 @@
     <row r="68" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="16"/>
       <c r="B68" s="6"/>
-      <c r="C68" s="100" t="s">
-        <v>232</v>
+      <c r="C68" s="92" t="s">
+        <v>228</v>
       </c>
       <c r="D68" s="10"/>
       <c r="E68" s="6"/>
@@ -3772,7 +3807,7 @@
     <row r="69" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="100"/>
+      <c r="C69" s="92"/>
       <c r="D69" s="10"/>
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
@@ -3810,8 +3845,8 @@
     <row r="71" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="16"/>
       <c r="B71" s="6"/>
-      <c r="C71" s="100" t="s">
-        <v>233</v>
+      <c r="C71" s="92" t="s">
+        <v>275</v>
       </c>
       <c r="D71" s="10"/>
       <c r="E71" s="6"/>
@@ -3831,7 +3866,7 @@
     <row r="72" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16"/>
       <c r="B72" s="6"/>
-      <c r="C72" s="100"/>
+      <c r="C72" s="92"/>
       <c r="D72" s="10"/>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
@@ -3869,8 +3904,8 @@
     <row r="74" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16"/>
       <c r="B74" s="6"/>
-      <c r="C74" s="100" t="s">
-        <v>110</v>
+      <c r="C74" s="92" t="s">
+        <v>107</v>
       </c>
       <c r="D74" s="10"/>
       <c r="E74" s="6"/>
@@ -3890,7 +3925,7 @@
     <row r="75" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="16"/>
       <c r="B75" s="6"/>
-      <c r="C75" s="100"/>
+      <c r="C75" s="92"/>
       <c r="D75" s="10"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
@@ -3928,7 +3963,7 @@
     <row r="77" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="16"/>
       <c r="B77" s="6"/>
-      <c r="C77" s="104" t="s">
+      <c r="C77" s="93" t="s">
         <v>54</v>
       </c>
       <c r="D77" s="7"/>
@@ -3949,7 +3984,7 @@
     <row r="78" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="16"/>
       <c r="B78" s="6"/>
-      <c r="C78" s="104"/>
+      <c r="C78" s="93"/>
       <c r="D78" s="7"/>
       <c r="E78" s="6"/>
       <c r="F78" s="6"/>
@@ -3968,8 +4003,8 @@
     <row r="79" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="16"/>
       <c r="B79" s="6"/>
-      <c r="C79" s="106" t="s">
-        <v>88</v>
+      <c r="C79" s="95" t="s">
+        <v>85</v>
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="6"/>
@@ -4039,7 +4074,7 @@
     <row r="80" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="16"/>
       <c r="B80" s="6"/>
-      <c r="C80" s="106"/>
+      <c r="C80" s="95"/>
       <c r="D80" s="7"/>
       <c r="E80" s="6"/>
       <c r="F80" s="6"/>
@@ -4167,18 +4202,18 @@
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5"/>
-      <c r="F84" s="105"/>
-      <c r="G84" s="105"/>
+      <c r="F84" s="94"/>
+      <c r="G84" s="94"/>
       <c r="H84" s="6"/>
       <c r="I84" s="37" t="s">
         <v>56</v>
       </c>
       <c r="J84" s="37"/>
       <c r="K84" s="6"/>
-      <c r="L84" s="103" t="s">
+      <c r="L84" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="M84" s="103"/>
+      <c r="M84" s="91"/>
       <c r="N84" s="39"/>
       <c r="O84" s="5"/>
       <c r="P84" s="5"/>
@@ -4204,95 +4239,93 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C87" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C88" s="4" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C89" s="4" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C90" s="85" t="s">
-        <v>186</v>
+      <c r="C90" s="84" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C91" s="85" t="s">
-        <v>226</v>
+      <c r="C91" s="84" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C92" s="85" t="s">
+      <c r="C92" s="84" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C93" s="84" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C94" s="84" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C95" s="84" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C96" s="84" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C97" s="84" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C93" s="85" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C94" s="85" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C95" s="85" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C96" s="85" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C97" s="85" t="s">
-        <v>247</v>
-      </c>
-    </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C98" s="85" t="s">
-        <v>248</v>
+      <c r="C98" s="84" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C99" s="85"/>
+      <c r="C99" s="84"/>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C100" s="85"/>
+      <c r="C100" s="84"/>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C101" s="85"/>
+      <c r="C101" s="84"/>
     </row>
     <row r="102" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C102" s="85"/>
+      <c r="C102" s="84"/>
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C103" s="85"/>
+      <c r="C103" s="84"/>
     </row>
     <row r="104" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C104" s="84"/>
+      <c r="C104" s="83"/>
     </row>
     <row r="105" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C105" s="84"/>
+      <c r="C105" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="L84:M84"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B2:O3"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="C11:C12"/>
     <mergeCell ref="C62:C63"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C21:C22"/>
@@ -4308,12 +4341,14 @@
     <mergeCell ref="C55:C56"/>
     <mergeCell ref="C58:C59"/>
     <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B2:O3"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="E6:K6"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="L84:M84"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C74:C75"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4348,7 +4383,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C3" s="57"/>
       <c r="D3" s="57"/>
@@ -4356,34 +4391,34 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="107"/>
       <c r="B4" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="107"/>
       <c r="B5" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -4397,19 +4432,19 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" s="60" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F6" s="60" t="s">
-        <v>115</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -4442,92 +4477,92 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C1" s="69"/>
+        <v>141</v>
+      </c>
+      <c r="C1" s="68"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C2" s="59"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C3" s="58"/>
       <c r="E3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C5" s="66"/>
+        <v>138</v>
+      </c>
+      <c r="C5" s="65"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>143</v>
-      </c>
-      <c r="C6" s="67"/>
+        <v>140</v>
+      </c>
+      <c r="C6" s="66"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>142</v>
-      </c>
-      <c r="C7" s="68"/>
+        <v>139</v>
+      </c>
+      <c r="C7" s="67"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>149</v>
-      </c>
-      <c r="C10" s="70"/>
+        <v>146</v>
+      </c>
+      <c r="C10" s="69"/>
       <c r="D10" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>145</v>
-      </c>
-      <c r="C11" s="71"/>
+        <v>142</v>
+      </c>
+      <c r="C11" s="70"/>
       <c r="D11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>147</v>
-      </c>
-      <c r="C12" s="72"/>
+        <v>144</v>
+      </c>
+      <c r="C12" s="71"/>
       <c r="D12">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>148</v>
-      </c>
-      <c r="C13" s="68"/>
+        <v>145</v>
+      </c>
+      <c r="C13" s="67"/>
       <c r="D13">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -4535,12 +4570,12 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C40" s="54"/>
     </row>
@@ -4646,10 +4681,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H79"/>
+  <dimension ref="B2:H59"/>
   <sheetViews>
-    <sheetView topLeftCell="D40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="D37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4668,178 +4703,190 @@
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="40"/>
       <c r="C2" s="41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F2" s="41" t="s">
         <v>35</v>
       </c>
       <c r="G2" s="41" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H2" s="41" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="121" t="s">
         <v>39</v>
       </c>
       <c r="C3" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="E3" s="44" t="s">
         <v>65</v>
-      </c>
-      <c r="E3" s="44" t="s">
-        <v>66</v>
       </c>
       <c r="F3" s="44"/>
       <c r="G3" s="44" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="H3" s="44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="109"/>
-      <c r="C4" s="112" t="s">
+      <c r="B4" s="122"/>
+      <c r="C4" s="124" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="112" t="s">
+      <c r="D4" s="124" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="44" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="F4" s="44"/>
       <c r="G4" s="44"/>
       <c r="H4" s="44" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="G6" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" s="44" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="123"/>
+      <c r="C7" s="123"/>
+      <c r="D7" s="123"/>
+      <c r="E7" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="44" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="109"/>
-      <c r="C5" s="109"/>
-      <c r="D5" s="109"/>
-      <c r="E5" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="F5" s="44" t="s">
-        <v>136</v>
-      </c>
-      <c r="G5" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="H5" s="44" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="109"/>
-      <c r="C6" s="109"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="F6" s="44" t="s">
-        <v>138</v>
-      </c>
-      <c r="G6" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="H6" s="44" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="110"/>
-      <c r="C7" s="110"/>
-      <c r="D7" s="110"/>
-      <c r="E7" s="44" t="s">
+      <c r="H7" s="44" t="s">
         <v>132</v>
-      </c>
-      <c r="F7" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="G7" s="44" t="s">
-        <v>134</v>
-      </c>
-      <c r="H7" s="44" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="55"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
+      <c r="C8" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="F8" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="G8" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="H8" s="44" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="63"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="83" t="s">
-        <v>224</v>
+      <c r="C9" s="82"/>
+      <c r="D9" s="82" t="s">
+        <v>220</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="F9" s="44"/>
       <c r="G9" s="44" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="H9" s="44" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="82"/>
-      <c r="C10" s="83"/>
-      <c r="D10" s="86" t="s">
-        <v>239</v>
+      <c r="B10" s="81"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="85" t="s">
+        <v>234</v>
       </c>
       <c r="E10" s="44" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="F10" s="44"/>
       <c r="G10" s="44" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="H10" s="44" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="81"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82" t="s">
+        <v>233</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>247</v>
+      </c>
+      <c r="F11" s="44" t="s">
+        <v>232</v>
+      </c>
+      <c r="G11" s="44" t="s">
+        <v>239</v>
+      </c>
+      <c r="H11" s="44" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="82"/>
-      <c r="C11" s="83"/>
-      <c r="D11" s="83" t="s">
-        <v>238</v>
-      </c>
-      <c r="E11" s="44" t="s">
-        <v>252</v>
-      </c>
-      <c r="F11" s="44" t="s">
-        <v>237</v>
-      </c>
-      <c r="G11" s="44" t="s">
-        <v>244</v>
-      </c>
-      <c r="H11" s="44" t="s">
-        <v>246</v>
-      </c>
-    </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="82"/>
-      <c r="C12" s="83"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="89"/>
       <c r="D12" s="89"/>
       <c r="E12" s="44"/>
       <c r="F12" s="44"/>
@@ -4847,730 +4894,678 @@
       <c r="H12" s="44"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="82"/>
-      <c r="C13" s="83"/>
-      <c r="D13" s="89" t="s">
-        <v>254</v>
-      </c>
-      <c r="E13" s="44" t="s">
-        <v>256</v>
-      </c>
-      <c r="F13" s="44" t="s">
-        <v>255</v>
-      </c>
-      <c r="G13" s="44" t="s">
-        <v>257</v>
-      </c>
-      <c r="H13" s="44" t="s">
-        <v>258</v>
-      </c>
+      <c r="B13" s="88"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="82"/>
-      <c r="C14" s="83"/>
-      <c r="D14" s="83"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="89"/>
       <c r="E14" s="44"/>
       <c r="F14" s="44"/>
       <c r="G14" s="44"/>
       <c r="H14" s="44"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="82"/>
-      <c r="C15" s="83"/>
-      <c r="D15" s="83" t="s">
+      <c r="B15" s="81"/>
+      <c r="C15" s="82"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="55"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+    </row>
+    <row r="17" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="115" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="113" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="113" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="116"/>
+      <c r="C18" s="114"/>
+      <c r="D18" s="114"/>
+      <c r="E18" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="G18" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="H18" s="47" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="116"/>
+      <c r="C19" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="46" t="s">
+        <v>156</v>
+      </c>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46" t="s">
+        <v>152</v>
+      </c>
+      <c r="H19" s="47" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="116"/>
+      <c r="C20" s="113" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="113" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="116"/>
+      <c r="C21" s="114"/>
+      <c r="D21" s="114"/>
+      <c r="E21" s="46" t="s">
+        <v>159</v>
+      </c>
+      <c r="F21" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="G21" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="H21" s="46" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="116"/>
+      <c r="C22" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="47" t="s">
+        <v>285</v>
+      </c>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47" t="s">
+        <v>161</v>
+      </c>
+      <c r="H22" s="47" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="116"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="90"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="116"/>
+      <c r="C24" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="D24" s="90" t="s">
+        <v>249</v>
+      </c>
+      <c r="E24" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="F24" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="G24" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="H24" s="47" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="116"/>
+      <c r="C25" s="47" t="s">
+        <v>279</v>
+      </c>
+      <c r="D25" s="90" t="s">
+        <v>258</v>
+      </c>
+      <c r="E25" s="47" t="s">
+        <v>254</v>
+      </c>
+      <c r="F25" s="47" t="s">
+        <v>259</v>
+      </c>
+      <c r="G25" s="47" t="s">
+        <v>255</v>
+      </c>
+      <c r="H25" s="47" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B26" s="116"/>
+      <c r="C26" s="47" t="s">
+        <v>281</v>
+      </c>
+      <c r="D26" s="90" t="s">
+        <v>257</v>
+      </c>
+      <c r="E26" s="47" t="s">
+        <v>260</v>
+      </c>
+      <c r="F26" s="125" t="s">
+        <v>262</v>
+      </c>
+      <c r="G26" s="47" t="s">
+        <v>261</v>
+      </c>
+      <c r="H26" s="47" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="116"/>
+      <c r="C27" s="47" t="s">
+        <v>282</v>
+      </c>
+      <c r="D27" s="47" t="s">
+        <v>274</v>
+      </c>
+      <c r="E27" s="47" t="s">
         <v>263</v>
       </c>
-      <c r="E15" s="44" t="s">
-        <v>259</v>
-      </c>
-      <c r="F15" s="44" t="s">
+      <c r="F27" s="47" t="s">
         <v>264</v>
       </c>
-      <c r="G15" s="44" t="s">
-        <v>260</v>
-      </c>
-      <c r="H15" s="44" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B16" s="82"/>
-      <c r="C16" s="83"/>
-      <c r="D16" s="83" t="s">
-        <v>262</v>
-      </c>
-      <c r="E16" s="44" t="s">
+      <c r="G27" s="47" t="s">
         <v>265</v>
       </c>
-      <c r="F16" s="90" t="s">
-        <v>267</v>
-      </c>
-      <c r="G16" s="44" t="s">
-        <v>266</v>
-      </c>
-      <c r="H16" s="44" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="82"/>
-      <c r="C17" s="83"/>
-      <c r="D17" s="83"/>
-      <c r="E17" s="44" t="s">
-        <v>268</v>
-      </c>
-      <c r="F17" s="44" t="s">
-        <v>269</v>
-      </c>
-      <c r="G17" s="44" t="s">
-        <v>270</v>
-      </c>
-      <c r="H17" s="44" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="82"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="83"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="82"/>
-      <c r="C19" s="83"/>
-      <c r="D19" s="83"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="55"/>
-      <c r="C20" s="56" t="s">
+      <c r="H27" s="47" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="116"/>
+      <c r="C28" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="72" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="72" t="s">
+        <v>163</v>
+      </c>
+      <c r="F28" s="72" t="s">
+        <v>165</v>
+      </c>
+      <c r="G28" s="72" t="s">
+        <v>164</v>
+      </c>
+      <c r="H28" s="72" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="116"/>
+      <c r="C29" s="108" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="108" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="108" t="s">
+        <v>172</v>
+      </c>
+      <c r="F29" s="117" t="s">
+        <v>174</v>
+      </c>
+      <c r="G29" s="117" t="s">
+        <v>238</v>
+      </c>
+      <c r="H29" s="108" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="116"/>
+      <c r="C30" s="109"/>
+      <c r="D30" s="109"/>
+      <c r="E30" s="109"/>
+      <c r="F30" s="118"/>
+      <c r="G30" s="118"/>
+      <c r="H30" s="109"/>
+    </row>
+    <row r="31" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B31" s="116"/>
+      <c r="C31" s="80" t="s">
+        <v>276</v>
+      </c>
+      <c r="D31" s="78" t="s">
+        <v>169</v>
+      </c>
+      <c r="E31" s="77" t="s">
+        <v>170</v>
+      </c>
+      <c r="F31" s="76" t="s">
+        <v>209</v>
+      </c>
+      <c r="G31" s="77" t="s">
+        <v>171</v>
+      </c>
+      <c r="H31" s="77" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B32" s="116"/>
+      <c r="C32" s="108" t="s">
+        <v>277</v>
+      </c>
+      <c r="D32" s="108" t="s">
+        <v>177</v>
+      </c>
+      <c r="E32" s="79" t="s">
+        <v>178</v>
+      </c>
+      <c r="F32" s="76" t="s">
+        <v>207</v>
+      </c>
+      <c r="G32" s="77" t="s">
+        <v>184</v>
+      </c>
+      <c r="H32" s="72" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B33" s="116"/>
+      <c r="C33" s="109"/>
+      <c r="D33" s="109"/>
+      <c r="E33" s="79" t="s">
+        <v>180</v>
+      </c>
+      <c r="F33" s="76" t="s">
+        <v>208</v>
+      </c>
+      <c r="G33" s="77" t="s">
+        <v>181</v>
+      </c>
+      <c r="H33" s="77" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="B34" s="116"/>
+      <c r="C34" s="73" t="s">
+        <v>278</v>
+      </c>
+      <c r="D34" s="80" t="s">
+        <v>176</v>
+      </c>
+      <c r="E34" s="79" t="s">
+        <v>189</v>
+      </c>
+      <c r="F34" s="76" t="s">
+        <v>206</v>
+      </c>
+      <c r="G34" s="79" t="s">
+        <v>190</v>
+      </c>
+      <c r="H34" s="79" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35" s="116"/>
+      <c r="C35" s="120" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="120" t="s">
+        <v>45</v>
+      </c>
+      <c r="E35" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="F35" s="48"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="48" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" s="116"/>
+      <c r="C36" s="120"/>
+      <c r="D36" s="120"/>
+      <c r="E36" s="48" t="s">
+        <v>192</v>
+      </c>
+      <c r="F36" s="76" t="s">
+        <v>204</v>
+      </c>
+      <c r="G36" s="48" t="s">
+        <v>193</v>
+      </c>
+      <c r="H36" s="48" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B37" s="116"/>
+      <c r="C37" s="108" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="108" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="72" t="s">
+        <v>194</v>
+      </c>
+      <c r="F37" s="76" t="s">
+        <v>201</v>
+      </c>
+      <c r="G37" s="72" t="s">
+        <v>195</v>
+      </c>
+      <c r="H37" s="72" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B38" s="116"/>
+      <c r="C38" s="109"/>
+      <c r="D38" s="109"/>
+      <c r="E38" s="72" t="s">
+        <v>196</v>
+      </c>
+      <c r="F38" s="76" t="s">
+        <v>202</v>
+      </c>
+      <c r="G38" s="72" t="s">
+        <v>200</v>
+      </c>
+      <c r="H38" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B39" s="116"/>
+      <c r="C39" s="79" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" s="79" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39" s="79" t="s">
+        <v>78</v>
+      </c>
+      <c r="F39" s="76" t="s">
+        <v>203</v>
+      </c>
+      <c r="G39" s="79" t="s">
+        <v>205</v>
+      </c>
+      <c r="H39" s="79" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B40" s="116"/>
+      <c r="C40" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40" s="108" t="s">
+        <v>50</v>
+      </c>
+      <c r="E40" s="72" t="s">
+        <v>210</v>
+      </c>
+      <c r="F40" s="76" t="s">
+        <v>215</v>
+      </c>
+      <c r="G40" s="72" t="s">
+        <v>214</v>
+      </c>
+      <c r="H40" s="72" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B41" s="116"/>
+      <c r="C41" s="109"/>
+      <c r="D41" s="109"/>
+      <c r="E41" s="72" t="s">
+        <v>216</v>
+      </c>
+      <c r="F41" s="76" t="s">
+        <v>211</v>
+      </c>
+      <c r="G41" s="72" t="s">
+        <v>217</v>
+      </c>
+      <c r="H41" s="72" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" s="110" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="119" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42" s="119" t="s">
+        <v>58</v>
+      </c>
+      <c r="E42" s="45" t="s">
+        <v>284</v>
+      </c>
+      <c r="F42" s="45"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="45" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" s="111"/>
+      <c r="C43" s="119"/>
+      <c r="D43" s="119"/>
+      <c r="E43" s="45" t="s">
+        <v>286</v>
+      </c>
+      <c r="F43" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="G43" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="H43" s="45" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44" s="111"/>
+      <c r="C44" s="61"/>
+      <c r="D44" s="61"/>
+      <c r="E44" s="61"/>
+      <c r="F44" s="61"/>
+      <c r="G44" s="61"/>
+      <c r="H44" s="61"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B45" s="112"/>
+      <c r="C45" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="F45" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="G45" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="H45" s="45" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B46" s="62"/>
+      <c r="C46" s="64"/>
+      <c r="D46" s="64" t="s">
+        <v>126</v>
+      </c>
+      <c r="E46" s="61"/>
+      <c r="F46" s="61"/>
+      <c r="G46" s="61"/>
+      <c r="H46" s="61"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B47" s="62"/>
+      <c r="C47" s="64"/>
+      <c r="D47" s="64" t="s">
         <v>122</v>
       </c>
-      <c r="D20" s="56" t="s">
+      <c r="E47" s="61"/>
+      <c r="F47" s="61"/>
+      <c r="G47" s="61"/>
+      <c r="H47" s="61"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B48" s="62"/>
+      <c r="C48" s="64"/>
+      <c r="D48" s="64" t="s">
         <v>123</v>
       </c>
-      <c r="E20" s="44" t="s">
-        <v>154</v>
-      </c>
-      <c r="F20" s="44" t="s">
-        <v>275</v>
-      </c>
-      <c r="G20" s="44" t="s">
-        <v>276</v>
-      </c>
-      <c r="H20" s="44" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="121" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="116" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="116" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="122"/>
-      <c r="C22" s="117"/>
-      <c r="D22" s="117"/>
-      <c r="E22" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="F22" s="46" t="s">
+      <c r="E48" s="61"/>
+      <c r="F48" s="61"/>
+      <c r="G48" s="61"/>
+      <c r="H48" s="61"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B49" s="62"/>
+      <c r="C49" s="64"/>
+      <c r="D49" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="G22" s="46" t="s">
-        <v>157</v>
-      </c>
-      <c r="H22" s="47" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="122"/>
-      <c r="C23" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="D23" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="E23" s="46" t="s">
-        <v>159</v>
-      </c>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46" t="s">
-        <v>155</v>
-      </c>
-      <c r="H23" s="47" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="122"/>
-      <c r="C24" s="116" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="116" t="s">
-        <v>74</v>
-      </c>
-      <c r="E24" s="46" t="s">
-        <v>160</v>
-      </c>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="46" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="122"/>
-      <c r="C25" s="117"/>
-      <c r="D25" s="117"/>
-      <c r="E25" s="46" t="s">
-        <v>162</v>
-      </c>
-      <c r="F25" s="47" t="s">
-        <v>156</v>
-      </c>
-      <c r="G25" s="46" t="s">
-        <v>163</v>
-      </c>
-      <c r="H25" s="46" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="122"/>
-      <c r="C26" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="47" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" s="47" t="s">
-        <v>164</v>
-      </c>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47" t="s">
-        <v>165</v>
-      </c>
-      <c r="H26" s="47" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="122"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="47"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="122"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="47"/>
-    </row>
-    <row r="29" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="122"/>
-      <c r="C29" s="73" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="73" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" s="73" t="s">
-        <v>167</v>
-      </c>
-      <c r="F29" s="73" t="s">
-        <v>169</v>
-      </c>
-      <c r="G29" s="73" t="s">
-        <v>168</v>
-      </c>
-      <c r="H29" s="73" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="122"/>
-      <c r="C30" s="113" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="113" t="s">
-        <v>47</v>
-      </c>
-      <c r="E30" s="113" t="s">
-        <v>176</v>
-      </c>
-      <c r="F30" s="123" t="s">
-        <v>178</v>
-      </c>
-      <c r="G30" s="123" t="s">
-        <v>243</v>
-      </c>
-      <c r="H30" s="113" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="122"/>
-      <c r="C31" s="114"/>
-      <c r="D31" s="114"/>
-      <c r="E31" s="114"/>
-      <c r="F31" s="124"/>
-      <c r="G31" s="124"/>
-      <c r="H31" s="114"/>
-    </row>
-    <row r="32" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B32" s="122"/>
-      <c r="C32" s="81"/>
-      <c r="D32" s="79" t="s">
-        <v>173</v>
-      </c>
-      <c r="E32" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="F32" s="77" t="s">
-        <v>213</v>
-      </c>
-      <c r="G32" s="78" t="s">
-        <v>175</v>
-      </c>
-      <c r="H32" s="78" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B33" s="122"/>
-      <c r="C33" s="113"/>
-      <c r="D33" s="113" t="s">
-        <v>181</v>
-      </c>
-      <c r="E33" s="80" t="s">
-        <v>182</v>
-      </c>
-      <c r="F33" s="77" t="s">
-        <v>211</v>
-      </c>
-      <c r="G33" s="78" t="s">
-        <v>188</v>
-      </c>
-      <c r="H33" s="73" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B34" s="122"/>
-      <c r="C34" s="114"/>
-      <c r="D34" s="114"/>
-      <c r="E34" s="80" t="s">
-        <v>184</v>
-      </c>
-      <c r="F34" s="77" t="s">
-        <v>212</v>
-      </c>
-      <c r="G34" s="78" t="s">
-        <v>185</v>
-      </c>
-      <c r="H34" s="78" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" ht="66" x14ac:dyDescent="0.3">
-      <c r="B35" s="122"/>
-      <c r="C35" s="74"/>
-      <c r="D35" s="81" t="s">
-        <v>180</v>
-      </c>
-      <c r="E35" s="80" t="s">
-        <v>193</v>
-      </c>
-      <c r="F35" s="77" t="s">
-        <v>210</v>
-      </c>
-      <c r="G35" s="80" t="s">
-        <v>194</v>
-      </c>
-      <c r="H35" s="80" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="122"/>
-      <c r="C36" s="111" t="s">
-        <v>41</v>
-      </c>
-      <c r="D36" s="111" t="s">
-        <v>45</v>
-      </c>
-      <c r="E36" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="F36" s="48"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="48" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="122"/>
-      <c r="C37" s="111"/>
-      <c r="D37" s="111"/>
-      <c r="E37" s="48" t="s">
-        <v>196</v>
-      </c>
-      <c r="F37" s="77" t="s">
-        <v>208</v>
-      </c>
-      <c r="G37" s="48" t="s">
-        <v>197</v>
-      </c>
-      <c r="H37" s="48" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B38" s="122"/>
-      <c r="C38" s="113" t="s">
-        <v>44</v>
-      </c>
-      <c r="D38" s="113" t="s">
-        <v>52</v>
-      </c>
-      <c r="E38" s="73" t="s">
-        <v>198</v>
-      </c>
-      <c r="F38" s="77" t="s">
-        <v>205</v>
-      </c>
-      <c r="G38" s="73" t="s">
-        <v>199</v>
-      </c>
-      <c r="H38" s="73" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B39" s="122"/>
-      <c r="C39" s="114"/>
-      <c r="D39" s="114"/>
-      <c r="E39" s="73" t="s">
-        <v>200</v>
-      </c>
-      <c r="F39" s="77" t="s">
-        <v>206</v>
-      </c>
-      <c r="G39" s="73" t="s">
-        <v>204</v>
-      </c>
-      <c r="H39" s="73" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B40" s="122"/>
-      <c r="C40" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="D40" s="80" t="s">
-        <v>51</v>
-      </c>
-      <c r="E40" s="80" t="s">
-        <v>80</v>
-      </c>
-      <c r="F40" s="77" t="s">
-        <v>207</v>
-      </c>
-      <c r="G40" s="80" t="s">
-        <v>209</v>
-      </c>
-      <c r="H40" s="80" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B41" s="122"/>
-      <c r="C41" s="113" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="113" t="s">
-        <v>50</v>
-      </c>
-      <c r="E41" s="73" t="s">
-        <v>214</v>
-      </c>
-      <c r="F41" s="77" t="s">
-        <v>219</v>
-      </c>
-      <c r="G41" s="73" t="s">
-        <v>218</v>
-      </c>
-      <c r="H41" s="73" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B42" s="122"/>
-      <c r="C42" s="114"/>
-      <c r="D42" s="114"/>
-      <c r="E42" s="73" t="s">
-        <v>220</v>
-      </c>
-      <c r="F42" s="77" t="s">
-        <v>215</v>
-      </c>
-      <c r="G42" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="H42" s="73" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B43" s="122"/>
-      <c r="C43" s="81"/>
-      <c r="D43" s="81"/>
-      <c r="E43" s="80"/>
-      <c r="F43" s="80"/>
-      <c r="G43" s="80"/>
-      <c r="H43" s="80"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B44" s="122"/>
-      <c r="C44" s="81"/>
-      <c r="D44" s="81"/>
-      <c r="E44" s="80"/>
-      <c r="F44" s="80"/>
-      <c r="G44" s="80"/>
-      <c r="H44" s="80"/>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B45" s="122"/>
-      <c r="C45" s="81"/>
-      <c r="D45" s="81"/>
-      <c r="E45" s="80"/>
-      <c r="F45" s="80"/>
-      <c r="G45" s="80"/>
-      <c r="H45" s="80"/>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B46" s="118" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B47" s="119"/>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B48" s="119"/>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B49" s="120"/>
+      <c r="E49" s="61"/>
+      <c r="F49" s="61"/>
+      <c r="G49" s="61"/>
+      <c r="H49" s="61"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B50" s="62"/>
+      <c r="C50" s="64"/>
+      <c r="D50" s="64" t="s">
+        <v>125</v>
+      </c>
+      <c r="E50" s="61"/>
+      <c r="F50" s="61"/>
+      <c r="G50" s="61"/>
+      <c r="H50" s="61"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B51" s="62"/>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B52" s="62"/>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B53" s="62"/>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B54" s="62"/>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B55" s="62"/>
-    </row>
-    <row r="63" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="D63" s="76" t="s">
-        <v>177</v>
-      </c>
-      <c r="E63" s="78" t="s">
-        <v>190</v>
-      </c>
-      <c r="F63" s="77" t="s">
-        <v>179</v>
-      </c>
-      <c r="G63" s="78" t="s">
-        <v>187</v>
-      </c>
-      <c r="H63" s="75" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="70" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C70" s="115" t="s">
-        <v>57</v>
-      </c>
-      <c r="D70" s="115" t="s">
-        <v>59</v>
-      </c>
-      <c r="E70" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="F70" s="45"/>
-      <c r="G70" s="45"/>
-      <c r="H70" s="45" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="71" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C71" s="115"/>
-      <c r="D71" s="115"/>
-      <c r="E71" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="F71" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="G71" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="H71" s="45" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="72" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C72" s="61"/>
-      <c r="D72" s="61"/>
-      <c r="E72" s="61"/>
-      <c r="F72" s="61"/>
-      <c r="G72" s="61"/>
-      <c r="H72" s="61"/>
-    </row>
-    <row r="73" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C73" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="D73" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="E73" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="F73" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="G73" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="H73" s="45" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="74" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C74" s="64"/>
-      <c r="D74" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="E74" s="61"/>
-      <c r="F74" s="61"/>
-      <c r="G74" s="61"/>
-      <c r="H74" s="61"/>
-    </row>
-    <row r="75" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C75" s="64"/>
-      <c r="D75" s="64" t="s">
-        <v>125</v>
-      </c>
-      <c r="E75" s="61"/>
-      <c r="F75" s="61"/>
-      <c r="G75" s="61"/>
-      <c r="H75" s="61"/>
-    </row>
-    <row r="76" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C76" s="64"/>
-      <c r="D76" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="E76" s="61"/>
-      <c r="F76" s="61"/>
-      <c r="G76" s="61"/>
-      <c r="H76" s="61"/>
-    </row>
-    <row r="77" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C77" s="64"/>
-      <c r="D77" s="64" t="s">
-        <v>127</v>
-      </c>
-      <c r="E77" s="61"/>
-      <c r="F77" s="61"/>
-      <c r="G77" s="61"/>
-      <c r="H77" s="61"/>
-    </row>
-    <row r="78" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C78" s="64"/>
-      <c r="D78" s="64" t="s">
-        <v>128</v>
-      </c>
-      <c r="E78" s="61"/>
-      <c r="F78" s="61"/>
-      <c r="G78" s="61"/>
-      <c r="H78" s="61"/>
-    </row>
-    <row r="79" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C79" s="64"/>
-      <c r="D79" s="64"/>
-      <c r="E79" s="61"/>
-      <c r="F79" s="61"/>
-      <c r="G79" s="61"/>
-      <c r="H79" s="61"/>
+      <c r="C51" s="64"/>
+      <c r="D51" s="64"/>
+      <c r="E51" s="61"/>
+      <c r="F51" s="61"/>
+      <c r="G51" s="61"/>
+      <c r="H51" s="61"/>
+    </row>
+    <row r="59" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="D59" s="75" t="s">
+        <v>173</v>
+      </c>
+      <c r="E59" s="77" t="s">
+        <v>186</v>
+      </c>
+      <c r="F59" s="76" t="s">
+        <v>175</v>
+      </c>
+      <c r="G59" s="77" t="s">
+        <v>183</v>
+      </c>
+      <c r="H59" s="74" t="s">
+        <v>185</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="B21:B45"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="C30:C31"/>
     <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C35:C36"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="D4:D7"/>
-    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B17:B41"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="F29:F30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Auto push 2023-03-27 18:01:52.42
</commit_message>
<xml_diff>
--- a/project/CheeYoonMovie.xlsx
+++ b/project/CheeYoonMovie.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="284">
   <si>
     <t>이용자 권한과 기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -225,12 +225,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>관
-리
-자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>통합, 테스트 및 수정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -243,50 +237,38 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>회원리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원들 리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pageNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">main/main.jsp </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>로그인</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>관리자모드 로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원리스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원들 리스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>allView.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pageNum</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메인페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>main.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">main/main.jsp </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>사용자 모드 로그인</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -311,10 +293,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MAllViewService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>회원탈퇴</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -331,10 +309,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">member/mAllView.jsp </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Service</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -344,14 +318,6 @@
   </si>
   <si>
     <t>Controller 요청 경로</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>allView.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALoginService.java</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1118,10 +1084,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>월요일 검색사이트, 관리자모드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>수요일 평점 리스트? 영화랭킹? 마이메뉴?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1162,19 +1124,42 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>admin/adminLogin.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>adminLoginView.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>withdrawal.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>관리자모드 로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>adminLogin.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AdminLoginService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userList.do</t>
+  </si>
+  <si>
+    <t>userList.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserListService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">admin/userList.jsp </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>월요일 검색사이트, 관리자모드 회원리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardList.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1712,7 +1697,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1986,12 +1971,51 @@
     <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2001,50 +2025,35 @@
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2053,12 +2062,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2069,27 +2072,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2440,7 +2422,7 @@
   <dimension ref="A1:BP105"/>
   <sheetViews>
     <sheetView topLeftCell="A58" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J73" sqref="J73"/>
+      <selection activeCell="O95" sqref="O95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.25" defaultRowHeight="11.25" x14ac:dyDescent="0.3"/>
@@ -2459,41 +2441,41 @@
     <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="100" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="101"/>
-      <c r="M2" s="101"/>
-      <c r="N2" s="101"/>
-      <c r="O2" s="101"/>
+      <c r="B2" s="94" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+      <c r="O2" s="95"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="101"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="101"/>
-      <c r="L3" s="101"/>
-      <c r="M3" s="101"/>
-      <c r="N3" s="101"/>
-      <c r="O3" s="101"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="95"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
@@ -2538,32 +2520,32 @@
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20"/>
-      <c r="C6" s="102" t="s">
+      <c r="C6" s="96" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="38"/>
-      <c r="E6" s="104" t="s">
+      <c r="E6" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="104"/>
-      <c r="G6" s="104"/>
-      <c r="H6" s="104"/>
-      <c r="I6" s="104"/>
-      <c r="J6" s="104"/>
-      <c r="K6" s="105"/>
-      <c r="L6" s="106" t="s">
+      <c r="F6" s="98"/>
+      <c r="G6" s="98"/>
+      <c r="H6" s="98"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="104"/>
-      <c r="N6" s="104"/>
-      <c r="O6" s="104"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="98"/>
+      <c r="O6" s="98"/>
       <c r="P6" s="21"/>
       <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="103"/>
+      <c r="C7" s="97"/>
       <c r="D7" s="22"/>
       <c r="E7" s="86">
         <v>20</v>
@@ -2663,7 +2645,7 @@
     <row r="11" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="96" t="s">
+      <c r="C11" s="101" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="10"/>
@@ -2684,7 +2666,7 @@
     <row r="12" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="96"/>
+      <c r="C12" s="101"/>
       <c r="D12" s="10"/>
       <c r="E12" s="8"/>
       <c r="F12" s="6"/>
@@ -2722,7 +2704,7 @@
     <row r="14" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="99" t="s">
+      <c r="C14" s="93" t="s">
         <v>32</v>
       </c>
       <c r="D14" s="10"/>
@@ -2743,7 +2725,7 @@
     <row r="15" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="99"/>
+      <c r="C15" s="93"/>
       <c r="D15" s="10"/>
       <c r="E15" s="8"/>
       <c r="F15" s="6"/>
@@ -2781,7 +2763,7 @@
     <row r="17" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="96" t="s">
+      <c r="C17" s="101" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="10"/>
@@ -2802,7 +2784,7 @@
     <row r="18" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="96"/>
+      <c r="C18" s="101"/>
       <c r="D18" s="10"/>
       <c r="E18" s="8"/>
       <c r="F18" s="6"/>
@@ -2861,8 +2843,8 @@
     <row r="21" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="97" t="s">
-        <v>221</v>
+      <c r="C21" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="37"/>
@@ -2882,7 +2864,7 @@
     <row r="22" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="97"/>
+      <c r="C22" s="103"/>
       <c r="D22" s="10"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
@@ -2920,7 +2902,7 @@
     <row r="24" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="97" t="s">
+      <c r="C24" s="103" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="10"/>
@@ -2941,7 +2923,7 @@
     <row r="25" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="97"/>
+      <c r="C25" s="103"/>
       <c r="D25" s="10"/>
       <c r="E25" s="6"/>
       <c r="F25" s="8"/>
@@ -2979,8 +2961,8 @@
     <row r="27" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="97" t="s">
-        <v>87</v>
+      <c r="C27" s="103" t="s">
+        <v>79</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="6"/>
@@ -3000,7 +2982,7 @@
     <row r="28" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="97"/>
+      <c r="C28" s="103"/>
       <c r="D28" s="10"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -3038,8 +3020,8 @@
     <row r="30" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="97" t="s">
-        <v>88</v>
+      <c r="C30" s="103" t="s">
+        <v>80</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="6"/>
@@ -3059,7 +3041,7 @@
     <row r="31" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="97"/>
+      <c r="C31" s="103"/>
       <c r="D31" s="10"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -3097,8 +3079,8 @@
     <row r="33" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="97" t="s">
-        <v>229</v>
+      <c r="C33" s="103" t="s">
+        <v>221</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="6"/>
@@ -3118,7 +3100,7 @@
     <row r="34" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="6"/>
-      <c r="C34" s="97"/>
+      <c r="C34" s="103"/>
       <c r="D34" s="10"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -3156,8 +3138,8 @@
     <row r="36" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="16"/>
       <c r="B36" s="6"/>
-      <c r="C36" s="97" t="s">
-        <v>89</v>
+      <c r="C36" s="103" t="s">
+        <v>81</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="6"/>
@@ -3177,7 +3159,7 @@
     <row r="37" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
       <c r="B37" s="6"/>
-      <c r="C37" s="97"/>
+      <c r="C37" s="103"/>
       <c r="D37" s="10"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
@@ -3236,7 +3218,7 @@
     <row r="40" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="6"/>
-      <c r="C40" s="98" t="s">
+      <c r="C40" s="104" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="10"/>
@@ -3257,7 +3239,7 @@
     <row r="41" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="98"/>
+      <c r="C41" s="104"/>
       <c r="D41" s="10"/>
       <c r="E41" s="6"/>
       <c r="F41" s="8"/>
@@ -3295,8 +3277,8 @@
     <row r="43" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="16"/>
       <c r="B43" s="6"/>
-      <c r="C43" s="98" t="s">
-        <v>223</v>
+      <c r="C43" s="104" t="s">
+        <v>215</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="6"/>
@@ -3316,7 +3298,7 @@
     <row r="44" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="98"/>
+      <c r="C44" s="104"/>
       <c r="D44" s="10"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
@@ -3354,8 +3336,8 @@
     <row r="46" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16"/>
       <c r="B46" s="6"/>
-      <c r="C46" s="98" t="s">
-        <v>225</v>
+      <c r="C46" s="104" t="s">
+        <v>217</v>
       </c>
       <c r="D46" s="10"/>
       <c r="E46" s="6"/>
@@ -3374,7 +3356,7 @@
     <row r="47" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="98"/>
+      <c r="C47" s="104"/>
       <c r="D47" s="10"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
@@ -3412,8 +3394,8 @@
     <row r="49" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="16"/>
       <c r="B49" s="6"/>
-      <c r="C49" s="98" t="s">
-        <v>226</v>
+      <c r="C49" s="104" t="s">
+        <v>218</v>
       </c>
       <c r="D49" s="10"/>
       <c r="E49" s="6"/>
@@ -3433,7 +3415,7 @@
     <row r="50" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="98"/>
+      <c r="C50" s="104"/>
       <c r="D50" s="10"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
@@ -3471,8 +3453,8 @@
     <row r="52" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="16"/>
       <c r="B52" s="6"/>
-      <c r="C52" s="98" t="s">
-        <v>109</v>
+      <c r="C52" s="104" t="s">
+        <v>101</v>
       </c>
       <c r="D52" s="10"/>
       <c r="E52" s="6"/>
@@ -3492,7 +3474,7 @@
     <row r="53" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16"/>
       <c r="B53" s="6"/>
-      <c r="C53" s="98"/>
+      <c r="C53" s="104"/>
       <c r="D53" s="10"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
@@ -3530,8 +3512,8 @@
     <row r="55" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="98" t="s">
-        <v>227</v>
+      <c r="C55" s="104" t="s">
+        <v>219</v>
       </c>
       <c r="D55" s="10"/>
       <c r="E55" s="6"/>
@@ -3550,7 +3532,7 @@
     <row r="56" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="16"/>
       <c r="B56" s="6"/>
-      <c r="C56" s="98"/>
+      <c r="C56" s="104"/>
       <c r="D56" s="10"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
@@ -3588,8 +3570,8 @@
     <row r="58" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="98" t="s">
-        <v>224</v>
+      <c r="C58" s="104" t="s">
+        <v>216</v>
       </c>
       <c r="D58" s="10"/>
       <c r="E58" s="6"/>
@@ -3609,7 +3591,7 @@
     <row r="59" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="16"/>
       <c r="B59" s="6"/>
-      <c r="C59" s="98"/>
+      <c r="C59" s="104"/>
       <c r="D59" s="10"/>
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
@@ -3668,8 +3650,8 @@
     <row r="62" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="16"/>
       <c r="B62" s="6"/>
-      <c r="C62" s="92" t="s">
-        <v>90</v>
+      <c r="C62" s="102" t="s">
+        <v>82</v>
       </c>
       <c r="D62" s="10"/>
       <c r="E62" s="6"/>
@@ -3689,7 +3671,7 @@
     <row r="63" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="16"/>
       <c r="B63" s="6"/>
-      <c r="C63" s="92"/>
+      <c r="C63" s="102"/>
       <c r="D63" s="10"/>
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
@@ -3727,8 +3709,8 @@
     <row r="65" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="16"/>
       <c r="B65" s="6"/>
-      <c r="C65" s="92" t="s">
-        <v>108</v>
+      <c r="C65" s="102" t="s">
+        <v>100</v>
       </c>
       <c r="D65" s="10"/>
       <c r="E65" s="6"/>
@@ -3748,7 +3730,7 @@
     <row r="66" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="16"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="92"/>
+      <c r="C66" s="102"/>
       <c r="D66" s="10"/>
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
@@ -3786,8 +3768,8 @@
     <row r="68" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="16"/>
       <c r="B68" s="6"/>
-      <c r="C68" s="92" t="s">
-        <v>228</v>
+      <c r="C68" s="102" t="s">
+        <v>220</v>
       </c>
       <c r="D68" s="10"/>
       <c r="E68" s="6"/>
@@ -3807,7 +3789,7 @@
     <row r="69" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="92"/>
+      <c r="C69" s="102"/>
       <c r="D69" s="10"/>
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
@@ -3845,8 +3827,8 @@
     <row r="71" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="16"/>
       <c r="B71" s="6"/>
-      <c r="C71" s="92" t="s">
-        <v>275</v>
+      <c r="C71" s="102" t="s">
+        <v>266</v>
       </c>
       <c r="D71" s="10"/>
       <c r="E71" s="6"/>
@@ -3866,7 +3848,7 @@
     <row r="72" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16"/>
       <c r="B72" s="6"/>
-      <c r="C72" s="92"/>
+      <c r="C72" s="102"/>
       <c r="D72" s="10"/>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
@@ -3904,8 +3886,8 @@
     <row r="74" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16"/>
       <c r="B74" s="6"/>
-      <c r="C74" s="92" t="s">
-        <v>107</v>
+      <c r="C74" s="102" t="s">
+        <v>99</v>
       </c>
       <c r="D74" s="10"/>
       <c r="E74" s="6"/>
@@ -3925,7 +3907,7 @@
     <row r="75" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="16"/>
       <c r="B75" s="6"/>
-      <c r="C75" s="92"/>
+      <c r="C75" s="102"/>
       <c r="D75" s="10"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
@@ -3963,8 +3945,8 @@
     <row r="77" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="16"/>
       <c r="B77" s="6"/>
-      <c r="C77" s="93" t="s">
-        <v>54</v>
+      <c r="C77" s="106" t="s">
+        <v>53</v>
       </c>
       <c r="D77" s="7"/>
       <c r="E77" s="6"/>
@@ -3984,7 +3966,7 @@
     <row r="78" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="16"/>
       <c r="B78" s="6"/>
-      <c r="C78" s="93"/>
+      <c r="C78" s="106"/>
       <c r="D78" s="7"/>
       <c r="E78" s="6"/>
       <c r="F78" s="6"/>
@@ -4003,8 +3985,8 @@
     <row r="79" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="16"/>
       <c r="B79" s="6"/>
-      <c r="C79" s="95" t="s">
-        <v>85</v>
+      <c r="C79" s="108" t="s">
+        <v>77</v>
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="6"/>
@@ -4074,7 +4056,7 @@
     <row r="80" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="16"/>
       <c r="B80" s="6"/>
-      <c r="C80" s="95"/>
+      <c r="C80" s="108"/>
       <c r="D80" s="7"/>
       <c r="E80" s="6"/>
       <c r="F80" s="6"/>
@@ -4202,18 +4184,18 @@
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5"/>
-      <c r="F84" s="94"/>
-      <c r="G84" s="94"/>
+      <c r="F84" s="107"/>
+      <c r="G84" s="107"/>
       <c r="H84" s="6"/>
       <c r="I84" s="37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J84" s="37"/>
       <c r="K84" s="6"/>
-      <c r="L84" s="91" t="s">
-        <v>55</v>
-      </c>
-      <c r="M84" s="91"/>
+      <c r="L84" s="105" t="s">
+        <v>54</v>
+      </c>
+      <c r="M84" s="105"/>
       <c r="N84" s="39"/>
       <c r="O84" s="5"/>
       <c r="P84" s="5"/>
@@ -4239,62 +4221,62 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C87" s="4" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C88" s="4" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C89" s="4" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C90" s="84" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C91" s="84" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C92" s="84" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C93" s="84" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C94" s="84" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C95" s="84" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C96" s="84" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C97" s="84" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C98" s="84" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.3">
@@ -4320,12 +4302,14 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B2:O3"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="E6:K6"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="L84:M84"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C74:C75"/>
     <mergeCell ref="C62:C63"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C21:C22"/>
@@ -4341,14 +4325,12 @@
     <mergeCell ref="C55:C56"/>
     <mergeCell ref="C58:C59"/>
     <mergeCell ref="C33:C34"/>
-    <mergeCell ref="L84:M84"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B2:O3"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="C11:C12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4379,46 +4361,46 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="109" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C3" s="57"/>
       <c r="D3" s="57"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="107"/>
+      <c r="A4" s="109"/>
       <c r="B4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="109"/>
+      <c r="B5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="107"/>
-      <c r="B5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -4432,19 +4414,19 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F6" s="60" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -4477,65 +4459,65 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C1" s="68"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C2" s="59"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C3" s="58"/>
       <c r="E3" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C5" s="65"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C6" s="66"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C7" s="67"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C10" s="69"/>
       <c r="D10" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C11" s="70"/>
       <c r="D11">
@@ -4544,7 +4526,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C12" s="71"/>
       <c r="D12">
@@ -4553,7 +4535,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C13" s="67"/>
       <c r="D13">
@@ -4562,7 +4544,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -4570,12 +4552,12 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C40" s="54"/>
     </row>
@@ -4681,10 +4663,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H59"/>
+  <dimension ref="B2:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="D34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4703,185 +4685,185 @@
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="40"/>
       <c r="C2" s="41" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="41" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F2" s="41" t="s">
         <v>35</v>
       </c>
       <c r="G2" s="41" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H2" s="41" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="121" t="s">
+      <c r="B3" s="110" t="s">
         <v>39</v>
       </c>
       <c r="C3" s="43" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E3" s="44" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F3" s="44"/>
       <c r="G3" s="44" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="H3" s="44" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="122"/>
-      <c r="C4" s="124" t="s">
+      <c r="B4" s="111"/>
+      <c r="C4" s="114" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="124" t="s">
+      <c r="D4" s="114" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="44" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="F4" s="44"/>
       <c r="G4" s="44"/>
       <c r="H4" s="44" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="111"/>
+      <c r="C5" s="111"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="G5" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="111"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="111"/>
+      <c r="E6" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="G6" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="H6" s="44" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="122"/>
-      <c r="C5" s="122"/>
-      <c r="D5" s="122"/>
-      <c r="E5" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="F5" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="G5" s="44" t="s">
-        <v>134</v>
-      </c>
-      <c r="H5" s="44" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="122"/>
-      <c r="C6" s="122"/>
-      <c r="D6" s="122"/>
-      <c r="E6" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="F6" s="44" t="s">
-        <v>135</v>
-      </c>
-      <c r="G6" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="H6" s="44" t="s">
-        <v>136</v>
-      </c>
-    </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="123"/>
-      <c r="C7" s="123"/>
-      <c r="D7" s="123"/>
+      <c r="B7" s="112"/>
+      <c r="C7" s="112"/>
+      <c r="D7" s="112"/>
       <c r="E7" s="44" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="F7" s="44" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="G7" s="44" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="H7" s="44" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="55"/>
       <c r="C8" s="56" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D8" s="56" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E8" s="44" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="F8" s="44" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="G8" s="44" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="H8" s="44" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="63"/>
       <c r="C9" s="82"/>
       <c r="D9" s="82" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="F9" s="44"/>
       <c r="G9" s="44" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H9" s="44" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="81"/>
       <c r="C10" s="82"/>
       <c r="D10" s="85" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E10" s="44" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="F10" s="44"/>
       <c r="G10" s="44" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="H10" s="44" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="81"/>
       <c r="C11" s="82"/>
       <c r="D11" s="82" t="s">
+        <v>225</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>239</v>
+      </c>
+      <c r="F11" s="44" t="s">
+        <v>224</v>
+      </c>
+      <c r="G11" s="44" t="s">
+        <v>231</v>
+      </c>
+      <c r="H11" s="44" t="s">
         <v>233</v>
-      </c>
-      <c r="E11" s="44" t="s">
-        <v>247</v>
-      </c>
-      <c r="F11" s="44" t="s">
-        <v>232</v>
-      </c>
-      <c r="G11" s="44" t="s">
-        <v>239</v>
-      </c>
-      <c r="H11" s="44" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
@@ -4930,115 +4912,115 @@
       <c r="H16" s="44"/>
     </row>
     <row r="17" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="115" t="s">
+      <c r="B17" s="121" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="113" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="113" t="s">
-        <v>68</v>
+      <c r="C17" s="117" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="117" t="s">
+        <v>64</v>
       </c>
       <c r="E17" s="46" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="F17" s="46"/>
       <c r="G17" s="46"/>
       <c r="H17" s="46" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="116"/>
-      <c r="C18" s="114"/>
-      <c r="D18" s="114"/>
+      <c r="B18" s="122"/>
+      <c r="C18" s="118"/>
+      <c r="D18" s="118"/>
       <c r="E18" s="46" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F18" s="46" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G18" s="46" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="H18" s="47" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="116"/>
+      <c r="B19" s="122"/>
       <c r="C19" s="46" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D19" s="46" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E19" s="46" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="F19" s="46"/>
       <c r="G19" s="46" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="H19" s="47" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="116"/>
-      <c r="C20" s="113" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="113" t="s">
-        <v>73</v>
+      <c r="B20" s="122"/>
+      <c r="C20" s="117" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="117" t="s">
+        <v>69</v>
       </c>
       <c r="E20" s="46" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="F20" s="46"/>
       <c r="G20" s="46"/>
       <c r="H20" s="46" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="116"/>
-      <c r="C21" s="114"/>
-      <c r="D21" s="114"/>
+      <c r="B21" s="122"/>
+      <c r="C21" s="118"/>
+      <c r="D21" s="118"/>
       <c r="E21" s="46" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="F21" s="47" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="G21" s="46" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="H21" s="46" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="116"/>
+      <c r="B22" s="122"/>
       <c r="C22" s="47" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D22" s="47" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E22" s="47" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="F22" s="47"/>
       <c r="G22" s="47" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="H22" s="47" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="116"/>
+      <c r="B23" s="122"/>
       <c r="C23" s="47"/>
       <c r="D23" s="90"/>
       <c r="E23" s="47"/>
@@ -5047,91 +5029,91 @@
       <c r="H23" s="47"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="116"/>
+      <c r="B24" s="122"/>
       <c r="C24" s="47" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="D24" s="90" t="s">
+        <v>241</v>
+      </c>
+      <c r="E24" s="47" t="s">
+        <v>243</v>
+      </c>
+      <c r="F24" s="47" t="s">
+        <v>242</v>
+      </c>
+      <c r="G24" s="47" t="s">
+        <v>244</v>
+      </c>
+      <c r="H24" s="47" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="122"/>
+      <c r="C25" s="47" t="s">
+        <v>270</v>
+      </c>
+      <c r="D25" s="90" t="s">
+        <v>250</v>
+      </c>
+      <c r="E25" s="47" t="s">
+        <v>246</v>
+      </c>
+      <c r="F25" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="G25" s="47" t="s">
+        <v>247</v>
+      </c>
+      <c r="H25" s="47" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B26" s="122"/>
+      <c r="C26" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="D26" s="90" t="s">
         <v>249</v>
       </c>
-      <c r="E24" s="47" t="s">
-        <v>251</v>
-      </c>
-      <c r="F24" s="47" t="s">
-        <v>250</v>
-      </c>
-      <c r="G24" s="47" t="s">
+      <c r="E26" s="47" t="s">
         <v>252</v>
       </c>
-      <c r="H24" s="47" t="s">
+      <c r="F26" s="92" t="s">
+        <v>254</v>
+      </c>
+      <c r="G26" s="47" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="116"/>
-      <c r="C25" s="47" t="s">
-        <v>279</v>
-      </c>
-      <c r="D25" s="90" t="s">
+      <c r="H26" s="47" t="s">
         <v>258</v>
       </c>
-      <c r="E25" s="47" t="s">
-        <v>254</v>
-      </c>
-      <c r="F25" s="47" t="s">
-        <v>259</v>
-      </c>
-      <c r="G25" s="47" t="s">
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="122"/>
+      <c r="C27" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="D27" s="47" t="s">
+        <v>265</v>
+      </c>
+      <c r="E27" s="47" t="s">
         <v>255</v>
       </c>
-      <c r="H25" s="47" t="s">
+      <c r="F27" s="47" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B26" s="116"/>
-      <c r="C26" s="47" t="s">
-        <v>281</v>
-      </c>
-      <c r="D26" s="90" t="s">
+      <c r="G27" s="47" t="s">
         <v>257</v>
       </c>
-      <c r="E26" s="47" t="s">
-        <v>260</v>
-      </c>
-      <c r="F26" s="125" t="s">
-        <v>262</v>
-      </c>
-      <c r="G26" s="47" t="s">
-        <v>261</v>
-      </c>
-      <c r="H26" s="47" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="116"/>
-      <c r="C27" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="D27" s="47" t="s">
-        <v>274</v>
-      </c>
-      <c r="E27" s="47" t="s">
-        <v>263</v>
-      </c>
-      <c r="F27" s="47" t="s">
-        <v>264</v>
-      </c>
-      <c r="G27" s="47" t="s">
-        <v>265</v>
-      </c>
       <c r="H27" s="47" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="116"/>
+      <c r="B28" s="122"/>
       <c r="C28" s="72" t="s">
         <v>42</v>
       </c>
@@ -5139,202 +5121,202 @@
         <v>46</v>
       </c>
       <c r="E28" s="72" t="s">
+        <v>283</v>
+      </c>
+      <c r="F28" s="72" t="s">
+        <v>157</v>
+      </c>
+      <c r="G28" s="72" t="s">
+        <v>156</v>
+      </c>
+      <c r="H28" s="72" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="122"/>
+      <c r="C29" s="115" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="115" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="115" t="s">
+        <v>164</v>
+      </c>
+      <c r="F29" s="123" t="s">
+        <v>166</v>
+      </c>
+      <c r="G29" s="123" t="s">
+        <v>230</v>
+      </c>
+      <c r="H29" s="115" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="122"/>
+      <c r="C30" s="116"/>
+      <c r="D30" s="116"/>
+      <c r="E30" s="116"/>
+      <c r="F30" s="124"/>
+      <c r="G30" s="124"/>
+      <c r="H30" s="116"/>
+    </row>
+    <row r="31" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B31" s="122"/>
+      <c r="C31" s="80" t="s">
+        <v>267</v>
+      </c>
+      <c r="D31" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="E31" s="77" t="s">
+        <v>162</v>
+      </c>
+      <c r="F31" s="76" t="s">
+        <v>201</v>
+      </c>
+      <c r="G31" s="77" t="s">
         <v>163</v>
       </c>
-      <c r="F28" s="72" t="s">
-        <v>165</v>
-      </c>
-      <c r="G28" s="72" t="s">
+      <c r="H31" s="77" t="s">
         <v>164</v>
       </c>
-      <c r="H28" s="72" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="116"/>
-      <c r="C29" s="108" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="108" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29" s="108" t="s">
+    </row>
+    <row r="32" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B32" s="122"/>
+      <c r="C32" s="115" t="s">
+        <v>268</v>
+      </c>
+      <c r="D32" s="115" t="s">
+        <v>169</v>
+      </c>
+      <c r="E32" s="79" t="s">
+        <v>170</v>
+      </c>
+      <c r="F32" s="76" t="s">
+        <v>199</v>
+      </c>
+      <c r="G32" s="77" t="s">
+        <v>176</v>
+      </c>
+      <c r="H32" s="72" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B33" s="122"/>
+      <c r="C33" s="116"/>
+      <c r="D33" s="116"/>
+      <c r="E33" s="79" t="s">
         <v>172</v>
       </c>
-      <c r="F29" s="117" t="s">
-        <v>174</v>
-      </c>
-      <c r="G29" s="117" t="s">
-        <v>238</v>
-      </c>
-      <c r="H29" s="108" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="116"/>
-      <c r="C30" s="109"/>
-      <c r="D30" s="109"/>
-      <c r="E30" s="109"/>
-      <c r="F30" s="118"/>
-      <c r="G30" s="118"/>
-      <c r="H30" s="109"/>
-    </row>
-    <row r="31" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B31" s="116"/>
-      <c r="C31" s="80" t="s">
-        <v>276</v>
-      </c>
-      <c r="D31" s="78" t="s">
-        <v>169</v>
-      </c>
-      <c r="E31" s="77" t="s">
-        <v>170</v>
-      </c>
-      <c r="F31" s="76" t="s">
-        <v>209</v>
-      </c>
-      <c r="G31" s="77" t="s">
-        <v>171</v>
-      </c>
-      <c r="H31" s="77" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B32" s="116"/>
-      <c r="C32" s="108" t="s">
-        <v>277</v>
-      </c>
-      <c r="D32" s="108" t="s">
-        <v>177</v>
-      </c>
-      <c r="E32" s="79" t="s">
-        <v>178</v>
-      </c>
-      <c r="F32" s="76" t="s">
-        <v>207</v>
-      </c>
-      <c r="G32" s="77" t="s">
-        <v>184</v>
-      </c>
-      <c r="H32" s="72" t="s">
+      <c r="F33" s="76" t="s">
+        <v>200</v>
+      </c>
+      <c r="G33" s="77" t="s">
+        <v>173</v>
+      </c>
+      <c r="H33" s="77" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="B34" s="122"/>
+      <c r="C34" s="73" t="s">
+        <v>269</v>
+      </c>
+      <c r="D34" s="80" t="s">
+        <v>168</v>
+      </c>
+      <c r="E34" s="79" t="s">
+        <v>181</v>
+      </c>
+      <c r="F34" s="76" t="s">
+        <v>198</v>
+      </c>
+      <c r="G34" s="79" t="s">
+        <v>182</v>
+      </c>
+      <c r="H34" s="79" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B33" s="116"/>
-      <c r="C33" s="109"/>
-      <c r="D33" s="109"/>
-      <c r="E33" s="79" t="s">
-        <v>180</v>
-      </c>
-      <c r="F33" s="76" t="s">
-        <v>208</v>
-      </c>
-      <c r="G33" s="77" t="s">
-        <v>181</v>
-      </c>
-      <c r="H33" s="77" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="66" x14ac:dyDescent="0.3">
-      <c r="B34" s="116"/>
-      <c r="C34" s="73" t="s">
-        <v>278</v>
-      </c>
-      <c r="D34" s="80" t="s">
-        <v>176</v>
-      </c>
-      <c r="E34" s="79" t="s">
-        <v>189</v>
-      </c>
-      <c r="F34" s="76" t="s">
-        <v>206</v>
-      </c>
-      <c r="G34" s="79" t="s">
-        <v>190</v>
-      </c>
-      <c r="H34" s="79" t="s">
-        <v>187</v>
-      </c>
-    </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="116"/>
-      <c r="C35" s="120" t="s">
+      <c r="B35" s="122"/>
+      <c r="C35" s="113" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="120" t="s">
+      <c r="D35" s="113" t="s">
         <v>45</v>
       </c>
       <c r="E35" s="48" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F35" s="48"/>
       <c r="G35" s="49"/>
       <c r="H35" s="48" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="116"/>
-      <c r="C36" s="120"/>
-      <c r="D36" s="120"/>
+      <c r="B36" s="122"/>
+      <c r="C36" s="113"/>
+      <c r="D36" s="113"/>
       <c r="E36" s="48" t="s">
+        <v>184</v>
+      </c>
+      <c r="F36" s="76" t="s">
+        <v>196</v>
+      </c>
+      <c r="G36" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="H36" s="48" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B37" s="122"/>
+      <c r="C37" s="115" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="115" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="72" t="s">
+        <v>186</v>
+      </c>
+      <c r="F37" s="76" t="s">
+        <v>193</v>
+      </c>
+      <c r="G37" s="72" t="s">
+        <v>187</v>
+      </c>
+      <c r="H37" s="72" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B38" s="122"/>
+      <c r="C38" s="116"/>
+      <c r="D38" s="116"/>
+      <c r="E38" s="72" t="s">
+        <v>188</v>
+      </c>
+      <c r="F38" s="76" t="s">
+        <v>194</v>
+      </c>
+      <c r="G38" s="72" t="s">
         <v>192</v>
       </c>
-      <c r="F36" s="76" t="s">
-        <v>204</v>
-      </c>
-      <c r="G36" s="48" t="s">
-        <v>193</v>
-      </c>
-      <c r="H36" s="48" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B37" s="116"/>
-      <c r="C37" s="108" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" s="108" t="s">
-        <v>52</v>
-      </c>
-      <c r="E37" s="72" t="s">
-        <v>194</v>
-      </c>
-      <c r="F37" s="76" t="s">
-        <v>201</v>
-      </c>
-      <c r="G37" s="72" t="s">
-        <v>195</v>
-      </c>
-      <c r="H37" s="72" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B38" s="116"/>
-      <c r="C38" s="109"/>
-      <c r="D38" s="109"/>
-      <c r="E38" s="72" t="s">
-        <v>196</v>
-      </c>
-      <c r="F38" s="76" t="s">
-        <v>202</v>
-      </c>
-      <c r="G38" s="72" t="s">
-        <v>200</v>
-      </c>
       <c r="H38" s="72" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B39" s="116"/>
+      <c r="B39" s="122"/>
       <c r="C39" s="79" t="s">
         <v>48</v>
       </c>
@@ -5342,127 +5324,121 @@
         <v>51</v>
       </c>
       <c r="E39" s="79" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F39" s="76" t="s">
+        <v>195</v>
+      </c>
+      <c r="G39" s="79" t="s">
+        <v>197</v>
+      </c>
+      <c r="H39" s="79" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B40" s="122"/>
+      <c r="C40" s="115" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40" s="115" t="s">
+        <v>50</v>
+      </c>
+      <c r="E40" s="72" t="s">
+        <v>202</v>
+      </c>
+      <c r="F40" s="76" t="s">
+        <v>207</v>
+      </c>
+      <c r="G40" s="72" t="s">
+        <v>206</v>
+      </c>
+      <c r="H40" s="72" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B41" s="122"/>
+      <c r="C41" s="116"/>
+      <c r="D41" s="116"/>
+      <c r="E41" s="72" t="s">
+        <v>208</v>
+      </c>
+      <c r="F41" s="76" t="s">
         <v>203</v>
       </c>
-      <c r="G39" s="79" t="s">
+      <c r="G41" s="72" t="s">
+        <v>209</v>
+      </c>
+      <c r="H41" s="72" t="s">
         <v>205</v>
       </c>
-      <c r="H39" s="79" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B40" s="116"/>
-      <c r="C40" s="108" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40" s="108" t="s">
-        <v>50</v>
-      </c>
-      <c r="E40" s="72" t="s">
-        <v>210</v>
-      </c>
-      <c r="F40" s="76" t="s">
-        <v>215</v>
-      </c>
-      <c r="G40" s="72" t="s">
-        <v>214</v>
-      </c>
-      <c r="H40" s="72" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B41" s="116"/>
-      <c r="C41" s="109"/>
-      <c r="D41" s="109"/>
-      <c r="E41" s="72" t="s">
-        <v>216</v>
-      </c>
-      <c r="F41" s="76" t="s">
-        <v>211</v>
-      </c>
-      <c r="G41" s="72" t="s">
-        <v>217</v>
-      </c>
-      <c r="H41" s="72" t="s">
-        <v>213</v>
-      </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B42" s="110" t="s">
-        <v>53</v>
-      </c>
-      <c r="C42" s="119" t="s">
+      <c r="B42" s="119"/>
+      <c r="C42" s="91"/>
+      <c r="D42" s="91" t="s">
+        <v>275</v>
+      </c>
+      <c r="E42" s="45" t="s">
+        <v>276</v>
+      </c>
+      <c r="F42" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="G42" s="45" t="s">
+        <v>277</v>
+      </c>
+      <c r="H42" s="45" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" s="119"/>
+      <c r="C43" s="61"/>
+      <c r="D43" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="119" t="s">
+      <c r="E43" s="91" t="s">
+        <v>278</v>
+      </c>
+      <c r="F43" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="E42" s="45" t="s">
-        <v>284</v>
-      </c>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B43" s="111"/>
-      <c r="C43" s="119"/>
-      <c r="D43" s="119"/>
-      <c r="E43" s="45" t="s">
-        <v>286</v>
-      </c>
-      <c r="F43" s="45" t="s">
-        <v>114</v>
-      </c>
       <c r="G43" s="45" t="s">
-        <v>84</v>
+        <v>280</v>
       </c>
       <c r="H43" s="45" t="s">
-        <v>83</v>
+        <v>281</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B44" s="111"/>
-      <c r="C44" s="61"/>
-      <c r="D44" s="61"/>
-      <c r="E44" s="61"/>
-      <c r="F44" s="61"/>
-      <c r="G44" s="61"/>
-      <c r="H44" s="61"/>
+      <c r="B44" s="120"/>
+      <c r="C44" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="64"/>
+      <c r="E44" s="91"/>
+      <c r="F44" s="91"/>
+      <c r="G44" s="91"/>
+      <c r="H44" s="91"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B45" s="112"/>
-      <c r="C45" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="D45" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="E45" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="F45" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="G45" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="H45" s="45" t="s">
-        <v>79</v>
-      </c>
+      <c r="B45" s="62"/>
+      <c r="C45" s="64"/>
+      <c r="D45" s="64" t="s">
+        <v>118</v>
+      </c>
+      <c r="E45" s="61"/>
+      <c r="F45" s="61"/>
+      <c r="G45" s="61"/>
+      <c r="H45" s="61"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B46" s="62"/>
       <c r="C46" s="64"/>
       <c r="D46" s="64" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="E46" s="61"/>
       <c r="F46" s="61"/>
@@ -5473,7 +5449,7 @@
       <c r="B47" s="62"/>
       <c r="C47" s="64"/>
       <c r="D47" s="64" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E47" s="61"/>
       <c r="F47" s="61"/>
@@ -5484,7 +5460,7 @@
       <c r="B48" s="62"/>
       <c r="C48" s="64"/>
       <c r="D48" s="64" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E48" s="61"/>
       <c r="F48" s="61"/>
@@ -5495,7 +5471,7 @@
       <c r="B49" s="62"/>
       <c r="C49" s="64"/>
       <c r="D49" s="64" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E49" s="61"/>
       <c r="F49" s="61"/>
@@ -5505,49 +5481,40 @@
     <row r="50" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B50" s="62"/>
       <c r="C50" s="64"/>
-      <c r="D50" s="64" t="s">
-        <v>125</v>
-      </c>
+      <c r="D50" s="64"/>
       <c r="E50" s="61"/>
       <c r="F50" s="61"/>
       <c r="G50" s="61"/>
       <c r="H50" s="61"/>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B51" s="62"/>
-      <c r="C51" s="64"/>
-      <c r="D51" s="64"/>
-      <c r="E51" s="61"/>
-      <c r="F51" s="61"/>
-      <c r="G51" s="61"/>
-      <c r="H51" s="61"/>
-    </row>
-    <row r="59" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="D59" s="75" t="s">
-        <v>173</v>
-      </c>
-      <c r="E59" s="77" t="s">
-        <v>186</v>
-      </c>
-      <c r="F59" s="76" t="s">
+    <row r="58" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="D58" s="75" t="s">
+        <v>165</v>
+      </c>
+      <c r="E58" s="77" t="s">
+        <v>178</v>
+      </c>
+      <c r="F58" s="76" t="s">
+        <v>167</v>
+      </c>
+      <c r="G58" s="77" t="s">
         <v>175</v>
       </c>
-      <c r="G59" s="77" t="s">
-        <v>183</v>
-      </c>
-      <c r="H59" s="74" t="s">
-        <v>185</v>
+      <c r="H58" s="74" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
+  <mergeCells count="23">
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B17:B41"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="F29:F30"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="D35:D36"/>
@@ -5557,15 +5524,11 @@
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="D29:D30"/>
     <mergeCell ref="C29:C30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B17:B41"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="E29:E30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Auto push 2023-03-28 18:03:20.22
</commit_message>
<xml_diff>
--- a/project/CheeYoonMovie.xlsx
+++ b/project/CheeYoonMovie.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12240" activeTab="3"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="8" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="296">
   <si>
     <t>이용자 권한과 기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -342,10 +342,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>관리자 등록, 삭제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>영화 검색, 조회</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -410,18 +406,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>평점 관리 (삭제)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자유게시판 관리 (보기, 삭제)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화 상세보기, 배우 상세보기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>배우 검색, 조회</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -483,10 +467,6 @@
   </si>
   <si>
     <t>인물 수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원 제재</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -900,15 +880,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>상영 예고작 리스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>영화 랭킹 리스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원 제재 (회원 목록)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1064,10 +1036,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>화요일 관리자모드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>26일요일 영화 상세보기, 평점 등록,수정,삭제</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1084,18 +1052,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>수요일 평점 리스트? 영화랭킹? 마이메뉴?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>평점 삭제</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>영화 등록, 수정 (인물)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>자유게시판 댓글 등록</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1143,23 +1103,108 @@
     <t>userList.do</t>
   </si>
   <si>
+    <t>UserListService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardList.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>userList.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UserListService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">admin/userList.jsp </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>월요일 검색사이트, 관리자모드 회원리스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boardList.do</t>
+    <t>admin/userList.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예고편 리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>trailerList.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TrailerListService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movie/trailerList.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movie/movieRanking.jsp</t>
+  </si>
+  <si>
+    <t>MovieRankingService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movieRanking.do</t>
+  </si>
+  <si>
+    <t>영화 랭킹 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type,pageNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movie/ratingList.jsp</t>
+  </si>
+  <si>
+    <t>RatingListService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ratingList.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평점리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>월요일 검색사이트,  관리자모드 회원리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화요일 영화랭킹, 평점리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수요일 관리자? 마이메뉴?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 상세보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상영 예고작 리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평점 리스트 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 로그인, 회원목록 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 등록, 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자유게시판 글, 댓글, 평점 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 제재 관리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1697,7 +1742,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1977,6 +2022,36 @@
     <xf numFmtId="0" fontId="11" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2001,31 +2076,40 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2037,40 +2121,7 @@
     <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2421,8 +2472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BP105"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="O95" sqref="O95"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="V44" sqref="V44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.25" defaultRowHeight="11.25" x14ac:dyDescent="0.3"/>
@@ -2441,41 +2492,41 @@
     <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="104" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="95"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
+      <c r="N2" s="105"/>
+      <c r="O2" s="105"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
-      <c r="N3" s="95"/>
-      <c r="O3" s="95"/>
+      <c r="B3" s="105"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="105"/>
+      <c r="K3" s="105"/>
+      <c r="L3" s="105"/>
+      <c r="M3" s="105"/>
+      <c r="N3" s="105"/>
+      <c r="O3" s="105"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
@@ -2520,32 +2571,32 @@
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20"/>
-      <c r="C6" s="96" t="s">
+      <c r="C6" s="106" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="38"/>
-      <c r="E6" s="98" t="s">
+      <c r="E6" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="98"/>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="98"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="100" t="s">
+      <c r="F6" s="108"/>
+      <c r="G6" s="108"/>
+      <c r="H6" s="108"/>
+      <c r="I6" s="108"/>
+      <c r="J6" s="108"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="110" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="98"/>
-      <c r="N6" s="98"/>
-      <c r="O6" s="98"/>
+      <c r="M6" s="108"/>
+      <c r="N6" s="108"/>
+      <c r="O6" s="108"/>
       <c r="P6" s="21"/>
       <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="97"/>
+      <c r="C7" s="107"/>
       <c r="D7" s="22"/>
       <c r="E7" s="86">
         <v>20</v>
@@ -2645,7 +2696,7 @@
     <row r="11" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="101" t="s">
+      <c r="C11" s="100" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="10"/>
@@ -2666,7 +2717,7 @@
     <row r="12" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="101"/>
+      <c r="C12" s="100"/>
       <c r="D12" s="10"/>
       <c r="E12" s="8"/>
       <c r="F12" s="6"/>
@@ -2704,7 +2755,7 @@
     <row r="14" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="93" t="s">
+      <c r="C14" s="103" t="s">
         <v>32</v>
       </c>
       <c r="D14" s="10"/>
@@ -2725,7 +2776,7 @@
     <row r="15" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="93"/>
+      <c r="C15" s="103"/>
       <c r="D15" s="10"/>
       <c r="E15" s="8"/>
       <c r="F15" s="6"/>
@@ -2763,7 +2814,7 @@
     <row r="17" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="101" t="s">
+      <c r="C17" s="100" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="10"/>
@@ -2784,7 +2835,7 @@
     <row r="18" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="101"/>
+      <c r="C18" s="100"/>
       <c r="D18" s="10"/>
       <c r="E18" s="8"/>
       <c r="F18" s="6"/>
@@ -2843,8 +2894,8 @@
     <row r="21" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="103" t="s">
-        <v>213</v>
+      <c r="C21" s="101" t="s">
+        <v>208</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="37"/>
@@ -2864,7 +2915,7 @@
     <row r="22" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="103"/>
+      <c r="C22" s="101"/>
       <c r="D22" s="10"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
@@ -2902,7 +2953,7 @@
     <row r="24" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="103" t="s">
+      <c r="C24" s="101" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="10"/>
@@ -2923,7 +2974,7 @@
     <row r="25" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="103"/>
+      <c r="C25" s="101"/>
       <c r="D25" s="10"/>
       <c r="E25" s="6"/>
       <c r="F25" s="8"/>
@@ -2961,7 +3012,7 @@
     <row r="27" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="103" t="s">
+      <c r="C27" s="101" t="s">
         <v>79</v>
       </c>
       <c r="D27" s="10"/>
@@ -2982,7 +3033,7 @@
     <row r="28" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="103"/>
+      <c r="C28" s="101"/>
       <c r="D28" s="10"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -3020,7 +3071,7 @@
     <row r="30" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="103" t="s">
+      <c r="C30" s="101" t="s">
         <v>80</v>
       </c>
       <c r="D30" s="10"/>
@@ -3041,7 +3092,7 @@
     <row r="31" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="103"/>
+      <c r="C31" s="101"/>
       <c r="D31" s="10"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -3079,8 +3130,8 @@
     <row r="33" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="103" t="s">
-        <v>221</v>
+      <c r="C33" s="101" t="s">
+        <v>214</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="6"/>
@@ -3100,7 +3151,7 @@
     <row r="34" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="6"/>
-      <c r="C34" s="103"/>
+      <c r="C34" s="101"/>
       <c r="D34" s="10"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -3138,7 +3189,7 @@
     <row r="36" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="16"/>
       <c r="B36" s="6"/>
-      <c r="C36" s="103" t="s">
+      <c r="C36" s="101" t="s">
         <v>81</v>
       </c>
       <c r="D36" s="10"/>
@@ -3159,7 +3210,7 @@
     <row r="37" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
       <c r="B37" s="6"/>
-      <c r="C37" s="103"/>
+      <c r="C37" s="101"/>
       <c r="D37" s="10"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
@@ -3218,7 +3269,7 @@
     <row r="40" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="6"/>
-      <c r="C40" s="104" t="s">
+      <c r="C40" s="102" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="10"/>
@@ -3239,7 +3290,7 @@
     <row r="41" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="104"/>
+      <c r="C41" s="102"/>
       <c r="D41" s="10"/>
       <c r="E41" s="6"/>
       <c r="F41" s="8"/>
@@ -3277,8 +3328,8 @@
     <row r="43" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="16"/>
       <c r="B43" s="6"/>
-      <c r="C43" s="104" t="s">
-        <v>215</v>
+      <c r="C43" s="102" t="s">
+        <v>210</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="6"/>
@@ -3298,7 +3349,7 @@
     <row r="44" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="104"/>
+      <c r="C44" s="102"/>
       <c r="D44" s="10"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
@@ -3336,8 +3387,8 @@
     <row r="46" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16"/>
       <c r="B46" s="6"/>
-      <c r="C46" s="104" t="s">
-        <v>217</v>
+      <c r="C46" s="102" t="s">
+        <v>212</v>
       </c>
       <c r="D46" s="10"/>
       <c r="E46" s="6"/>
@@ -3356,7 +3407,7 @@
     <row r="47" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="104"/>
+      <c r="C47" s="102"/>
       <c r="D47" s="10"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
@@ -3394,8 +3445,8 @@
     <row r="49" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="16"/>
       <c r="B49" s="6"/>
-      <c r="C49" s="104" t="s">
-        <v>218</v>
+      <c r="C49" s="102" t="s">
+        <v>290</v>
       </c>
       <c r="D49" s="10"/>
       <c r="E49" s="6"/>
@@ -3415,7 +3466,7 @@
     <row r="50" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="104"/>
+      <c r="C50" s="102"/>
       <c r="D50" s="10"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
@@ -3453,8 +3504,8 @@
     <row r="52" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="16"/>
       <c r="B52" s="6"/>
-      <c r="C52" s="104" t="s">
-        <v>101</v>
+      <c r="C52" s="102" t="s">
+        <v>289</v>
       </c>
       <c r="D52" s="10"/>
       <c r="E52" s="6"/>
@@ -3474,7 +3525,7 @@
     <row r="53" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16"/>
       <c r="B53" s="6"/>
-      <c r="C53" s="104"/>
+      <c r="C53" s="102"/>
       <c r="D53" s="10"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
@@ -3512,8 +3563,8 @@
     <row r="55" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="104" t="s">
-        <v>219</v>
+      <c r="C55" s="102" t="s">
+        <v>213</v>
       </c>
       <c r="D55" s="10"/>
       <c r="E55" s="6"/>
@@ -3523,16 +3574,16 @@
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
       <c r="L55" s="6"/>
-      <c r="M55" s="6"/>
+      <c r="M55" s="37"/>
       <c r="N55" s="6"/>
-      <c r="O55" s="37"/>
+      <c r="O55" s="6"/>
       <c r="P55" s="16"/>
       <c r="Q55" s="5"/>
     </row>
     <row r="56" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="16"/>
       <c r="B56" s="6"/>
-      <c r="C56" s="104"/>
+      <c r="C56" s="102"/>
       <c r="D56" s="10"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
@@ -3542,7 +3593,7 @@
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
       <c r="L56" s="6"/>
-      <c r="M56" s="6"/>
+      <c r="M56" s="8"/>
       <c r="N56" s="6"/>
       <c r="O56" s="6"/>
       <c r="P56" s="16"/>
@@ -3570,8 +3621,8 @@
     <row r="58" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="104" t="s">
-        <v>216</v>
+      <c r="C58" s="102" t="s">
+        <v>211</v>
       </c>
       <c r="D58" s="10"/>
       <c r="E58" s="6"/>
@@ -3591,7 +3642,7 @@
     <row r="59" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="16"/>
       <c r="B59" s="6"/>
-      <c r="C59" s="104"/>
+      <c r="C59" s="102"/>
       <c r="D59" s="10"/>
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
@@ -3626,13 +3677,13 @@
       <c r="P60" s="16"/>
       <c r="Q60" s="5"/>
     </row>
-    <row r="61" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="16"/>
       <c r="B61" s="6"/>
-      <c r="C61" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D61" s="6"/>
+      <c r="C61" s="102" t="s">
+        <v>291</v>
+      </c>
+      <c r="D61" s="10"/>
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
@@ -3642,7 +3693,7 @@
       <c r="K61" s="6"/>
       <c r="L61" s="6"/>
       <c r="M61" s="6"/>
-      <c r="N61" s="6"/>
+      <c r="N61" s="37"/>
       <c r="O61" s="6"/>
       <c r="P61" s="16"/>
       <c r="Q61" s="5"/>
@@ -3650,9 +3701,7 @@
     <row r="62" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="16"/>
       <c r="B62" s="6"/>
-      <c r="C62" s="102" t="s">
-        <v>82</v>
-      </c>
+      <c r="C62" s="102"/>
       <c r="D62" s="10"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
@@ -3662,7 +3711,7 @@
       <c r="J62" s="6"/>
       <c r="K62" s="6"/>
       <c r="L62" s="6"/>
-      <c r="M62" s="6"/>
+      <c r="M62" s="8"/>
       <c r="N62" s="6"/>
       <c r="O62" s="6"/>
       <c r="P62" s="16"/>
@@ -3671,7 +3720,7 @@
     <row r="63" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="16"/>
       <c r="B63" s="6"/>
-      <c r="C63" s="102"/>
+      <c r="C63" s="10"/>
       <c r="D63" s="10"/>
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
@@ -3687,11 +3736,13 @@
       <c r="P63" s="16"/>
       <c r="Q63" s="5"/>
     </row>
-    <row r="64" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="16"/>
       <c r="B64" s="6"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
+      <c r="C64" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" s="6"/>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
@@ -3709,8 +3760,8 @@
     <row r="65" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="16"/>
       <c r="B65" s="6"/>
-      <c r="C65" s="102" t="s">
-        <v>100</v>
+      <c r="C65" s="96" t="s">
+        <v>292</v>
       </c>
       <c r="D65" s="10"/>
       <c r="E65" s="6"/>
@@ -3720,7 +3771,7 @@
       <c r="I65" s="6"/>
       <c r="J65" s="6"/>
       <c r="K65" s="6"/>
-      <c r="L65" s="6"/>
+      <c r="L65" s="37"/>
       <c r="M65" s="6"/>
       <c r="N65" s="6"/>
       <c r="O65" s="6"/>
@@ -3730,7 +3781,7 @@
     <row r="66" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="16"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="102"/>
+      <c r="C66" s="96"/>
       <c r="D66" s="10"/>
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
@@ -3739,7 +3790,7 @@
       <c r="I66" s="6"/>
       <c r="J66" s="6"/>
       <c r="K66" s="6"/>
-      <c r="L66" s="6"/>
+      <c r="L66" s="8"/>
       <c r="M66" s="6"/>
       <c r="N66" s="6"/>
       <c r="O66" s="6"/>
@@ -3768,8 +3819,8 @@
     <row r="68" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="16"/>
       <c r="B68" s="6"/>
-      <c r="C68" s="102" t="s">
-        <v>220</v>
+      <c r="C68" s="96" t="s">
+        <v>293</v>
       </c>
       <c r="D68" s="10"/>
       <c r="E68" s="6"/>
@@ -3789,7 +3840,7 @@
     <row r="69" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="102"/>
+      <c r="C69" s="96"/>
       <c r="D69" s="10"/>
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
@@ -3799,7 +3850,7 @@
       <c r="J69" s="6"/>
       <c r="K69" s="6"/>
       <c r="L69" s="6"/>
-      <c r="M69" s="11"/>
+      <c r="M69" s="6"/>
       <c r="N69" s="6"/>
       <c r="O69" s="6"/>
       <c r="P69" s="16"/>
@@ -3827,8 +3878,8 @@
     <row r="71" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="16"/>
       <c r="B71" s="6"/>
-      <c r="C71" s="102" t="s">
-        <v>266</v>
+      <c r="C71" s="96" t="s">
+        <v>294</v>
       </c>
       <c r="D71" s="10"/>
       <c r="E71" s="6"/>
@@ -3848,7 +3899,7 @@
     <row r="72" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16"/>
       <c r="B72" s="6"/>
-      <c r="C72" s="102"/>
+      <c r="C72" s="96"/>
       <c r="D72" s="10"/>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
@@ -3858,7 +3909,7 @@
       <c r="J72" s="6"/>
       <c r="K72" s="6"/>
       <c r="L72" s="6"/>
-      <c r="M72" s="6"/>
+      <c r="M72" s="11"/>
       <c r="N72" s="6"/>
       <c r="O72" s="6"/>
       <c r="P72" s="16"/>
@@ -3886,8 +3937,8 @@
     <row r="74" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16"/>
       <c r="B74" s="6"/>
-      <c r="C74" s="102" t="s">
-        <v>99</v>
+      <c r="C74" s="96" t="s">
+        <v>295</v>
       </c>
       <c r="D74" s="10"/>
       <c r="E74" s="6"/>
@@ -3907,7 +3958,7 @@
     <row r="75" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="16"/>
       <c r="B75" s="6"/>
-      <c r="C75" s="102"/>
+      <c r="C75" s="96"/>
       <c r="D75" s="10"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
@@ -3945,7 +3996,7 @@
     <row r="77" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="16"/>
       <c r="B77" s="6"/>
-      <c r="C77" s="106" t="s">
+      <c r="C77" s="97" t="s">
         <v>53</v>
       </c>
       <c r="D77" s="7"/>
@@ -3966,7 +4017,7 @@
     <row r="78" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="16"/>
       <c r="B78" s="6"/>
-      <c r="C78" s="106"/>
+      <c r="C78" s="97"/>
       <c r="D78" s="7"/>
       <c r="E78" s="6"/>
       <c r="F78" s="6"/>
@@ -3985,7 +4036,7 @@
     <row r="79" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="16"/>
       <c r="B79" s="6"/>
-      <c r="C79" s="108" t="s">
+      <c r="C79" s="99" t="s">
         <v>77</v>
       </c>
       <c r="D79" s="7"/>
@@ -4056,7 +4107,7 @@
     <row r="80" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="16"/>
       <c r="B80" s="6"/>
-      <c r="C80" s="108"/>
+      <c r="C80" s="99"/>
       <c r="D80" s="7"/>
       <c r="E80" s="6"/>
       <c r="F80" s="6"/>
@@ -4184,18 +4235,18 @@
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5"/>
-      <c r="F84" s="107"/>
-      <c r="G84" s="107"/>
+      <c r="F84" s="98"/>
+      <c r="G84" s="98"/>
       <c r="H84" s="6"/>
       <c r="I84" s="37" t="s">
         <v>55</v>
       </c>
       <c r="J84" s="37"/>
       <c r="K84" s="6"/>
-      <c r="L84" s="105" t="s">
+      <c r="L84" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="M84" s="105"/>
+      <c r="M84" s="95"/>
       <c r="N84" s="39"/>
       <c r="O84" s="5"/>
       <c r="P84" s="5"/>
@@ -4221,62 +4272,62 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C87" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C88" s="4" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C89" s="4" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C90" s="84" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C91" s="84" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C92" s="84" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C93" s="84" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C94" s="84" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C95" s="84" t="s">
-        <v>259</v>
+        <v>287</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C96" s="84" t="s">
-        <v>264</v>
+        <v>288</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C97" s="84" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C98" s="84" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.3">
@@ -4302,15 +4353,13 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="L84:M84"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B2:O3"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="C11:C12"/>
     <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="C62:C63"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="C24:C25"/>
@@ -4325,12 +4374,14 @@
     <mergeCell ref="C55:C56"/>
     <mergeCell ref="C58:C59"/>
     <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B2:O3"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="E6:K6"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="L84:M84"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="C79:C80"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4361,46 +4412,46 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="109" t="s">
+      <c r="A3" s="111" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" s="57"/>
       <c r="D3" s="57"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="109"/>
+      <c r="A4" s="111"/>
       <c r="B4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="111"/>
+      <c r="B5" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="109"/>
-      <c r="B5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -4414,19 +4465,19 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="60" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="60" t="s">
-        <v>104</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -4459,65 +4510,65 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C1" s="68"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2" s="59"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3" s="58"/>
       <c r="E3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C5" s="65"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C6" s="66"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C7" s="67"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C10" s="69"/>
       <c r="D10" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C11" s="70"/>
       <c r="D11">
@@ -4526,7 +4577,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C12" s="71"/>
       <c r="D12">
@@ -4535,7 +4586,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C13" s="67"/>
       <c r="D13">
@@ -4544,7 +4595,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -4552,12 +4603,12 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C40" s="54"/>
     </row>
@@ -4663,10 +4714,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H58"/>
+  <dimension ref="B2:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29:G30"/>
+    <sheetView topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4704,7 +4755,7 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="110" t="s">
+      <c r="B3" s="123" t="s">
         <v>39</v>
       </c>
       <c r="C3" s="43" t="s">
@@ -4718,167 +4769,177 @@
       </c>
       <c r="F3" s="44"/>
       <c r="G3" s="44" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="H3" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="111"/>
-      <c r="C4" s="114" t="s">
+      <c r="B4" s="124"/>
+      <c r="C4" s="126" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="114" t="s">
+      <c r="D4" s="126" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="44" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="F4" s="44"/>
       <c r="G4" s="44"/>
       <c r="H4" s="44" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="124"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
+      <c r="E5" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="44" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="111"/>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="F5" s="44" t="s">
-        <v>125</v>
-      </c>
       <c r="G5" s="44" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="H5" s="44" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="111"/>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
+      <c r="B6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
       <c r="E6" s="44" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F6" s="44" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G6" s="44" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H6" s="44" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="112"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
+      <c r="B7" s="125"/>
+      <c r="C7" s="125"/>
+      <c r="D7" s="125"/>
       <c r="E7" s="44" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F7" s="44" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G7" s="44" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="H7" s="44" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="55"/>
       <c r="C8" s="56" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D8" s="56" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E8" s="44" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F8" s="44" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="G8" s="44" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="H8" s="44" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="63"/>
       <c r="C9" s="82"/>
       <c r="D9" s="82" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F9" s="44"/>
       <c r="G9" s="44" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H9" s="44" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="81"/>
       <c r="C10" s="82"/>
       <c r="D10" s="85" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="E10" s="44" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="F10" s="44"/>
       <c r="G10" s="44" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="H10" s="44" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="81"/>
       <c r="C11" s="82"/>
       <c r="D11" s="82" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="E11" s="44" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="F11" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="G11" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="G11" s="44" t="s">
-        <v>231</v>
-      </c>
       <c r="H11" s="44" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="88"/>
       <c r="C12" s="89"/>
-      <c r="D12" s="89"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
+      <c r="D12" s="94" t="s">
+        <v>280</v>
+      </c>
+      <c r="E12" s="44" t="s">
+        <v>279</v>
+      </c>
+      <c r="F12" s="44" t="s">
+        <v>281</v>
+      </c>
+      <c r="G12" s="44" t="s">
+        <v>278</v>
+      </c>
+      <c r="H12" s="44" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="88"/>
-      <c r="C13" s="89"/>
-      <c r="D13" s="89"/>
+      <c r="B13" s="93"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
       <c r="E13" s="44"/>
       <c r="F13" s="44"/>
       <c r="G13" s="44"/>
@@ -4887,559 +4948,571 @@
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="88"/>
       <c r="C14" s="89"/>
-      <c r="D14" s="89"/>
-      <c r="E14" s="44"/>
+      <c r="D14" s="89" t="s">
+        <v>285</v>
+      </c>
+      <c r="E14" s="44" t="s">
+        <v>284</v>
+      </c>
       <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
+      <c r="G14" s="44" t="s">
+        <v>283</v>
+      </c>
+      <c r="H14" s="44" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="81"/>
-      <c r="C15" s="82"/>
-      <c r="D15" s="82"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="89"/>
       <c r="E15" s="44"/>
       <c r="F15" s="44"/>
       <c r="G15" s="44"/>
       <c r="H15" s="44"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="55"/>
-      <c r="C16" s="89"/>
-      <c r="D16" s="89"/>
-      <c r="E16" s="44"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="82"/>
+      <c r="D16" s="89" t="s">
+        <v>273</v>
+      </c>
+      <c r="E16" s="44" t="s">
+        <v>274</v>
+      </c>
       <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-    </row>
-    <row r="17" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="121" t="s">
+      <c r="G16" s="44" t="s">
+        <v>275</v>
+      </c>
+      <c r="H16" s="44" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="55"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+    </row>
+    <row r="18" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="117" t="s">
+      <c r="C18" s="116" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="117" t="s">
+      <c r="D18" s="116" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="122"/>
-      <c r="C18" s="118"/>
-      <c r="D18" s="118"/>
       <c r="E18" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="119"/>
+      <c r="C19" s="117"/>
+      <c r="D19" s="117"/>
+      <c r="E19" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="46" t="s">
-        <v>113</v>
-      </c>
-      <c r="G18" s="46" t="s">
+      <c r="F19" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="H19" s="47" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="119"/>
+      <c r="C20" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="H20" s="47" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="119"/>
+      <c r="C21" s="116" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="116" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="119"/>
+      <c r="C22" s="117"/>
+      <c r="D22" s="117"/>
+      <c r="E22" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="H18" s="47" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="122"/>
-      <c r="C19" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="46" t="s">
+      <c r="F22" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="G22" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="H22" s="46" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="119"/>
+      <c r="C23" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="47" t="s">
+        <v>264</v>
+      </c>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46" t="s">
-        <v>144</v>
-      </c>
-      <c r="H19" s="47" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="122"/>
-      <c r="C20" s="117" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="117" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="46" t="s">
-        <v>149</v>
-      </c>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46" t="s">
+      <c r="H23" s="47" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="119"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="90"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="119"/>
+      <c r="C25" s="47" t="s">
+        <v>261</v>
+      </c>
+      <c r="D25" s="90" t="s">
+        <v>234</v>
+      </c>
+      <c r="E25" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="F25" s="47" t="s">
+        <v>235</v>
+      </c>
+      <c r="G25" s="47" t="s">
+        <v>237</v>
+      </c>
+      <c r="H25" s="47" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="119"/>
+      <c r="C26" s="47" t="s">
+        <v>260</v>
+      </c>
+      <c r="D26" s="90" t="s">
+        <v>243</v>
+      </c>
+      <c r="E26" s="47" t="s">
+        <v>239</v>
+      </c>
+      <c r="F26" s="47" t="s">
+        <v>244</v>
+      </c>
+      <c r="G26" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="H26" s="47" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B27" s="119"/>
+      <c r="C27" s="47" t="s">
+        <v>262</v>
+      </c>
+      <c r="D27" s="90" t="s">
+        <v>242</v>
+      </c>
+      <c r="E27" s="47" t="s">
+        <v>245</v>
+      </c>
+      <c r="F27" s="92" t="s">
+        <v>247</v>
+      </c>
+      <c r="G27" s="47" t="s">
+        <v>246</v>
+      </c>
+      <c r="H27" s="47" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="119"/>
+      <c r="C28" s="47" t="s">
+        <v>263</v>
+      </c>
+      <c r="D28" s="47" t="s">
+        <v>256</v>
+      </c>
+      <c r="E28" s="47" t="s">
+        <v>248</v>
+      </c>
+      <c r="F28" s="47" t="s">
+        <v>249</v>
+      </c>
+      <c r="G28" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="H28" s="47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="119"/>
+      <c r="C29" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="72" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="72" t="s">
+        <v>270</v>
+      </c>
+      <c r="F29" s="72" t="s">
+        <v>152</v>
+      </c>
+      <c r="G29" s="72" t="s">
+        <v>151</v>
+      </c>
+      <c r="H29" s="72" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="119"/>
+      <c r="C30" s="112" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="112" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="112" t="s">
+        <v>159</v>
+      </c>
+      <c r="F30" s="120" t="s">
+        <v>161</v>
+      </c>
+      <c r="G30" s="120" t="s">
+        <v>223</v>
+      </c>
+      <c r="H30" s="112" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="119"/>
+      <c r="C31" s="113"/>
+      <c r="D31" s="113"/>
+      <c r="E31" s="113"/>
+      <c r="F31" s="121"/>
+      <c r="G31" s="121"/>
+      <c r="H31" s="113"/>
+    </row>
+    <row r="32" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B32" s="119"/>
+      <c r="C32" s="80" t="s">
+        <v>257</v>
+      </c>
+      <c r="D32" s="78" t="s">
+        <v>156</v>
+      </c>
+      <c r="E32" s="77" t="s">
+        <v>157</v>
+      </c>
+      <c r="F32" s="76" t="s">
+        <v>196</v>
+      </c>
+      <c r="G32" s="77" t="s">
+        <v>158</v>
+      </c>
+      <c r="H32" s="77" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B33" s="119"/>
+      <c r="C33" s="112" t="s">
+        <v>258</v>
+      </c>
+      <c r="D33" s="112" t="s">
+        <v>164</v>
+      </c>
+      <c r="E33" s="79" t="s">
+        <v>165</v>
+      </c>
+      <c r="F33" s="76" t="s">
+        <v>194</v>
+      </c>
+      <c r="G33" s="77" t="s">
+        <v>171</v>
+      </c>
+      <c r="H33" s="72" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B34" s="119"/>
+      <c r="C34" s="113"/>
+      <c r="D34" s="113"/>
+      <c r="E34" s="79" t="s">
+        <v>167</v>
+      </c>
+      <c r="F34" s="76" t="s">
+        <v>195</v>
+      </c>
+      <c r="G34" s="77" t="s">
+        <v>168</v>
+      </c>
+      <c r="H34" s="77" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="B35" s="119"/>
+      <c r="C35" s="73" t="s">
+        <v>259</v>
+      </c>
+      <c r="D35" s="80" t="s">
+        <v>163</v>
+      </c>
+      <c r="E35" s="79" t="s">
+        <v>176</v>
+      </c>
+      <c r="F35" s="76" t="s">
+        <v>193</v>
+      </c>
+      <c r="G35" s="79" t="s">
+        <v>177</v>
+      </c>
+      <c r="H35" s="79" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" s="119"/>
+      <c r="C36" s="122" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="122" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="F36" s="48"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="48" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37" s="119"/>
+      <c r="C37" s="122"/>
+      <c r="D37" s="122"/>
+      <c r="E37" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="F37" s="76" t="s">
+        <v>191</v>
+      </c>
+      <c r="G37" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="H37" s="48" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="122"/>
-      <c r="C21" s="118"/>
-      <c r="D21" s="118"/>
-      <c r="E21" s="46" t="s">
-        <v>151</v>
-      </c>
-      <c r="F21" s="47" t="s">
-        <v>145</v>
-      </c>
-      <c r="G21" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="H21" s="46" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="122"/>
-      <c r="C22" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="47" t="s">
-        <v>274</v>
-      </c>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="H22" s="47" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="122"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="90"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="122"/>
-      <c r="C24" s="47" t="s">
+    <row r="38" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B38" s="119"/>
+      <c r="C38" s="112" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="112" t="s">
+        <v>52</v>
+      </c>
+      <c r="E38" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="F38" s="76" t="s">
+        <v>188</v>
+      </c>
+      <c r="G38" s="72" t="s">
+        <v>182</v>
+      </c>
+      <c r="H38" s="72" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B39" s="119"/>
+      <c r="C39" s="113"/>
+      <c r="D39" s="113"/>
+      <c r="E39" s="72" t="s">
+        <v>183</v>
+      </c>
+      <c r="F39" s="76" t="s">
+        <v>189</v>
+      </c>
+      <c r="G39" s="72" t="s">
+        <v>187</v>
+      </c>
+      <c r="H39" s="72" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B40" s="119"/>
+      <c r="C40" s="79" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="79" t="s">
+        <v>51</v>
+      </c>
+      <c r="E40" s="79" t="s">
+        <v>73</v>
+      </c>
+      <c r="F40" s="76" t="s">
+        <v>190</v>
+      </c>
+      <c r="G40" s="79" t="s">
+        <v>192</v>
+      </c>
+      <c r="H40" s="79" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B41" s="119"/>
+      <c r="C41" s="112" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="112" t="s">
+        <v>50</v>
+      </c>
+      <c r="E41" s="72" t="s">
+        <v>197</v>
+      </c>
+      <c r="F41" s="76" t="s">
+        <v>202</v>
+      </c>
+      <c r="G41" s="72" t="s">
+        <v>201</v>
+      </c>
+      <c r="H41" s="72" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B42" s="119"/>
+      <c r="C42" s="113"/>
+      <c r="D42" s="113"/>
+      <c r="E42" s="72" t="s">
+        <v>203</v>
+      </c>
+      <c r="F42" s="76" t="s">
+        <v>198</v>
+      </c>
+      <c r="G42" s="72" t="s">
+        <v>204</v>
+      </c>
+      <c r="H42" s="72" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" s="114"/>
+      <c r="C43" s="91"/>
+      <c r="D43" s="91" t="s">
+        <v>265</v>
+      </c>
+      <c r="E43" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="F43" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="G43" s="45" t="s">
+        <v>267</v>
+      </c>
+      <c r="H43" s="45" t="s">
         <v>271</v>
       </c>
-      <c r="D24" s="90" t="s">
-        <v>241</v>
-      </c>
-      <c r="E24" s="47" t="s">
-        <v>243</v>
-      </c>
-      <c r="F24" s="47" t="s">
-        <v>242</v>
-      </c>
-      <c r="G24" s="47" t="s">
-        <v>244</v>
-      </c>
-      <c r="H24" s="47" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="122"/>
-      <c r="C25" s="47" t="s">
-        <v>270</v>
-      </c>
-      <c r="D25" s="90" t="s">
-        <v>250</v>
-      </c>
-      <c r="E25" s="47" t="s">
-        <v>246</v>
-      </c>
-      <c r="F25" s="47" t="s">
-        <v>251</v>
-      </c>
-      <c r="G25" s="47" t="s">
-        <v>247</v>
-      </c>
-      <c r="H25" s="47" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B26" s="122"/>
-      <c r="C26" s="47" t="s">
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44" s="114"/>
+      <c r="C44" s="61"/>
+      <c r="D44" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="E44" s="91" t="s">
+        <v>268</v>
+      </c>
+      <c r="F44" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="G44" s="45" t="s">
+        <v>269</v>
+      </c>
+      <c r="H44" s="45" t="s">
         <v>272</v>
       </c>
-      <c r="D26" s="90" t="s">
-        <v>249</v>
-      </c>
-      <c r="E26" s="47" t="s">
-        <v>252</v>
-      </c>
-      <c r="F26" s="92" t="s">
-        <v>254</v>
-      </c>
-      <c r="G26" s="47" t="s">
-        <v>253</v>
-      </c>
-      <c r="H26" s="47" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="122"/>
-      <c r="C27" s="47" t="s">
-        <v>273</v>
-      </c>
-      <c r="D27" s="47" t="s">
-        <v>265</v>
-      </c>
-      <c r="E27" s="47" t="s">
-        <v>255</v>
-      </c>
-      <c r="F27" s="47" t="s">
-        <v>256</v>
-      </c>
-      <c r="G27" s="47" t="s">
-        <v>257</v>
-      </c>
-      <c r="H27" s="47" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="122"/>
-      <c r="C28" s="72" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="72" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="72" t="s">
-        <v>283</v>
-      </c>
-      <c r="F28" s="72" t="s">
-        <v>157</v>
-      </c>
-      <c r="G28" s="72" t="s">
-        <v>156</v>
-      </c>
-      <c r="H28" s="72" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="122"/>
-      <c r="C29" s="115" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="115" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29" s="115" t="s">
-        <v>164</v>
-      </c>
-      <c r="F29" s="123" t="s">
-        <v>166</v>
-      </c>
-      <c r="G29" s="123" t="s">
-        <v>230</v>
-      </c>
-      <c r="H29" s="115" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="122"/>
-      <c r="C30" s="116"/>
-      <c r="D30" s="116"/>
-      <c r="E30" s="116"/>
-      <c r="F30" s="124"/>
-      <c r="G30" s="124"/>
-      <c r="H30" s="116"/>
-    </row>
-    <row r="31" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B31" s="122"/>
-      <c r="C31" s="80" t="s">
-        <v>267</v>
-      </c>
-      <c r="D31" s="78" t="s">
-        <v>161</v>
-      </c>
-      <c r="E31" s="77" t="s">
-        <v>162</v>
-      </c>
-      <c r="F31" s="76" t="s">
-        <v>201</v>
-      </c>
-      <c r="G31" s="77" t="s">
-        <v>163</v>
-      </c>
-      <c r="H31" s="77" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B32" s="122"/>
-      <c r="C32" s="115" t="s">
-        <v>268</v>
-      </c>
-      <c r="D32" s="115" t="s">
-        <v>169</v>
-      </c>
-      <c r="E32" s="79" t="s">
-        <v>170</v>
-      </c>
-      <c r="F32" s="76" t="s">
-        <v>199</v>
-      </c>
-      <c r="G32" s="77" t="s">
-        <v>176</v>
-      </c>
-      <c r="H32" s="72" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B33" s="122"/>
-      <c r="C33" s="116"/>
-      <c r="D33" s="116"/>
-      <c r="E33" s="79" t="s">
-        <v>172</v>
-      </c>
-      <c r="F33" s="76" t="s">
-        <v>200</v>
-      </c>
-      <c r="G33" s="77" t="s">
-        <v>173</v>
-      </c>
-      <c r="H33" s="77" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="66" x14ac:dyDescent="0.3">
-      <c r="B34" s="122"/>
-      <c r="C34" s="73" t="s">
-        <v>269</v>
-      </c>
-      <c r="D34" s="80" t="s">
-        <v>168</v>
-      </c>
-      <c r="E34" s="79" t="s">
-        <v>181</v>
-      </c>
-      <c r="F34" s="76" t="s">
-        <v>198</v>
-      </c>
-      <c r="G34" s="79" t="s">
-        <v>182</v>
-      </c>
-      <c r="H34" s="79" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="122"/>
-      <c r="C35" s="113" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" s="113" t="s">
-        <v>45</v>
-      </c>
-      <c r="E35" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="F35" s="48"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="48" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="122"/>
-      <c r="C36" s="113"/>
-      <c r="D36" s="113"/>
-      <c r="E36" s="48" t="s">
-        <v>184</v>
-      </c>
-      <c r="F36" s="76" t="s">
-        <v>196</v>
-      </c>
-      <c r="G36" s="48" t="s">
-        <v>185</v>
-      </c>
-      <c r="H36" s="48" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B37" s="122"/>
-      <c r="C37" s="115" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" s="115" t="s">
-        <v>52</v>
-      </c>
-      <c r="E37" s="72" t="s">
-        <v>186</v>
-      </c>
-      <c r="F37" s="76" t="s">
-        <v>193</v>
-      </c>
-      <c r="G37" s="72" t="s">
-        <v>187</v>
-      </c>
-      <c r="H37" s="72" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B38" s="122"/>
-      <c r="C38" s="116"/>
-      <c r="D38" s="116"/>
-      <c r="E38" s="72" t="s">
-        <v>188</v>
-      </c>
-      <c r="F38" s="76" t="s">
-        <v>194</v>
-      </c>
-      <c r="G38" s="72" t="s">
-        <v>192</v>
-      </c>
-      <c r="H38" s="72" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B39" s="122"/>
-      <c r="C39" s="79" t="s">
-        <v>48</v>
-      </c>
-      <c r="D39" s="79" t="s">
-        <v>51</v>
-      </c>
-      <c r="E39" s="79" t="s">
-        <v>73</v>
-      </c>
-      <c r="F39" s="76" t="s">
-        <v>195</v>
-      </c>
-      <c r="G39" s="79" t="s">
-        <v>197</v>
-      </c>
-      <c r="H39" s="79" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B40" s="122"/>
-      <c r="C40" s="115" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40" s="115" t="s">
-        <v>50</v>
-      </c>
-      <c r="E40" s="72" t="s">
-        <v>202</v>
-      </c>
-      <c r="F40" s="76" t="s">
-        <v>207</v>
-      </c>
-      <c r="G40" s="72" t="s">
-        <v>206</v>
-      </c>
-      <c r="H40" s="72" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B41" s="122"/>
-      <c r="C41" s="116"/>
-      <c r="D41" s="116"/>
-      <c r="E41" s="72" t="s">
-        <v>208</v>
-      </c>
-      <c r="F41" s="76" t="s">
-        <v>203</v>
-      </c>
-      <c r="G41" s="72" t="s">
-        <v>209</v>
-      </c>
-      <c r="H41" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B42" s="119"/>
-      <c r="C42" s="91"/>
-      <c r="D42" s="91" t="s">
-        <v>275</v>
-      </c>
-      <c r="E42" s="45" t="s">
-        <v>276</v>
-      </c>
-      <c r="F42" s="45" t="s">
-        <v>106</v>
-      </c>
-      <c r="G42" s="45" t="s">
-        <v>277</v>
-      </c>
-      <c r="H42" s="45" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B43" s="119"/>
-      <c r="C43" s="61"/>
-      <c r="D43" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="E43" s="91" t="s">
-        <v>278</v>
-      </c>
-      <c r="F43" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="G43" s="45" t="s">
-        <v>280</v>
-      </c>
-      <c r="H43" s="45" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B44" s="120"/>
-      <c r="C44" s="45" t="s">
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B45" s="115"/>
+      <c r="C45" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="D44" s="64"/>
-      <c r="E44" s="91"/>
-      <c r="F44" s="91"/>
-      <c r="G44" s="91"/>
-      <c r="H44" s="91"/>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B45" s="62"/>
-      <c r="C45" s="64"/>
-      <c r="D45" s="64" t="s">
-        <v>118</v>
-      </c>
-      <c r="E45" s="61"/>
-      <c r="F45" s="61"/>
-      <c r="G45" s="61"/>
-      <c r="H45" s="61"/>
+      <c r="D45" s="64"/>
+      <c r="E45" s="91"/>
+      <c r="F45" s="91"/>
+      <c r="G45" s="91"/>
+      <c r="H45" s="91"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B46" s="62"/>
       <c r="C46" s="64"/>
-      <c r="D46" s="64" t="s">
-        <v>114</v>
-      </c>
+      <c r="D46" s="64"/>
       <c r="E46" s="61"/>
       <c r="F46" s="61"/>
       <c r="G46" s="61"/>
@@ -5449,7 +5522,7 @@
       <c r="B47" s="62"/>
       <c r="C47" s="64"/>
       <c r="D47" s="64" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E47" s="61"/>
       <c r="F47" s="61"/>
@@ -5460,7 +5533,7 @@
       <c r="B48" s="62"/>
       <c r="C48" s="64"/>
       <c r="D48" s="64" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E48" s="61"/>
       <c r="F48" s="61"/>
@@ -5471,7 +5544,7 @@
       <c r="B49" s="62"/>
       <c r="C49" s="64"/>
       <c r="D49" s="64" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E49" s="61"/>
       <c r="F49" s="61"/>
@@ -5481,54 +5554,65 @@
     <row r="50" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B50" s="62"/>
       <c r="C50" s="64"/>
-      <c r="D50" s="64"/>
+      <c r="D50" s="64" t="s">
+        <v>113</v>
+      </c>
       <c r="E50" s="61"/>
       <c r="F50" s="61"/>
       <c r="G50" s="61"/>
       <c r="H50" s="61"/>
     </row>
-    <row r="58" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="D58" s="75" t="s">
-        <v>165</v>
-      </c>
-      <c r="E58" s="77" t="s">
-        <v>178</v>
-      </c>
-      <c r="F58" s="76" t="s">
-        <v>167</v>
-      </c>
-      <c r="G58" s="77" t="s">
-        <v>175</v>
-      </c>
-      <c r="H58" s="74" t="s">
-        <v>177</v>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B51" s="62"/>
+      <c r="C51" s="64"/>
+      <c r="D51" s="64"/>
+      <c r="E51" s="61"/>
+      <c r="F51" s="61"/>
+      <c r="G51" s="61"/>
+      <c r="H51" s="61"/>
+    </row>
+    <row r="59" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="D59" s="75" t="s">
+        <v>160</v>
+      </c>
+      <c r="E59" s="77" t="s">
+        <v>173</v>
+      </c>
+      <c r="F59" s="76" t="s">
+        <v>162</v>
+      </c>
+      <c r="G59" s="77" t="s">
+        <v>170</v>
+      </c>
+      <c r="H59" s="74" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B17:B41"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C30:C31"/>
     <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C36:C37"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="D4:D7"/>
-    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="B18:B42"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C33:C34"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Auto push 2023-03-29 18:03:38.12
</commit_message>
<xml_diff>
--- a/project/CheeYoonMovie.xlsx
+++ b/project/CheeYoonMovie.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12240"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12240" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="8" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="302">
   <si>
     <t>이용자 권한과 기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -237,10 +237,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>회원리스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>회원들 리스트</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -454,10 +450,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>영화 등록</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>영화 수정(개봉예정,상영작,종료)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -650,10 +642,6 @@
   </si>
   <si>
     <t>boardContent.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>댓글 리스트 출력</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -662,11 +650,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>boardNo
-commentPageNum</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>댓글 삭제</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -695,19 +678,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CommentListService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CommentModifyViewService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>board/commentList.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>commentList.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1205,6 +1176,57 @@
   </si>
   <si>
     <t>회원 제재 관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이게제일좋음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원상세보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userDetail.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserDetailService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user/userDetail.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RegisterMovie.java</t>
+  </si>
+  <si>
+    <t>등록페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin/insert.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insertView.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insertMovie.do</t>
+  </si>
+  <si>
+    <t>영화등록처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MovieDto속성들
+tagDto 여러개</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1742,7 +1764,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1966,137 +1988,155 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2109,20 +2149,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2472,8 +2500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BP105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="V44" sqref="V44"/>
+    <sheetView topLeftCell="A67" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.25" defaultRowHeight="11.25" x14ac:dyDescent="0.3"/>
@@ -2492,41 +2520,41 @@
     <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="104" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="105"/>
-      <c r="M2" s="105"/>
-      <c r="N2" s="105"/>
-      <c r="O2" s="105"/>
+      <c r="B2" s="97" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="105"/>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="105"/>
-      <c r="L3" s="105"/>
-      <c r="M3" s="105"/>
-      <c r="N3" s="105"/>
-      <c r="O3" s="105"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
@@ -2571,64 +2599,64 @@
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20"/>
-      <c r="C6" s="106" t="s">
+      <c r="C6" s="99" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="38"/>
-      <c r="E6" s="108" t="s">
+      <c r="E6" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="108"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="108"/>
-      <c r="I6" s="108"/>
-      <c r="J6" s="108"/>
-      <c r="K6" s="109"/>
-      <c r="L6" s="110" t="s">
+      <c r="F6" s="101"/>
+      <c r="G6" s="101"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="101"/>
+      <c r="J6" s="101"/>
+      <c r="K6" s="102"/>
+      <c r="L6" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="108"/>
-      <c r="N6" s="108"/>
-      <c r="O6" s="108"/>
+      <c r="M6" s="101"/>
+      <c r="N6" s="101"/>
+      <c r="O6" s="101"/>
       <c r="P6" s="21"/>
       <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="107"/>
+      <c r="C7" s="100"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="86">
+      <c r="E7" s="84">
         <v>20</v>
       </c>
-      <c r="F7" s="86">
+      <c r="F7" s="84">
         <v>21</v>
       </c>
-      <c r="G7" s="86">
+      <c r="G7" s="84">
         <v>22</v>
       </c>
-      <c r="H7" s="86">
+      <c r="H7" s="84">
         <v>23</v>
       </c>
-      <c r="I7" s="86">
+      <c r="I7" s="84">
         <v>24</v>
       </c>
-      <c r="J7" s="86">
+      <c r="J7" s="84">
         <v>25</v>
       </c>
-      <c r="K7" s="87">
+      <c r="K7" s="85">
         <v>26</v>
       </c>
-      <c r="L7" s="86">
+      <c r="L7" s="84">
         <v>27</v>
       </c>
-      <c r="M7" s="86">
+      <c r="M7" s="84">
         <v>28</v>
       </c>
-      <c r="N7" s="86">
+      <c r="N7" s="84">
         <v>29</v>
       </c>
-      <c r="O7" s="86">
+      <c r="O7" s="84">
         <v>30</v>
       </c>
       <c r="P7" s="23"/>
@@ -2696,7 +2724,7 @@
     <row r="11" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="100" t="s">
+      <c r="C11" s="104" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="10"/>
@@ -2717,7 +2745,7 @@
     <row r="12" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="100"/>
+      <c r="C12" s="104"/>
       <c r="D12" s="10"/>
       <c r="E12" s="8"/>
       <c r="F12" s="6"/>
@@ -2755,7 +2783,7 @@
     <row r="14" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="103" t="s">
+      <c r="C14" s="96" t="s">
         <v>32</v>
       </c>
       <c r="D14" s="10"/>
@@ -2776,7 +2804,7 @@
     <row r="15" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="103"/>
+      <c r="C15" s="96"/>
       <c r="D15" s="10"/>
       <c r="E15" s="8"/>
       <c r="F15" s="6"/>
@@ -2814,7 +2842,7 @@
     <row r="17" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="100" t="s">
+      <c r="C17" s="104" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="10"/>
@@ -2835,7 +2863,7 @@
     <row r="18" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="100"/>
+      <c r="C18" s="104"/>
       <c r="D18" s="10"/>
       <c r="E18" s="8"/>
       <c r="F18" s="6"/>
@@ -2894,8 +2922,8 @@
     <row r="21" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="101" t="s">
-        <v>208</v>
+      <c r="C21" s="106" t="s">
+        <v>201</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="37"/>
@@ -2915,7 +2943,7 @@
     <row r="22" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="101"/>
+      <c r="C22" s="106"/>
       <c r="D22" s="10"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
@@ -2953,7 +2981,7 @@
     <row r="24" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="101" t="s">
+      <c r="C24" s="106" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="10"/>
@@ -2974,7 +3002,7 @@
     <row r="25" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="101"/>
+      <c r="C25" s="106"/>
       <c r="D25" s="10"/>
       <c r="E25" s="6"/>
       <c r="F25" s="8"/>
@@ -3012,8 +3040,8 @@
     <row r="27" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="101" t="s">
-        <v>79</v>
+      <c r="C27" s="106" t="s">
+        <v>78</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="6"/>
@@ -3033,7 +3061,7 @@
     <row r="28" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="101"/>
+      <c r="C28" s="106"/>
       <c r="D28" s="10"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -3071,8 +3099,8 @@
     <row r="30" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="101" t="s">
-        <v>80</v>
+      <c r="C30" s="106" t="s">
+        <v>79</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="6"/>
@@ -3092,7 +3120,7 @@
     <row r="31" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="101"/>
+      <c r="C31" s="106"/>
       <c r="D31" s="10"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -3130,8 +3158,8 @@
     <row r="33" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="101" t="s">
-        <v>214</v>
+      <c r="C33" s="106" t="s">
+        <v>207</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="6"/>
@@ -3151,7 +3179,7 @@
     <row r="34" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="6"/>
-      <c r="C34" s="101"/>
+      <c r="C34" s="106"/>
       <c r="D34" s="10"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -3189,8 +3217,8 @@
     <row r="36" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="16"/>
       <c r="B36" s="6"/>
-      <c r="C36" s="101" t="s">
-        <v>81</v>
+      <c r="C36" s="106" t="s">
+        <v>80</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="6"/>
@@ -3210,7 +3238,7 @@
     <row r="37" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
       <c r="B37" s="6"/>
-      <c r="C37" s="101"/>
+      <c r="C37" s="106"/>
       <c r="D37" s="10"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
@@ -3269,7 +3297,7 @@
     <row r="40" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="6"/>
-      <c r="C40" s="102" t="s">
+      <c r="C40" s="107" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="10"/>
@@ -3290,7 +3318,7 @@
     <row r="41" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="102"/>
+      <c r="C41" s="107"/>
       <c r="D41" s="10"/>
       <c r="E41" s="6"/>
       <c r="F41" s="8"/>
@@ -3328,8 +3356,8 @@
     <row r="43" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="16"/>
       <c r="B43" s="6"/>
-      <c r="C43" s="102" t="s">
-        <v>210</v>
+      <c r="C43" s="107" t="s">
+        <v>203</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="6"/>
@@ -3349,7 +3377,7 @@
     <row r="44" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="102"/>
+      <c r="C44" s="107"/>
       <c r="D44" s="10"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
@@ -3387,8 +3415,8 @@
     <row r="46" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16"/>
       <c r="B46" s="6"/>
-      <c r="C46" s="102" t="s">
-        <v>212</v>
+      <c r="C46" s="107" t="s">
+        <v>205</v>
       </c>
       <c r="D46" s="10"/>
       <c r="E46" s="6"/>
@@ -3407,7 +3435,7 @@
     <row r="47" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="102"/>
+      <c r="C47" s="107"/>
       <c r="D47" s="10"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
@@ -3445,8 +3473,8 @@
     <row r="49" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="16"/>
       <c r="B49" s="6"/>
-      <c r="C49" s="102" t="s">
-        <v>290</v>
+      <c r="C49" s="107" t="s">
+        <v>283</v>
       </c>
       <c r="D49" s="10"/>
       <c r="E49" s="6"/>
@@ -3466,7 +3494,7 @@
     <row r="50" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="102"/>
+      <c r="C50" s="107"/>
       <c r="D50" s="10"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
@@ -3504,8 +3532,8 @@
     <row r="52" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="16"/>
       <c r="B52" s="6"/>
-      <c r="C52" s="102" t="s">
-        <v>289</v>
+      <c r="C52" s="107" t="s">
+        <v>282</v>
       </c>
       <c r="D52" s="10"/>
       <c r="E52" s="6"/>
@@ -3525,7 +3553,7 @@
     <row r="53" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16"/>
       <c r="B53" s="6"/>
-      <c r="C53" s="102"/>
+      <c r="C53" s="107"/>
       <c r="D53" s="10"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
@@ -3563,8 +3591,8 @@
     <row r="55" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="102" t="s">
-        <v>213</v>
+      <c r="C55" s="107" t="s">
+        <v>206</v>
       </c>
       <c r="D55" s="10"/>
       <c r="E55" s="6"/>
@@ -3583,7 +3611,7 @@
     <row r="56" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="16"/>
       <c r="B56" s="6"/>
-      <c r="C56" s="102"/>
+      <c r="C56" s="107"/>
       <c r="D56" s="10"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
@@ -3621,8 +3649,8 @@
     <row r="58" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="102" t="s">
-        <v>211</v>
+      <c r="C58" s="107" t="s">
+        <v>204</v>
       </c>
       <c r="D58" s="10"/>
       <c r="E58" s="6"/>
@@ -3642,7 +3670,7 @@
     <row r="59" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="16"/>
       <c r="B59" s="6"/>
-      <c r="C59" s="102"/>
+      <c r="C59" s="107"/>
       <c r="D59" s="10"/>
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
@@ -3680,8 +3708,8 @@
     <row r="61" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="16"/>
       <c r="B61" s="6"/>
-      <c r="C61" s="102" t="s">
-        <v>291</v>
+      <c r="C61" s="107" t="s">
+        <v>284</v>
       </c>
       <c r="D61" s="10"/>
       <c r="E61" s="6"/>
@@ -3701,7 +3729,7 @@
     <row r="62" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="16"/>
       <c r="B62" s="6"/>
-      <c r="C62" s="102"/>
+      <c r="C62" s="107"/>
       <c r="D62" s="10"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
@@ -3760,8 +3788,8 @@
     <row r="65" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="16"/>
       <c r="B65" s="6"/>
-      <c r="C65" s="96" t="s">
-        <v>292</v>
+      <c r="C65" s="105" t="s">
+        <v>285</v>
       </c>
       <c r="D65" s="10"/>
       <c r="E65" s="6"/>
@@ -3781,7 +3809,7 @@
     <row r="66" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="16"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="96"/>
+      <c r="C66" s="105"/>
       <c r="D66" s="10"/>
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
@@ -3819,8 +3847,8 @@
     <row r="68" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="16"/>
       <c r="B68" s="6"/>
-      <c r="C68" s="96" t="s">
-        <v>293</v>
+      <c r="C68" s="105" t="s">
+        <v>286</v>
       </c>
       <c r="D68" s="10"/>
       <c r="E68" s="6"/>
@@ -3840,7 +3868,7 @@
     <row r="69" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="96"/>
+      <c r="C69" s="105"/>
       <c r="D69" s="10"/>
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
@@ -3878,8 +3906,8 @@
     <row r="71" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="16"/>
       <c r="B71" s="6"/>
-      <c r="C71" s="96" t="s">
-        <v>294</v>
+      <c r="C71" s="105" t="s">
+        <v>287</v>
       </c>
       <c r="D71" s="10"/>
       <c r="E71" s="6"/>
@@ -3899,7 +3927,7 @@
     <row r="72" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16"/>
       <c r="B72" s="6"/>
-      <c r="C72" s="96"/>
+      <c r="C72" s="105"/>
       <c r="D72" s="10"/>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
@@ -3937,8 +3965,8 @@
     <row r="74" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16"/>
       <c r="B74" s="6"/>
-      <c r="C74" s="96" t="s">
-        <v>295</v>
+      <c r="C74" s="105" t="s">
+        <v>288</v>
       </c>
       <c r="D74" s="10"/>
       <c r="E74" s="6"/>
@@ -3958,7 +3986,7 @@
     <row r="75" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="16"/>
       <c r="B75" s="6"/>
-      <c r="C75" s="96"/>
+      <c r="C75" s="105"/>
       <c r="D75" s="10"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
@@ -3996,7 +4024,7 @@
     <row r="77" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="16"/>
       <c r="B77" s="6"/>
-      <c r="C77" s="97" t="s">
+      <c r="C77" s="109" t="s">
         <v>53</v>
       </c>
       <c r="D77" s="7"/>
@@ -4017,7 +4045,7 @@
     <row r="78" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="16"/>
       <c r="B78" s="6"/>
-      <c r="C78" s="97"/>
+      <c r="C78" s="109"/>
       <c r="D78" s="7"/>
       <c r="E78" s="6"/>
       <c r="F78" s="6"/>
@@ -4036,8 +4064,8 @@
     <row r="79" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="16"/>
       <c r="B79" s="6"/>
-      <c r="C79" s="99" t="s">
-        <v>77</v>
+      <c r="C79" s="111" t="s">
+        <v>76</v>
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="6"/>
@@ -4107,7 +4135,7 @@
     <row r="80" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="16"/>
       <c r="B80" s="6"/>
-      <c r="C80" s="99"/>
+      <c r="C80" s="111"/>
       <c r="D80" s="7"/>
       <c r="E80" s="6"/>
       <c r="F80" s="6"/>
@@ -4235,18 +4263,18 @@
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5"/>
-      <c r="F84" s="98"/>
-      <c r="G84" s="98"/>
+      <c r="F84" s="110"/>
+      <c r="G84" s="110"/>
       <c r="H84" s="6"/>
       <c r="I84" s="37" t="s">
         <v>55</v>
       </c>
       <c r="J84" s="37"/>
       <c r="K84" s="6"/>
-      <c r="L84" s="95" t="s">
+      <c r="L84" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="M84" s="95"/>
+      <c r="M84" s="108"/>
       <c r="N84" s="39"/>
       <c r="O84" s="5"/>
       <c r="P84" s="5"/>
@@ -4272,93 +4300,94 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C87" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C88" s="4" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C89" s="4" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C90" s="84" t="s">
-        <v>169</v>
+      <c r="C90" s="82" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C91" s="84" t="s">
-        <v>209</v>
+      <c r="C91" s="82" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C92" s="84" t="s">
-        <v>222</v>
+      <c r="C92" s="82" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C93" s="84" t="s">
-        <v>252</v>
+      <c r="C93" s="82" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C94" s="84" t="s">
-        <v>286</v>
+      <c r="C94" s="82" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C95" s="84" t="s">
-        <v>287</v>
+      <c r="C95" s="82" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C96" s="84" t="s">
-        <v>288</v>
+      <c r="C96" s="82" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C97" s="84" t="s">
-        <v>227</v>
+      <c r="C97" s="82" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C98" s="84" t="s">
-        <v>228</v>
+      <c r="C98" s="82" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C99" s="84"/>
+      <c r="C99" s="82"/>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C100" s="84"/>
+      <c r="C100" s="82"/>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C101" s="84"/>
+      <c r="C101" s="82"/>
     </row>
     <row r="102" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C102" s="84"/>
+      <c r="C102" s="82"/>
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C103" s="84"/>
+      <c r="C103" s="82"/>
     </row>
     <row r="104" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C104" s="83"/>
+      <c r="C104" s="81"/>
     </row>
     <row r="105" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C105" s="83"/>
+      <c r="C105" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B2:O3"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="E6:K6"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="L84:M84"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="C79:C80"/>
     <mergeCell ref="C65:C66"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C21:C22"/>
@@ -4375,13 +4404,12 @@
     <mergeCell ref="C58:C59"/>
     <mergeCell ref="C33:C34"/>
     <mergeCell ref="C61:C62"/>
-    <mergeCell ref="L84:M84"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B2:O3"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="C11:C12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4412,46 +4440,46 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="112" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="57"/>
       <c r="D3" s="57"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="111"/>
+      <c r="A4" s="112"/>
       <c r="B4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="112"/>
+      <c r="B5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="111"/>
-      <c r="B5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -4465,19 +4493,19 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="60" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="60" t="s">
-        <v>100</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -4500,7 +4528,7 @@
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4510,65 +4538,68 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C1" s="68"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" s="59"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C3" s="58"/>
       <c r="E3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C5" s="65"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C6" s="66"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C7" s="67"/>
+      <c r="E7" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C10" s="69"/>
       <c r="D10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C11" s="70"/>
       <c r="D11">
@@ -4577,7 +4608,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C12" s="71"/>
       <c r="D12">
@@ -4586,7 +4617,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C13" s="67"/>
       <c r="D13">
@@ -4595,7 +4626,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -4603,12 +4634,12 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C40" s="54"/>
     </row>
@@ -4714,10 +4745,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H59"/>
+  <dimension ref="B2:H57"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4736,883 +4767,942 @@
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="40"/>
       <c r="C2" s="41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F2" s="41" t="s">
         <v>35</v>
       </c>
       <c r="G2" s="41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H2" s="41" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="115" t="s">
         <v>39</v>
       </c>
       <c r="C3" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="E3" s="44" t="s">
         <v>60</v>
-      </c>
-      <c r="E3" s="44" t="s">
-        <v>61</v>
       </c>
       <c r="F3" s="44"/>
       <c r="G3" s="44" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="H3" s="44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="124"/>
-      <c r="C4" s="126" t="s">
+      <c r="B4" s="116"/>
+      <c r="C4" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="126" t="s">
+      <c r="D4" s="119" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="44" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="F4" s="44"/>
       <c r="G4" s="44"/>
       <c r="H4" s="44" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="124"/>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
+      <c r="B5" s="116"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="116"/>
       <c r="E5" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="116"/>
+      <c r="C6" s="116"/>
+      <c r="D6" s="116"/>
+      <c r="E6" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="F6" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="G5" s="44" t="s">
+      <c r="G6" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="H5" s="44" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="124"/>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="F6" s="44" t="s">
-        <v>122</v>
-      </c>
-      <c r="G6" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="H6" s="44" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="125"/>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
+      <c r="B7" s="117"/>
+      <c r="C7" s="117"/>
+      <c r="D7" s="117"/>
       <c r="E7" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="F7" s="44" t="s">
-        <v>101</v>
-      </c>
-      <c r="G7" s="44" t="s">
-        <v>118</v>
-      </c>
       <c r="H7" s="44" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="55"/>
       <c r="C8" s="56" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="D8" s="56" t="s">
-        <v>108</v>
-      </c>
       <c r="E8" s="44" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F8" s="44" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G8" s="44" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="H8" s="44" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="63"/>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82" t="s">
-        <v>207</v>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80" t="s">
+        <v>200</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="F9" s="44"/>
       <c r="G9" s="44" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="H9" s="44" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="81"/>
-      <c r="C10" s="82"/>
-      <c r="D10" s="85" t="s">
-        <v>219</v>
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="83" t="s">
+        <v>212</v>
       </c>
       <c r="E10" s="44" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F10" s="44"/>
       <c r="G10" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="H10" s="44" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80" t="s">
+        <v>211</v>
+      </c>
+      <c r="E11" s="44" t="s">
         <v>225</v>
       </c>
-      <c r="H10" s="44" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="81"/>
-      <c r="C11" s="82"/>
-      <c r="D11" s="82" t="s">
-        <v>218</v>
-      </c>
-      <c r="E11" s="44" t="s">
-        <v>232</v>
-      </c>
       <c r="F11" s="44" t="s">
+        <v>210</v>
+      </c>
+      <c r="G11" s="44" t="s">
         <v>217</v>
       </c>
-      <c r="G11" s="44" t="s">
-        <v>224</v>
-      </c>
       <c r="H11" s="44" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="88"/>
-      <c r="C12" s="89"/>
-      <c r="D12" s="94" t="s">
-        <v>280</v>
+      <c r="B12" s="86"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="92" t="s">
+        <v>273</v>
       </c>
       <c r="E12" s="44" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F12" s="44" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="G12" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="H12" s="44" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="91"/>
+      <c r="C13" s="92"/>
+      <c r="D13" s="87" t="s">
         <v>278</v>
       </c>
-      <c r="H12" s="44" t="s">
+      <c r="E13" s="44" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="93"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="94"/>
-      <c r="E13" s="44"/>
       <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
+      <c r="G13" s="44" t="s">
+        <v>276</v>
+      </c>
+      <c r="H13" s="44" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="88"/>
-      <c r="C14" s="89"/>
-      <c r="D14" s="89" t="s">
-        <v>285</v>
-      </c>
-      <c r="E14" s="44" t="s">
-        <v>284</v>
-      </c>
+      <c r="B14" s="86"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="44"/>
       <c r="F14" s="44"/>
-      <c r="G14" s="44" t="s">
-        <v>283</v>
-      </c>
-      <c r="H14" s="44" t="s">
-        <v>282</v>
-      </c>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="88"/>
-      <c r="C15" s="89"/>
-      <c r="D15" s="89"/>
+      <c r="B15" s="86"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="87"/>
       <c r="E15" s="44"/>
       <c r="F15" s="44"/>
       <c r="G15" s="44"/>
       <c r="H15" s="44"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="81"/>
-      <c r="C16" s="82"/>
-      <c r="D16" s="89" t="s">
-        <v>273</v>
+      <c r="B16" s="79"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="87" t="s">
+        <v>266</v>
       </c>
       <c r="E16" s="44" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="F16" s="44"/>
       <c r="G16" s="44" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="H16" s="44" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="55"/>
-      <c r="C17" s="89"/>
-      <c r="D17" s="89"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="87"/>
       <c r="E17" s="44"/>
       <c r="F17" s="44"/>
       <c r="G17" s="44"/>
       <c r="H17" s="44"/>
     </row>
     <row r="18" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="118" t="s">
+      <c r="B18" s="124" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="116" t="s">
+      <c r="C18" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="122" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="116" t="s">
-        <v>64</v>
-      </c>
       <c r="E18" s="46" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F18" s="46"/>
       <c r="G18" s="46"/>
       <c r="H18" s="46" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="119"/>
-      <c r="C19" s="117"/>
-      <c r="D19" s="117"/>
+      <c r="B19" s="125"/>
+      <c r="C19" s="123"/>
+      <c r="D19" s="123"/>
       <c r="E19" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="G19" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="H19" s="47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="125"/>
+      <c r="C20" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="G19" s="46" t="s">
+      <c r="D20" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="46" t="s">
         <v>141</v>
-      </c>
-      <c r="H19" s="47" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="119"/>
-      <c r="C20" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="46" t="s">
-        <v>143</v>
       </c>
       <c r="F20" s="46"/>
       <c r="G20" s="46" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H20" s="47" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="125"/>
+      <c r="C21" s="122" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="122" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="46" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="119"/>
-      <c r="C21" s="116" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="116" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="46" t="s">
-        <v>144</v>
       </c>
       <c r="F21" s="46"/>
       <c r="G21" s="46"/>
       <c r="H21" s="46" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="125"/>
+      <c r="C22" s="123"/>
+      <c r="D22" s="123"/>
+      <c r="E22" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="F22" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="G22" s="46" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="119"/>
-      <c r="C22" s="117"/>
-      <c r="D22" s="117"/>
-      <c r="E22" s="46" t="s">
+      <c r="H22" s="46" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="125"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="94" t="s">
+        <v>290</v>
+      </c>
+      <c r="E23" s="47" t="s">
+        <v>292</v>
+      </c>
+      <c r="F23" s="47" t="s">
+        <v>291</v>
+      </c>
+      <c r="G23" s="47" t="s">
+        <v>293</v>
+      </c>
+      <c r="H23" s="47" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="125"/>
+      <c r="C24" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="47" t="s">
+        <v>257</v>
+      </c>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="F22" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="G22" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="H22" s="46" t="s">
+      <c r="H24" s="47" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="125"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="94"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="125"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="125"/>
+      <c r="C27" s="47" t="s">
+        <v>254</v>
+      </c>
+      <c r="D27" s="88" t="s">
+        <v>227</v>
+      </c>
+      <c r="E27" s="47" t="s">
+        <v>229</v>
+      </c>
+      <c r="F27" s="47" t="s">
+        <v>228</v>
+      </c>
+      <c r="G27" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="H27" s="47" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="125"/>
+      <c r="C28" s="47" t="s">
+        <v>253</v>
+      </c>
+      <c r="D28" s="88" t="s">
+        <v>236</v>
+      </c>
+      <c r="E28" s="47" t="s">
+        <v>232</v>
+      </c>
+      <c r="F28" s="47" t="s">
+        <v>237</v>
+      </c>
+      <c r="G28" s="47" t="s">
+        <v>233</v>
+      </c>
+      <c r="H28" s="47" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B29" s="125"/>
+      <c r="C29" s="47" t="s">
+        <v>255</v>
+      </c>
+      <c r="D29" s="88" t="s">
+        <v>235</v>
+      </c>
+      <c r="E29" s="47" t="s">
+        <v>238</v>
+      </c>
+      <c r="F29" s="90" t="s">
+        <v>240</v>
+      </c>
+      <c r="G29" s="47" t="s">
+        <v>239</v>
+      </c>
+      <c r="H29" s="47" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="125"/>
+      <c r="C30" s="47" t="s">
+        <v>256</v>
+      </c>
+      <c r="D30" s="47" t="s">
+        <v>249</v>
+      </c>
+      <c r="E30" s="47" t="s">
+        <v>241</v>
+      </c>
+      <c r="F30" s="47" t="s">
+        <v>242</v>
+      </c>
+      <c r="G30" s="47" t="s">
+        <v>243</v>
+      </c>
+      <c r="H30" s="47" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="125"/>
+      <c r="C31" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="72" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="72" t="s">
+        <v>263</v>
+      </c>
+      <c r="F31" s="72" t="s">
+        <v>150</v>
+      </c>
+      <c r="G31" s="72" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="119"/>
-      <c r="C23" s="47" t="s">
+      <c r="H31" s="72" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="125"/>
+      <c r="C32" s="113" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="113" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="113" t="s">
+        <v>157</v>
+      </c>
+      <c r="F32" s="126" t="s">
+        <v>158</v>
+      </c>
+      <c r="G32" s="126" t="s">
+        <v>216</v>
+      </c>
+      <c r="H32" s="113" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33" s="125"/>
+      <c r="C33" s="114"/>
+      <c r="D33" s="114"/>
+      <c r="E33" s="114"/>
+      <c r="F33" s="127"/>
+      <c r="G33" s="127"/>
+      <c r="H33" s="114"/>
+    </row>
+    <row r="34" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B34" s="125"/>
+      <c r="C34" s="78" t="s">
+        <v>250</v>
+      </c>
+      <c r="D34" s="76" t="s">
+        <v>154</v>
+      </c>
+      <c r="E34" s="75" t="s">
+        <v>155</v>
+      </c>
+      <c r="F34" s="74" t="s">
+        <v>189</v>
+      </c>
+      <c r="G34" s="75" t="s">
+        <v>156</v>
+      </c>
+      <c r="H34" s="75" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B35" s="125"/>
+      <c r="C35" s="113" t="s">
+        <v>251</v>
+      </c>
+      <c r="D35" s="113" t="s">
+        <v>160</v>
+      </c>
+      <c r="E35" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="F35" s="74" t="s">
+        <v>187</v>
+      </c>
+      <c r="G35" s="75" t="s">
+        <v>166</v>
+      </c>
+      <c r="H35" s="72" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B36" s="125"/>
+      <c r="C36" s="114"/>
+      <c r="D36" s="114"/>
+      <c r="E36" s="77" t="s">
+        <v>163</v>
+      </c>
+      <c r="F36" s="74" t="s">
+        <v>188</v>
+      </c>
+      <c r="G36" s="75" t="s">
+        <v>164</v>
+      </c>
+      <c r="H36" s="75" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="B37" s="125"/>
+      <c r="C37" s="73" t="s">
+        <v>252</v>
+      </c>
+      <c r="D37" s="78" t="s">
+        <v>159</v>
+      </c>
+      <c r="E37" s="77" t="s">
+        <v>169</v>
+      </c>
+      <c r="F37" s="74" t="s">
+        <v>186</v>
+      </c>
+      <c r="G37" s="77" t="s">
+        <v>170</v>
+      </c>
+      <c r="H37" s="77" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38" s="125"/>
+      <c r="C38" s="118" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="118" t="s">
+        <v>45</v>
+      </c>
+      <c r="E38" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="47" t="s">
+      <c r="F38" s="48"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="48" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B39" s="125"/>
+      <c r="C39" s="118"/>
+      <c r="D39" s="118"/>
+      <c r="E39" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="F39" s="74" t="s">
+        <v>184</v>
+      </c>
+      <c r="G39" s="48" t="s">
+        <v>173</v>
+      </c>
+      <c r="H39" s="48" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B40" s="125"/>
+      <c r="C40" s="113" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="113" t="s">
+        <v>52</v>
+      </c>
+      <c r="E40" s="72" t="s">
+        <v>174</v>
+      </c>
+      <c r="F40" s="74" t="s">
+        <v>181</v>
+      </c>
+      <c r="G40" s="72" t="s">
+        <v>175</v>
+      </c>
+      <c r="H40" s="72" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B41" s="125"/>
+      <c r="C41" s="114"/>
+      <c r="D41" s="114"/>
+      <c r="E41" s="72" t="s">
+        <v>176</v>
+      </c>
+      <c r="F41" s="74" t="s">
+        <v>182</v>
+      </c>
+      <c r="G41" s="72" t="s">
+        <v>180</v>
+      </c>
+      <c r="H41" s="72" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B42" s="125"/>
+      <c r="C42" s="77" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="77" t="s">
+        <v>51</v>
+      </c>
+      <c r="E42" s="77" t="s">
+        <v>72</v>
+      </c>
+      <c r="F42" s="74" t="s">
+        <v>183</v>
+      </c>
+      <c r="G42" s="77" t="s">
+        <v>185</v>
+      </c>
+      <c r="H42" s="77" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B43" s="125"/>
+      <c r="C43" s="113" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" s="113" t="s">
+        <v>50</v>
+      </c>
+      <c r="E43" s="72" t="s">
+        <v>190</v>
+      </c>
+      <c r="F43" s="74" t="s">
+        <v>195</v>
+      </c>
+      <c r="G43" s="72" t="s">
+        <v>194</v>
+      </c>
+      <c r="H43" s="72" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B44" s="125"/>
+      <c r="C44" s="114"/>
+      <c r="D44" s="114"/>
+      <c r="E44" s="72" t="s">
+        <v>196</v>
+      </c>
+      <c r="F44" s="74" t="s">
+        <v>191</v>
+      </c>
+      <c r="G44" s="72" t="s">
+        <v>197</v>
+      </c>
+      <c r="H44" s="72" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B45" s="120"/>
+      <c r="C45" s="89"/>
+      <c r="D45" s="89" t="s">
+        <v>258</v>
+      </c>
+      <c r="E45" s="45" t="s">
+        <v>259</v>
+      </c>
+      <c r="F45" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="G45" s="45" t="s">
+        <v>260</v>
+      </c>
+      <c r="H45" s="45" t="s">
         <v>264</v>
       </c>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="H23" s="47" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="119"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="90"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="119"/>
-      <c r="C25" s="47" t="s">
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B46" s="120"/>
+      <c r="C46" s="61"/>
+      <c r="D46" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="E46" s="89" t="s">
         <v>261</v>
       </c>
-      <c r="D25" s="90" t="s">
-        <v>234</v>
-      </c>
-      <c r="E25" s="47" t="s">
-        <v>236</v>
-      </c>
-      <c r="F25" s="47" t="s">
-        <v>235</v>
-      </c>
-      <c r="G25" s="47" t="s">
-        <v>237</v>
-      </c>
-      <c r="H25" s="47" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="119"/>
-      <c r="C26" s="47" t="s">
-        <v>260</v>
-      </c>
-      <c r="D26" s="90" t="s">
-        <v>243</v>
-      </c>
-      <c r="E26" s="47" t="s">
-        <v>239</v>
-      </c>
-      <c r="F26" s="47" t="s">
-        <v>244</v>
-      </c>
-      <c r="G26" s="47" t="s">
-        <v>240</v>
-      </c>
-      <c r="H26" s="47" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B27" s="119"/>
-      <c r="C27" s="47" t="s">
+      <c r="F46" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="G46" s="45" t="s">
         <v>262</v>
       </c>
-      <c r="D27" s="90" t="s">
-        <v>242</v>
-      </c>
-      <c r="E27" s="47" t="s">
-        <v>245</v>
-      </c>
-      <c r="F27" s="92" t="s">
-        <v>247</v>
-      </c>
-      <c r="G27" s="47" t="s">
-        <v>246</v>
-      </c>
-      <c r="H27" s="47" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="119"/>
-      <c r="C28" s="47" t="s">
-        <v>263</v>
-      </c>
-      <c r="D28" s="47" t="s">
-        <v>256</v>
-      </c>
-      <c r="E28" s="47" t="s">
-        <v>248</v>
-      </c>
-      <c r="F28" s="47" t="s">
-        <v>249</v>
-      </c>
-      <c r="G28" s="47" t="s">
-        <v>250</v>
-      </c>
-      <c r="H28" s="47" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="119"/>
-      <c r="C29" s="72" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="72" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" s="72" t="s">
-        <v>270</v>
-      </c>
-      <c r="F29" s="72" t="s">
-        <v>152</v>
-      </c>
-      <c r="G29" s="72" t="s">
-        <v>151</v>
-      </c>
-      <c r="H29" s="72" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="119"/>
-      <c r="C30" s="112" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="112" t="s">
-        <v>47</v>
-      </c>
-      <c r="E30" s="112" t="s">
-        <v>159</v>
-      </c>
-      <c r="F30" s="120" t="s">
-        <v>161</v>
-      </c>
-      <c r="G30" s="120" t="s">
-        <v>223</v>
-      </c>
-      <c r="H30" s="112" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="119"/>
-      <c r="C31" s="113"/>
-      <c r="D31" s="113"/>
-      <c r="E31" s="113"/>
-      <c r="F31" s="121"/>
-      <c r="G31" s="121"/>
-      <c r="H31" s="113"/>
-    </row>
-    <row r="32" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B32" s="119"/>
-      <c r="C32" s="80" t="s">
-        <v>257</v>
-      </c>
-      <c r="D32" s="78" t="s">
-        <v>156</v>
-      </c>
-      <c r="E32" s="77" t="s">
-        <v>157</v>
-      </c>
-      <c r="F32" s="76" t="s">
-        <v>196</v>
-      </c>
-      <c r="G32" s="77" t="s">
-        <v>158</v>
-      </c>
-      <c r="H32" s="77" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B33" s="119"/>
-      <c r="C33" s="112" t="s">
-        <v>258</v>
-      </c>
-      <c r="D33" s="112" t="s">
-        <v>164</v>
-      </c>
-      <c r="E33" s="79" t="s">
-        <v>165</v>
-      </c>
-      <c r="F33" s="76" t="s">
-        <v>194</v>
-      </c>
-      <c r="G33" s="77" t="s">
-        <v>171</v>
-      </c>
-      <c r="H33" s="72" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B34" s="119"/>
-      <c r="C34" s="113"/>
-      <c r="D34" s="113"/>
-      <c r="E34" s="79" t="s">
-        <v>167</v>
-      </c>
-      <c r="F34" s="76" t="s">
-        <v>195</v>
-      </c>
-      <c r="G34" s="77" t="s">
-        <v>168</v>
-      </c>
-      <c r="H34" s="77" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" ht="66" x14ac:dyDescent="0.3">
-      <c r="B35" s="119"/>
-      <c r="C35" s="73" t="s">
-        <v>259</v>
-      </c>
-      <c r="D35" s="80" t="s">
-        <v>163</v>
-      </c>
-      <c r="E35" s="79" t="s">
-        <v>176</v>
-      </c>
-      <c r="F35" s="76" t="s">
-        <v>193</v>
-      </c>
-      <c r="G35" s="79" t="s">
-        <v>177</v>
-      </c>
-      <c r="H35" s="79" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="119"/>
-      <c r="C36" s="122" t="s">
-        <v>41</v>
-      </c>
-      <c r="D36" s="122" t="s">
-        <v>45</v>
-      </c>
-      <c r="E36" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="F36" s="48"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="48" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="119"/>
-      <c r="C37" s="122"/>
-      <c r="D37" s="122"/>
-      <c r="E37" s="48" t="s">
-        <v>179</v>
-      </c>
-      <c r="F37" s="76" t="s">
-        <v>191</v>
-      </c>
-      <c r="G37" s="48" t="s">
-        <v>180</v>
-      </c>
-      <c r="H37" s="48" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B38" s="119"/>
-      <c r="C38" s="112" t="s">
-        <v>44</v>
-      </c>
-      <c r="D38" s="112" t="s">
-        <v>52</v>
-      </c>
-      <c r="E38" s="72" t="s">
-        <v>181</v>
-      </c>
-      <c r="F38" s="76" t="s">
-        <v>188</v>
-      </c>
-      <c r="G38" s="72" t="s">
-        <v>182</v>
-      </c>
-      <c r="H38" s="72" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B39" s="119"/>
-      <c r="C39" s="113"/>
-      <c r="D39" s="113"/>
-      <c r="E39" s="72" t="s">
-        <v>183</v>
-      </c>
-      <c r="F39" s="76" t="s">
-        <v>189</v>
-      </c>
-      <c r="G39" s="72" t="s">
-        <v>187</v>
-      </c>
-      <c r="H39" s="72" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B40" s="119"/>
-      <c r="C40" s="79" t="s">
-        <v>48</v>
-      </c>
-      <c r="D40" s="79" t="s">
-        <v>51</v>
-      </c>
-      <c r="E40" s="79" t="s">
-        <v>73</v>
-      </c>
-      <c r="F40" s="76" t="s">
-        <v>190</v>
-      </c>
-      <c r="G40" s="79" t="s">
-        <v>192</v>
-      </c>
-      <c r="H40" s="79" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B41" s="119"/>
-      <c r="C41" s="112" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="112" t="s">
-        <v>50</v>
-      </c>
-      <c r="E41" s="72" t="s">
-        <v>197</v>
-      </c>
-      <c r="F41" s="76" t="s">
-        <v>202</v>
-      </c>
-      <c r="G41" s="72" t="s">
-        <v>201</v>
-      </c>
-      <c r="H41" s="72" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B42" s="119"/>
-      <c r="C42" s="113"/>
-      <c r="D42" s="113"/>
-      <c r="E42" s="72" t="s">
-        <v>203</v>
-      </c>
-      <c r="F42" s="76" t="s">
-        <v>198</v>
-      </c>
-      <c r="G42" s="72" t="s">
-        <v>204</v>
-      </c>
-      <c r="H42" s="72" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B43" s="114"/>
-      <c r="C43" s="91"/>
-      <c r="D43" s="91" t="s">
+      <c r="H46" s="45" t="s">
         <v>265</v>
       </c>
-      <c r="E43" s="45" t="s">
-        <v>266</v>
-      </c>
-      <c r="F43" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="G43" s="45" t="s">
-        <v>267</v>
-      </c>
-      <c r="H43" s="45" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B44" s="114"/>
-      <c r="C44" s="61"/>
-      <c r="D44" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="E44" s="91" t="s">
-        <v>268</v>
-      </c>
-      <c r="F44" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="G44" s="45" t="s">
-        <v>269</v>
-      </c>
-      <c r="H44" s="45" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B45" s="115"/>
-      <c r="C45" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="64"/>
-      <c r="E45" s="91"/>
-      <c r="F45" s="91"/>
-      <c r="G45" s="91"/>
-      <c r="H45" s="91"/>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B46" s="62"/>
-      <c r="C46" s="64"/>
-      <c r="D46" s="64"/>
-      <c r="E46" s="61"/>
-      <c r="F46" s="61"/>
-      <c r="G46" s="61"/>
-      <c r="H46" s="61"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B47" s="62"/>
-      <c r="C47" s="64"/>
-      <c r="D47" s="64" t="s">
-        <v>110</v>
-      </c>
-      <c r="E47" s="61"/>
-      <c r="F47" s="61"/>
-      <c r="G47" s="61"/>
-      <c r="H47" s="61"/>
+      <c r="B47" s="121"/>
+      <c r="C47" s="45"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="89"/>
+      <c r="F47" s="89"/>
+      <c r="G47" s="89"/>
+      <c r="H47" s="89"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B48" s="62"/>
       <c r="C48" s="64"/>
-      <c r="D48" s="64" t="s">
-        <v>111</v>
-      </c>
+      <c r="D48" s="64"/>
       <c r="E48" s="61"/>
       <c r="F48" s="61"/>
       <c r="G48" s="61"/>
       <c r="H48" s="61"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B49" s="62"/>
+      <c r="B49" s="93"/>
       <c r="C49" s="64"/>
-      <c r="D49" s="64" t="s">
-        <v>112</v>
-      </c>
-      <c r="E49" s="61"/>
-      <c r="F49" s="61"/>
-      <c r="G49" s="61"/>
-      <c r="H49" s="61"/>
+      <c r="D49" s="64"/>
+      <c r="E49" s="89"/>
+      <c r="F49" s="89"/>
+      <c r="G49" s="89"/>
+      <c r="H49" s="89"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B50" s="62"/>
       <c r="C50" s="64"/>
       <c r="D50" s="64" t="s">
-        <v>113</v>
-      </c>
-      <c r="E50" s="61"/>
+        <v>296</v>
+      </c>
+      <c r="E50" s="61" t="s">
+        <v>298</v>
+      </c>
       <c r="F50" s="61"/>
-      <c r="G50" s="61"/>
-      <c r="H50" s="61"/>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B51" s="62"/>
+      <c r="G50" s="89"/>
+      <c r="H50" s="89" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B51" s="93"/>
       <c r="C51" s="64"/>
-      <c r="D51" s="64"/>
-      <c r="E51" s="61"/>
-      <c r="F51" s="61"/>
-      <c r="G51" s="61"/>
-      <c r="H51" s="61"/>
-    </row>
-    <row r="59" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="D59" s="75" t="s">
-        <v>160</v>
-      </c>
-      <c r="E59" s="77" t="s">
-        <v>173</v>
-      </c>
-      <c r="F59" s="76" t="s">
-        <v>162</v>
-      </c>
-      <c r="G59" s="77" t="s">
-        <v>170</v>
-      </c>
-      <c r="H59" s="74" t="s">
-        <v>172</v>
-      </c>
+      <c r="D51" s="64" t="s">
+        <v>300</v>
+      </c>
+      <c r="E51" s="89" t="s">
+        <v>299</v>
+      </c>
+      <c r="F51" s="128" t="s">
+        <v>301</v>
+      </c>
+      <c r="G51" s="89" t="s">
+        <v>295</v>
+      </c>
+      <c r="H51" s="89" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B52" s="93"/>
+      <c r="C52" s="64"/>
+      <c r="D52" s="64"/>
+      <c r="E52" s="89"/>
+      <c r="F52" s="89"/>
+      <c r="G52" s="89"/>
+      <c r="H52" s="89"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B53" s="93"/>
+      <c r="C53" s="64"/>
+      <c r="D53" s="64"/>
+      <c r="E53" s="89"/>
+      <c r="F53" s="89"/>
+      <c r="G53" s="89"/>
+      <c r="H53" s="89"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B54" s="62"/>
+      <c r="C54" s="64"/>
+      <c r="D54" s="64" t="s">
+        <v>109</v>
+      </c>
+      <c r="E54" s="61"/>
+      <c r="F54" s="61"/>
+      <c r="G54" s="61"/>
+      <c r="H54" s="61"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B55" s="62"/>
+      <c r="C55" s="64"/>
+      <c r="D55" s="64" t="s">
+        <v>110</v>
+      </c>
+      <c r="E55" s="61"/>
+      <c r="F55" s="61"/>
+      <c r="G55" s="61"/>
+      <c r="H55" s="61"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B56" s="62"/>
+      <c r="C56" s="64"/>
+      <c r="D56" s="64" t="s">
+        <v>111</v>
+      </c>
+      <c r="E56" s="61"/>
+      <c r="F56" s="61"/>
+      <c r="G56" s="61"/>
+      <c r="H56" s="61"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B57" s="62"/>
+      <c r="C57" s="64"/>
+      <c r="D57" s="64"/>
+      <c r="E57" s="61"/>
+      <c r="F57" s="61"/>
+      <c r="G57" s="61"/>
+      <c r="H57" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="B18:B44"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="C32:C33"/>
     <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C38:C39"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="D4:D7"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="B18:B42"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C33:C34"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Auto push 2023-03-29 23:04:00.21
</commit_message>
<xml_diff>
--- a/project/CheeYoonMovie.xlsx
+++ b/project/CheeYoonMovie.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="303">
   <si>
     <t>이용자 권한과 기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1203,22 +1203,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RegisterMovie.java</t>
-  </si>
-  <si>
     <t>등록페이지</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>admin/insert.jsp</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insertView.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insertMovie.do</t>
   </si>
   <si>
     <t>영화등록처리</t>
@@ -1227,6 +1217,22 @@
   <si>
     <t>MovieDto속성들
 tagDto 여러개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RegisterMovie.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RegisterMovie.java</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2053,6 +2059,33 @@
     <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2077,30 +2110,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2110,6 +2119,33 @@
     <xf numFmtId="0" fontId="11" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2119,38 +2155,8 @@
     <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2520,41 +2526,41 @@
     <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="106" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="107"/>
+      <c r="G2" s="107"/>
+      <c r="H2" s="107"/>
+      <c r="I2" s="107"/>
+      <c r="J2" s="107"/>
+      <c r="K2" s="107"/>
+      <c r="L2" s="107"/>
+      <c r="M2" s="107"/>
+      <c r="N2" s="107"/>
+      <c r="O2" s="107"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
+      <c r="B3" s="107"/>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="107"/>
+      <c r="H3" s="107"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
+      <c r="K3" s="107"/>
+      <c r="L3" s="107"/>
+      <c r="M3" s="107"/>
+      <c r="N3" s="107"/>
+      <c r="O3" s="107"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
@@ -2599,32 +2605,32 @@
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20"/>
-      <c r="C6" s="99" t="s">
+      <c r="C6" s="108" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="38"/>
-      <c r="E6" s="101" t="s">
+      <c r="E6" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="101"/>
-      <c r="G6" s="101"/>
-      <c r="H6" s="101"/>
-      <c r="I6" s="101"/>
-      <c r="J6" s="101"/>
-      <c r="K6" s="102"/>
-      <c r="L6" s="103" t="s">
+      <c r="F6" s="110"/>
+      <c r="G6" s="110"/>
+      <c r="H6" s="110"/>
+      <c r="I6" s="110"/>
+      <c r="J6" s="110"/>
+      <c r="K6" s="111"/>
+      <c r="L6" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="101"/>
-      <c r="N6" s="101"/>
-      <c r="O6" s="101"/>
+      <c r="M6" s="110"/>
+      <c r="N6" s="110"/>
+      <c r="O6" s="110"/>
       <c r="P6" s="21"/>
       <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="100"/>
+      <c r="C7" s="109"/>
       <c r="D7" s="22"/>
       <c r="E7" s="84">
         <v>20</v>
@@ -2724,7 +2730,7 @@
     <row r="11" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="104" t="s">
+      <c r="C11" s="102" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="10"/>
@@ -2745,7 +2751,7 @@
     <row r="12" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="104"/>
+      <c r="C12" s="102"/>
       <c r="D12" s="10"/>
       <c r="E12" s="8"/>
       <c r="F12" s="6"/>
@@ -2783,7 +2789,7 @@
     <row r="14" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="96" t="s">
+      <c r="C14" s="105" t="s">
         <v>32</v>
       </c>
       <c r="D14" s="10"/>
@@ -2804,7 +2810,7 @@
     <row r="15" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="96"/>
+      <c r="C15" s="105"/>
       <c r="D15" s="10"/>
       <c r="E15" s="8"/>
       <c r="F15" s="6"/>
@@ -2842,7 +2848,7 @@
     <row r="17" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="104" t="s">
+      <c r="C17" s="102" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="10"/>
@@ -2863,7 +2869,7 @@
     <row r="18" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="104"/>
+      <c r="C18" s="102"/>
       <c r="D18" s="10"/>
       <c r="E18" s="8"/>
       <c r="F18" s="6"/>
@@ -2922,7 +2928,7 @@
     <row r="21" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="106" t="s">
+      <c r="C21" s="103" t="s">
         <v>201</v>
       </c>
       <c r="D21" s="10"/>
@@ -2943,7 +2949,7 @@
     <row r="22" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="106"/>
+      <c r="C22" s="103"/>
       <c r="D22" s="10"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
@@ -2981,7 +2987,7 @@
     <row r="24" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="106" t="s">
+      <c r="C24" s="103" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="10"/>
@@ -3002,7 +3008,7 @@
     <row r="25" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="106"/>
+      <c r="C25" s="103"/>
       <c r="D25" s="10"/>
       <c r="E25" s="6"/>
       <c r="F25" s="8"/>
@@ -3040,7 +3046,7 @@
     <row r="27" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="106" t="s">
+      <c r="C27" s="103" t="s">
         <v>78</v>
       </c>
       <c r="D27" s="10"/>
@@ -3061,7 +3067,7 @@
     <row r="28" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="106"/>
+      <c r="C28" s="103"/>
       <c r="D28" s="10"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -3099,7 +3105,7 @@
     <row r="30" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="106" t="s">
+      <c r="C30" s="103" t="s">
         <v>79</v>
       </c>
       <c r="D30" s="10"/>
@@ -3120,7 +3126,7 @@
     <row r="31" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="106"/>
+      <c r="C31" s="103"/>
       <c r="D31" s="10"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -3158,7 +3164,7 @@
     <row r="33" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="106" t="s">
+      <c r="C33" s="103" t="s">
         <v>207</v>
       </c>
       <c r="D33" s="10"/>
@@ -3179,7 +3185,7 @@
     <row r="34" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="6"/>
-      <c r="C34" s="106"/>
+      <c r="C34" s="103"/>
       <c r="D34" s="10"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -3217,7 +3223,7 @@
     <row r="36" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="16"/>
       <c r="B36" s="6"/>
-      <c r="C36" s="106" t="s">
+      <c r="C36" s="103" t="s">
         <v>80</v>
       </c>
       <c r="D36" s="10"/>
@@ -3238,7 +3244,7 @@
     <row r="37" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
       <c r="B37" s="6"/>
-      <c r="C37" s="106"/>
+      <c r="C37" s="103"/>
       <c r="D37" s="10"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
@@ -3297,7 +3303,7 @@
     <row r="40" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="6"/>
-      <c r="C40" s="107" t="s">
+      <c r="C40" s="104" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="10"/>
@@ -3318,7 +3324,7 @@
     <row r="41" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="107"/>
+      <c r="C41" s="104"/>
       <c r="D41" s="10"/>
       <c r="E41" s="6"/>
       <c r="F41" s="8"/>
@@ -3356,7 +3362,7 @@
     <row r="43" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="16"/>
       <c r="B43" s="6"/>
-      <c r="C43" s="107" t="s">
+      <c r="C43" s="104" t="s">
         <v>203</v>
       </c>
       <c r="D43" s="10"/>
@@ -3377,7 +3383,7 @@
     <row r="44" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="107"/>
+      <c r="C44" s="104"/>
       <c r="D44" s="10"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
@@ -3415,7 +3421,7 @@
     <row r="46" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16"/>
       <c r="B46" s="6"/>
-      <c r="C46" s="107" t="s">
+      <c r="C46" s="104" t="s">
         <v>205</v>
       </c>
       <c r="D46" s="10"/>
@@ -3435,7 +3441,7 @@
     <row r="47" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="107"/>
+      <c r="C47" s="104"/>
       <c r="D47" s="10"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
@@ -3473,7 +3479,7 @@
     <row r="49" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="16"/>
       <c r="B49" s="6"/>
-      <c r="C49" s="107" t="s">
+      <c r="C49" s="104" t="s">
         <v>283</v>
       </c>
       <c r="D49" s="10"/>
@@ -3494,7 +3500,7 @@
     <row r="50" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="107"/>
+      <c r="C50" s="104"/>
       <c r="D50" s="10"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
@@ -3532,7 +3538,7 @@
     <row r="52" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="16"/>
       <c r="B52" s="6"/>
-      <c r="C52" s="107" t="s">
+      <c r="C52" s="104" t="s">
         <v>282</v>
       </c>
       <c r="D52" s="10"/>
@@ -3553,7 +3559,7 @@
     <row r="53" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16"/>
       <c r="B53" s="6"/>
-      <c r="C53" s="107"/>
+      <c r="C53" s="104"/>
       <c r="D53" s="10"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
@@ -3591,7 +3597,7 @@
     <row r="55" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="107" t="s">
+      <c r="C55" s="104" t="s">
         <v>206</v>
       </c>
       <c r="D55" s="10"/>
@@ -3611,7 +3617,7 @@
     <row r="56" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="16"/>
       <c r="B56" s="6"/>
-      <c r="C56" s="107"/>
+      <c r="C56" s="104"/>
       <c r="D56" s="10"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
@@ -3649,7 +3655,7 @@
     <row r="58" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="107" t="s">
+      <c r="C58" s="104" t="s">
         <v>204</v>
       </c>
       <c r="D58" s="10"/>
@@ -3670,7 +3676,7 @@
     <row r="59" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="16"/>
       <c r="B59" s="6"/>
-      <c r="C59" s="107"/>
+      <c r="C59" s="104"/>
       <c r="D59" s="10"/>
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
@@ -3708,7 +3714,7 @@
     <row r="61" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="16"/>
       <c r="B61" s="6"/>
-      <c r="C61" s="107" t="s">
+      <c r="C61" s="104" t="s">
         <v>284</v>
       </c>
       <c r="D61" s="10"/>
@@ -3729,7 +3735,7 @@
     <row r="62" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="16"/>
       <c r="B62" s="6"/>
-      <c r="C62" s="107"/>
+      <c r="C62" s="104"/>
       <c r="D62" s="10"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
@@ -3788,7 +3794,7 @@
     <row r="65" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="16"/>
       <c r="B65" s="6"/>
-      <c r="C65" s="105" t="s">
+      <c r="C65" s="98" t="s">
         <v>285</v>
       </c>
       <c r="D65" s="10"/>
@@ -3809,7 +3815,7 @@
     <row r="66" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="16"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="105"/>
+      <c r="C66" s="98"/>
       <c r="D66" s="10"/>
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
@@ -3847,7 +3853,7 @@
     <row r="68" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="16"/>
       <c r="B68" s="6"/>
-      <c r="C68" s="105" t="s">
+      <c r="C68" s="98" t="s">
         <v>286</v>
       </c>
       <c r="D68" s="10"/>
@@ -3868,7 +3874,7 @@
     <row r="69" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="105"/>
+      <c r="C69" s="98"/>
       <c r="D69" s="10"/>
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
@@ -3906,7 +3912,7 @@
     <row r="71" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="16"/>
       <c r="B71" s="6"/>
-      <c r="C71" s="105" t="s">
+      <c r="C71" s="98" t="s">
         <v>287</v>
       </c>
       <c r="D71" s="10"/>
@@ -3927,7 +3933,7 @@
     <row r="72" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16"/>
       <c r="B72" s="6"/>
-      <c r="C72" s="105"/>
+      <c r="C72" s="98"/>
       <c r="D72" s="10"/>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
@@ -3965,7 +3971,7 @@
     <row r="74" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16"/>
       <c r="B74" s="6"/>
-      <c r="C74" s="105" t="s">
+      <c r="C74" s="98" t="s">
         <v>288</v>
       </c>
       <c r="D74" s="10"/>
@@ -3986,7 +3992,7 @@
     <row r="75" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="16"/>
       <c r="B75" s="6"/>
-      <c r="C75" s="105"/>
+      <c r="C75" s="98"/>
       <c r="D75" s="10"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
@@ -4024,7 +4030,7 @@
     <row r="77" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="16"/>
       <c r="B77" s="6"/>
-      <c r="C77" s="109" t="s">
+      <c r="C77" s="99" t="s">
         <v>53</v>
       </c>
       <c r="D77" s="7"/>
@@ -4045,7 +4051,7 @@
     <row r="78" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="16"/>
       <c r="B78" s="6"/>
-      <c r="C78" s="109"/>
+      <c r="C78" s="99"/>
       <c r="D78" s="7"/>
       <c r="E78" s="6"/>
       <c r="F78" s="6"/>
@@ -4064,7 +4070,7 @@
     <row r="79" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="16"/>
       <c r="B79" s="6"/>
-      <c r="C79" s="111" t="s">
+      <c r="C79" s="101" t="s">
         <v>76</v>
       </c>
       <c r="D79" s="7"/>
@@ -4135,7 +4141,7 @@
     <row r="80" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="16"/>
       <c r="B80" s="6"/>
-      <c r="C80" s="111"/>
+      <c r="C80" s="101"/>
       <c r="D80" s="7"/>
       <c r="E80" s="6"/>
       <c r="F80" s="6"/>
@@ -4263,18 +4269,18 @@
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5"/>
-      <c r="F84" s="110"/>
-      <c r="G84" s="110"/>
+      <c r="F84" s="100"/>
+      <c r="G84" s="100"/>
       <c r="H84" s="6"/>
       <c r="I84" s="37" t="s">
         <v>55</v>
       </c>
       <c r="J84" s="37"/>
       <c r="K84" s="6"/>
-      <c r="L84" s="108" t="s">
+      <c r="L84" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="M84" s="108"/>
+      <c r="M84" s="97"/>
       <c r="N84" s="39"/>
       <c r="O84" s="5"/>
       <c r="P84" s="5"/>
@@ -4381,13 +4387,12 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="L84:M84"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B2:O3"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="C11:C12"/>
     <mergeCell ref="C65:C66"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C21:C22"/>
@@ -4404,12 +4409,13 @@
     <mergeCell ref="C58:C59"/>
     <mergeCell ref="C33:C34"/>
     <mergeCell ref="C61:C62"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B2:O3"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="E6:K6"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="L84:M84"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="C79:C80"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4440,7 +4446,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="112" t="s">
+      <c r="A3" s="113" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -4450,7 +4456,7 @@
       <c r="D3" s="57"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="112"/>
+      <c r="A4" s="113"/>
       <c r="B4" s="1" t="s">
         <v>83</v>
       </c>
@@ -4465,7 +4471,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="112"/>
+      <c r="A5" s="113"/>
       <c r="B5" s="1" t="s">
         <v>84</v>
       </c>
@@ -4747,8 +4753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" topLeftCell="B37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4786,7 +4792,7 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="125" t="s">
         <v>39</v>
       </c>
       <c r="C3" s="43" t="s">
@@ -4807,11 +4813,11 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="116"/>
-      <c r="C4" s="119" t="s">
+      <c r="B4" s="126"/>
+      <c r="C4" s="128" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="119" t="s">
+      <c r="D4" s="128" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="44" t="s">
@@ -4824,9 +4830,9 @@
       </c>
     </row>
     <row r="5" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="116"/>
-      <c r="C5" s="116"/>
-      <c r="D5" s="116"/>
+      <c r="B5" s="126"/>
+      <c r="C5" s="126"/>
+      <c r="D5" s="126"/>
       <c r="E5" s="44" t="s">
         <v>102</v>
       </c>
@@ -4841,9 +4847,9 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="116"/>
-      <c r="C6" s="116"/>
-      <c r="D6" s="116"/>
+      <c r="B6" s="126"/>
+      <c r="C6" s="126"/>
+      <c r="D6" s="126"/>
       <c r="E6" s="44" t="s">
         <v>103</v>
       </c>
@@ -4858,9 +4864,9 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="117"/>
-      <c r="C7" s="117"/>
-      <c r="D7" s="117"/>
+      <c r="B7" s="127"/>
+      <c r="C7" s="127"/>
+      <c r="D7" s="127"/>
       <c r="E7" s="44" t="s">
         <v>114</v>
       </c>
@@ -5029,13 +5035,13 @@
       <c r="H17" s="44"/>
     </row>
     <row r="18" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="124" t="s">
+      <c r="B18" s="120" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="122" t="s">
+      <c r="C18" s="118" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="122" t="s">
+      <c r="D18" s="118" t="s">
         <v>63</v>
       </c>
       <c r="E18" s="46" t="s">
@@ -5048,9 +5054,9 @@
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="125"/>
-      <c r="C19" s="123"/>
-      <c r="D19" s="123"/>
+      <c r="B19" s="121"/>
+      <c r="C19" s="119"/>
+      <c r="D19" s="119"/>
       <c r="E19" s="46" t="s">
         <v>64</v>
       </c>
@@ -5065,7 +5071,7 @@
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="125"/>
+      <c r="B20" s="121"/>
       <c r="C20" s="46" t="s">
         <v>65</v>
       </c>
@@ -5084,11 +5090,11 @@
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="125"/>
-      <c r="C21" s="122" t="s">
+      <c r="B21" s="121"/>
+      <c r="C21" s="118" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="122" t="s">
+      <c r="D21" s="118" t="s">
         <v>68</v>
       </c>
       <c r="E21" s="46" t="s">
@@ -5101,9 +5107,9 @@
       </c>
     </row>
     <row r="22" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="125"/>
-      <c r="C22" s="123"/>
-      <c r="D22" s="123"/>
+      <c r="B22" s="121"/>
+      <c r="C22" s="119"/>
+      <c r="D22" s="119"/>
       <c r="E22" s="46" t="s">
         <v>144</v>
       </c>
@@ -5118,7 +5124,7 @@
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="125"/>
+      <c r="B23" s="121"/>
       <c r="C23" s="47"/>
       <c r="D23" s="94" t="s">
         <v>290</v>
@@ -5137,7 +5143,7 @@
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="125"/>
+      <c r="B24" s="121"/>
       <c r="C24" s="47" t="s">
         <v>70</v>
       </c>
@@ -5156,7 +5162,7 @@
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="125"/>
+      <c r="B25" s="121"/>
       <c r="C25" s="47"/>
       <c r="D25" s="94"/>
       <c r="E25" s="47"/>
@@ -5165,7 +5171,7 @@
       <c r="H25" s="47"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="125"/>
+      <c r="B26" s="121"/>
       <c r="C26" s="47"/>
       <c r="D26" s="88"/>
       <c r="E26" s="47"/>
@@ -5174,7 +5180,7 @@
       <c r="H26" s="47"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="125"/>
+      <c r="B27" s="121"/>
       <c r="C27" s="47" t="s">
         <v>254</v>
       </c>
@@ -5195,7 +5201,7 @@
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="125"/>
+      <c r="B28" s="121"/>
       <c r="C28" s="47" t="s">
         <v>253</v>
       </c>
@@ -5216,7 +5222,7 @@
       </c>
     </row>
     <row r="29" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B29" s="125"/>
+      <c r="B29" s="121"/>
       <c r="C29" s="47" t="s">
         <v>255</v>
       </c>
@@ -5237,7 +5243,7 @@
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="125"/>
+      <c r="B30" s="121"/>
       <c r="C30" s="47" t="s">
         <v>256</v>
       </c>
@@ -5258,7 +5264,7 @@
       </c>
     </row>
     <row r="31" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="125"/>
+      <c r="B31" s="121"/>
       <c r="C31" s="72" t="s">
         <v>42</v>
       </c>
@@ -5279,37 +5285,37 @@
       </c>
     </row>
     <row r="32" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="125"/>
-      <c r="C32" s="113" t="s">
+      <c r="B32" s="121"/>
+      <c r="C32" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="113" t="s">
+      <c r="D32" s="114" t="s">
         <v>47</v>
       </c>
-      <c r="E32" s="113" t="s">
+      <c r="E32" s="114" t="s">
         <v>157</v>
       </c>
-      <c r="F32" s="126" t="s">
+      <c r="F32" s="122" t="s">
         <v>158</v>
       </c>
-      <c r="G32" s="126" t="s">
+      <c r="G32" s="122" t="s">
         <v>216</v>
       </c>
-      <c r="H32" s="113" t="s">
+      <c r="H32" s="114" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="125"/>
-      <c r="C33" s="114"/>
-      <c r="D33" s="114"/>
-      <c r="E33" s="114"/>
-      <c r="F33" s="127"/>
-      <c r="G33" s="127"/>
-      <c r="H33" s="114"/>
+      <c r="B33" s="121"/>
+      <c r="C33" s="115"/>
+      <c r="D33" s="115"/>
+      <c r="E33" s="115"/>
+      <c r="F33" s="123"/>
+      <c r="G33" s="123"/>
+      <c r="H33" s="115"/>
     </row>
     <row r="34" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B34" s="125"/>
+      <c r="B34" s="121"/>
       <c r="C34" s="78" t="s">
         <v>250</v>
       </c>
@@ -5330,11 +5336,11 @@
       </c>
     </row>
     <row r="35" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B35" s="125"/>
-      <c r="C35" s="113" t="s">
+      <c r="B35" s="121"/>
+      <c r="C35" s="114" t="s">
         <v>251</v>
       </c>
-      <c r="D35" s="113" t="s">
+      <c r="D35" s="114" t="s">
         <v>160</v>
       </c>
       <c r="E35" s="77" t="s">
@@ -5351,9 +5357,9 @@
       </c>
     </row>
     <row r="36" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B36" s="125"/>
-      <c r="C36" s="114"/>
-      <c r="D36" s="114"/>
+      <c r="B36" s="121"/>
+      <c r="C36" s="115"/>
+      <c r="D36" s="115"/>
       <c r="E36" s="77" t="s">
         <v>163</v>
       </c>
@@ -5368,7 +5374,7 @@
       </c>
     </row>
     <row r="37" spans="2:8" ht="66" x14ac:dyDescent="0.3">
-      <c r="B37" s="125"/>
+      <c r="B37" s="121"/>
       <c r="C37" s="73" t="s">
         <v>252</v>
       </c>
@@ -5389,11 +5395,11 @@
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="125"/>
-      <c r="C38" s="118" t="s">
+      <c r="B38" s="121"/>
+      <c r="C38" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="D38" s="118" t="s">
+      <c r="D38" s="124" t="s">
         <v>45</v>
       </c>
       <c r="E38" s="48" t="s">
@@ -5406,9 +5412,9 @@
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B39" s="125"/>
-      <c r="C39" s="118"/>
-      <c r="D39" s="118"/>
+      <c r="B39" s="121"/>
+      <c r="C39" s="124"/>
+      <c r="D39" s="124"/>
       <c r="E39" s="48" t="s">
         <v>172</v>
       </c>
@@ -5423,11 +5429,11 @@
       </c>
     </row>
     <row r="40" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B40" s="125"/>
-      <c r="C40" s="113" t="s">
+      <c r="B40" s="121"/>
+      <c r="C40" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="D40" s="113" t="s">
+      <c r="D40" s="114" t="s">
         <v>52</v>
       </c>
       <c r="E40" s="72" t="s">
@@ -5444,9 +5450,9 @@
       </c>
     </row>
     <row r="41" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B41" s="125"/>
-      <c r="C41" s="114"/>
-      <c r="D41" s="114"/>
+      <c r="B41" s="121"/>
+      <c r="C41" s="115"/>
+      <c r="D41" s="115"/>
       <c r="E41" s="72" t="s">
         <v>176</v>
       </c>
@@ -5461,7 +5467,7 @@
       </c>
     </row>
     <row r="42" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B42" s="125"/>
+      <c r="B42" s="121"/>
       <c r="C42" s="77" t="s">
         <v>48</v>
       </c>
@@ -5482,11 +5488,11 @@
       </c>
     </row>
     <row r="43" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B43" s="125"/>
-      <c r="C43" s="113" t="s">
+      <c r="B43" s="121"/>
+      <c r="C43" s="114" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="113" t="s">
+      <c r="D43" s="114" t="s">
         <v>50</v>
       </c>
       <c r="E43" s="72" t="s">
@@ -5503,9 +5509,9 @@
       </c>
     </row>
     <row r="44" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B44" s="125"/>
-      <c r="C44" s="114"/>
-      <c r="D44" s="114"/>
+      <c r="B44" s="121"/>
+      <c r="C44" s="115"/>
+      <c r="D44" s="115"/>
       <c r="E44" s="72" t="s">
         <v>196</v>
       </c>
@@ -5520,7 +5526,7 @@
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B45" s="120"/>
+      <c r="B45" s="116"/>
       <c r="C45" s="89"/>
       <c r="D45" s="89" t="s">
         <v>258</v>
@@ -5539,7 +5545,7 @@
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B46" s="120"/>
+      <c r="B46" s="116"/>
       <c r="C46" s="61"/>
       <c r="D46" s="45" t="s">
         <v>56</v>
@@ -5558,7 +5564,7 @@
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B47" s="121"/>
+      <c r="B47" s="117"/>
       <c r="C47" s="45"/>
       <c r="D47" s="64"/>
       <c r="E47" s="89"/>
@@ -5588,34 +5594,34 @@
       <c r="B50" s="62"/>
       <c r="C50" s="64"/>
       <c r="D50" s="64" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E50" s="61" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F50" s="61"/>
       <c r="G50" s="89"/>
       <c r="H50" s="89" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="51" spans="2:8" ht="33" x14ac:dyDescent="0.3">
       <c r="B51" s="93"/>
       <c r="C51" s="64"/>
       <c r="D51" s="64" t="s">
+        <v>297</v>
+      </c>
+      <c r="E51" s="89" t="s">
+        <v>301</v>
+      </c>
+      <c r="F51" s="96" t="s">
+        <v>298</v>
+      </c>
+      <c r="G51" s="89" t="s">
+        <v>302</v>
+      </c>
+      <c r="H51" s="89" t="s">
         <v>300</v>
-      </c>
-      <c r="E51" s="89" t="s">
-        <v>299</v>
-      </c>
-      <c r="F51" s="128" t="s">
-        <v>301</v>
-      </c>
-      <c r="G51" s="89" t="s">
-        <v>295</v>
-      </c>
-      <c r="H51" s="89" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.3">
@@ -5680,6 +5686,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="D4:D7"/>
     <mergeCell ref="H32:H33"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="C40:C41"/>
@@ -5696,13 +5709,6 @@
     <mergeCell ref="D43:D44"/>
     <mergeCell ref="D35:D36"/>
     <mergeCell ref="C35:C36"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="D4:D7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Auto push 2023-03-30 18:01:52.52
</commit_message>
<xml_diff>
--- a/project/CheeYoonMovie.xlsx
+++ b/project/CheeYoonMovie.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="325">
   <si>
     <t>이용자 권한과 기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -450,15 +450,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>영화 수정(개봉예정,상영작,종료)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>인물 등록</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>인물 수정</t>
+    <t xml:space="preserve">user/register.jsp </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>register.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">user/login.jsp </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RegisterService.java</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -466,26 +470,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">user/register.jsp </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>register.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">user/login.jsp </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RegisterService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>loginView.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>userId</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -578,10 +562,6 @@
   </si>
   <si>
     <t>logout.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>modifyView.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1090,22 +1070,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>예고편 리스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>trailerList.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TrailerListService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>movie/trailerList.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>movie/movieRanking.jsp</t>
   </si>
   <si>
@@ -1211,28 +1175,144 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>영화등록처리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MovieDto속성들
-tagDto 여러개</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>insert.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>loginView.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>modifyView.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>findPassword.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user/findPassword.jsp</t>
+  </si>
+  <si>
+    <t>passwordResult.do</t>
+  </si>
+  <si>
+    <t>PasswordResultService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user/passwordResult.jsp</t>
+  </si>
+  <si>
+    <t>userId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InsertService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insertMovie.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MovieDto속성들</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InsertMovie.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insertTag.do</t>
+  </si>
+  <si>
+    <t>insertTrailer.do</t>
+  </si>
+  <si>
+    <t>refreshMovie.do</t>
+  </si>
+  <si>
+    <t>영화 태그 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 예고편 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 새로고침</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InsertTag.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movieId,tag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>insert.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RegisterMovie.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RegisterMovie.java</t>
+    <t>InsertTrailer.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TrailerDto속성들</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RefreshMovie.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>updateMovieView.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UpdateMovieView</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movieId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin/updateMovie.jsp</t>
+  </si>
+  <si>
+    <t>updateMovie.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MovieDto속성들</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UpdateMovie.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1770,7 +1850,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2062,12 +2142,48 @@
     <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2077,39 +2193,6 @@
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2119,6 +2202,21 @@
     <xf numFmtId="0" fontId="11" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2141,21 +2239,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2526,41 +2609,41 @@
     <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="99" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
-      <c r="N2" s="107"/>
-      <c r="O2" s="107"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
+      <c r="N2" s="100"/>
+      <c r="O2" s="100"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="107"/>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="107"/>
-      <c r="O3" s="107"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
@@ -2605,32 +2688,32 @@
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20"/>
-      <c r="C6" s="108" t="s">
+      <c r="C6" s="101" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="38"/>
-      <c r="E6" s="110" t="s">
+      <c r="E6" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="110"/>
-      <c r="J6" s="110"/>
-      <c r="K6" s="111"/>
-      <c r="L6" s="112" t="s">
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="103"/>
+      <c r="J6" s="103"/>
+      <c r="K6" s="104"/>
+      <c r="L6" s="105" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="110"/>
-      <c r="N6" s="110"/>
-      <c r="O6" s="110"/>
+      <c r="M6" s="103"/>
+      <c r="N6" s="103"/>
+      <c r="O6" s="103"/>
       <c r="P6" s="21"/>
       <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="109"/>
+      <c r="C7" s="102"/>
       <c r="D7" s="22"/>
       <c r="E7" s="84">
         <v>20</v>
@@ -2730,7 +2813,7 @@
     <row r="11" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="102" t="s">
+      <c r="C11" s="106" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="10"/>
@@ -2751,7 +2834,7 @@
     <row r="12" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="102"/>
+      <c r="C12" s="106"/>
       <c r="D12" s="10"/>
       <c r="E12" s="8"/>
       <c r="F12" s="6"/>
@@ -2789,7 +2872,7 @@
     <row r="14" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="105" t="s">
+      <c r="C14" s="98" t="s">
         <v>32</v>
       </c>
       <c r="D14" s="10"/>
@@ -2810,7 +2893,7 @@
     <row r="15" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="105"/>
+      <c r="C15" s="98"/>
       <c r="D15" s="10"/>
       <c r="E15" s="8"/>
       <c r="F15" s="6"/>
@@ -2848,7 +2931,7 @@
     <row r="17" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="102" t="s">
+      <c r="C17" s="106" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="10"/>
@@ -2869,7 +2952,7 @@
     <row r="18" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="102"/>
+      <c r="C18" s="106"/>
       <c r="D18" s="10"/>
       <c r="E18" s="8"/>
       <c r="F18" s="6"/>
@@ -2928,8 +3011,8 @@
     <row r="21" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="103" t="s">
-        <v>201</v>
+      <c r="C21" s="108" t="s">
+        <v>196</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="37"/>
@@ -2949,7 +3032,7 @@
     <row r="22" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="103"/>
+      <c r="C22" s="108"/>
       <c r="D22" s="10"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
@@ -2987,7 +3070,7 @@
     <row r="24" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="103" t="s">
+      <c r="C24" s="108" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="10"/>
@@ -3008,7 +3091,7 @@
     <row r="25" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="103"/>
+      <c r="C25" s="108"/>
       <c r="D25" s="10"/>
       <c r="E25" s="6"/>
       <c r="F25" s="8"/>
@@ -3046,7 +3129,7 @@
     <row r="27" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="103" t="s">
+      <c r="C27" s="108" t="s">
         <v>78</v>
       </c>
       <c r="D27" s="10"/>
@@ -3067,7 +3150,7 @@
     <row r="28" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="103"/>
+      <c r="C28" s="108"/>
       <c r="D28" s="10"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -3105,7 +3188,7 @@
     <row r="30" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="103" t="s">
+      <c r="C30" s="108" t="s">
         <v>79</v>
       </c>
       <c r="D30" s="10"/>
@@ -3126,7 +3209,7 @@
     <row r="31" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="103"/>
+      <c r="C31" s="108"/>
       <c r="D31" s="10"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -3164,8 +3247,8 @@
     <row r="33" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="103" t="s">
-        <v>207</v>
+      <c r="C33" s="108" t="s">
+        <v>202</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="6"/>
@@ -3185,7 +3268,7 @@
     <row r="34" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="6"/>
-      <c r="C34" s="103"/>
+      <c r="C34" s="108"/>
       <c r="D34" s="10"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -3223,7 +3306,7 @@
     <row r="36" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="16"/>
       <c r="B36" s="6"/>
-      <c r="C36" s="103" t="s">
+      <c r="C36" s="108" t="s">
         <v>80</v>
       </c>
       <c r="D36" s="10"/>
@@ -3244,7 +3327,7 @@
     <row r="37" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
       <c r="B37" s="6"/>
-      <c r="C37" s="103"/>
+      <c r="C37" s="108"/>
       <c r="D37" s="10"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
@@ -3303,7 +3386,7 @@
     <row r="40" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="6"/>
-      <c r="C40" s="104" t="s">
+      <c r="C40" s="109" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="10"/>
@@ -3324,7 +3407,7 @@
     <row r="41" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="104"/>
+      <c r="C41" s="109"/>
       <c r="D41" s="10"/>
       <c r="E41" s="6"/>
       <c r="F41" s="8"/>
@@ -3362,8 +3445,8 @@
     <row r="43" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="16"/>
       <c r="B43" s="6"/>
-      <c r="C43" s="104" t="s">
-        <v>203</v>
+      <c r="C43" s="109" t="s">
+        <v>198</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="6"/>
@@ -3383,7 +3466,7 @@
     <row r="44" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="104"/>
+      <c r="C44" s="109"/>
       <c r="D44" s="10"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
@@ -3421,8 +3504,8 @@
     <row r="46" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16"/>
       <c r="B46" s="6"/>
-      <c r="C46" s="104" t="s">
-        <v>205</v>
+      <c r="C46" s="109" t="s">
+        <v>200</v>
       </c>
       <c r="D46" s="10"/>
       <c r="E46" s="6"/>
@@ -3441,7 +3524,7 @@
     <row r="47" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="104"/>
+      <c r="C47" s="109"/>
       <c r="D47" s="10"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
@@ -3479,8 +3562,8 @@
     <row r="49" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="16"/>
       <c r="B49" s="6"/>
-      <c r="C49" s="104" t="s">
-        <v>283</v>
+      <c r="C49" s="109" t="s">
+        <v>274</v>
       </c>
       <c r="D49" s="10"/>
       <c r="E49" s="6"/>
@@ -3500,7 +3583,7 @@
     <row r="50" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="104"/>
+      <c r="C50" s="109"/>
       <c r="D50" s="10"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
@@ -3538,8 +3621,8 @@
     <row r="52" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="16"/>
       <c r="B52" s="6"/>
-      <c r="C52" s="104" t="s">
-        <v>282</v>
+      <c r="C52" s="109" t="s">
+        <v>273</v>
       </c>
       <c r="D52" s="10"/>
       <c r="E52" s="6"/>
@@ -3559,7 +3642,7 @@
     <row r="53" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16"/>
       <c r="B53" s="6"/>
-      <c r="C53" s="104"/>
+      <c r="C53" s="109"/>
       <c r="D53" s="10"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
@@ -3597,8 +3680,8 @@
     <row r="55" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="104" t="s">
-        <v>206</v>
+      <c r="C55" s="109" t="s">
+        <v>201</v>
       </c>
       <c r="D55" s="10"/>
       <c r="E55" s="6"/>
@@ -3617,7 +3700,7 @@
     <row r="56" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="16"/>
       <c r="B56" s="6"/>
-      <c r="C56" s="104"/>
+      <c r="C56" s="109"/>
       <c r="D56" s="10"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
@@ -3655,8 +3738,8 @@
     <row r="58" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="104" t="s">
-        <v>204</v>
+      <c r="C58" s="109" t="s">
+        <v>199</v>
       </c>
       <c r="D58" s="10"/>
       <c r="E58" s="6"/>
@@ -3676,7 +3759,7 @@
     <row r="59" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="16"/>
       <c r="B59" s="6"/>
-      <c r="C59" s="104"/>
+      <c r="C59" s="109"/>
       <c r="D59" s="10"/>
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
@@ -3714,8 +3797,8 @@
     <row r="61" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="16"/>
       <c r="B61" s="6"/>
-      <c r="C61" s="104" t="s">
-        <v>284</v>
+      <c r="C61" s="109" t="s">
+        <v>275</v>
       </c>
       <c r="D61" s="10"/>
       <c r="E61" s="6"/>
@@ -3735,7 +3818,7 @@
     <row r="62" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="16"/>
       <c r="B62" s="6"/>
-      <c r="C62" s="104"/>
+      <c r="C62" s="109"/>
       <c r="D62" s="10"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
@@ -3794,8 +3877,8 @@
     <row r="65" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="16"/>
       <c r="B65" s="6"/>
-      <c r="C65" s="98" t="s">
-        <v>285</v>
+      <c r="C65" s="107" t="s">
+        <v>276</v>
       </c>
       <c r="D65" s="10"/>
       <c r="E65" s="6"/>
@@ -3815,7 +3898,7 @@
     <row r="66" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="16"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="98"/>
+      <c r="C66" s="107"/>
       <c r="D66" s="10"/>
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
@@ -3853,8 +3936,8 @@
     <row r="68" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="16"/>
       <c r="B68" s="6"/>
-      <c r="C68" s="98" t="s">
-        <v>286</v>
+      <c r="C68" s="107" t="s">
+        <v>277</v>
       </c>
       <c r="D68" s="10"/>
       <c r="E68" s="6"/>
@@ -3874,7 +3957,7 @@
     <row r="69" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="98"/>
+      <c r="C69" s="107"/>
       <c r="D69" s="10"/>
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
@@ -3912,8 +3995,8 @@
     <row r="71" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="16"/>
       <c r="B71" s="6"/>
-      <c r="C71" s="98" t="s">
-        <v>287</v>
+      <c r="C71" s="107" t="s">
+        <v>278</v>
       </c>
       <c r="D71" s="10"/>
       <c r="E71" s="6"/>
@@ -3933,7 +4016,7 @@
     <row r="72" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16"/>
       <c r="B72" s="6"/>
-      <c r="C72" s="98"/>
+      <c r="C72" s="107"/>
       <c r="D72" s="10"/>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
@@ -3971,8 +4054,8 @@
     <row r="74" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16"/>
       <c r="B74" s="6"/>
-      <c r="C74" s="98" t="s">
-        <v>288</v>
+      <c r="C74" s="107" t="s">
+        <v>279</v>
       </c>
       <c r="D74" s="10"/>
       <c r="E74" s="6"/>
@@ -3992,7 +4075,7 @@
     <row r="75" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="16"/>
       <c r="B75" s="6"/>
-      <c r="C75" s="98"/>
+      <c r="C75" s="107"/>
       <c r="D75" s="10"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
@@ -4030,7 +4113,7 @@
     <row r="77" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="16"/>
       <c r="B77" s="6"/>
-      <c r="C77" s="99" t="s">
+      <c r="C77" s="111" t="s">
         <v>53</v>
       </c>
       <c r="D77" s="7"/>
@@ -4051,7 +4134,7 @@
     <row r="78" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="16"/>
       <c r="B78" s="6"/>
-      <c r="C78" s="99"/>
+      <c r="C78" s="111"/>
       <c r="D78" s="7"/>
       <c r="E78" s="6"/>
       <c r="F78" s="6"/>
@@ -4070,7 +4153,7 @@
     <row r="79" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="16"/>
       <c r="B79" s="6"/>
-      <c r="C79" s="101" t="s">
+      <c r="C79" s="113" t="s">
         <v>76</v>
       </c>
       <c r="D79" s="7"/>
@@ -4141,7 +4224,7 @@
     <row r="80" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="16"/>
       <c r="B80" s="6"/>
-      <c r="C80" s="101"/>
+      <c r="C80" s="113"/>
       <c r="D80" s="7"/>
       <c r="E80" s="6"/>
       <c r="F80" s="6"/>
@@ -4269,18 +4352,18 @@
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5"/>
-      <c r="F84" s="100"/>
-      <c r="G84" s="100"/>
+      <c r="F84" s="112"/>
+      <c r="G84" s="112"/>
       <c r="H84" s="6"/>
       <c r="I84" s="37" t="s">
         <v>55</v>
       </c>
       <c r="J84" s="37"/>
       <c r="K84" s="6"/>
-      <c r="L84" s="97" t="s">
+      <c r="L84" s="110" t="s">
         <v>54</v>
       </c>
-      <c r="M84" s="97"/>
+      <c r="M84" s="110"/>
       <c r="N84" s="39"/>
       <c r="O84" s="5"/>
       <c r="P84" s="5"/>
@@ -4306,62 +4389,62 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C87" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C88" s="4" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C89" s="4" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C90" s="82" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C91" s="82" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C92" s="82" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C93" s="82" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C94" s="82" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C95" s="82" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C96" s="82" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C97" s="82" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C98" s="82" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.3">
@@ -4387,12 +4470,13 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B2:O3"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="E6:K6"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="L84:M84"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="C79:C80"/>
     <mergeCell ref="C65:C66"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C21:C22"/>
@@ -4409,13 +4493,12 @@
     <mergeCell ref="C58:C59"/>
     <mergeCell ref="C33:C34"/>
     <mergeCell ref="C61:C62"/>
-    <mergeCell ref="L84:M84"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B2:O3"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="C11:C12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4446,7 +4529,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="113" t="s">
+      <c r="A3" s="114" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -4456,7 +4539,7 @@
       <c r="D3" s="57"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="113"/>
+      <c r="A4" s="114"/>
       <c r="B4" s="1" t="s">
         <v>83</v>
       </c>
@@ -4471,7 +4554,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="113"/>
+      <c r="A5" s="114"/>
       <c r="B5" s="1" t="s">
         <v>84</v>
       </c>
@@ -4544,7 +4627,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C1" s="68"/>
     </row>
@@ -4560,7 +4643,7 @@
       </c>
       <c r="C3" s="58"/>
       <c r="E3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -4570,42 +4653,42 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C5" s="65"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C6" s="66"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C7" s="67"/>
       <c r="E7" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C10" s="69"/>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C11" s="70"/>
       <c r="D11">
@@ -4614,7 +4697,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C12" s="71"/>
       <c r="D12">
@@ -4623,7 +4706,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C13" s="67"/>
       <c r="D13">
@@ -4632,7 +4715,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -4640,7 +4723,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -4751,10 +4834,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H57"/>
+  <dimension ref="B2:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4792,7 +4875,7 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="125" t="s">
+      <c r="B3" s="117" t="s">
         <v>39</v>
       </c>
       <c r="C3" s="43" t="s">
@@ -4806,78 +4889,78 @@
       </c>
       <c r="F3" s="44"/>
       <c r="G3" s="44" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="H3" s="44" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="126"/>
-      <c r="C4" s="128" t="s">
+      <c r="B4" s="118"/>
+      <c r="C4" s="121" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="128" t="s">
+      <c r="D4" s="121" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="44" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F4" s="44"/>
       <c r="G4" s="44"/>
       <c r="H4" s="44" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="126"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="126"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
       <c r="E5" s="44" t="s">
         <v>102</v>
       </c>
       <c r="F5" s="44" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G5" s="44" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H5" s="44" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="126"/>
-      <c r="C6" s="126"/>
-      <c r="D6" s="126"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
       <c r="E6" s="44" t="s">
         <v>103</v>
       </c>
       <c r="F6" s="44" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G6" s="44" t="s">
         <v>105</v>
       </c>
       <c r="H6" s="44" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="127"/>
-      <c r="C7" s="127"/>
-      <c r="D7" s="127"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119"/>
       <c r="E7" s="44" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F7" s="44" t="s">
         <v>100</v>
       </c>
       <c r="G7" s="44" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H7" s="44" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
@@ -4889,105 +4972,105 @@
         <v>107</v>
       </c>
       <c r="E8" s="44" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F8" s="44" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G8" s="44" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="H8" s="44" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="63"/>
       <c r="C9" s="80"/>
       <c r="D9" s="80" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="F9" s="44"/>
       <c r="G9" s="44" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H9" s="44" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="79"/>
       <c r="C10" s="80"/>
       <c r="D10" s="83" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E10" s="44" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F10" s="44"/>
       <c r="G10" s="44" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H10" s="44" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="79"/>
       <c r="C11" s="80"/>
       <c r="D11" s="80" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E11" s="44" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F11" s="44" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G11" s="44" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="H11" s="44" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="86"/>
       <c r="C12" s="87"/>
       <c r="D12" s="92" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="E12" s="44" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="F12" s="44" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="G12" s="44" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="H12" s="44" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="91"/>
       <c r="C13" s="92"/>
       <c r="D13" s="87" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="E13" s="44" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="F13" s="44"/>
       <c r="G13" s="44" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="H13" s="44" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
@@ -5011,19 +5094,11 @@
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="79"/>
       <c r="C16" s="80"/>
-      <c r="D16" s="87" t="s">
-        <v>266</v>
-      </c>
-      <c r="E16" s="44" t="s">
-        <v>267</v>
-      </c>
+      <c r="D16" s="87"/>
+      <c r="E16" s="44"/>
       <c r="F16" s="44"/>
-      <c r="G16" s="44" t="s">
-        <v>268</v>
-      </c>
-      <c r="H16" s="44" t="s">
-        <v>269</v>
-      </c>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="55"/>
@@ -5035,28 +5110,28 @@
       <c r="H17" s="44"/>
     </row>
     <row r="18" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="120" t="s">
+      <c r="B18" s="126" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="118" t="s">
+      <c r="C18" s="124" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="118" t="s">
+      <c r="D18" s="124" t="s">
         <v>63</v>
       </c>
       <c r="E18" s="46" t="s">
-        <v>112</v>
+        <v>289</v>
       </c>
       <c r="F18" s="46"/>
       <c r="G18" s="46"/>
       <c r="H18" s="46" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="121"/>
-      <c r="C19" s="119"/>
-      <c r="D19" s="119"/>
+      <c r="B19" s="127"/>
+      <c r="C19" s="125"/>
+      <c r="D19" s="125"/>
       <c r="E19" s="46" t="s">
         <v>64</v>
       </c>
@@ -5064,616 +5139,674 @@
         <v>108</v>
       </c>
       <c r="G19" s="46" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H19" s="47" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="121"/>
-      <c r="C20" s="46" t="s">
+      <c r="B20" s="127"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="97" t="s">
+        <v>297</v>
+      </c>
+      <c r="E20" s="47" t="s">
+        <v>291</v>
+      </c>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="127"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="97" t="s">
+        <v>298</v>
+      </c>
+      <c r="E21" s="47" t="s">
+        <v>293</v>
+      </c>
+      <c r="F21" s="47" t="s">
+        <v>296</v>
+      </c>
+      <c r="G21" s="47" t="s">
+        <v>294</v>
+      </c>
+      <c r="H21" s="47" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="127"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="127"/>
+      <c r="C23" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="46" t="s">
+      <c r="D23" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="46" t="s">
+      <c r="E23" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="H23" s="47" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="127"/>
+      <c r="C24" s="124" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="124" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="46" t="s">
+        <v>290</v>
+      </c>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="127"/>
+      <c r="C25" s="125"/>
+      <c r="D25" s="125"/>
+      <c r="E25" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="F25" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="G25" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="H25" s="46" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="127"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="94" t="s">
+        <v>281</v>
+      </c>
+      <c r="E26" s="47" t="s">
+        <v>283</v>
+      </c>
+      <c r="F26" s="47" t="s">
+        <v>282</v>
+      </c>
+      <c r="G26" s="47" t="s">
+        <v>284</v>
+      </c>
+      <c r="H26" s="47" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="127"/>
+      <c r="C27" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46" t="s">
-        <v>137</v>
-      </c>
-      <c r="H20" s="47" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="121"/>
-      <c r="C21" s="118" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="118" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" s="46" t="s">
-        <v>142</v>
-      </c>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="121"/>
-      <c r="C22" s="119"/>
-      <c r="D22" s="119"/>
-      <c r="E22" s="46" t="s">
+      <c r="H27" s="47" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="127"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="94"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="47"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="127"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="88"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="127"/>
+      <c r="C30" s="47" t="s">
+        <v>249</v>
+      </c>
+      <c r="D30" s="88" t="s">
+        <v>222</v>
+      </c>
+      <c r="E30" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="F30" s="47" t="s">
+        <v>223</v>
+      </c>
+      <c r="G30" s="47" t="s">
+        <v>225</v>
+      </c>
+      <c r="H30" s="47" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="127"/>
+      <c r="C31" s="47" t="s">
+        <v>248</v>
+      </c>
+      <c r="D31" s="88" t="s">
+        <v>231</v>
+      </c>
+      <c r="E31" s="47" t="s">
+        <v>227</v>
+      </c>
+      <c r="F31" s="47" t="s">
+        <v>232</v>
+      </c>
+      <c r="G31" s="47" t="s">
+        <v>228</v>
+      </c>
+      <c r="H31" s="47" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B32" s="127"/>
+      <c r="C32" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="D32" s="88" t="s">
+        <v>230</v>
+      </c>
+      <c r="E32" s="47" t="s">
+        <v>233</v>
+      </c>
+      <c r="F32" s="90" t="s">
+        <v>235</v>
+      </c>
+      <c r="G32" s="47" t="s">
+        <v>234</v>
+      </c>
+      <c r="H32" s="47" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33" s="127"/>
+      <c r="C33" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="D33" s="47" t="s">
+        <v>244</v>
+      </c>
+      <c r="E33" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="F33" s="47" t="s">
+        <v>237</v>
+      </c>
+      <c r="G33" s="47" t="s">
+        <v>238</v>
+      </c>
+      <c r="H33" s="47" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="127"/>
+      <c r="C34" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="72" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="72" t="s">
+        <v>258</v>
+      </c>
+      <c r="F34" s="72" t="s">
+        <v>145</v>
+      </c>
+      <c r="G34" s="72" t="s">
         <v>144</v>
       </c>
-      <c r="F22" s="47" t="s">
-        <v>138</v>
-      </c>
-      <c r="G22" s="46" t="s">
-        <v>145</v>
-      </c>
-      <c r="H22" s="46" t="s">
+      <c r="H34" s="72" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="121"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="94" t="s">
-        <v>290</v>
-      </c>
-      <c r="E23" s="47" t="s">
-        <v>292</v>
-      </c>
-      <c r="F23" s="47" t="s">
-        <v>291</v>
-      </c>
-      <c r="G23" s="47" t="s">
-        <v>293</v>
-      </c>
-      <c r="H23" s="47" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="121"/>
-      <c r="C24" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="47" t="s">
-        <v>257</v>
-      </c>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47" t="s">
+    <row r="35" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="127"/>
+      <c r="C35" s="115" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="115" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" s="115" t="s">
+        <v>152</v>
+      </c>
+      <c r="F35" s="128" t="s">
+        <v>153</v>
+      </c>
+      <c r="G35" s="128" t="s">
+        <v>211</v>
+      </c>
+      <c r="H35" s="115" t="s">
         <v>146</v>
       </c>
-      <c r="H24" s="47" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="121"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="94"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="121"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="121"/>
-      <c r="C27" s="47" t="s">
-        <v>254</v>
-      </c>
-      <c r="D27" s="88" t="s">
-        <v>227</v>
-      </c>
-      <c r="E27" s="47" t="s">
-        <v>229</v>
-      </c>
-      <c r="F27" s="47" t="s">
-        <v>228</v>
-      </c>
-      <c r="G27" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="H27" s="47" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="121"/>
-      <c r="C28" s="47" t="s">
-        <v>253</v>
-      </c>
-      <c r="D28" s="88" t="s">
-        <v>236</v>
-      </c>
-      <c r="E28" s="47" t="s">
-        <v>232</v>
-      </c>
-      <c r="F28" s="47" t="s">
-        <v>237</v>
-      </c>
-      <c r="G28" s="47" t="s">
-        <v>233</v>
-      </c>
-      <c r="H28" s="47" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B29" s="121"/>
-      <c r="C29" s="47" t="s">
-        <v>255</v>
-      </c>
-      <c r="D29" s="88" t="s">
-        <v>235</v>
-      </c>
-      <c r="E29" s="47" t="s">
-        <v>238</v>
-      </c>
-      <c r="F29" s="90" t="s">
-        <v>240</v>
-      </c>
-      <c r="G29" s="47" t="s">
-        <v>239</v>
-      </c>
-      <c r="H29" s="47" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="121"/>
-      <c r="C30" s="47" t="s">
-        <v>256</v>
-      </c>
-      <c r="D30" s="47" t="s">
-        <v>249</v>
-      </c>
-      <c r="E30" s="47" t="s">
-        <v>241</v>
-      </c>
-      <c r="F30" s="47" t="s">
-        <v>242</v>
-      </c>
-      <c r="G30" s="47" t="s">
-        <v>243</v>
-      </c>
-      <c r="H30" s="47" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="121"/>
-      <c r="C31" s="72" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="72" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="72" t="s">
-        <v>263</v>
-      </c>
-      <c r="F31" s="72" t="s">
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" s="127"/>
+      <c r="C36" s="116"/>
+      <c r="D36" s="116"/>
+      <c r="E36" s="116"/>
+      <c r="F36" s="129"/>
+      <c r="G36" s="129"/>
+      <c r="H36" s="116"/>
+    </row>
+    <row r="37" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B37" s="127"/>
+      <c r="C37" s="78" t="s">
+        <v>245</v>
+      </c>
+      <c r="D37" s="76" t="s">
+        <v>149</v>
+      </c>
+      <c r="E37" s="75" t="s">
         <v>150</v>
       </c>
-      <c r="G31" s="72" t="s">
-        <v>149</v>
-      </c>
-      <c r="H31" s="72" t="s">
+      <c r="F37" s="74" t="s">
+        <v>184</v>
+      </c>
+      <c r="G37" s="75" t="s">
+        <v>151</v>
+      </c>
+      <c r="H37" s="75" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="121"/>
-      <c r="C32" s="114" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="114" t="s">
-        <v>47</v>
-      </c>
-      <c r="E32" s="114" t="s">
+    <row r="38" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B38" s="127"/>
+      <c r="C38" s="115" t="s">
+        <v>246</v>
+      </c>
+      <c r="D38" s="115" t="s">
+        <v>155</v>
+      </c>
+      <c r="E38" s="77" t="s">
+        <v>156</v>
+      </c>
+      <c r="F38" s="74" t="s">
+        <v>182</v>
+      </c>
+      <c r="G38" s="75" t="s">
+        <v>161</v>
+      </c>
+      <c r="H38" s="72" t="s">
         <v>157</v>
       </c>
-      <c r="F32" s="122" t="s">
+    </row>
+    <row r="39" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B39" s="127"/>
+      <c r="C39" s="116"/>
+      <c r="D39" s="116"/>
+      <c r="E39" s="77" t="s">
         <v>158</v>
       </c>
-      <c r="G32" s="122" t="s">
-        <v>216</v>
-      </c>
-      <c r="H32" s="114" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="121"/>
-      <c r="C33" s="115"/>
-      <c r="D33" s="115"/>
-      <c r="E33" s="115"/>
-      <c r="F33" s="123"/>
-      <c r="G33" s="123"/>
-      <c r="H33" s="115"/>
-    </row>
-    <row r="34" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B34" s="121"/>
-      <c r="C34" s="78" t="s">
-        <v>250</v>
-      </c>
-      <c r="D34" s="76" t="s">
+      <c r="F39" s="74" t="s">
+        <v>183</v>
+      </c>
+      <c r="G39" s="75" t="s">
+        <v>159</v>
+      </c>
+      <c r="H39" s="75" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="B40" s="127"/>
+      <c r="C40" s="73" t="s">
+        <v>247</v>
+      </c>
+      <c r="D40" s="78" t="s">
         <v>154</v>
       </c>
-      <c r="E34" s="75" t="s">
-        <v>155</v>
-      </c>
-      <c r="F34" s="74" t="s">
-        <v>189</v>
-      </c>
-      <c r="G34" s="75" t="s">
-        <v>156</v>
-      </c>
-      <c r="H34" s="75" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B35" s="121"/>
-      <c r="C35" s="114" t="s">
-        <v>251</v>
-      </c>
-      <c r="D35" s="114" t="s">
-        <v>160</v>
-      </c>
-      <c r="E35" s="77" t="s">
-        <v>161</v>
-      </c>
-      <c r="F35" s="74" t="s">
-        <v>187</v>
-      </c>
-      <c r="G35" s="75" t="s">
-        <v>166</v>
-      </c>
-      <c r="H35" s="72" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B36" s="121"/>
-      <c r="C36" s="115"/>
-      <c r="D36" s="115"/>
-      <c r="E36" s="77" t="s">
-        <v>163</v>
-      </c>
-      <c r="F36" s="74" t="s">
-        <v>188</v>
-      </c>
-      <c r="G36" s="75" t="s">
+      <c r="E40" s="77" t="s">
         <v>164</v>
-      </c>
-      <c r="H36" s="75" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" ht="66" x14ac:dyDescent="0.3">
-      <c r="B37" s="121"/>
-      <c r="C37" s="73" t="s">
-        <v>252</v>
-      </c>
-      <c r="D37" s="78" t="s">
-        <v>159</v>
-      </c>
-      <c r="E37" s="77" t="s">
-        <v>169</v>
-      </c>
-      <c r="F37" s="74" t="s">
-        <v>186</v>
-      </c>
-      <c r="G37" s="77" t="s">
-        <v>170</v>
-      </c>
-      <c r="H37" s="77" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="121"/>
-      <c r="C38" s="124" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" s="124" t="s">
-        <v>45</v>
-      </c>
-      <c r="E38" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="F38" s="48"/>
-      <c r="G38" s="49"/>
-      <c r="H38" s="48" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B39" s="121"/>
-      <c r="C39" s="124"/>
-      <c r="D39" s="124"/>
-      <c r="E39" s="48" t="s">
-        <v>172</v>
-      </c>
-      <c r="F39" s="74" t="s">
-        <v>184</v>
-      </c>
-      <c r="G39" s="48" t="s">
-        <v>173</v>
-      </c>
-      <c r="H39" s="48" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B40" s="121"/>
-      <c r="C40" s="114" t="s">
-        <v>44</v>
-      </c>
-      <c r="D40" s="114" t="s">
-        <v>52</v>
-      </c>
-      <c r="E40" s="72" t="s">
-        <v>174</v>
       </c>
       <c r="F40" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="G40" s="72" t="s">
+      <c r="G40" s="77" t="s">
+        <v>165</v>
+      </c>
+      <c r="H40" s="77" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B41" s="127"/>
+      <c r="C41" s="120" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" s="120" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="F41" s="48"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="48" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" s="127"/>
+      <c r="C42" s="120"/>
+      <c r="D42" s="120"/>
+      <c r="E42" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="F42" s="74" t="s">
+        <v>179</v>
+      </c>
+      <c r="G42" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="H42" s="48" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B43" s="127"/>
+      <c r="C43" s="115" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" s="115" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" s="72" t="s">
+        <v>169</v>
+      </c>
+      <c r="F43" s="74" t="s">
+        <v>176</v>
+      </c>
+      <c r="G43" s="72" t="s">
+        <v>170</v>
+      </c>
+      <c r="H43" s="72" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B44" s="127"/>
+      <c r="C44" s="116"/>
+      <c r="D44" s="116"/>
+      <c r="E44" s="72" t="s">
+        <v>171</v>
+      </c>
+      <c r="F44" s="74" t="s">
+        <v>177</v>
+      </c>
+      <c r="G44" s="72" t="s">
         <v>175</v>
       </c>
-      <c r="H40" s="72" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B41" s="121"/>
-      <c r="C41" s="115"/>
-      <c r="D41" s="115"/>
-      <c r="E41" s="72" t="s">
-        <v>176</v>
-      </c>
-      <c r="F41" s="74" t="s">
-        <v>182</v>
-      </c>
-      <c r="G41" s="72" t="s">
+      <c r="H44" s="72" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B45" s="127"/>
+      <c r="C45" s="77" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="77" t="s">
+        <v>51</v>
+      </c>
+      <c r="E45" s="77" t="s">
+        <v>72</v>
+      </c>
+      <c r="F45" s="74" t="s">
+        <v>178</v>
+      </c>
+      <c r="G45" s="77" t="s">
         <v>180</v>
       </c>
-      <c r="H41" s="72" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B42" s="121"/>
-      <c r="C42" s="77" t="s">
-        <v>48</v>
-      </c>
-      <c r="D42" s="77" t="s">
-        <v>51</v>
-      </c>
-      <c r="E42" s="77" t="s">
-        <v>72</v>
-      </c>
-      <c r="F42" s="74" t="s">
-        <v>183</v>
-      </c>
-      <c r="G42" s="77" t="s">
+      <c r="H45" s="77" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B46" s="127"/>
+      <c r="C46" s="115" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="115" t="s">
+        <v>50</v>
+      </c>
+      <c r="E46" s="72" t="s">
         <v>185</v>
       </c>
-      <c r="H42" s="77" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B43" s="121"/>
-      <c r="C43" s="114" t="s">
-        <v>49</v>
-      </c>
-      <c r="D43" s="114" t="s">
-        <v>50</v>
-      </c>
-      <c r="E43" s="72" t="s">
+      <c r="F46" s="74" t="s">
         <v>190</v>
       </c>
-      <c r="F43" s="74" t="s">
-        <v>195</v>
-      </c>
-      <c r="G43" s="72" t="s">
-        <v>194</v>
-      </c>
-      <c r="H43" s="72" t="s">
+      <c r="G46" s="72" t="s">
+        <v>189</v>
+      </c>
+      <c r="H46" s="72" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B47" s="127"/>
+      <c r="C47" s="116"/>
+      <c r="D47" s="116"/>
+      <c r="E47" s="72" t="s">
+        <v>191</v>
+      </c>
+      <c r="F47" s="74" t="s">
+        <v>186</v>
+      </c>
+      <c r="G47" s="72" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="44" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B44" s="121"/>
-      <c r="C44" s="115"/>
-      <c r="D44" s="115"/>
-      <c r="E44" s="72" t="s">
-        <v>196</v>
-      </c>
-      <c r="F44" s="74" t="s">
-        <v>191</v>
-      </c>
-      <c r="G44" s="72" t="s">
-        <v>197</v>
-      </c>
-      <c r="H44" s="72" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B45" s="116"/>
-      <c r="C45" s="89"/>
-      <c r="D45" s="89" t="s">
-        <v>258</v>
-      </c>
-      <c r="E45" s="45" t="s">
+      <c r="H47" s="72" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B48" s="122"/>
+      <c r="C48" s="89"/>
+      <c r="D48" s="89" t="s">
+        <v>253</v>
+      </c>
+      <c r="E48" s="45" t="s">
+        <v>254</v>
+      </c>
+      <c r="F48" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="G48" s="45" t="s">
+        <v>255</v>
+      </c>
+      <c r="H48" s="45" t="s">
         <v>259</v>
       </c>
-      <c r="F45" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="G45" s="45" t="s">
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B49" s="122"/>
+      <c r="C49" s="61"/>
+      <c r="D49" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="E49" s="89" t="s">
+        <v>256</v>
+      </c>
+      <c r="F49" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="G49" s="45" t="s">
+        <v>257</v>
+      </c>
+      <c r="H49" s="45" t="s">
         <v>260</v>
       </c>
-      <c r="H45" s="45" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B46" s="116"/>
-      <c r="C46" s="61"/>
-      <c r="D46" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="E46" s="89" t="s">
-        <v>261</v>
-      </c>
-      <c r="F46" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="G46" s="45" t="s">
-        <v>262</v>
-      </c>
-      <c r="H46" s="45" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B47" s="117"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="64"/>
-      <c r="E47" s="89"/>
-      <c r="F47" s="89"/>
-      <c r="G47" s="89"/>
-      <c r="H47" s="89"/>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B48" s="62"/>
-      <c r="C48" s="64"/>
-      <c r="D48" s="64"/>
-      <c r="E48" s="61"/>
-      <c r="F48" s="61"/>
-      <c r="G48" s="61"/>
-      <c r="H48" s="61"/>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B49" s="93"/>
-      <c r="C49" s="64"/>
-      <c r="D49" s="64"/>
-      <c r="E49" s="89"/>
-      <c r="F49" s="89"/>
-      <c r="G49" s="89"/>
-      <c r="H49" s="89"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B50" s="62"/>
-      <c r="C50" s="64"/>
+      <c r="B50" s="123"/>
+      <c r="C50" s="45"/>
       <c r="D50" s="64" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="E50" s="61" t="s">
+        <v>288</v>
+      </c>
+      <c r="F50" s="61"/>
+      <c r="G50" s="89" t="s">
         <v>299</v>
       </c>
-      <c r="F50" s="61"/>
-      <c r="G50" s="89"/>
       <c r="H50" s="89" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B51" s="93"/>
+        <v>287</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B51" s="62"/>
       <c r="C51" s="64"/>
       <c r="D51" s="64" t="s">
-        <v>297</v>
+        <v>308</v>
       </c>
       <c r="E51" s="89" t="s">
+        <v>300</v>
+      </c>
+      <c r="F51" s="96" t="s">
         <v>301</v>
-      </c>
-      <c r="F51" s="96" t="s">
-        <v>298</v>
       </c>
       <c r="G51" s="89" t="s">
         <v>302</v>
       </c>
       <c r="H51" s="89" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B52" s="93"/>
       <c r="C52" s="64"/>
-      <c r="D52" s="64"/>
-      <c r="E52" s="89"/>
-      <c r="F52" s="89"/>
-      <c r="G52" s="89"/>
-      <c r="H52" s="89"/>
+      <c r="D52" s="64" t="s">
+        <v>306</v>
+      </c>
+      <c r="E52" s="89" t="s">
+        <v>303</v>
+      </c>
+      <c r="F52" s="89" t="s">
+        <v>311</v>
+      </c>
+      <c r="G52" s="89" t="s">
+        <v>310</v>
+      </c>
+      <c r="H52" s="89" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B53" s="93"/>
+      <c r="B53" s="62"/>
       <c r="C53" s="64"/>
-      <c r="D53" s="64"/>
-      <c r="E53" s="89"/>
-      <c r="F53" s="89"/>
-      <c r="G53" s="89"/>
-      <c r="H53" s="89"/>
+      <c r="D53" s="64" t="s">
+        <v>307</v>
+      </c>
+      <c r="E53" s="89" t="s">
+        <v>304</v>
+      </c>
+      <c r="F53" s="89" t="s">
+        <v>314</v>
+      </c>
+      <c r="G53" s="89" t="s">
+        <v>313</v>
+      </c>
+      <c r="H53" s="89" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B54" s="62"/>
+      <c r="B54" s="93"/>
       <c r="C54" s="64"/>
       <c r="D54" s="64" t="s">
-        <v>109</v>
-      </c>
-      <c r="E54" s="61"/>
-      <c r="F54" s="61"/>
-      <c r="G54" s="61"/>
-      <c r="H54" s="61"/>
+        <v>309</v>
+      </c>
+      <c r="E54" s="89" t="s">
+        <v>305</v>
+      </c>
+      <c r="F54" s="89"/>
+      <c r="G54" s="89" t="s">
+        <v>315</v>
+      </c>
+      <c r="H54" s="89" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B55" s="62"/>
+      <c r="B55" s="93"/>
       <c r="C55" s="64"/>
       <c r="D55" s="64" t="s">
-        <v>110</v>
-      </c>
-      <c r="E55" s="61"/>
-      <c r="F55" s="61"/>
-      <c r="G55" s="61"/>
-      <c r="H55" s="61"/>
+        <v>316</v>
+      </c>
+      <c r="E55" s="89" t="s">
+        <v>317</v>
+      </c>
+      <c r="F55" s="89" t="s">
+        <v>319</v>
+      </c>
+      <c r="G55" s="89" t="s">
+        <v>318</v>
+      </c>
+      <c r="H55" s="89" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B56" s="62"/>
+      <c r="B56" s="93"/>
       <c r="C56" s="64"/>
-      <c r="D56" s="64" t="s">
-        <v>111</v>
-      </c>
-      <c r="E56" s="61"/>
-      <c r="F56" s="61"/>
-      <c r="G56" s="61"/>
-      <c r="H56" s="61"/>
+      <c r="D56" s="64"/>
+      <c r="E56" s="89" t="s">
+        <v>321</v>
+      </c>
+      <c r="F56" s="89" t="s">
+        <v>322</v>
+      </c>
+      <c r="G56" s="89" t="s">
+        <v>323</v>
+      </c>
+      <c r="H56" s="89" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B57" s="62"/>
@@ -5684,31 +5817,58 @@
       <c r="G57" s="61"/>
       <c r="H57" s="61"/>
     </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B58" s="62"/>
+      <c r="C58" s="64"/>
+      <c r="D58" s="64"/>
+      <c r="E58" s="61"/>
+      <c r="F58" s="61"/>
+      <c r="G58" s="61"/>
+      <c r="H58" s="61"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B59" s="62"/>
+      <c r="C59" s="64"/>
+      <c r="D59" s="64"/>
+      <c r="E59" s="61"/>
+      <c r="F59" s="61"/>
+      <c r="G59" s="61"/>
+      <c r="H59" s="61"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B60" s="62"/>
+      <c r="C60" s="64"/>
+      <c r="D60" s="64"/>
+      <c r="E60" s="61"/>
+      <c r="F60" s="61"/>
+      <c r="G60" s="61"/>
+      <c r="H60" s="61"/>
+    </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B18:B47"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="C35:C36"/>
     <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C41:C42"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="D4:D7"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="B18:B44"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="C35:C36"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>